<commit_message>
Added Group 34's (BotII) requirements to the spreadsheet
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D5FC9DF-D770-4083-83A8-0CCEE3BAA020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlbea\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F6E724-2CB7-496C-9C74-D7BD6635FE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Tested By</t>
   </si>
@@ -76,9 +81,6 @@
   </si>
   <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t>Text</t>
   </si>
   <si>
     <t>Implemented In</t>
@@ -105,13 +107,124 @@
   </si>
   <si>
     <t>cut and paste the screenshot of each page in this part of the spreadsheet, please. use as much space is needed.</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>BOT II shall return a list of game move(s) to game manager</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.sendMove</t>
+  </si>
+  <si>
+    <t>Bot II shall receive the game board from the gamemanger</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.requestMove</t>
+  </si>
+  <si>
+    <t>Bot II shall implement a fixed strategy against either BotI or person to determine what move(s) should be made</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.implementBotStrategy</t>
+  </si>
+  <si>
+    <t>Bot II shall be able to capture pieces</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.implement BotStrategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot II shall follow game rules of checkers according to  https://en.wikipedia.org/wiki/English_draughts </t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.determineMoves</t>
+  </si>
+  <si>
+    <t>BotII shall be able to make one or more moves on the given game board/state</t>
+  </si>
+  <si>
+    <t>Bot II shall be given a request to make its move and return its move within the same function call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot II shall evaluate multiple different moves </t>
+  </si>
+  <si>
+    <t>BotII shall be able to play against BotI with the same interface</t>
+  </si>
+  <si>
+    <t>BotII shall be able handle logic where a piece is a king</t>
+  </si>
+  <si>
+    <t>BotII Shall assign a basic elo rating to each set of moves (normal, jump move)</t>
+  </si>
+  <si>
+    <t>BotII shall ensure the move attempted is valid move</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.isValidMove</t>
+  </si>
+  <si>
+    <t>BotII shall ensure it can check both ways to move (diagonal left, diagonal right)</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.checkSingleMove</t>
+  </si>
+  <si>
+    <t>BotII shall be able to check the validity of a  normal move and a jump/capture move</t>
+  </si>
+  <si>
+    <t>BotII shall be able to determine how many moves or rows a piece is away from becoming a king after a move</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.movesToKing</t>
+  </si>
+  <si>
+    <t>BotII shall increase the ELO rating for a move depending on how far away the piece is from becoming king</t>
+  </si>
+  <si>
+    <t>BotII shall increase the elo rating for a jump/capture move</t>
+  </si>
+  <si>
+    <t>BotII shall sort possible moves according to the selected strategy (aggressive or passive) based on their ELO ratings</t>
+  </si>
+  <si>
+    <t>BotII shall select the highest ELO-rated move when playing aggressively and the lowest ELO-rated move when playing passively</t>
+  </si>
+  <si>
+    <t>BotII shall update its strategy during gameplay based on the current board state</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.playStyle</t>
+  </si>
+  <si>
+    <t>BotII shall switch to defensive strategy when at a numerical disadvantage</t>
+  </si>
+  <si>
+    <t>BotII shall determine if thegiven board is a start board (i.e. BotII has made no moves and the opponent has made 0 or 1 moves)</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.isFirstMove</t>
+  </si>
+  <si>
+    <t>BotII shall make a basic move if the given game board is a start game board</t>
+  </si>
+  <si>
+    <t>uta.cse3310.Bot.BotII.startMove</t>
+  </si>
+  <si>
+    <t>BotII shall, before every move determination flush the moves object</t>
+  </si>
+  <si>
+    <t>BotII shall, for every piece that belongs to it, determine the moves that piece can make, add it to a list and sort that list by ELO rating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +259,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,28 +601,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.06640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -550,7 +660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -558,19 +668,19 @@
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="43.5">
+    </row>
+    <row r="4" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -578,50 +688,373 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="S4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="B7">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
+      <c r="B9">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>34</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>34</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Group 33's (BotI) requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlbea\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitlynnhernandez/cse3310/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F6E724-2CB7-496C-9C74-D7BD6635FE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5092EB4F-20FA-4D40-944D-F789170B0D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>Tested By</t>
   </si>
@@ -218,13 +218,139 @@
   </si>
   <si>
     <t>BotII shall, for every piece that belongs to it, determine the moves that piece can make, add it to a list and sort that list by ELO rating</t>
+  </si>
+  <si>
+    <t>Bot 1 shall use a fixed strategy to determine its moves when playing against the user or Bot II.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall receive the current game board state from the Game Manager via the requestMove(Board board) method.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall return its selected move(s) to the Game Manager via the sendMove()method.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall communicate with the Game Manager via function calls</t>
+  </si>
+  <si>
+    <t>Bot 1 shall be able to play against Bot 2 using the same interface.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall not store any game state locally; all state will reside with the Game Manager.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot 1 shall correctly determine and evaluate all legal moves, including normal and capture moves, for all its pieces on the board. </t>
+  </si>
+  <si>
+    <t>Bot 1 shall utilize a LinkedList&lt;Move&gt; to represent and manage sequences of moves, including potential chains for multi-jump captures.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall avoid moves that expose its pieces to immediate counter-capture, especially in the passive strategy. The defensive strategy will lower the score of such moves to discourage risky decisions.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall send all move(s) to the Game Manager in a single transmission when multiple captures occur.</t>
+  </si>
+  <si>
+    <t>Bot 1 shall follow the rules for the game that come from https://en.wikipedia.org/wiki/English_draughts</t>
+  </si>
+  <si>
+    <t>Bot I shall use this function to dynamically change the strategy depending on the output of countallPieces()</t>
+  </si>
+  <si>
+    <t>Bot I shall count the board for all the pieces</t>
+  </si>
+  <si>
+    <t>Bot I shall play more aggressively (push forward more) if it has more pieces than the player.</t>
+  </si>
+  <si>
+    <t>Bot I shall play more cautiously if it has less pieces than player.</t>
+  </si>
+  <si>
+    <t>Bot I shall advance a space if the square is empty given that the space does not have an enemy piece on it.</t>
+  </si>
+  <si>
+    <t>Bot I shall evaluate and add a capturing move if the move exists and is legal.</t>
+  </si>
+  <si>
+    <t>Bot I shall identify whether a given move is a capturing move by evaluating the distance between the start and destination squares and checking for an opponent piece in between.</t>
+  </si>
+  <si>
+    <t>Bot I shall determine if a move places its piece in a vulnerable location where it can be captured by the opponent.</t>
+  </si>
+  <si>
+    <t>Bot I shall evaluate if a given board position can be used by the opponent to attack.</t>
+  </si>
+  <si>
+    <t>Bot I shall check if a move leaves the piece protected by an adjacent friendly piece.</t>
+  </si>
+  <si>
+    <t>Bot I shall detect if a square is occupied by a friendly piece to determine support.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot I shall know the boundaries of the board so prevent plays made out of the board. </t>
+  </si>
+  <si>
+    <t>Bot1.java / requestMove()</t>
+  </si>
+  <si>
+    <t>Bot1.java / sendMove()</t>
+  </si>
+  <si>
+    <t>Bot1.java / requestMove(), sendMove()</t>
+  </si>
+  <si>
+    <t>Bot1.java / requestMove(), flushMoves()</t>
+  </si>
+  <si>
+    <t>Bot1.java / determineMoves(), playNormalMove(), playCapture()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot1.java / sendMove(), determineMoves() </t>
+  </si>
+  <si>
+    <t>Bot1.java / passiveStrategyImplementation()</t>
+  </si>
+  <si>
+    <t>BotI.java / isAggressive()</t>
+  </si>
+  <si>
+    <t>BotI.java / countallPieces()</t>
+  </si>
+  <si>
+    <t>BotI.java /  aggressiveStrategyImplementation</t>
+  </si>
+  <si>
+    <t>BotI.java /  passiveStrategyImplementation</t>
+  </si>
+  <si>
+    <t>BotI.java / playNormalMove</t>
+  </si>
+  <si>
+    <t>BotI.java / playCapture</t>
+  </si>
+  <si>
+    <t>BotI.java / isCapturingMove</t>
+  </si>
+  <si>
+    <t>BotI.java / insideDangerRegion</t>
+  </si>
+  <si>
+    <t>BotI.java / canBeAttackedFrom</t>
+  </si>
+  <si>
+    <t>BotI.java / hasBackupAfterMove</t>
+  </si>
+  <si>
+    <t>BotI.java / hasSupportAt</t>
+  </si>
+  <si>
+    <t>BotI.java / isInsideBoard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +362,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,12 +391,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -601,28 +739,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.06640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -660,7 +798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -680,7 +818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -703,7 +841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -717,7 +855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -731,7 +869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -745,7 +883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -759,7 +897,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -773,7 +911,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -787,7 +925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -801,7 +939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -815,7 +953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -829,7 +967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -843,7 +981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -857,7 +995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -871,7 +1009,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -885,7 +1023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -899,7 +1037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -913,7 +1051,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -927,7 +1065,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -941,7 +1079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -955,7 +1093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -969,7 +1107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -983,7 +1121,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -997,7 +1135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1011,7 +1149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1025,7 +1163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1039,7 +1177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1051,6 +1189,328 @@
       </c>
       <c r="D29" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>33</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>33</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>33</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>33</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>33</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>33</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>33</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>33</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>33</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>33</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>33</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>33</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>33</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>33</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>33</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>33</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <v>33</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Join Game requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitlynnhernandez/cse3310/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5092EB4F-20FA-4D40-944D-F789170B0D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F7FD75-C49B-6F41-B2A5-ABF000868AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="136">
   <si>
     <t>Tested By</t>
   </si>
@@ -344,6 +344,108 @@
   </si>
   <si>
     <t>BotI.java / isInsideBoard</t>
+  </si>
+  <si>
+    <t>The program shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/displayWaitlist()</t>
+  </si>
+  <si>
+    <t>The program shall display a button for a game against another user.</t>
+  </si>
+  <si>
+    <t>webapp/index.html</t>
+  </si>
+  <si>
+    <t>The program shall display a button for a game against a bot.</t>
+  </si>
+  <si>
+    <t>The program shall update the waitlist as players login and join/leave a game.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/add(), joingame/Waitlist.js/remove()</t>
+  </si>
+  <si>
+    <t>The program shall display a notification with updates to the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/DisplayNotification.js/displayNotification()</t>
+  </si>
+  <si>
+    <t>The program will display a notification to the user when they are next to join a game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The program shall have display a button to spectate a game of 2 bots playing against each other. </t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestSpectateBotVsBot()</t>
+  </si>
+  <si>
+    <t>The program will display players that choose to replay and new players at the bottom of the waitlist.</t>
+  </si>
+  <si>
+    <t>The program will load usernames and IDs in waitlist and display them within 2 seconds of logging in/joining a game.</t>
+  </si>
+  <si>
+    <t>The web interface of the Join Game component will be written in HTML5.</t>
+  </si>
+  <si>
+    <t>The program will be compatible with the web browsers Chrome, Firefox, and Safari.</t>
+  </si>
+  <si>
+    <t>joingame</t>
+  </si>
+  <si>
+    <t>The interactive and dynamic functionality within the component will be written in JavaScript.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js, Data.js, Displaynotification.js, MatchMaking.js, Waitlist.js</t>
+  </si>
+  <si>
+    <t>When the button to play against another player is pressed, the program will send the player information along with the game mode to the Page Manager component to initalize the pairing up process to begin a game.</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestPlayerMatch()</t>
+  </si>
+  <si>
+    <t>When the button to play against a bot is pressed, the program will send the player information along with the game mode to the Page Manager component to intialize the process to start a game against a bot.</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestBotMatch()</t>
+  </si>
+  <si>
+    <t>When a player(s) requests to join a game, the program removes their name from the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/remove()</t>
+  </si>
+  <si>
+    <t>When a player(s) logins successfully, the program adds their name to the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/add()</t>
+  </si>
+  <si>
+    <t>The program will receive player information (username and ID) from the Page Manager through a websocket.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js/handlePlayerData()</t>
+  </si>
+  <si>
+    <t>The program will create a player instance based on the provided data from the Page Manager.</t>
+  </si>
+  <si>
+    <t>joingame/Data.js/constructor()</t>
+  </si>
+  <si>
+    <t>The program will send player information (username and ID) and their selected game mode to the Page Manager through a websocket.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js/sendPlayerAttributes()</t>
+  </si>
+  <si>
+    <t>When the button to spectate a game of two bots playing against each other, the program will send players' username and ID along with the game mode to Page Manager to intialize the process to start the game</t>
   </si>
 </sst>
 </file>
@@ -391,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -399,10 +501,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -739,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1300,7 @@
       <c r="C30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1215,7 +1314,7 @@
       <c r="C31" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1229,7 +1328,7 @@
       <c r="C32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1243,7 +1342,7 @@
       <c r="C33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1257,7 +1356,7 @@
       <c r="C34" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1271,7 +1370,7 @@
       <c r="C35" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1285,7 +1384,7 @@
       <c r="C36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1299,7 +1398,7 @@
       <c r="C37" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1313,7 +1412,7 @@
       <c r="C38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1327,7 +1426,7 @@
       <c r="C39" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1341,7 +1440,7 @@
       <c r="C40" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1352,10 +1451,10 @@
       <c r="B41">
         <v>33</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1366,10 +1465,10 @@
       <c r="B42">
         <v>33</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1380,10 +1479,10 @@
       <c r="B43">
         <v>33</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1394,10 +1493,10 @@
       <c r="B44">
         <v>33</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1408,10 +1507,10 @@
       <c r="B45">
         <v>33</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1422,10 +1521,10 @@
       <c r="B46">
         <v>33</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1436,10 +1535,10 @@
       <c r="B47">
         <v>33</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1450,10 +1549,10 @@
       <c r="B48">
         <v>33</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1464,10 +1563,10 @@
       <c r="B49">
         <v>33</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1478,10 +1577,10 @@
       <c r="B50">
         <v>33</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1492,10 +1591,10 @@
       <c r="B51">
         <v>33</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1506,11 +1605,291 @@
       <c r="B52">
         <v>33</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>26</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <v>26</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>26</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>26</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>26</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>26</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>26</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>26</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63">
+        <v>26</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64">
+        <v>26</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <v>26</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>26</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>26</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <v>26</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69">
+        <v>26</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <v>26</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <v>26</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72">
+        <v>26</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushing Game Termination Requirements to github
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pravesh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F7FD75-C49B-6F41-B2A5-ABF000868AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD270C-8AC9-7F45-A3C3-D515C5874C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="760" windowWidth="28520" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="153">
   <si>
     <t>Tested By</t>
   </si>
@@ -446,13 +446,64 @@
   </si>
   <si>
     <t>When the button to spectate a game of two bots playing against each other, the program will send players' username and ID along with the game mode to Page Manager to intialize the process to start the game</t>
+  </si>
+  <si>
+    <t>After a game concludes, the players go to the end of the line waiting for the new game</t>
+  </si>
+  <si>
+    <t>The results of every game played will be stored into a database, and shall be used for building the contents of the leaderboard.</t>
+  </si>
+  <si>
+    <t>The system will detect a draw, if one occurs</t>
+  </si>
+  <si>
+    <t>The system will have an understanding of the game rules in order to detect winnings after each play, and check for legalMoves to terminate the game</t>
+  </si>
+  <si>
+    <t>The subsytem will send game termination information to database, only when the game ends through a final summary</t>
+  </si>
+  <si>
+    <t>The subsystem will send a final termination message to game play once a match is over</t>
+  </si>
+  <si>
+    <t>The subsystem will handle a confirmation response from the database.</t>
+  </si>
+  <si>
+    <t>The subsytem will track the captured pieces, in order to determine who has lost the game</t>
+  </si>
+  <si>
+    <t>The subsystem will keep track of the player scores after a move, as well as update them</t>
+  </si>
+  <si>
+    <t>GameTermination.java/checkGameOver()</t>
+  </si>
+  <si>
+    <t>GameResult.java/saveResultsToDatabase()</t>
+  </si>
+  <si>
+    <t>GameResult.java/checkForLegalMoves(), getWinner()</t>
+  </si>
+  <si>
+    <t>GameTermination.java/saveResultsToDatabase()</t>
+  </si>
+  <si>
+    <t>GameTermination.java/endGame(), sendResults()</t>
+  </si>
+  <si>
+    <t>GameResult.java/confirmDataStored()</t>
+  </si>
+  <si>
+    <t>GameResult.java/trackCapturedPieces()</t>
+  </si>
+  <si>
+    <t>GameResult.java/updateScores(), getScore()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +522,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -493,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -502,6 +559,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -838,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S72"/>
+  <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1892,6 +1952,132 @@
         <v>113</v>
       </c>
     </row>
+    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73">
+        <v>35</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <v>35</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75">
+        <v>35</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76">
+        <v>35</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <v>35</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78">
+        <v>35</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79">
+        <v>35</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <v>35</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81">
+        <v>35</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating final requirements spreadsheet
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pravesh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD270C-8AC9-7F45-A3C3-D515C5874C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D670A50-AFBE-499F-9E35-6D987A8002CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="760" windowWidth="28520" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="193">
   <si>
     <t>Tested By</t>
   </si>
@@ -497,13 +497,134 @@
   </si>
   <si>
     <t>GameResult.java/updateScores(), getScore()</t>
+  </si>
+  <si>
+    <t>The game will run as a Java program with JavaScript/HTML clients.</t>
+  </si>
+  <si>
+    <t>The rules follow English Draughts from Wikipedia.</t>
+  </si>
+  <si>
+    <t>Display a standard 8x8 checkers board grid with alternating dark and light squares. Board layout should be clear and consistent, with the dark square at the bottom left corner.</t>
+  </si>
+  <si>
+    <t>Display checker pieces for both players. Regular and king pieces should be visually different, and valid moves must be highlighted when a piece is selected.</t>
+  </si>
+  <si>
+    <t>The game will allow selection of pieces and display valid move destinations by commuicating with other teams. Display feedback for illegal moves, captures, and multiple jump possibilities, as provided by other responsible teams to the game display team.</t>
+  </si>
+  <si>
+    <t>Display current player's turn, player names (ID).</t>
+  </si>
+  <si>
+    <t>Implement method for other teams to send messages to the players.</t>
+  </si>
+  <si>
+    <t>Keep game board hidden until the game starts. Enable or disable move interface based on game state and player's turn. This must be controlled by page manager.</t>
+  </si>
+  <si>
+    <t>Provide buttons for resigning, and offering draw.</t>
+  </si>
+  <si>
+    <t>Indicate who moves first.</t>
+  </si>
+  <si>
+    <t>Display all valid moves for a selected piece. Valid moves are determined by backend and visualized on the board.</t>
+  </si>
+  <si>
+    <t>Send all player moves to the backend. Game display collects and formats movement data.</t>
+  </si>
+  <si>
+    <t>Support multiple concurrent game instances by designing the checkers board as a reusable class.</t>
+  </si>
+  <si>
+    <t>Automatically rotate the board 180 degrees for the black player to maintain player perspective.</t>
+  </si>
+  <si>
+    <t>Implement robust error handling in UI functions with clear feedback.</t>
+  </si>
+  <si>
+    <t>Define a standardized JSON message format for client-server communications with type-based message handling.</t>
+  </si>
+  <si>
+    <t>Automatically promote pieces to kings upon reaching the opponent's back row and update visuals.</t>
+  </si>
+  <si>
+    <t>Manage game state transitions and update UI appropriately during turn changes or game completion.</t>
+  </si>
+  <si>
+    <t>Notify players of game events such as opponent moves and game end.</t>
+  </si>
+  <si>
+    <t>Prevent duplication of event listeners.</t>
+  </si>
+  <si>
+    <t>Java WebSocket Server
+connection object in client JS</t>
+  </si>
+  <si>
+    <t>CheckersBoard class construction and design pattern</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.handle_checkers_piece_click()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.update_board_style(), game_display_checkers.js/CheckersBoard.create_checkers_board()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.update_board_style(), CSS styling in game_display_checkers.js/update_board_style()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.handle_checkers_piece_click(), game_display_checkers.js/CheckersBoard.show_possible_moves()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.update_current_player(), game_id</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/game_display_popup_messages()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.create_checkers_board()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/handle_resign(), game_display_checkers.js/offer_draw(), game_display_checkers.js/add_game_display_user_control_event_listener()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard constructor, game_display_checkers.js/update_current_player()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.show_possible_moves(), game_display_checkers.js/return_allowed_moves(), game_display_checkers.js/is_valid_move()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.move_checkers_piece(), WebSocket message: {type: "move", ...}</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.rotateBoardIfBlack()</t>
+  </si>
+  <si>
+    <t>Try/catch blocks, game_display_checkers.js/game_display_popup_messages()</t>
+  </si>
+  <si>
+    <t>WebSocket message formatting in game_display_checkers.js/game_display_handle_websocket_received_data()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/move_checkers_piece(), game_display_checkers.js/update_board_style()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/update_current_player(), game_display_checkers.js/game_display_handle_websocket_received_data()</t>
+  </si>
+  <si>
+    <t>Message handling in game_display_checkers.js/game_display_handle_websocket_received_data()</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/register_buttons_to_event_listener()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,6 +650,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -550,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -564,6 +691,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,28 +1028,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S81"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="81" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -957,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -977,7 +1107,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1000,7 +1130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1014,7 +1144,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1028,7 +1158,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1042,7 +1172,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1056,7 +1186,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1070,7 +1200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1084,7 +1214,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1098,7 +1228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1112,7 +1242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1126,7 +1256,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1140,7 +1270,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1154,7 +1284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1168,7 +1298,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1182,7 +1312,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1196,7 +1326,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1210,7 +1340,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1224,7 +1354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1238,7 +1368,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1252,7 +1382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1266,7 +1396,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1280,7 +1410,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1294,7 +1424,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1308,7 +1438,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1322,7 +1452,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1336,7 +1466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1350,7 +1480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1364,7 +1494,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1378,7 +1508,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1392,7 +1522,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1406,7 +1536,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1420,7 +1550,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1434,7 +1564,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1448,7 +1578,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1462,7 +1592,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1476,7 +1606,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1490,7 +1620,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1504,7 +1634,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1518,7 +1648,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1532,7 +1662,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1546,7 +1676,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -1560,7 +1690,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -1574,7 +1704,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -1588,7 +1718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -1602,7 +1732,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -1616,7 +1746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1630,7 +1760,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1644,7 +1774,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -1658,7 +1788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -1672,7 +1802,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1686,7 +1816,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -1700,7 +1830,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -1714,7 +1844,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -1728,7 +1858,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -1742,7 +1872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -1756,7 +1886,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -1770,7 +1900,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -1784,7 +1914,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -1798,7 +1928,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -1812,7 +1942,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -1826,7 +1956,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -1840,7 +1970,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -1854,7 +1984,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
@@ -1868,7 +1998,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
@@ -1882,7 +2012,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
@@ -1896,7 +2026,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
@@ -1910,7 +2040,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
@@ -1924,7 +2054,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -1938,7 +2068,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
@@ -1952,7 +2082,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
@@ -1966,7 +2096,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
@@ -1980,7 +2110,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -1994,7 +2124,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
@@ -2008,7 +2138,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
@@ -2022,7 +2152,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
@@ -2036,7 +2166,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
@@ -2050,7 +2180,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
@@ -2064,7 +2194,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -2076,6 +2206,286 @@
       </c>
       <c r="D81" s="1" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <v>27</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>80</v>
+      </c>
+      <c r="B83">
+        <v>27</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>81</v>
+      </c>
+      <c r="B84" s="6">
+        <v>27</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>82</v>
+      </c>
+      <c r="B85" s="6">
+        <v>27</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>83</v>
+      </c>
+      <c r="B86" s="6">
+        <v>27</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="6">
+        <v>84</v>
+      </c>
+      <c r="B87" s="6">
+        <v>27</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>85</v>
+      </c>
+      <c r="B88" s="6">
+        <v>27</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>86</v>
+      </c>
+      <c r="B89" s="6">
+        <v>27</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>87</v>
+      </c>
+      <c r="B90" s="6">
+        <v>27</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>88</v>
+      </c>
+      <c r="B91" s="6">
+        <v>27</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>89</v>
+      </c>
+      <c r="B92" s="6">
+        <v>27</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>90</v>
+      </c>
+      <c r="B93" s="6">
+        <v>27</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>91</v>
+      </c>
+      <c r="B94" s="6">
+        <v>27</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>92</v>
+      </c>
+      <c r="B95" s="6">
+        <v>27</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>93</v>
+      </c>
+      <c r="B96" s="6">
+        <v>27</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>94</v>
+      </c>
+      <c r="B97" s="6">
+        <v>27</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>95</v>
+      </c>
+      <c r="B98" s="6">
+        <v>27</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
+        <v>96</v>
+      </c>
+      <c r="B99" s="6">
+        <v>27</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="6">
+        <v>97</v>
+      </c>
+      <c r="B100" s="6">
+        <v>27</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>98</v>
+      </c>
+      <c r="B101" s="6">
+        <v>27</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added GamePlay requirements to the Final Requirements spreadsheet
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D670A50-AFBE-499F-9E35-6D987A8002CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015FAE43-4A49-4945-A8E0-B7350BCF26AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="215">
   <si>
     <t>Tested By</t>
   </si>
@@ -618,6 +618,72 @@
   </si>
   <si>
     <t>game_display_checkers.js/register_buttons_to_event_listener()</t>
+  </si>
+  <si>
+    <t>Game Play shall determine whether a move is legal or not and decides whether a piece has been captured.</t>
+  </si>
+  <si>
+    <t>A checker's piece shall not move to a spot taken by another checker's piece.  If the user attempts to move in a spot that is taken send an error message to Game Manager</t>
+  </si>
+  <si>
+    <t>A checker's piece shall only move diagonally up the board unless it is marked by a crown, allowing the piece to move diagonally up and down.</t>
+  </si>
+  <si>
+    <t>A checker's piece shall not move beyond the border of the playing field.</t>
+  </si>
+  <si>
+    <t>Game Play shall communicate with Game Manager, notifying whether the requested move is legal and whether a piece has been captured.</t>
+  </si>
+  <si>
+    <t>A player shall not be allowed to move checker pieces of their oponent</t>
+  </si>
+  <si>
+    <t>The user is able to make multiple successive jumps during one turn, if each jump captures an opponents piece and follows the rules associated with the user's cheker piece (i.e a king could do this in either a backwards or forwards direction, and a regular piece is only able to do this in a forward direction)</t>
+  </si>
+  <si>
+    <t>The user must capture an opponent's piece if a legal move is presented/available</t>
+  </si>
+  <si>
+    <t>The bot should be subject to the same rules as the user</t>
+  </si>
+  <si>
+    <t>A king checker piece is not able to move both up and down during one turn. It must choose to either move up or down</t>
+  </si>
+  <si>
+    <t>If the user is presented two different opportunities to capture an opponents checker piece during their turn, they are allowed to chose which checker's piece they capture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A king checker piece shall be held to the same capture rules as a regular checker piece. </t>
+  </si>
+  <si>
+    <t>A captured piece shall be removed from the game</t>
+  </si>
+  <si>
+    <t>A pieces move length shall be proportional to the amount of the opponent's pieces the moving piece jumps over.</t>
+  </si>
+  <si>
+    <t>GamePlay.GamePlay.returnBoard</t>
+  </si>
+  <si>
+    <t>GamePlay.rules.isLegal</t>
+  </si>
+  <si>
+    <t>GamePlay.rules.inBounds</t>
+  </si>
+  <si>
+    <t>GamePlay.rules.canMovePiece</t>
+  </si>
+  <si>
+    <t>GamePlay.rules.isLegal / GamePlay.GamePlay.returnBoard</t>
+  </si>
+  <si>
+    <t>GamePlay.rules.returnBoard</t>
+  </si>
+  <si>
+    <t>GamePlay shall return a list of possible moves a player can take during their turn</t>
+  </si>
+  <si>
+    <t>GamePlay.GamePlay.returnMoves</t>
   </si>
 </sst>
 </file>
@@ -677,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -691,8 +757,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1028,28 +1092,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S101"/>
+  <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1087,7 +1151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1107,7 +1171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1130,7 +1194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1144,7 +1208,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1158,7 +1222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1172,7 +1236,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1186,7 +1250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1200,7 +1264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1214,7 +1278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1228,7 +1292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1242,7 +1306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1256,7 +1320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1270,7 +1334,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1284,7 +1348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1298,7 +1362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1312,7 +1376,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1326,7 +1390,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1340,7 +1404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1354,7 +1418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1368,7 +1432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1382,7 +1446,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1396,7 +1460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1410,7 +1474,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1424,7 +1488,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1438,7 +1502,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1452,7 +1516,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1466,7 +1530,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1480,7 +1544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1494,7 +1558,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1508,7 +1572,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1522,7 +1586,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1536,7 +1600,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1550,7 +1614,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1564,7 +1628,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1578,7 +1642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1592,7 +1656,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1606,7 +1670,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1620,7 +1684,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1634,7 +1698,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1648,7 +1712,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1662,7 +1726,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1676,7 +1740,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>41</v>
       </c>
@@ -1690,7 +1754,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>42</v>
       </c>
@@ -1704,7 +1768,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>43</v>
       </c>
@@ -1718,7 +1782,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>44</v>
       </c>
@@ -1732,7 +1796,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>45</v>
       </c>
@@ -1746,7 +1810,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1760,7 +1824,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1774,7 +1838,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>48</v>
       </c>
@@ -1788,7 +1852,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>49</v>
       </c>
@@ -1802,7 +1866,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1816,7 +1880,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>51</v>
       </c>
@@ -1830,7 +1894,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>52</v>
       </c>
@@ -1844,7 +1908,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>53</v>
       </c>
@@ -1858,7 +1922,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>54</v>
       </c>
@@ -1872,7 +1936,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>55</v>
       </c>
@@ -1886,7 +1950,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>56</v>
       </c>
@@ -1900,7 +1964,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>57</v>
       </c>
@@ -1914,7 +1978,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>58</v>
       </c>
@@ -1928,7 +1992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>59</v>
       </c>
@@ -1942,7 +2006,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>60</v>
       </c>
@@ -1956,7 +2020,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>61</v>
       </c>
@@ -1970,7 +2034,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>62</v>
       </c>
@@ -1984,7 +2048,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>63</v>
       </c>
@@ -1998,7 +2062,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>64</v>
       </c>
@@ -2012,7 +2076,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>65</v>
       </c>
@@ -2026,7 +2090,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>66</v>
       </c>
@@ -2040,7 +2104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>67</v>
       </c>
@@ -2054,7 +2118,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>68</v>
       </c>
@@ -2068,7 +2132,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>69</v>
       </c>
@@ -2082,7 +2146,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>70</v>
       </c>
@@ -2096,7 +2160,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>71</v>
       </c>
@@ -2110,7 +2174,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>72</v>
       </c>
@@ -2124,7 +2188,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>73</v>
       </c>
@@ -2138,7 +2202,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>74</v>
       </c>
@@ -2152,7 +2216,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>75</v>
       </c>
@@ -2166,7 +2230,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>76</v>
       </c>
@@ -2180,7 +2244,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>77</v>
       </c>
@@ -2194,7 +2258,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>78</v>
       </c>
@@ -2208,8 +2272,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="6">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82">
         <v>79</v>
       </c>
       <c r="B82">
@@ -2218,12 +2282,12 @@
       <c r="C82" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="6">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83">
         <v>80</v>
       </c>
       <c r="B83">
@@ -2232,260 +2296,470 @@
       <c r="C83" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="6">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84">
         <v>81</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84">
         <v>27</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="6">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85">
         <v>82</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85">
         <v>27</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="6">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86">
         <v>83</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86">
         <v>27</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="6">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87">
         <v>84</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87">
         <v>27</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="6">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88">
         <v>85</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88">
         <v>27</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="6">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89">
         <v>86</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89">
         <v>27</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="6">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90">
         <v>87</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90">
         <v>27</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="6">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91">
         <v>88</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91">
         <v>27</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="D91" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="6">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92">
         <v>89</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92">
         <v>27</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="6">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93">
         <v>90</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93">
         <v>27</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="6">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A94">
         <v>91</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94">
         <v>27</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="6">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A95">
         <v>92</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95">
         <v>27</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="6">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A96">
         <v>93</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96">
         <v>27</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="6">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A97">
         <v>94</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97">
         <v>27</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="6">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A98">
         <v>95</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98">
         <v>27</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="6">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A99">
         <v>96</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99">
         <v>27</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D99" s="5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="6">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A100">
         <v>97</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100">
         <v>27</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="D100" s="5" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="6">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A101">
         <v>98</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101">
         <v>27</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="5" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102">
+        <v>36</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103">
+        <v>36</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104">
+        <v>36</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105">
+        <v>36</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106">
+        <v>36</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107">
+        <v>36</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108">
+        <v>36</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109">
+        <v>36</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110">
+        <v>36</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111">
+        <v>36</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>109</v>
+      </c>
+      <c r="B112">
+        <v>36</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113">
+        <v>36</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114">
+        <v>36</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>112</v>
+      </c>
+      <c r="B115">
+        <v>36</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116">
+        <v>36</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Pm to final reqs
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/cmb6906_mavs_uta_edu/Documents/2024-2025/Spring/Fundamentals of SE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{879BA1B7-AEFB-1F4C-96A0-906E7F19F358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{879BA1B7-AEFB-1F4C-96A0-906E7F19F358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39493073-E4FC-43A9-95E0-73D5DF3F67C1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="310">
   <si>
     <t>Tested By</t>
   </si>
@@ -79,6 +81,9 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Requirement</t>
   </si>
   <si>
     <t>Implemented In</t>
@@ -107,9 +112,6 @@
     <t>cut and paste the screenshot of each page in this part of the spreadsheet, please. use as much space is needed.</t>
   </si>
   <si>
-    <t>Requirement</t>
-  </si>
-  <si>
     <t>BOT II shall return a list of game move(s) to game manager</t>
   </si>
   <si>
@@ -221,30 +223,51 @@
     <t>Bot 1 shall use a fixed strategy to determine its moves when playing against the user or Bot II.</t>
   </si>
   <si>
+    <t>Bot1.java / requestMove()</t>
+  </si>
+  <si>
     <t>Bot 1 shall receive the current game board state from the Game Manager via the requestMove(Board board) method.</t>
   </si>
   <si>
     <t>Bot 1 shall return its selected move(s) to the Game Manager via the sendMove()method.</t>
   </si>
   <si>
+    <t>Bot1.java / sendMove()</t>
+  </si>
+  <si>
     <t>Bot 1 shall communicate with the Game Manager via function calls</t>
   </si>
   <si>
+    <t>Bot1.java / requestMove(), sendMove()</t>
+  </si>
+  <si>
     <t>Bot 1 shall be able to play against Bot 2 using the same interface.</t>
   </si>
   <si>
     <t>Bot 1 shall not store any game state locally; all state will reside with the Game Manager.</t>
   </si>
   <si>
+    <t>Bot1.java / requestMove(), flushMoves()</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bot 1 shall correctly determine and evaluate all legal moves, including normal and capture moves, for all its pieces on the board. </t>
   </si>
   <si>
+    <t>Bot1.java / determineMoves(), playNormalMove(), playCapture()</t>
+  </si>
+  <si>
     <t>Bot 1 shall utilize a LinkedList&lt;Move&gt; to represent and manage sequences of moves, including potential chains for multi-jump captures.</t>
   </si>
   <si>
+    <t xml:space="preserve">Bot1.java / sendMove(), determineMoves() </t>
+  </si>
+  <si>
     <t>Bot 1 shall avoid moves that expose its pieces to immediate counter-capture, especially in the passive strategy. The defensive strategy will lower the score of such moves to discourage risky decisions.</t>
   </si>
   <si>
+    <t>Bot1.java / passiveStrategyImplementation()</t>
+  </si>
+  <si>
     <t>Bot 1 shall send all move(s) to the Game Manager in a single transmission when multiple captures occur.</t>
   </si>
   <si>
@@ -254,93 +277,72 @@
     <t>Bot I shall use this function to dynamically change the strategy depending on the output of countallPieces()</t>
   </si>
   <si>
+    <t>BotI.java / isAggressive()</t>
+  </si>
+  <si>
     <t>Bot I shall count the board for all the pieces</t>
   </si>
   <si>
+    <t>BotI.java / countallPieces()</t>
+  </si>
+  <si>
     <t>Bot I shall play more aggressively (push forward more) if it has more pieces than the player.</t>
   </si>
   <si>
+    <t>BotI.java /  aggressiveStrategyImplementation</t>
+  </si>
+  <si>
     <t>Bot I shall play more cautiously if it has less pieces than player.</t>
   </si>
   <si>
+    <t>BotI.java /  passiveStrategyImplementation</t>
+  </si>
+  <si>
     <t>Bot I shall advance a space if the square is empty given that the space does not have an enemy piece on it.</t>
   </si>
   <si>
+    <t>BotI.java / playNormalMove</t>
+  </si>
+  <si>
     <t>Bot I shall evaluate and add a capturing move if the move exists and is legal.</t>
   </si>
   <si>
+    <t>BotI.java / playCapture</t>
+  </si>
+  <si>
     <t>Bot I shall identify whether a given move is a capturing move by evaluating the distance between the start and destination squares and checking for an opponent piece in between.</t>
   </si>
   <si>
+    <t>BotI.java / isCapturingMove</t>
+  </si>
+  <si>
     <t>Bot I shall determine if a move places its piece in a vulnerable location where it can be captured by the opponent.</t>
   </si>
   <si>
+    <t>BotI.java / insideDangerRegion</t>
+  </si>
+  <si>
     <t>Bot I shall evaluate if a given board position can be used by the opponent to attack.</t>
   </si>
   <si>
+    <t>BotI.java / canBeAttackedFrom</t>
+  </si>
+  <si>
     <t>Bot I shall check if a move leaves the piece protected by an adjacent friendly piece.</t>
   </si>
   <si>
+    <t>BotI.java / hasBackupAfterMove</t>
+  </si>
+  <si>
     <t>Bot I shall detect if a square is occupied by a friendly piece to determine support.</t>
   </si>
   <si>
+    <t>BotI.java / hasSupportAt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bot I shall know the boundaries of the board so prevent plays made out of the board. </t>
   </si>
   <si>
-    <t>Bot1.java / requestMove()</t>
-  </si>
-  <si>
-    <t>Bot1.java / sendMove()</t>
-  </si>
-  <si>
-    <t>Bot1.java / requestMove(), sendMove()</t>
-  </si>
-  <si>
-    <t>Bot1.java / requestMove(), flushMoves()</t>
-  </si>
-  <si>
-    <t>Bot1.java / determineMoves(), playNormalMove(), playCapture()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bot1.java / sendMove(), determineMoves() </t>
-  </si>
-  <si>
-    <t>Bot1.java / passiveStrategyImplementation()</t>
-  </si>
-  <si>
-    <t>BotI.java / isAggressive()</t>
-  </si>
-  <si>
-    <t>BotI.java / countallPieces()</t>
-  </si>
-  <si>
-    <t>BotI.java /  aggressiveStrategyImplementation</t>
-  </si>
-  <si>
-    <t>BotI.java /  passiveStrategyImplementation</t>
-  </si>
-  <si>
-    <t>BotI.java / playNormalMove</t>
-  </si>
-  <si>
-    <t>BotI.java / playCapture</t>
-  </si>
-  <si>
-    <t>BotI.java / isCapturingMove</t>
-  </si>
-  <si>
-    <t>BotI.java / insideDangerRegion</t>
-  </si>
-  <si>
-    <t>BotI.java / canBeAttackedFrom</t>
-  </si>
-  <si>
-    <t>BotI.java / hasBackupAfterMove</t>
-  </si>
-  <si>
-    <t>BotI.java / hasSupportAt</t>
-  </si>
-  <si>
     <t>BotI.java / isInsideBoard</t>
   </si>
   <si>
@@ -449,199 +451,214 @@
     <t>After a game concludes, the players go to the end of the line waiting for the new game</t>
   </si>
   <si>
+    <t>GameTermination.java/checkGameOver()</t>
+  </si>
+  <si>
     <t>The results of every game played will be stored into a database, and shall be used for building the contents of the leaderboard.</t>
   </si>
   <si>
+    <t>GameResult.java/saveResultsToDatabase()</t>
+  </si>
+  <si>
     <t>The system will detect a draw, if one occurs</t>
   </si>
   <si>
     <t>The system will have an understanding of the game rules in order to detect winnings after each play, and check for legalMoves to terminate the game</t>
   </si>
   <si>
+    <t>GameResult.java/checkForLegalMoves(), getWinner()</t>
+  </si>
+  <si>
     <t>The subsytem will send game termination information to database, only when the game ends through a final summary</t>
   </si>
   <si>
+    <t>GameTermination.java/saveResultsToDatabase()</t>
+  </si>
+  <si>
     <t>The subsystem will send a final termination message to game play once a match is over</t>
   </si>
   <si>
+    <t>GameTermination.java/endGame(), sendResults()</t>
+  </si>
+  <si>
     <t>The subsystem will handle a confirmation response from the database.</t>
   </si>
   <si>
+    <t>GameResult.java/confirmDataStored()</t>
+  </si>
+  <si>
     <t>The subsytem will track the captured pieces, in order to determine who has lost the game</t>
   </si>
   <si>
+    <t>GameResult.java/trackCapturedPieces()</t>
+  </si>
+  <si>
     <t>The subsystem will keep track of the player scores after a move, as well as update them</t>
   </si>
   <si>
-    <t>GameTermination.java/checkGameOver()</t>
-  </si>
-  <si>
-    <t>GameResult.java/saveResultsToDatabase()</t>
-  </si>
-  <si>
-    <t>GameResult.java/checkForLegalMoves(), getWinner()</t>
-  </si>
-  <si>
-    <t>GameTermination.java/saveResultsToDatabase()</t>
-  </si>
-  <si>
-    <t>GameTermination.java/endGame(), sendResults()</t>
-  </si>
-  <si>
-    <t>GameResult.java/confirmDataStored()</t>
-  </si>
-  <si>
-    <t>GameResult.java/trackCapturedPieces()</t>
-  </si>
-  <si>
     <t>GameResult.java/updateScores(), getScore()</t>
   </si>
   <si>
     <t>The game will run as a Java program with JavaScript/HTML clients.</t>
-  </si>
-  <si>
-    <t>The rules follow English Draughts from Wikipedia.</t>
-  </si>
-  <si>
-    <t>Display a standard 8x8 checkers board grid with alternating dark and light squares. Board layout should be clear and consistent, with the dark square at the bottom left corner.</t>
-  </si>
-  <si>
-    <t>Display checker pieces for both players. Regular and king pieces should be visually different, and valid moves must be highlighted when a piece is selected.</t>
-  </si>
-  <si>
-    <t>The game will allow selection of pieces and display valid move destinations by commuicating with other teams. Display feedback for illegal moves, captures, and multiple jump possibilities, as provided by other responsible teams to the game display team.</t>
-  </si>
-  <si>
-    <t>Display current player's turn, player names (ID).</t>
-  </si>
-  <si>
-    <t>Implement method for other teams to send messages to the players.</t>
-  </si>
-  <si>
-    <t>Keep game board hidden until the game starts. Enable or disable move interface based on game state and player's turn. This must be controlled by page manager.</t>
-  </si>
-  <si>
-    <t>Provide buttons for resigning, and offering draw.</t>
-  </si>
-  <si>
-    <t>Indicate who moves first.</t>
-  </si>
-  <si>
-    <t>Display all valid moves for a selected piece. Valid moves are determined by backend and visualized on the board.</t>
-  </si>
-  <si>
-    <t>Send all player moves to the backend. Game display collects and formats movement data.</t>
-  </si>
-  <si>
-    <t>Support multiple concurrent game instances by designing the checkers board as a reusable class.</t>
-  </si>
-  <si>
-    <t>Automatically rotate the board 180 degrees for the black player to maintain player perspective.</t>
-  </si>
-  <si>
-    <t>Implement robust error handling in UI functions with clear feedback.</t>
-  </si>
-  <si>
-    <t>Define a standardized JSON message format for client-server communications with type-based message handling.</t>
-  </si>
-  <si>
-    <t>Automatically promote pieces to kings upon reaching the opponent's back row and update visuals.</t>
-  </si>
-  <si>
-    <t>Manage game state transitions and update UI appropriately during turn changes or game completion.</t>
-  </si>
-  <si>
-    <t>Notify players of game events such as opponent moves and game end.</t>
-  </si>
-  <si>
-    <t>Prevent duplication of event listeners.</t>
   </si>
   <si>
     <t>Java WebSocket Server
 connection object in client JS</t>
   </si>
   <si>
+    <t>The rules follow English Draughts from Wikipedia.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.handle_checkers_piece_click()</t>
+  </si>
+  <si>
+    <t>Display a standard 8x8 checkers board grid with alternating dark and light squares. Board layout should be clear and consistent, with the dark square at the bottom left corner.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.update_board_style(), game_display_checkers.js/CheckersBoard.create_checkers_board()</t>
+  </si>
+  <si>
+    <t>Display checker pieces for both players. Regular and king pieces should be visually different, and valid moves must be highlighted when a piece is selected.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.update_board_style(), CSS styling in game_display_checkers.js/update_board_style()</t>
+  </si>
+  <si>
+    <t>The game will allow selection of pieces and display valid move destinations by commuicating with other teams. Display feedback for illegal moves, captures, and multiple jump possibilities, as provided by other responsible teams to the game display team.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.handle_checkers_piece_click(), game_display_checkers.js/CheckersBoard.show_possible_moves()</t>
+  </si>
+  <si>
+    <t>Display current player's turn, player names (ID).</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.update_current_player(), game_id</t>
+  </si>
+  <si>
+    <t>Implement method for other teams to send messages to the players.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/game_display_popup_messages()</t>
+  </si>
+  <si>
+    <t>Keep game board hidden until the game starts. Enable or disable move interface based on game state and player's turn. This must be controlled by page manager.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.create_checkers_board()</t>
+  </si>
+  <si>
+    <t>Provide buttons for resigning, and offering draw.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/handle_resign(), game_display_checkers.js/offer_draw(), game_display_checkers.js/add_game_display_user_control_event_listener()</t>
+  </si>
+  <si>
+    <t>Indicate who moves first.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard constructor, game_display_checkers.js/update_current_player()</t>
+  </si>
+  <si>
+    <t>Display all valid moves for a selected piece. Valid moves are determined by backend and visualized on the board.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.show_possible_moves(), game_display_checkers.js/return_allowed_moves(), game_display_checkers.js/is_valid_move()</t>
+  </si>
+  <si>
+    <t>Send all player moves to the backend. Game display collects and formats movement data.</t>
+  </si>
+  <si>
+    <t>game_display_checkers.js/CheckersBoard.move_checkers_piece(), WebSocket message: {type: "move", ...}</t>
+  </si>
+  <si>
+    <t>Support multiple concurrent game instances by designing the checkers board as a reusable class.</t>
+  </si>
+  <si>
     <t>CheckersBoard class construction and design pattern</t>
   </si>
   <si>
-    <t>game_display_checkers.js/CheckersBoard.handle_checkers_piece_click()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.update_board_style(), game_display_checkers.js/CheckersBoard.create_checkers_board()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.update_board_style(), CSS styling in game_display_checkers.js/update_board_style()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.handle_checkers_piece_click(), game_display_checkers.js/CheckersBoard.show_possible_moves()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.update_current_player(), game_id</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/game_display_popup_messages()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.create_checkers_board()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/handle_resign(), game_display_checkers.js/offer_draw(), game_display_checkers.js/add_game_display_user_control_event_listener()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard constructor, game_display_checkers.js/update_current_player()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.show_possible_moves(), game_display_checkers.js/return_allowed_moves(), game_display_checkers.js/is_valid_move()</t>
-  </si>
-  <si>
-    <t>game_display_checkers.js/CheckersBoard.move_checkers_piece(), WebSocket message: {type: "move", ...}</t>
+    <t>Automatically rotate the board 180 degrees for the black player to maintain player perspective.</t>
   </si>
   <si>
     <t>game_display_checkers.js/CheckersBoard.rotateBoardIfBlack()</t>
   </si>
   <si>
+    <t>Implement robust error handling in UI functions with clear feedback.</t>
+  </si>
+  <si>
     <t>Try/catch blocks, game_display_checkers.js/game_display_popup_messages()</t>
   </si>
   <si>
+    <t>Define a standardized JSON message format for client-server communications with type-based message handling.</t>
+  </si>
+  <si>
     <t>WebSocket message formatting in game_display_checkers.js/game_display_handle_websocket_received_data()</t>
   </si>
   <si>
+    <t>Automatically promote pieces to kings upon reaching the opponent's back row and update visuals.</t>
+  </si>
+  <si>
     <t>game_display_checkers.js/move_checkers_piece(), game_display_checkers.js/update_board_style()</t>
   </si>
   <si>
+    <t>Manage game state transitions and update UI appropriately during turn changes or game completion.</t>
+  </si>
+  <si>
     <t>game_display_checkers.js/update_current_player(), game_display_checkers.js/game_display_handle_websocket_received_data()</t>
   </si>
   <si>
+    <t>Notify players of game events such as opponent moves and game end.</t>
+  </si>
+  <si>
     <t>Message handling in game_display_checkers.js/game_display_handle_websocket_received_data()</t>
   </si>
   <si>
+    <t>Prevent duplication of event listeners.</t>
+  </si>
+  <si>
     <t>game_display_checkers.js/register_buttons_to_event_listener()</t>
   </si>
   <si>
     <t>Game Play shall determine whether a move is legal or not and decides whether a piece has been captured.</t>
   </si>
   <si>
+    <t>GamePlay.GamePlay.returnBoard</t>
+  </si>
+  <si>
     <t>A checker's piece shall not move to a spot taken by another checker's piece.  If the user attempts to move in a spot that is taken send an error message to Game Manager</t>
   </si>
   <si>
+    <t>GamePlay.rules.isLegal</t>
+  </si>
+  <si>
     <t>A checker's piece shall only move diagonally up the board unless it is marked by a crown, allowing the piece to move diagonally up and down.</t>
   </si>
   <si>
     <t>A checker's piece shall not move beyond the border of the playing field.</t>
   </si>
   <si>
+    <t>GamePlay.rules.inBounds</t>
+  </si>
+  <si>
     <t>Game Play shall communicate with Game Manager, notifying whether the requested move is legal and whether a piece has been captured.</t>
   </si>
   <si>
     <t>A player shall not be allowed to move checker pieces of their oponent</t>
   </si>
   <si>
+    <t>GamePlay.rules.canMovePiece</t>
+  </si>
+  <si>
     <t>The user is able to make multiple successive jumps during one turn, if each jump captures an opponents piece and follows the rules associated with the user's cheker piece (i.e a king could do this in either a backwards or forwards direction, and a regular piece is only able to do this in a forward direction)</t>
   </si>
   <si>
     <t>The user must capture an opponent's piece if a legal move is presented/available</t>
   </si>
   <si>
+    <t>GamePlay.rules.isLegal / GamePlay.GamePlay.returnBoard</t>
+  </si>
+  <si>
     <t>The bot should be subject to the same rules as the user</t>
   </si>
   <si>
@@ -660,21 +677,6 @@
     <t>A pieces move length shall be proportional to the amount of the opponent's pieces the moving piece jumps over.</t>
   </si>
   <si>
-    <t>GamePlay.GamePlay.returnBoard</t>
-  </si>
-  <si>
-    <t>GamePlay.rules.isLegal</t>
-  </si>
-  <si>
-    <t>GamePlay.rules.inBounds</t>
-  </si>
-  <si>
-    <t>GamePlay.rules.canMovePiece</t>
-  </si>
-  <si>
-    <t>GamePlay.rules.isLegal / GamePlay.GamePlay.returnBoard</t>
-  </si>
-  <si>
     <t>GamePlay.rules.returnBoard</t>
   </si>
   <si>
@@ -684,87 +686,99 @@
     <t>GamePlay.GamePlay.returnMoves</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall allow the user to be matched with another user if the user desires to play against another user</t>
+  </si>
+  <si>
     <t>PairUp/Matchmaking/pair</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall allow the user to be matched with a bot if the user desires to play against a bot</t>
+  </si>
+  <si>
+    <t>The PairUp subsystem shall allow a bot to play against another bot</t>
+  </si>
+  <si>
+    <t>The PairUp subsystem shall manage a "matchmaking" pool with players that are looking for a match against another player</t>
+  </si>
+  <si>
     <t>PairUp/Matchmaking/matching</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall allow other subsystems to add/remove/search/clear players from the matchmaking pool</t>
+  </si>
+  <si>
     <t>PairUp/PairUp</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall allow other subsystems to "ping" the matchmaking pool, which tells the matchmaker to look for possible pairs in the current pool</t>
+  </si>
+  <si>
     <t>PairUp/ping</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall provide information of the two entities that were matched for a game to game manager</t>
+  </si>
+  <si>
+    <t>The PairUp subsystem shall keep track of information of players in queue, including their timeOfEntry, playerID, playerName, if their playAgainstBot, and wins</t>
+  </si>
+  <si>
     <t>PairUp/PlayerInMatchmaking/N/A</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall keep track of all match information before sending it to game manager</t>
+  </si>
+  <si>
     <t>PairUp/Match/N/A</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall implement a matchmaking algorithm to pair up players of the same skill range. The algorithm will instantly match those with a similar win count (+/- 1 win), but keep those that don't get matched instantly inside the matchmaking "pool".</t>
+  </si>
+  <si>
+    <t>The PairUp subsystem shall ensure that no player gets stuck in matchmaking for eternity, if a match can be made. A player will have a "priority" once they have been in queue for more than 60 seconds, pairing them with the next player that enters queue, regardless of their win count</t>
+  </si>
+  <si>
+    <t>The PairUp subsystem shall keep track of all players in the queue, using a LinkedHashMap that stores playerID as a key, and the "PlayerInMatchmaking" object as its value</t>
+  </si>
+  <si>
     <t>PairUp/Matchmaking</t>
   </si>
   <si>
+    <t>The PairUp subsystem shall routinely check for possible matches to prevent a standstill scenario. An asychrounous scheduler is used to "ping" the matching method, telling it to check for available pairings between players currently in the queue every 60 seconds.</t>
+  </si>
+  <si>
     <t>PairUp/MatchmakingScheduler</t>
   </si>
   <si>
+    <t>The PairUp subsystem will support direct matches, in which a player directly challenges another player to avoid going through the matchmaking process</t>
+  </si>
+  <si>
     <t>PairUp/PairUp/pair</t>
   </si>
   <si>
-    <t>The PairUp subsystem shall allow other subsystems to add/remove/search/clear players from the matchmaking pool</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall allow other subsystems to "ping" the matchmaking pool, which tells the matchmaker to look for possible pairs in the current pool</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall provide information of the two entities that were matched for a game to game manager</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall keep track of information of players in queue, including their timeOfEntry, playerID, playerName, if their playAgainstBot, and wins</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall keep track of all match information before sending it to game manager</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall implement a matchmaking algorithm to pair up players of the same skill range. The algorithm will instantly match those with a similar win count (+/- 1 win), but keep those that don't get matched instantly inside the matchmaking "pool".</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall ensure that no player gets stuck in matchmaking for eternity, if a match can be made. A player will have a "priority" once they have been in queue for more than 60 seconds, pairing them with the next player that enters queue, regardless of their win count</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall keep track of all players in the queue, using a LinkedHashMap that stores playerID as a key, and the "PlayerInMatchmaking" object as its value</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall routinely check for possible matches to prevent a standstill scenario. An asychrounous scheduler is used to "ping" the matching method, telling it to check for available pairings between players currently in the queue every 60 seconds.</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem will support direct matches, in which a player directly challenges another player to avoid going through the matchmaking process</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall allow the user to be matched with another user if the user desires to play against another user</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall allow the user to be matched with a bot if the user desires to play against a bot</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall allow a bot to play against another bot</t>
-  </si>
-  <si>
-    <t>The PairUp subsystem shall manage a "matchmaking" pool with players that are looking for a match against another player</t>
-  </si>
-  <si>
     <t>The Database shall store player information and ranking of all users who create an account.</t>
   </si>
   <si>
+    <t>Uta.cse3310.DB.insertUser </t>
+  </si>
+  <si>
     <t>The Database shall retrieve player account when page manager interface requests it by matching it to a players unique Username.</t>
   </si>
   <si>
+    <t>Uta.cse3310.DB.getLeaderboard </t>
+  </si>
+  <si>
     <t>The Database will be created in SQLite3</t>
   </si>
   <si>
+    <t>Uta.cse3310.DB. SQLiteConnector  </t>
+  </si>
+  <si>
     <t xml:space="preserve">The Database shall update the  rank for the winner and loser after a match has ended, which will be signaled by the game termination interface. </t>
   </si>
   <si>
+    <t>Uta.cse3310.DB. UpdatePlayer </t>
+  </si>
+  <si>
     <t xml:space="preserve">The Database shall display a query in which it orders all the accounts in ascending order by ranking having highest rank at the top. </t>
   </si>
   <si>
@@ -780,7 +794,13 @@
     <t>The DB shall return an error message “username unavailable” if the username entered in the login interface matches any entries in the player table Database.</t>
   </si>
   <si>
+    <t>Uta.cse3310.DB.ValidateUser  </t>
+  </si>
+  <si>
     <t>The DB will return player information and player ID to Pair up interface when it is requested and verified that a pair up is possible between players by the Pair up interface.</t>
+  </si>
+  <si>
+    <t>Uta.cse3310.DB.ValidateUser </t>
   </si>
   <si>
     <t>The player ranking shall be a calculated with the following formula
@@ -794,24 +814,6 @@
  dr equals the difference in ratings.</t>
   </si>
   <si>
-    <t>Uta.cse3310.DB.insertUser </t>
-  </si>
-  <si>
-    <t>Uta.cse3310.DB.getLeaderboard </t>
-  </si>
-  <si>
-    <t>Uta.cse3310.DB. SQLiteConnector  </t>
-  </si>
-  <si>
-    <t>Uta.cse3310.DB. UpdatePlayer </t>
-  </si>
-  <si>
-    <t>Uta.cse3310.DB.ValidateUser  </t>
-  </si>
-  <si>
-    <t>Uta.cse3310.DB.ValidateUser </t>
-  </si>
-  <si>
     <t>Uta.cse3310.DB.GetRank </t>
   </si>
   <si>
@@ -821,12 +823,21 @@
     <t>summary.html</t>
   </si>
   <si>
+    <t>U009</t>
+  </si>
+  <si>
+    <t>Summary:</t>
+  </si>
+  <si>
     <t>The results of every game played will be stored into a database. And shall be used for building the contents of the leaderboard</t>
   </si>
   <si>
     <t>summary.js</t>
   </si>
   <si>
+    <t>U010</t>
+  </si>
+  <si>
     <t>The leaderboard page shall display a search bar to search players ranks</t>
   </si>
   <si>
@@ -851,20 +862,146 @@
     <t>The leaderboard page shall have a back button that goes to main menu</t>
   </si>
   <si>
-    <t>U009</t>
-  </si>
-  <si>
-    <t>U010</t>
-  </si>
-  <si>
-    <t>Summary:</t>
+    <t>The system shall convert JSON messages from the frontend into Java objects and send them to the correct part of the backend (like the database, matchmaking, or game logic). It shall also convert Java objects back into JSON to send responses.</t>
+  </si>
+  <si>
+    <t>JSONconverter in pairup_subsys.java, UserEvent.java, App.java</t>
+  </si>
+  <si>
+    <t>The backend shall be written in Java and shall communicate with the frontend, which is made using JavaScript and HTML. The system shall work on any web browser.</t>
+  </si>
+  <si>
+    <t>PageManager.java</t>
+  </si>
+  <si>
+    <t>After a game concludes, a leaderboard will be shown using score data sourced from the gameplay session.</t>
+  </si>
+  <si>
+    <t>getUserScore() in Summary.java</t>
+  </si>
+  <si>
+    <t>The client interface will be a single HTML page that dynamically shows/hides relevant sections depending on the current game state.</t>
+  </si>
+  <si>
+    <t>Managed by frontend; enabled/disabled via received WebSocket events</t>
+  </si>
+  <si>
+    <t>All messages sent and received over WebSockets will be in JSON format, converted to Java using a custom JSONconverter.</t>
+  </si>
+  <si>
+    <t>public class App in App.java (extends WebSocketServer)</t>
+  </si>
+  <si>
+    <t>After a player makes a move, the system shall check the new game state and send an update to the players involved.</t>
+  </si>
+  <si>
+    <t>game_status in game_status.java, handleMoveRequest() in PageManager.java</t>
+  </si>
+  <si>
+    <t>Each client that connects to the system shall be given a unique ID, which shall be used to send messages and manage game logic.</t>
+  </si>
+  <si>
+    <t>int clientId in App.java, linked via UserEvent.id</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Java backend shall be event-driven. The GameManager shall run on a 1-second timer loop, and other parts of the system </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shall respond to events sent through WebSocket.</t>
+    </r>
+  </si>
+  <si>
+    <t>UserEvent in UserEvent.java, timer logic inside GameManager</t>
+  </si>
+  <si>
+    <t>When the backend gets a move from the frontend, it shall check if the move is valid, apply it using the GameManager, and send the updated game status to both players.</t>
+  </si>
+  <si>
+    <t>handleMoveRequest(UserEvent) in PageManager.java, makeMove() in GameManager.java</t>
+  </si>
+  <si>
+    <t>If a player resigns, the system shall log the event in the GameManager and send a message to both players to confirm the resignation and end the game.</t>
+  </si>
+  <si>
+    <t>handleResign(UserEvent) in PageManager.java, processResign() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>If a player offers a draw, the system shall notify the other player. If the draw is accepted, the game shall end and both players shall be notified.</t>
+  </si>
+  <si>
+    <t>handleDrawOffer(UserEvent) and handleDrawAccept(UserEvent) in PageManager.java</t>
+  </si>
+  <si>
+    <t>All event handler methods shall return a `UserEventReply` that includes a `game_status` object and a list of client IDs who should receive the message.</t>
+  </si>
+  <si>
+    <t>UserEventReply in UserEventReply.java, game_status in game_status.java</t>
+  </si>
+  <si>
+    <t>On game start, a show_game_display event will be sent to each player with their ID, assigned color, and starting player information.</t>
+  </si>
+  <si>
+    <t>buildShowGameDisplay() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>On game end (via win, resign, or draw), a hide_game_display event will be sent to all participants.</t>
+  </si>
+  <si>
+    <t>buildHideGameDisplay() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>The backend must support relaying move_made_by_other_player_or_bot messages to ensure clients update pieces visually.</t>
+  </si>
+  <si>
+    <t>processMove() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>Backend must support responding to get_allowed_moves requests and return a list of valid moves in valid_moves format.</t>
+  </si>
+  <si>
+    <t>processAllowedMovesRequest() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>The backend shall be able to send `notify_players` messages for things like game wins or losses, connection issues, or error alerts.</t>
+  </si>
+  <si>
+    <t>buildNotifyPlayers() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>The system shall return the game status for a player when given their player ID.</t>
+  </si>
+  <si>
+    <t>getGameinfo() in GameManagerSubsys.java</t>
+  </si>
+  <si>
+    <t>The system shall retrieve game-related data such as the current turn, winner, loser, and draw status from the controller.</t>
+  </si>
+  <si>
+    <t>Look up game sessions using client ID using GamePageController</t>
+  </si>
+  <si>
+    <t>getAllPlayerIDs(), processMove() in GamePageController.java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,6 +1045,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -917,7 +1073,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -925,11 +1081,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,6 +1200,33 @@
       <alignment horizontal="justify" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,8 +1256,8 @@
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>154</xdr:row>
-      <xdr:rowOff>145294</xdr:rowOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>716794</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1337,28 +1610,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S151"/>
+  <dimension ref="A1:S171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D139" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M147" sqref="M147"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1396,7 +1669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.95">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1404,19 +1677,19 @@
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="48">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1424,22 +1697,22 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.95">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1453,7 +1726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.95">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1467,7 +1740,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="32.1">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1481,7 +1754,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15.95">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1495,7 +1768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="32.1">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1509,7 +1782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="32.1">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1523,7 +1796,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="32.1">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1537,7 +1810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15.95">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1551,7 +1824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15.95">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1565,7 +1838,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15.95">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1579,7 +1852,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="32.1">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1593,7 +1866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15.95">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1607,7 +1880,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="32.1">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1621,7 +1894,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="32.1">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1635,7 +1908,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="32.1">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1649,7 +1922,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="32.1">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1663,7 +1936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.95">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1677,7 +1950,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="32.1">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1691,7 +1964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="48">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1705,7 +1978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="32.1">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1719,7 +1992,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="32.1">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1733,7 +2006,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="48">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1747,7 +2020,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="32.1">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1761,7 +2034,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="32.1">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1775,7 +2048,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="48">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1789,7 +2062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="32.1">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1800,10 +2073,10 @@
         <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="32.1">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1811,13 +2084,13 @@
         <v>33</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:4" ht="32.1">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1825,13 +2098,13 @@
         <v>33</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="32.1">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1839,13 +2112,13 @@
         <v>33</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32.1">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1853,13 +2126,13 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="32.1">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1867,13 +2140,13 @@
         <v>33</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="48">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1881,13 +2154,13 @@
         <v>33</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="48">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1895,13 +2168,13 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="63.95">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1909,13 +2182,13 @@
         <v>33</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="32.1">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1923,13 +2196,13 @@
         <v>33</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="32.1">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1937,13 +2210,13 @@
         <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="32.1">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1951,13 +2224,13 @@
         <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.95">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1965,13 +2238,13 @@
         <v>33</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="32.1">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1979,13 +2252,13 @@
         <v>33</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="32.1">
       <c r="A44">
         <v>41</v>
       </c>
@@ -1993,13 +2266,13 @@
         <v>33</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="32.1">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2007,13 +2280,13 @@
         <v>33</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="32.1">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2021,13 +2294,13 @@
         <v>33</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="48">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2035,13 +2308,13 @@
         <v>33</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32.1">
       <c r="A48">
         <v>45</v>
       </c>
@@ -2049,13 +2322,13 @@
         <v>33</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="32.1">
       <c r="A49">
         <v>46</v>
       </c>
@@ -2063,13 +2336,13 @@
         <v>33</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="32.1">
       <c r="A50">
         <v>47</v>
       </c>
@@ -2077,13 +2350,13 @@
         <v>33</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="32.1">
       <c r="A51">
         <v>48</v>
       </c>
@@ -2091,13 +2364,13 @@
         <v>33</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="32.1">
       <c r="A52">
         <v>49</v>
       </c>
@@ -2105,13 +2378,13 @@
         <v>33</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="48">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2125,7 +2398,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="32.1">
       <c r="A54">
         <v>51</v>
       </c>
@@ -2139,7 +2412,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="15.95">
       <c r="A55">
         <v>52</v>
       </c>
@@ -2153,7 +2426,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="32.1">
       <c r="A56">
         <v>53</v>
       </c>
@@ -2167,7 +2440,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="32.1">
       <c r="A57">
         <v>54</v>
       </c>
@@ -2181,7 +2454,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="32.1">
       <c r="A58">
         <v>55</v>
       </c>
@@ -2195,7 +2468,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="32.1">
       <c r="A59">
         <v>56</v>
       </c>
@@ -2209,7 +2482,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="32.1">
       <c r="A60">
         <v>57</v>
       </c>
@@ -2223,7 +2496,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="32.1">
       <c r="A61">
         <v>58</v>
       </c>
@@ -2237,7 +2510,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="32.1">
       <c r="A62">
         <v>59</v>
       </c>
@@ -2251,7 +2524,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="32.1">
       <c r="A63">
         <v>60</v>
       </c>
@@ -2265,7 +2538,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="32.1">
       <c r="A64">
         <v>61</v>
       </c>
@@ -2279,7 +2552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="63.95">
       <c r="A65">
         <v>62</v>
       </c>
@@ -2293,7 +2566,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="63.95">
       <c r="A66">
         <v>63</v>
       </c>
@@ -2307,7 +2580,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="32.1">
       <c r="A67">
         <v>64</v>
       </c>
@@ -2321,7 +2594,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="32.1">
       <c r="A68">
         <v>65</v>
       </c>
@@ -2335,7 +2608,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="32.1">
       <c r="A69">
         <v>66</v>
       </c>
@@ -2349,7 +2622,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="32.1">
       <c r="A70">
         <v>67</v>
       </c>
@@ -2363,7 +2636,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="48">
       <c r="A71">
         <v>68</v>
       </c>
@@ -2377,7 +2650,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="63.95">
       <c r="A72">
         <v>69</v>
       </c>
@@ -2391,7 +2664,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="32.1">
       <c r="A73">
         <v>70</v>
       </c>
@@ -2402,10 +2675,10 @@
         <v>136</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="48">
       <c r="A74">
         <v>71</v>
       </c>
@@ -2413,13 +2686,13 @@
         <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.95">
       <c r="A75">
         <v>72</v>
       </c>
@@ -2427,13 +2700,13 @@
         <v>35</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="48">
       <c r="A76">
         <v>73</v>
       </c>
@@ -2441,13 +2714,13 @@
         <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="48">
       <c r="A77">
         <v>74</v>
       </c>
@@ -2455,13 +2728,13 @@
         <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="32.1">
       <c r="A78">
         <v>75</v>
       </c>
@@ -2469,13 +2742,13 @@
         <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="32.1">
       <c r="A79">
         <v>76</v>
       </c>
@@ -2483,13 +2756,13 @@
         <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="32.1">
       <c r="A80">
         <v>77</v>
       </c>
@@ -2497,13 +2770,13 @@
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="32.1">
       <c r="A81">
         <v>78</v>
       </c>
@@ -2511,13 +2784,13 @@
         <v>35</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>79</v>
       </c>
@@ -2528,10 +2801,10 @@
         <v>153</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>80</v>
       </c>
@@ -2539,13 +2812,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>81</v>
       </c>
@@ -2553,13 +2826,13 @@
         <v>27</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>82</v>
       </c>
@@ -2567,13 +2840,13 @@
         <v>27</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>83</v>
       </c>
@@ -2581,13 +2854,13 @@
         <v>27</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>84</v>
       </c>
@@ -2595,13 +2868,13 @@
         <v>27</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>85</v>
       </c>
@@ -2609,13 +2882,13 @@
         <v>27</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>86</v>
       </c>
@@ -2623,13 +2896,13 @@
         <v>27</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>87</v>
       </c>
@@ -2637,13 +2910,13 @@
         <v>27</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>88</v>
       </c>
@@ -2651,13 +2924,13 @@
         <v>27</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>89</v>
       </c>
@@ -2665,13 +2938,13 @@
         <v>27</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>90</v>
       </c>
@@ -2679,13 +2952,13 @@
         <v>27</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>91</v>
       </c>
@@ -2693,13 +2966,13 @@
         <v>27</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>92</v>
       </c>
@@ -2707,13 +2980,13 @@
         <v>27</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>93</v>
       </c>
@@ -2721,13 +2994,13 @@
         <v>27</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>94</v>
       </c>
@@ -2735,13 +3008,13 @@
         <v>27</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>95</v>
       </c>
@@ -2749,13 +3022,13 @@
         <v>27</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>96</v>
       </c>
@@ -2763,13 +3036,13 @@
         <v>27</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>97</v>
       </c>
@@ -2777,13 +3050,13 @@
         <v>27</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>98</v>
       </c>
@@ -2791,13 +3064,13 @@
         <v>27</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="32.1">
       <c r="A102">
         <v>99</v>
       </c>
@@ -2808,10 +3081,10 @@
         <v>193</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="48">
       <c r="A103">
         <v>100</v>
       </c>
@@ -2819,13 +3092,13 @@
         <v>36</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="48">
       <c r="A104">
         <v>101</v>
       </c>
@@ -2833,13 +3106,13 @@
         <v>36</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="32.1">
       <c r="A105">
         <v>102</v>
       </c>
@@ -2847,13 +3120,13 @@
         <v>36</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="48">
       <c r="A106">
         <v>103</v>
       </c>
@@ -2861,13 +3134,13 @@
         <v>36</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="32.1">
       <c r="A107">
         <v>104</v>
       </c>
@@ -2875,13 +3148,13 @@
         <v>36</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="96">
       <c r="A108">
         <v>105</v>
       </c>
@@ -2889,13 +3162,13 @@
         <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="32.1">
       <c r="A109">
         <v>106</v>
       </c>
@@ -2903,13 +3176,13 @@
         <v>36</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15.95">
       <c r="A110">
         <v>107</v>
       </c>
@@ -2917,13 +3190,13 @@
         <v>36</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="32.1">
       <c r="A111">
         <v>108</v>
       </c>
@@ -2931,13 +3204,13 @@
         <v>36</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="48">
       <c r="A112">
         <v>109</v>
       </c>
@@ -2945,13 +3218,13 @@
         <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="32.1">
       <c r="A113">
         <v>110</v>
       </c>
@@ -2959,13 +3232,13 @@
         <v>36</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15.95">
       <c r="A114">
         <v>111</v>
       </c>
@@ -2973,13 +3246,13 @@
         <v>36</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="32.1">
       <c r="A115">
         <v>112</v>
       </c>
@@ -2987,13 +3260,13 @@
         <v>36</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="32.1">
       <c r="A116">
         <v>113</v>
       </c>
@@ -3007,7 +3280,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="48">
       <c r="A117">
         <v>114</v>
       </c>
@@ -3015,13 +3288,13 @@
         <v>31</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="32.1">
       <c r="A118">
         <v>115</v>
       </c>
@@ -3029,13 +3302,13 @@
         <v>31</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="32.1">
       <c r="A119">
         <v>116</v>
       </c>
@@ -3043,13 +3316,13 @@
         <v>31</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="48">
       <c r="A120">
         <v>117</v>
       </c>
@@ -3057,13 +3330,13 @@
         <v>31</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="48">
       <c r="A121">
         <v>118</v>
       </c>
@@ -3071,13 +3344,13 @@
         <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="48">
       <c r="A122">
         <v>119</v>
       </c>
@@ -3085,13 +3358,13 @@
         <v>31</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="32.1">
       <c r="A123">
         <v>120</v>
       </c>
@@ -3099,13 +3372,13 @@
         <v>31</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="48">
       <c r="A124">
         <v>121</v>
       </c>
@@ -3113,13 +3386,13 @@
         <v>31</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:4" ht="32.1">
       <c r="A125">
         <v>122</v>
       </c>
@@ -3130,10 +3403,10 @@
         <v>228</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="80.099999999999994">
       <c r="A126">
         <v>123</v>
       </c>
@@ -3141,13 +3414,13 @@
         <v>31</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="80.099999999999994">
       <c r="A127">
         <v>124</v>
       </c>
@@ -3155,13 +3428,13 @@
         <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="48">
       <c r="A128">
         <v>125</v>
       </c>
@@ -3169,13 +3442,13 @@
         <v>31</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" ht="80.099999999999994">
       <c r="A129">
         <v>126</v>
       </c>
@@ -3183,13 +3456,13 @@
         <v>31</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" ht="48">
       <c r="A130">
         <v>127</v>
       </c>
@@ -3197,13 +3470,13 @@
         <v>31</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="33.950000000000003">
       <c r="A131">
         <v>128</v>
       </c>
@@ -3214,10 +3487,10 @@
         <v>238</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" ht="51">
       <c r="A132">
         <v>129</v>
       </c>
@@ -3225,13 +3498,13 @@
         <v>30</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" ht="17.100000000000001">
       <c r="A133">
         <v>130</v>
       </c>
@@ -3239,13 +3512,13 @@
         <v>30</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" ht="51">
       <c r="A134">
         <v>131</v>
       </c>
@@ -3253,13 +3526,13 @@
         <v>30</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" ht="51">
       <c r="A135">
         <v>132</v>
       </c>
@@ -3267,13 +3540,13 @@
         <v>30</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="33.950000000000003">
       <c r="A136">
         <v>133</v>
       </c>
@@ -3281,13 +3554,13 @@
         <v>30</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="51">
       <c r="A137">
         <v>134</v>
       </c>
@@ -3295,13 +3568,13 @@
         <v>30</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="33.950000000000003">
       <c r="A138">
         <v>135</v>
       </c>
@@ -3309,13 +3582,13 @@
         <v>30</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" ht="68.099999999999994">
       <c r="A139">
         <v>136</v>
       </c>
@@ -3323,13 +3596,13 @@
         <v>30</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" ht="68.099999999999994">
       <c r="A140">
         <v>137</v>
       </c>
@@ -3337,13 +3610,13 @@
         <v>30</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="207.95">
       <c r="A141">
         <v>138</v>
       </c>
@@ -3351,13 +3624,13 @@
         <v>30</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D141" s="9" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" ht="15.95">
       <c r="A142">
         <v>139</v>
       </c>
@@ -3371,13 +3644,13 @@
         <v>257</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="R142" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="48">
       <c r="A143">
         <v>140</v>
       </c>
@@ -3385,16 +3658,16 @@
         <v>28</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D143" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" ht="32.1">
       <c r="A144">
         <v>141</v>
       </c>
@@ -3402,13 +3675,13 @@
         <v>28</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D144" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="15.95">
       <c r="A145">
         <v>142</v>
       </c>
@@ -3416,13 +3689,13 @@
         <v>28</v>
       </c>
       <c r="C145" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D145" t="s">
         <v>261</v>
       </c>
-      <c r="D145" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:4" ht="32.1">
       <c r="A146">
         <v>143</v>
       </c>
@@ -3430,13 +3703,13 @@
         <v>28</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D146" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="32.1">
       <c r="A147">
         <v>144</v>
       </c>
@@ -3444,13 +3717,13 @@
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D147" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="32.1">
       <c r="A148">
         <v>145</v>
       </c>
@@ -3458,13 +3731,13 @@
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D148" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="15.95">
       <c r="A149">
         <v>146</v>
       </c>
@@ -3472,13 +3745,13 @@
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D149" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="32.1">
       <c r="A150">
         <v>147</v>
       </c>
@@ -3486,13 +3759,13 @@
         <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D150" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="32.1">
       <c r="A151">
         <v>148</v>
       </c>
@@ -3500,10 +3773,290 @@
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D151" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="72.75">
+      <c r="A152">
+        <v>149</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D152" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="57.75">
+      <c r="A153">
+        <v>150</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D153" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="23.25">
+      <c r="A154">
+        <v>151</v>
+      </c>
+      <c r="B154">
+        <v>3</v>
+      </c>
+      <c r="C154" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D154" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="35.25">
+      <c r="A155">
+        <v>152</v>
+      </c>
+      <c r="B155">
+        <v>4</v>
+      </c>
+      <c r="C155" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D155" s="12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="35.25">
+      <c r="A156">
+        <v>153</v>
+      </c>
+      <c r="B156">
+        <v>5</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D156" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="43.5">
+      <c r="A157">
+        <v>154</v>
+      </c>
+      <c r="B157">
+        <v>6</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D157" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="43.5">
+      <c r="A158">
+        <v>155</v>
+      </c>
+      <c r="B158">
+        <v>7</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D158" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="57.75">
+      <c r="A159">
+        <v>156</v>
+      </c>
+      <c r="B159">
+        <v>8</v>
+      </c>
+      <c r="C159" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D159" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="57.75">
+      <c r="A160">
+        <v>157</v>
+      </c>
+      <c r="B160">
+        <v>9</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D160" s="14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="43.5">
+      <c r="A161">
+        <v>158</v>
+      </c>
+      <c r="B161">
+        <v>10</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D161" s="14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="43.5">
+      <c r="A162">
+        <v>159</v>
+      </c>
+      <c r="B162">
+        <v>11</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D162" s="14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="46.5">
+      <c r="A163">
+        <v>160</v>
+      </c>
+      <c r="B163">
+        <v>12</v>
+      </c>
+      <c r="C163" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D163" s="14" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="35.25">
+      <c r="A164">
+        <v>161</v>
+      </c>
+      <c r="B164">
+        <v>13</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D164" s="14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="35.25">
+      <c r="A165">
+        <v>162</v>
+      </c>
+      <c r="B165">
+        <v>14</v>
+      </c>
+      <c r="C165" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D165" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="35.25">
+      <c r="A166">
+        <v>163</v>
+      </c>
+      <c r="B166">
+        <v>15</v>
+      </c>
+      <c r="C166" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D166" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="35.25">
+      <c r="A167">
+        <v>164</v>
+      </c>
+      <c r="B167">
+        <v>16</v>
+      </c>
+      <c r="C167" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="D167" s="14" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="35.25">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168">
+        <v>17</v>
+      </c>
+      <c r="C168" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D168" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="23.25">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <v>18</v>
+      </c>
+      <c r="C169" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D169" s="15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="35.25">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170">
+        <v>19</v>
+      </c>
+      <c r="C170" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D170" s="15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="23.25">
+      <c r="A171">
+        <v>168</v>
+      </c>
+      <c r="B171">
+        <v>20</v>
+      </c>
+      <c r="C171" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="D171" s="17" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added group 32 game manager requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/cmb6906_mavs_uta_edu/Documents/2024-2025/Spring/Fundamentals of SE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\GitRepos\cse3310-sp25-002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{879BA1B7-AEFB-1F4C-96A0-906E7F19F358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39493073-E4FC-43A9-95E0-73D5DF3F67C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A7EB0-011B-4F4E-A4CE-1E991D561FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="380">
   <si>
     <t>Tested By</t>
   </si>
@@ -904,13 +904,289 @@
     <t>int clientId in App.java, linked via UserEvent.id</t>
   </si>
   <si>
+    <t>UserEvent in UserEvent.java, timer logic inside GameManager</t>
+  </si>
+  <si>
+    <t>When the backend gets a move from the frontend, it shall check if the move is valid, apply it using the GameManager, and send the updated game status to both players.</t>
+  </si>
+  <si>
+    <t>handleMoveRequest(UserEvent) in PageManager.java, makeMove() in GameManager.java</t>
+  </si>
+  <si>
+    <t>If a player resigns, the system shall log the event in the GameManager and send a message to both players to confirm the resignation and end the game.</t>
+  </si>
+  <si>
+    <t>handleResign(UserEvent) in PageManager.java, processResign() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>If a player offers a draw, the system shall notify the other player. If the draw is accepted, the game shall end and both players shall be notified.</t>
+  </si>
+  <si>
+    <t>handleDrawOffer(UserEvent) and handleDrawAccept(UserEvent) in PageManager.java</t>
+  </si>
+  <si>
+    <t>All event handler methods shall return a `UserEventReply` that includes a `game_status` object and a list of client IDs who should receive the message.</t>
+  </si>
+  <si>
+    <t>UserEventReply in UserEventReply.java, game_status in game_status.java</t>
+  </si>
+  <si>
+    <t>On game start, a show_game_display event will be sent to each player with their ID, assigned color, and starting player information.</t>
+  </si>
+  <si>
+    <t>buildShowGameDisplay() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>On game end (via win, resign, or draw), a hide_game_display event will be sent to all participants.</t>
+  </si>
+  <si>
+    <t>buildHideGameDisplay() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>The backend must support relaying move_made_by_other_player_or_bot messages to ensure clients update pieces visually.</t>
+  </si>
+  <si>
+    <t>processMove() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>Backend must support responding to get_allowed_moves requests and return a list of valid moves in valid_moves format.</t>
+  </si>
+  <si>
+    <t>processAllowedMovesRequest() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>The backend shall be able to send `notify_players` messages for things like game wins or losses, connection issues, or error alerts.</t>
+  </si>
+  <si>
+    <t>buildNotifyPlayers() in GameDisplayConnector.java</t>
+  </si>
+  <si>
+    <t>The system shall return the game status for a player when given their player ID.</t>
+  </si>
+  <si>
+    <t>getGameinfo() in GameManagerSubsys.java</t>
+  </si>
+  <si>
+    <t>The system shall retrieve game-related data such as the current turn, winner, loser, and draw status from the controller.</t>
+  </si>
+  <si>
+    <t>Look up game sessions using client ID using GamePageController</t>
+  </si>
+  <si>
+    <t>getAllPlayerIDs(), processMove() in GamePageController.java</t>
+  </si>
+  <si>
+    <t>The system shall have an object of squared data type for each individual board</t>
+  </si>
+  <si>
+    <t>GameManager/Board.getSquare, GameManager/Square.Square()</t>
+  </si>
+  <si>
+    <t>The board shall be a 2D array of Square objects</t>
+  </si>
+  <si>
+    <t>GameManager/Board.Board()</t>
+  </si>
+  <si>
+    <t>Move objects shall be linked list data structures to allow multiple steps in a single participant move</t>
+  </si>
+  <si>
+    <t>GameManager/Moves.Moves(), GameManager/move.Move()</t>
+  </si>
+  <si>
+    <t>The system shall enforce turn-based play using a boolean system</t>
+  </si>
+  <si>
+    <t>The system shall receive moves from players or bots and incorporate them from Square destination into the board</t>
+  </si>
+  <si>
+    <t>The system shall place each player ID to their designated board and team once they're matched together</t>
+  </si>
+  <si>
+    <t>GameManager/GamePairController.newMatch()</t>
+  </si>
+  <si>
+    <t>The system shall have colors of white and black randomly assigned to each player, where one is white and the other is black</t>
+  </si>
+  <si>
+    <t>GameManager/Game.Game</t>
+  </si>
+  <si>
+    <t>The system shall update the score of the player after a piece is captured</t>
+  </si>
+  <si>
+    <t>GameManager/Player.addScore()</t>
+  </si>
+  <si>
+    <t>The system shall process a given Move object and respond with an disapproval alert if it is illegal</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.processMove()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall contain information of the position of the piece occupying a square </t>
+  </si>
+  <si>
+    <t>GameManager/Square.getRow()|.getColumn()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall contain information of the type of piece occupying a square </t>
+  </si>
+  <si>
+    <t>GameManager/Square.getColor()|.isKing()</t>
+  </si>
+  <si>
+    <t>Move objects shall be utilized to encode the requested move from both players and bots</t>
+  </si>
+  <si>
+    <t>GameManager/Moves.makeMove()</t>
+  </si>
+  <si>
+    <t>Checks whether the game is active</t>
+  </si>
+  <si>
+    <t>GameManager/Game.gameActive()</t>
+  </si>
+  <si>
+    <t>Verfies whether slots are available to create a new game and creates one if so</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.createGame()</t>
+  </si>
+  <si>
+    <t>Deals with game termination and notifies GameTermination</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.terminateGame()</t>
+  </si>
+  <si>
+    <t>Deals with restarting the game</t>
+  </si>
+  <si>
+    <t>Initialises a new game with the relevant data to accomodate pairups</t>
+  </si>
+  <si>
+    <t>Deals with the piece count on the board</t>
+  </si>
+  <si>
+    <t>GameManager/Player.getPieces()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deals with the pieces taken </t>
+  </si>
+  <si>
+    <t>GameManager/Player.takePieces()</t>
+  </si>
+  <si>
+    <t>PageManager shall be able to receive game ID's and the current board</t>
+  </si>
+  <si>
+    <t>GameManager/GamePageController.sendBoard()</t>
+  </si>
+  <si>
+    <t>GamePlay shall be able to access a list of moves</t>
+  </si>
+  <si>
+    <t>GameManager/GamePageController.processMove()</t>
+  </si>
+  <si>
+    <t>The system will support a maximum of 10 concurrent games</t>
+  </si>
+  <si>
+    <t>GameManager</t>
+  </si>
+  <si>
+    <t>Returns the game called by the searched player ID</t>
+  </si>
+  <si>
+    <t>GameManager/GamePageController.returnGame(), GameManager/GameManager.findGameByPlayerId</t>
+  </si>
+  <si>
+    <t>Tracks captures being made</t>
+  </si>
+  <si>
+    <t>GameManager/Game.lastCapture()</t>
+  </si>
+  <si>
+    <t>Returns the winner and loser of the game</t>
+  </si>
+  <si>
+    <t>GameManager/Game.getWinner()|.getLoser(), GameManager/GamePageController.getWinner()|.getLoser()</t>
+  </si>
+  <si>
+    <t>Updates the state of the board</t>
+  </si>
+  <si>
+    <t>GameManager/Game.updateBoard(), GameManager/Board.getSquare()</t>
+  </si>
+  <si>
+    <t>Checks whether the player is a bot or not</t>
+  </si>
+  <si>
+    <t>GameManager/Game.isPlayer1Bot()|.isPlayer2Bot()</t>
+  </si>
+  <si>
+    <t>Checks if a player is in an active game</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.isPlayerInGame()</t>
+  </si>
+  <si>
+    <t>Returns active game count</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.getActiveGameCount()</t>
+  </si>
+  <si>
+    <t>Removes a player from game if needed</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.removePlayer()</t>
+  </si>
+  <si>
+    <t>Processes player requests to quit game</t>
+  </si>
+  <si>
+    <t>GameManager/GameManager.playerQuit()</t>
+  </si>
+  <si>
+    <t>Utilises pair made by GamePairController while creating games</t>
+  </si>
+  <si>
+    <t>Returns the player whose turn it is</t>
+  </si>
+  <si>
+    <t>GameManager/GamePageController.playerTurn()</t>
+  </si>
+  <si>
+    <t>Returns that the game was declared a draw</t>
+  </si>
+  <si>
+    <t>GameManager/GamePageController.getDraw()</t>
+  </si>
+  <si>
+    <t>GameManager/Game.progressGame()</t>
+  </si>
+  <si>
+    <t>The system shall manage the game state for each active match</t>
+  </si>
+  <si>
+    <t>GameManager/Game, GameManager/GameManager.requestBotMoves</t>
+  </si>
+  <si>
+    <t>The system shall receive moves performed by Bot 1 and Bot 2</t>
+  </si>
+  <si>
+    <t>GameManager/Game.switchTurn()</t>
+  </si>
+  <si>
+    <t>GameManager/Board.execute(), GameManager/Move.getStart()|.getDest()</t>
+  </si>
+  <si>
+    <t>U005</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">The Java backend shall be event-driven. The GameManager shall run on a 1-second timer loop, and other parts of the system </t>
     </r>
     <r>
@@ -919,107 +1195,24 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>shall respond to events sent through WebSocket.</t>
     </r>
-  </si>
-  <si>
-    <t>UserEvent in UserEvent.java, timer logic inside GameManager</t>
-  </si>
-  <si>
-    <t>When the backend gets a move from the frontend, it shall check if the move is valid, apply it using the GameManager, and send the updated game status to both players.</t>
-  </si>
-  <si>
-    <t>handleMoveRequest(UserEvent) in PageManager.java, makeMove() in GameManager.java</t>
-  </si>
-  <si>
-    <t>If a player resigns, the system shall log the event in the GameManager and send a message to both players to confirm the resignation and end the game.</t>
-  </si>
-  <si>
-    <t>handleResign(UserEvent) in PageManager.java, processResign() in GameDisplayConnector.java</t>
-  </si>
-  <si>
-    <t>If a player offers a draw, the system shall notify the other player. If the draw is accepted, the game shall end and both players shall be notified.</t>
-  </si>
-  <si>
-    <t>handleDrawOffer(UserEvent) and handleDrawAccept(UserEvent) in PageManager.java</t>
-  </si>
-  <si>
-    <t>All event handler methods shall return a `UserEventReply` that includes a `game_status` object and a list of client IDs who should receive the message.</t>
-  </si>
-  <si>
-    <t>UserEventReply in UserEventReply.java, game_status in game_status.java</t>
-  </si>
-  <si>
-    <t>On game start, a show_game_display event will be sent to each player with their ID, assigned color, and starting player information.</t>
-  </si>
-  <si>
-    <t>buildShowGameDisplay() in GameDisplayConnector.java</t>
-  </si>
-  <si>
-    <t>On game end (via win, resign, or draw), a hide_game_display event will be sent to all participants.</t>
-  </si>
-  <si>
-    <t>buildHideGameDisplay() in GameDisplayConnector.java</t>
-  </si>
-  <si>
-    <t>The backend must support relaying move_made_by_other_player_or_bot messages to ensure clients update pieces visually.</t>
-  </si>
-  <si>
-    <t>processMove() in GameDisplayConnector.java</t>
-  </si>
-  <si>
-    <t>Backend must support responding to get_allowed_moves requests and return a list of valid moves in valid_moves format.</t>
-  </si>
-  <si>
-    <t>processAllowedMovesRequest() in GameDisplayConnector.java</t>
-  </si>
-  <si>
-    <t>The backend shall be able to send `notify_players` messages for things like game wins or losses, connection issues, or error alerts.</t>
-  </si>
-  <si>
-    <t>buildNotifyPlayers() in GameDisplayConnector.java</t>
-  </si>
-  <si>
-    <t>The system shall return the game status for a player when given their player ID.</t>
-  </si>
-  <si>
-    <t>getGameinfo() in GameManagerSubsys.java</t>
-  </si>
-  <si>
-    <t>The system shall retrieve game-related data such as the current turn, winner, loser, and draw status from the controller.</t>
-  </si>
-  <si>
-    <t>Look up game sessions using client ID using GamePageController</t>
-  </si>
-  <si>
-    <t>getAllPlayerIDs(), processMove() in GamePageController.java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1029,32 +1222,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1062,6 +1232,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1073,7 +1244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1081,101 +1252,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1183,49 +1264,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1610,13 +1698,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S171"/>
+  <dimension ref="A1:S207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A172" sqref="A172"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
@@ -1626,12 +1714,12 @@
     <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1669,11 +1757,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.95">
-      <c r="A3" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1689,17 +1777,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="48">
-      <c r="A4">
+    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="12">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1712,2352 +1800,2922 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.95">
-      <c r="A5">
+    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="13">
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.95">
-      <c r="A6">
+    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="13">
         <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32.1">
-      <c r="A7">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="13">
         <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.95">
-      <c r="A8">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="13">
         <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="32.1">
-      <c r="A9">
+    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="32.1">
-      <c r="A10">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="32.1">
-      <c r="A11">
+    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="13">
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.95">
-      <c r="A12">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
         <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.95">
-      <c r="A13">
+    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="13">
         <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.95">
-      <c r="A14">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="13">
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="32.1">
-      <c r="A15">
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="13">
         <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.95">
-      <c r="A16">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="13">
         <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32.1">
-      <c r="A17">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="13">
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32.1">
-      <c r="A18">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <v>15</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="13">
         <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32.1">
-      <c r="A19">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="13">
         <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32.1">
-      <c r="A20">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>17</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="13">
         <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.95">
-      <c r="A21">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>18</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="13">
         <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32.1">
-      <c r="A22">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="13">
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48">
-      <c r="A23">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="13">
         <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32.1">
-      <c r="A24">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="13">
         <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32.1">
-      <c r="A25">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
         <v>22</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="13">
         <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48">
-      <c r="A26">
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <v>23</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="13">
         <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32.1">
-      <c r="A27">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
         <v>24</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="13">
         <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32.1">
-      <c r="A28">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
         <v>25</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="13">
         <v>34</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="48">
-      <c r="A29">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
         <v>26</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="13">
         <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="32.1">
-      <c r="A30">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
         <v>27</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="13">
         <v>33</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="32.1">
-      <c r="A31">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
         <v>28</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="13">
         <v>33</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32.1">
-      <c r="A32">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
         <v>29</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="13">
         <v>33</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32.1">
-      <c r="A33">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
         <v>30</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="13">
         <v>33</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32.1">
-      <c r="A34">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
         <v>31</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="13">
         <v>33</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32.1">
-      <c r="A35">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
         <v>32</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="13">
         <v>33</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="48">
-      <c r="A36">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
         <v>33</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="13">
         <v>33</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="48">
-      <c r="A37">
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
         <v>34</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="13">
         <v>33</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="63.95">
-      <c r="A38">
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
         <v>35</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="13">
         <v>33</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32.1">
-      <c r="A39">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
         <v>36</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="13">
         <v>33</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32.1">
-      <c r="A40">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
         <v>37</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="13">
         <v>33</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32.1">
-      <c r="A41">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
         <v>38</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="13">
         <v>33</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.95">
-      <c r="A42">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
         <v>39</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="13">
         <v>33</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32.1">
-      <c r="A43">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
         <v>40</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="13">
         <v>33</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="32.1">
-      <c r="A44">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
         <v>41</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="13">
         <v>33</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="32.1">
-      <c r="A45">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
         <v>42</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="13">
         <v>33</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32.1">
-      <c r="A46">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
         <v>43</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="13">
         <v>33</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="48">
-      <c r="A47">
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
         <v>44</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="13">
         <v>33</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="32.1">
-      <c r="A48">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
         <v>45</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="13">
         <v>33</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="32.1">
-      <c r="A49">
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
         <v>46</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="13">
         <v>33</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="32.1">
-      <c r="A50">
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
         <v>47</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="13">
         <v>33</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32.1">
-      <c r="A51">
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
         <v>48</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="13">
         <v>33</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="32.1">
-      <c r="A52">
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
         <v>49</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="13">
         <v>33</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48">
-      <c r="A53">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
         <v>50</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="13">
         <v>26</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="32.1">
-      <c r="A54">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
         <v>51</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="13">
         <v>26</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.95">
-      <c r="A55">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="13">
         <v>52</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="13">
         <v>26</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="32.1">
-      <c r="A56">
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
         <v>53</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="13">
         <v>26</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="32.1">
-      <c r="A57">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
         <v>54</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="13">
         <v>26</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="32.1">
-      <c r="A58">
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="13">
         <v>55</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="13">
         <v>26</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="32.1">
-      <c r="A59">
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="13">
         <v>56</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="13">
         <v>26</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="32.1">
-      <c r="A60">
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="13">
         <v>57</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="13">
         <v>26</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="32.1">
-      <c r="A61">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="13">
         <v>58</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="13">
         <v>26</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="32.1">
-      <c r="A62">
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="13">
         <v>59</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="13">
         <v>26</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="32.1">
-      <c r="A63">
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="13">
         <v>60</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="13">
         <v>26</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="32.1">
-      <c r="A64">
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="13">
         <v>61</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="13">
         <v>26</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="63.95">
-      <c r="A65">
+    <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="13">
         <v>62</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="13">
         <v>26</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="63.95">
-      <c r="A66">
+    <row r="66" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="13">
         <v>63</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="13">
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="32.1">
-      <c r="A67">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="13">
         <v>64</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="13">
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="32.1">
-      <c r="A68">
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
         <v>65</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="13">
         <v>26</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="16" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="32.1">
-      <c r="A69">
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="13">
         <v>66</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="13">
         <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="32.1">
-      <c r="A70">
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="13">
         <v>67</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="13">
         <v>26</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="48">
-      <c r="A71">
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="13">
         <v>68</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="13">
         <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="63.95">
-      <c r="A72">
+    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="13">
         <v>69</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="13">
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="32.1">
-      <c r="A73">
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="13">
         <v>70</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="13">
         <v>35</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="48">
-      <c r="A74">
+    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="13">
         <v>71</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="13">
         <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.95">
-      <c r="A75">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="13">
         <v>72</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="13">
         <v>35</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="48">
-      <c r="A76">
+    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="13">
         <v>73</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="13">
         <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="48">
-      <c r="A77">
+    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="13">
         <v>74</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="13">
         <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="32.1">
-      <c r="A78">
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="13">
         <v>75</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="13">
         <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="32.1">
-      <c r="A79">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="13">
         <v>76</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="13">
         <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="32.1">
-      <c r="A80">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="13">
         <v>77</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="13">
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="32.1">
-      <c r="A81">
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="13">
         <v>78</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="13">
         <v>35</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="16" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82">
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="13">
         <v>79</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="13">
         <v>27</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="15" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="13">
         <v>80</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="13">
         <v>27</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84">
+    <row r="84" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A84" s="13">
         <v>81</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="13">
         <v>27</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85">
+    <row r="85" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A85" s="13">
         <v>82</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="13">
         <v>27</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86">
+    <row r="86" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A86" s="13">
         <v>83</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="13">
         <v>27</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="13">
         <v>84</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="13">
         <v>27</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88">
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="13">
         <v>85</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="13">
         <v>27</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89">
+    <row r="89" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A89" s="13">
         <v>86</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="13">
         <v>27</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="13">
         <v>87</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="13">
         <v>27</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91">
+    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="13">
         <v>88</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="13">
         <v>27</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
-      <c r="A92">
+    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="13">
         <v>89</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="13">
         <v>27</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="15" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93">
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="13">
         <v>90</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="13">
         <v>27</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94">
+    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="13">
         <v>91</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="13">
         <v>27</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95">
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="13">
         <v>92</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="13">
         <v>27</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96">
+    <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="13">
         <v>93</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="13">
         <v>27</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="15" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97">
+    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="13">
         <v>94</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="13">
         <v>27</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98">
+    <row r="98" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="13">
         <v>95</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="13">
         <v>27</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="15" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99">
+    <row r="99" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="13">
         <v>96</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="13">
         <v>27</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="15" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100">
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="13">
         <v>97</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="13">
         <v>27</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="15" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="13">
         <v>98</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="13">
         <v>27</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="32.1">
-      <c r="A102">
+    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="13">
         <v>99</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="13">
         <v>36</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="48">
-      <c r="A103">
+    <row r="103" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A103" s="13">
         <v>100</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="13">
         <v>36</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="48">
-      <c r="A104">
+    <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="13">
         <v>101</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="13">
         <v>36</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="32.1">
-      <c r="A105">
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="13">
         <v>102</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="13">
         <v>36</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="15" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="48">
-      <c r="A106">
+    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="13">
         <v>103</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="13">
         <v>36</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="32.1">
-      <c r="A107">
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="13">
         <v>104</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="13">
         <v>36</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="15" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="96">
-      <c r="A108">
+    <row r="108" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A108" s="13">
         <v>105</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="13">
         <v>36</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="32.1">
-      <c r="A109">
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="13">
         <v>106</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="13">
         <v>36</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" s="15" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.95">
-      <c r="A110">
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="13">
         <v>107</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="13">
         <v>36</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="32.1">
-      <c r="A111">
+    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="13">
         <v>108</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="13">
         <v>36</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="48">
-      <c r="A112">
+    <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A112" s="13">
         <v>109</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="13">
         <v>36</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="32.1">
-      <c r="A113">
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="13">
         <v>110</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="13">
         <v>36</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.95">
-      <c r="A114">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="13">
         <v>111</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="13">
         <v>36</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="32.1">
-      <c r="A115">
+    <row r="115" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="13">
         <v>112</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="13">
         <v>36</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="15" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="32.1">
-      <c r="A116">
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="13">
         <v>113</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="13">
         <v>36</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="15" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="48">
-      <c r="A117">
+    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="13">
         <v>114</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="13">
         <v>31</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="15" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="32.1">
-      <c r="A118">
+    <row r="118" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="13">
         <v>115</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="13">
         <v>31</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" s="15" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="32.1">
-      <c r="A119">
+    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="13">
         <v>116</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="13">
         <v>31</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="15" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="48">
-      <c r="A120">
+    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="13">
         <v>117</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="13">
         <v>31</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="48">
-      <c r="A121">
+    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A121" s="13">
         <v>118</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="13">
         <v>31</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="15" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="48">
-      <c r="A122">
+    <row r="122" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A122" s="13">
         <v>119</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="13">
         <v>31</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="15" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="32.1">
-      <c r="A123">
+    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="13">
         <v>120</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="13">
         <v>31</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="15" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="48">
-      <c r="A124">
+    <row r="124" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A124" s="13">
         <v>121</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="13">
         <v>31</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="32.1">
-      <c r="A125">
+    <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="13">
         <v>122</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="13">
         <v>31</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="80.099999999999994">
-      <c r="A126">
+    <row r="126" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A126" s="13">
         <v>123</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="13">
         <v>31</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="80.099999999999994">
-      <c r="A127">
+    <row r="127" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A127" s="13">
         <v>124</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="13">
         <v>31</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" s="15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="48">
-      <c r="A128">
+    <row r="128" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A128" s="13">
         <v>125</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="13">
         <v>31</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D128" s="15" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="80.099999999999994">
-      <c r="A129">
+    <row r="129" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A129" s="13">
         <v>126</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="13">
         <v>31</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D129" s="15" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="48">
-      <c r="A130">
+    <row r="130" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A130" s="13">
         <v>127</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="13">
         <v>31</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D130" s="15" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="33.950000000000003">
-      <c r="A131">
+    <row r="131" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="13">
         <v>128</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="13">
         <v>30</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D131" s="9" t="s">
+      <c r="D131" s="17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="51">
-      <c r="A132">
+    <row r="132" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A132" s="13">
         <v>129</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="13">
         <v>30</v>
       </c>
-      <c r="C132" s="8" t="s">
+      <c r="C132" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="D132" s="9" t="s">
+      <c r="D132" s="17" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="17.100000000000001">
-      <c r="A133">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A133" s="13">
         <v>130</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="13">
         <v>30</v>
       </c>
-      <c r="C133" s="8" t="s">
+      <c r="C133" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D133" s="9" t="s">
+      <c r="D133" s="17" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="51">
-      <c r="A134">
+    <row r="134" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A134" s="13">
         <v>131</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="13">
         <v>30</v>
       </c>
-      <c r="C134" s="8" t="s">
+      <c r="C134" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="D134" s="9" t="s">
+      <c r="D134" s="17" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="51">
-      <c r="A135">
+    <row r="135" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A135" s="13">
         <v>132</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="13">
         <v>30</v>
       </c>
-      <c r="C135" s="8" t="s">
+      <c r="C135" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="D135" s="9" t="s">
+      <c r="D135" s="17" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="33.950000000000003">
-      <c r="A136">
+    <row r="136" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="13">
         <v>133</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="13">
         <v>30</v>
       </c>
-      <c r="C136" s="8" t="s">
+      <c r="C136" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="D136" s="9" t="s">
+      <c r="D136" s="17" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="51">
-      <c r="A137">
+    <row r="137" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A137" s="13">
         <v>134</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="13">
         <v>30</v>
       </c>
-      <c r="C137" s="8" t="s">
+      <c r="C137" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D137" s="9" t="s">
+      <c r="D137" s="17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="33.950000000000003">
-      <c r="A138">
+    <row r="138" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="13">
         <v>135</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="13">
         <v>30</v>
       </c>
-      <c r="C138" s="8" t="s">
+      <c r="C138" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="D138" s="9" t="s">
+      <c r="D138" s="17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="68.099999999999994">
-      <c r="A139">
+    <row r="139" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A139" s="13">
         <v>136</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="13">
         <v>30</v>
       </c>
-      <c r="C139" s="8" t="s">
+      <c r="C139" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="D139" s="9" t="s">
+      <c r="D139" s="17" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="68.099999999999994">
-      <c r="A140">
+    <row r="140" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A140" s="13">
         <v>137</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="13">
         <v>30</v>
       </c>
-      <c r="C140" s="8" t="s">
+      <c r="C140" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="D140" s="9" t="s">
+      <c r="D140" s="17" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="207.95">
-      <c r="A141">
+    <row r="141" spans="1:18" ht="195" x14ac:dyDescent="0.25">
+      <c r="A141" s="13">
         <v>138</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="13">
         <v>30</v>
       </c>
-      <c r="C141" s="6" t="s">
+      <c r="C141" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D141" s="9" t="s">
+      <c r="D141" s="17" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="15.95">
-      <c r="A142">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
         <v>139</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="14">
         <v>28</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="E142" s="4" t="s">
         <v>258</v>
       </c>
       <c r="R142" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="48">
-      <c r="A143">
+    <row r="143" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
         <v>140</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="14">
         <v>28</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="E143" s="1" t="s">
+      <c r="E143" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="32.1">
-      <c r="A144">
+    <row r="144" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A144" s="14">
         <v>141</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="14">
         <v>28</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="15" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="15.95">
-      <c r="A145">
+      <c r="E144" s="4"/>
+    </row>
+    <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="14">
         <v>142</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="14">
         <v>28</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="15" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="32.1">
-      <c r="A146">
+      <c r="E145" s="4"/>
+    </row>
+    <row r="146" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="14">
         <v>143</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="14">
         <v>28</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="15" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="32.1">
-      <c r="A147">
+      <c r="E146" s="4"/>
+    </row>
+    <row r="147" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A147" s="14">
         <v>144</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="14">
         <v>28</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="15" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" ht="32.1">
-      <c r="A148">
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
         <v>145</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="14">
         <v>28</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="15" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="15.95">
-      <c r="A149">
+      <c r="E148" s="4"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
         <v>146</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="14">
         <v>28</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="15" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" ht="32.1">
-      <c r="A150">
+      <c r="E149" s="4"/>
+    </row>
+    <row r="150" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
         <v>147</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="14">
         <v>28</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="15" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="32.1">
-      <c r="A151">
+      <c r="E150" s="4"/>
+    </row>
+    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
         <v>148</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="14">
         <v>28</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="15" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="72.75">
-      <c r="A152">
+      <c r="E151" s="4"/>
+    </row>
+    <row r="152" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
         <v>149</v>
       </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
-      <c r="C152" s="1" t="s">
+      <c r="B152" s="14">
+        <v>29</v>
+      </c>
+      <c r="C152" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="D152" s="10" t="s">
+      <c r="D152" s="18" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" ht="57.75">
-      <c r="A153">
+      <c r="E152" s="4"/>
+    </row>
+    <row r="153" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
         <v>150</v>
       </c>
-      <c r="B153">
-        <v>2</v>
-      </c>
-      <c r="C153" s="1" t="s">
+      <c r="B153" s="14">
+        <v>29</v>
+      </c>
+      <c r="C153" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="D153" s="12" t="s">
+      <c r="D153" s="18" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" ht="23.25">
-      <c r="A154">
+      <c r="E153" s="4"/>
+    </row>
+    <row r="154" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
         <v>151</v>
       </c>
-      <c r="B154">
-        <v>3</v>
-      </c>
-      <c r="C154" s="11" t="s">
+      <c r="B154" s="14">
+        <v>29</v>
+      </c>
+      <c r="C154" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D154" s="12" t="s">
+      <c r="D154" s="18" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" ht="35.25">
-      <c r="A155">
+      <c r="E154" s="4"/>
+    </row>
+    <row r="155" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
         <v>152</v>
       </c>
-      <c r="B155">
-        <v>4</v>
-      </c>
-      <c r="C155" s="11" t="s">
+      <c r="B155" s="14">
+        <v>29</v>
+      </c>
+      <c r="C155" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="D155" s="12" t="s">
+      <c r="D155" s="18" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" ht="35.25">
-      <c r="A156">
+      <c r="E155" s="4"/>
+    </row>
+    <row r="156" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
         <v>153</v>
       </c>
-      <c r="B156">
-        <v>5</v>
-      </c>
-      <c r="C156" s="11" t="s">
+      <c r="B156" s="14">
+        <v>29</v>
+      </c>
+      <c r="C156" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="D156" s="12" t="s">
+      <c r="D156" s="18" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" ht="43.5">
-      <c r="A157">
+      <c r="E156" s="4"/>
+    </row>
+    <row r="157" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
         <v>154</v>
       </c>
-      <c r="B157">
-        <v>6</v>
-      </c>
-      <c r="C157" s="1" t="s">
+      <c r="B157" s="14">
+        <v>29</v>
+      </c>
+      <c r="C157" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="D157" s="12" t="s">
+      <c r="D157" s="18" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" ht="43.5">
-      <c r="A158">
+      <c r="E157" s="4"/>
+    </row>
+    <row r="158" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
         <v>155</v>
       </c>
-      <c r="B158">
-        <v>7</v>
-      </c>
-      <c r="C158" s="1" t="s">
+      <c r="B158" s="14">
+        <v>29</v>
+      </c>
+      <c r="C158" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D158" s="12" t="s">
+      <c r="D158" s="18" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" ht="57.75">
-      <c r="A159">
+      <c r="E158" s="4"/>
+    </row>
+    <row r="159" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
         <v>156</v>
       </c>
-      <c r="B159">
-        <v>8</v>
-      </c>
-      <c r="C159" s="18" t="s">
+      <c r="B159" s="14">
+        <v>29</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D159" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="D159" s="12" t="s">
+      <c r="E159" s="4"/>
+    </row>
+    <row r="160" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>157</v>
+      </c>
+      <c r="B160" s="14">
+        <v>29</v>
+      </c>
+      <c r="C160" s="5" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" ht="57.75">
-      <c r="A160">
-        <v>157</v>
-      </c>
-      <c r="B160">
-        <v>9</v>
-      </c>
-      <c r="C160" s="1" t="s">
+      <c r="D160" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="D160" s="14" t="s">
+      <c r="E160" s="4"/>
+    </row>
+    <row r="161" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>158</v>
+      </c>
+      <c r="B161" s="14">
+        <v>29</v>
+      </c>
+      <c r="C161" s="5" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" ht="43.5">
-      <c r="A161">
-        <v>158</v>
-      </c>
-      <c r="B161">
-        <v>10</v>
-      </c>
-      <c r="C161" s="1" t="s">
+      <c r="D161" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="D161" s="14" t="s">
+      <c r="E161" s="4"/>
+    </row>
+    <row r="162" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>159</v>
+      </c>
+      <c r="B162" s="14">
+        <v>29</v>
+      </c>
+      <c r="C162" s="5" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" ht="43.5">
-      <c r="A162">
-        <v>159</v>
-      </c>
-      <c r="B162">
-        <v>11</v>
-      </c>
-      <c r="C162" s="1" t="s">
+      <c r="D162" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="D162" s="14" t="s">
+      <c r="E162" s="4"/>
+    </row>
+    <row r="163" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>160</v>
+      </c>
+      <c r="B163" s="14">
+        <v>29</v>
+      </c>
+      <c r="C163" s="8" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" ht="46.5">
-      <c r="A163">
-        <v>160</v>
-      </c>
-      <c r="B163">
-        <v>12</v>
-      </c>
-      <c r="C163" s="13" t="s">
+      <c r="D163" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="D163" s="14" t="s">
+      <c r="E163" s="4"/>
+    </row>
+    <row r="164" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>161</v>
+      </c>
+      <c r="B164" s="14">
+        <v>29</v>
+      </c>
+      <c r="C164" s="8" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="35.25">
-      <c r="A164">
-        <v>161</v>
-      </c>
-      <c r="B164">
-        <v>13</v>
-      </c>
-      <c r="C164" s="13" t="s">
+      <c r="D164" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D164" s="14" t="s">
+      <c r="E164" s="4"/>
+    </row>
+    <row r="165" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>162</v>
+      </c>
+      <c r="B165" s="14">
+        <v>29</v>
+      </c>
+      <c r="C165" s="8" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" ht="35.25">
-      <c r="A165">
-        <v>162</v>
-      </c>
-      <c r="B165">
-        <v>14</v>
-      </c>
-      <c r="C165" s="13" t="s">
+      <c r="D165" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="D165" s="14" t="s">
+      <c r="E165" s="4"/>
+    </row>
+    <row r="166" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>163</v>
+      </c>
+      <c r="B166" s="14">
+        <v>29</v>
+      </c>
+      <c r="C166" s="8" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" ht="35.25">
-      <c r="A166">
-        <v>163</v>
-      </c>
-      <c r="B166">
-        <v>15</v>
-      </c>
-      <c r="C166" s="13" t="s">
+      <c r="D166" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="D166" s="14" t="s">
+      <c r="E166" s="4"/>
+    </row>
+    <row r="167" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>164</v>
+      </c>
+      <c r="B167" s="14">
+        <v>29</v>
+      </c>
+      <c r="C167" s="8" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" ht="35.25">
-      <c r="A167">
-        <v>164</v>
-      </c>
-      <c r="B167">
-        <v>16</v>
-      </c>
-      <c r="C167" s="13" t="s">
+      <c r="D167" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="D167" s="14" t="s">
+      <c r="E167" s="4"/>
+    </row>
+    <row r="168" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>165</v>
+      </c>
+      <c r="B168" s="14">
+        <v>29</v>
+      </c>
+      <c r="C168" s="8" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" ht="35.25">
-      <c r="A168">
-        <v>165</v>
-      </c>
-      <c r="B168">
-        <v>17</v>
-      </c>
-      <c r="C168" s="13" t="s">
+      <c r="D168" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="D168" s="14" t="s">
+      <c r="E168" s="4"/>
+    </row>
+    <row r="169" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>166</v>
+      </c>
+      <c r="B169" s="14">
+        <v>29</v>
+      </c>
+      <c r="C169" s="8" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" ht="23.25">
-      <c r="A169">
-        <v>166</v>
-      </c>
-      <c r="B169">
-        <v>18</v>
-      </c>
-      <c r="C169" s="13" t="s">
+      <c r="D169" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="D169" s="15" t="s">
+      <c r="E169" s="4"/>
+    </row>
+    <row r="170" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>167</v>
+      </c>
+      <c r="B170" s="14">
+        <v>29</v>
+      </c>
+      <c r="C170" s="8" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" ht="35.25">
-      <c r="A170">
-        <v>167</v>
-      </c>
-      <c r="B170">
-        <v>19</v>
-      </c>
-      <c r="C170" s="13" t="s">
+      <c r="D170" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E170" s="4"/>
+    </row>
+    <row r="171" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>168</v>
+      </c>
+      <c r="B171" s="14">
+        <v>29</v>
+      </c>
+      <c r="C171" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="D170" s="15" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="23.25">
-      <c r="A171">
-        <v>168</v>
-      </c>
-      <c r="B171">
-        <v>20</v>
-      </c>
-      <c r="C171" s="16" t="s">
+      <c r="D171" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="D171" s="17" t="s">
+      <c r="E171" s="4"/>
+    </row>
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>169</v>
+      </c>
+      <c r="B172" s="14">
+        <v>32</v>
+      </c>
+      <c r="C172" s="4" t="s">
         <v>309</v>
       </c>
+      <c r="D172" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="E172" s="4"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>170</v>
+      </c>
+      <c r="B173" s="14">
+        <v>32</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D173" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="E173" s="4"/>
+    </row>
+    <row r="174" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>171</v>
+      </c>
+      <c r="B174" s="14">
+        <v>32</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D174" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="E174" s="4"/>
+    </row>
+    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>172</v>
+      </c>
+      <c r="B175" s="14">
+        <v>32</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D175" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="E175" s="4"/>
+    </row>
+    <row r="176" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>173</v>
+      </c>
+      <c r="B176" s="14">
+        <v>32</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D176" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="E176" s="4"/>
+    </row>
+    <row r="177" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>174</v>
+      </c>
+      <c r="B177" s="14">
+        <v>32</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D177" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="E177" s="4"/>
+    </row>
+    <row r="178" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>175</v>
+      </c>
+      <c r="B178" s="14">
+        <v>32</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D178" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="E178" s="4"/>
+    </row>
+    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="14">
+        <v>176</v>
+      </c>
+      <c r="B179" s="14">
+        <v>32</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="D179" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="E179" s="4"/>
+    </row>
+    <row r="180" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>177</v>
+      </c>
+      <c r="B180" s="14">
+        <v>32</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D180" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="E180" s="4"/>
+    </row>
+    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>178</v>
+      </c>
+      <c r="B181" s="14">
+        <v>32</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D181" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="E181" s="4"/>
+    </row>
+    <row r="182" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>179</v>
+      </c>
+      <c r="B182" s="14">
+        <v>32</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D182" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="E182" s="4"/>
+    </row>
+    <row r="183" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>180</v>
+      </c>
+      <c r="B183" s="14">
+        <v>32</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D183" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="E183" s="4"/>
+    </row>
+    <row r="184" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>181</v>
+      </c>
+      <c r="B184" s="14">
+        <v>32</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D184" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="E184" s="4"/>
+    </row>
+    <row r="185" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>182</v>
+      </c>
+      <c r="B185" s="14">
+        <v>32</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D185" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="E185" s="4"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>183</v>
+      </c>
+      <c r="B186" s="14">
+        <v>32</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D186" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="E186" s="4"/>
+    </row>
+    <row r="187" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>184</v>
+      </c>
+      <c r="B187" s="14">
+        <v>32</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D187" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="E187" s="4"/>
+    </row>
+    <row r="188" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>185</v>
+      </c>
+      <c r="B188" s="14">
+        <v>32</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D188" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="E188" s="4"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>186</v>
+      </c>
+      <c r="B189" s="14">
+        <v>32</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D189" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="E189" s="4"/>
+    </row>
+    <row r="190" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>187</v>
+      </c>
+      <c r="B190" s="14">
+        <v>32</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D190" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="E190" s="4"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>188</v>
+      </c>
+      <c r="B191" s="14">
+        <v>32</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="D191" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="E191" s="4"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>189</v>
+      </c>
+      <c r="B192" s="14">
+        <v>32</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D192" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="E192" s="4"/>
+    </row>
+    <row r="193" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>190</v>
+      </c>
+      <c r="B193" s="14">
+        <v>32</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D193" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E193" s="4"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>191</v>
+      </c>
+      <c r="B194" s="14">
+        <v>32</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D194" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="E194" s="4"/>
+    </row>
+    <row r="195" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>192</v>
+      </c>
+      <c r="B195" s="14">
+        <v>32</v>
+      </c>
+      <c r="C195" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D195" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>193</v>
+      </c>
+      <c r="B196" s="14">
+        <v>32</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D196" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="E196" s="4"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>194</v>
+      </c>
+      <c r="B197" s="14">
+        <v>32</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D197" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="E197" s="4"/>
+    </row>
+    <row r="198" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>195</v>
+      </c>
+      <c r="B198" s="14">
+        <v>32</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D198" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="E198" s="4"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>196</v>
+      </c>
+      <c r="B199" s="14">
+        <v>32</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D199" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="E199" s="4"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>197</v>
+      </c>
+      <c r="B200" s="14">
+        <v>32</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D200" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="E200" s="4"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>198</v>
+      </c>
+      <c r="B201" s="14">
+        <v>32</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D201" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="E201" s="4"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>199</v>
+      </c>
+      <c r="B202" s="14">
+        <v>32</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D202" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="E202" s="4"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>200</v>
+      </c>
+      <c r="B203" s="14">
+        <v>32</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D203" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="E203" s="4"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>201</v>
+      </c>
+      <c r="B204" s="14">
+        <v>32</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D204" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="E204" s="4"/>
+    </row>
+    <row r="205" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>202</v>
+      </c>
+      <c r="B205" s="14">
+        <v>32</v>
+      </c>
+      <c r="C205" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D205" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="E205" s="4"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>203</v>
+      </c>
+      <c r="B206" s="14">
+        <v>32</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D206" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="E206" s="4"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>204</v>
+      </c>
+      <c r="B207" s="14">
+        <v>32</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D207" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="E207" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Join Game modified requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/anh7674_mavs_uta_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BC9751C-A6C4-4E21-8EB6-DDB8B1DF3622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFE4871-967C-244C-B466-C827EC2CE343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="417">
   <si>
     <t>Tested By</t>
   </si>
@@ -346,106 +346,28 @@
     <t>BotI.java / isInsideBoard</t>
   </si>
   <si>
-    <t>The program shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined.</t>
-  </si>
-  <si>
     <t>joingame/Waitlist.js/displayWaitlist()</t>
   </si>
   <si>
-    <t>The program shall display a button for a game against another user.</t>
-  </si>
-  <si>
     <t>webapp/index.html</t>
   </si>
   <si>
-    <t>The program shall display a button for a game against a bot.</t>
-  </si>
-  <si>
-    <t>The program shall update the waitlist as players login and join/leave a game.</t>
-  </si>
-  <si>
     <t>joingame/Waitlist.js/add(), joingame/Waitlist.js/remove()</t>
   </si>
   <si>
-    <t>The program shall display a notification with updates to the waitlist.</t>
-  </si>
-  <si>
     <t>joingame/DisplayNotification.js/displayNotification()</t>
   </si>
   <si>
-    <t>The program will display a notification to the user when they are next to join a game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The program shall have display a button to spectate a game of 2 bots playing against each other. </t>
-  </si>
-  <si>
     <t>joingame/MatchMaker.js/requestSpectateBotVsBot()</t>
   </si>
   <si>
-    <t>The program will display players that choose to replay and new players at the bottom of the waitlist.</t>
-  </si>
-  <si>
-    <t>The program will load usernames and IDs in waitlist and display them within 2 seconds of logging in/joining a game.</t>
-  </si>
-  <si>
-    <t>The web interface of the Join Game component will be written in HTML5.</t>
-  </si>
-  <si>
-    <t>The program will be compatible with the web browsers Chrome, Firefox, and Safari.</t>
-  </si>
-  <si>
     <t>joingame</t>
   </si>
   <si>
-    <t>The interactive and dynamic functionality within the component will be written in JavaScript.</t>
-  </si>
-  <si>
     <t>joingame/Communication.js, Data.js, Displaynotification.js, MatchMaking.js, Waitlist.js</t>
   </si>
   <si>
-    <t>When the button to play against another player is pressed, the program will send the player information along with the game mode to the Page Manager component to initalize the pairing up process to begin a game.</t>
-  </si>
-  <si>
-    <t>joingame/MatchMaker.js/requestPlayerMatch()</t>
-  </si>
-  <si>
-    <t>When the button to play against a bot is pressed, the program will send the player information along with the game mode to the Page Manager component to intialize the process to start a game against a bot.</t>
-  </si>
-  <si>
-    <t>joingame/MatchMaker.js/requestBotMatch()</t>
-  </si>
-  <si>
-    <t>When a player(s) requests to join a game, the program removes their name from the waitlist.</t>
-  </si>
-  <si>
-    <t>joingame/Waitlist.js/remove()</t>
-  </si>
-  <si>
-    <t>When a player(s) logins successfully, the program adds their name to the waitlist.</t>
-  </si>
-  <si>
-    <t>joingame/Waitlist.js/add()</t>
-  </si>
-  <si>
-    <t>The program will receive player information (username and ID) from the Page Manager through a websocket.</t>
-  </si>
-  <si>
-    <t>joingame/Communication.js/handlePlayerData()</t>
-  </si>
-  <si>
-    <t>The program will create a player instance based on the provided data from the Page Manager.</t>
-  </si>
-  <si>
     <t>joingame/Data.js/constructor()</t>
-  </si>
-  <si>
-    <t>The program will send player information (username and ID) and their selected game mode to the Page Manager through a websocket.</t>
-  </si>
-  <si>
-    <t>joingame/Communication.js/sendPlayerAttributes()</t>
-  </si>
-  <si>
-    <t>When the button to spectate a game of two bots playing against each other, the program will send players' username and ID along with the game mode to Page Manager to intialize the process to start the game</t>
   </si>
   <si>
     <t>After a game concludes, the players go to the end of the line waiting for the new game</t>
@@ -1309,12 +1231,93 @@
   <si>
     <t>summary:</t>
   </si>
+  <si>
+    <t>The join game page shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined.</t>
+  </si>
+  <si>
+    <t>The join game page shall display a button for a game against another user.</t>
+  </si>
+  <si>
+    <t>The join game page shall display a button for a game against a bot.</t>
+  </si>
+  <si>
+    <t>The join game program shall update the waitlist as players login and join/leave a game.</t>
+  </si>
+  <si>
+    <t>The join game page shall display a notification with updates to the waitlist.</t>
+  </si>
+  <si>
+    <t>The join game page will display a notification to the user when they are next to join a game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The join game page shall have display a button to spectate a game of 2 bots playing against each other. </t>
+  </si>
+  <si>
+    <t>The join game page will display players that choose to replay and new players at the bottom of the waitlist.</t>
+  </si>
+  <si>
+    <t>The join game program will load usernames and IDs in waitlist and display them within 2 seconds of logging in/joining a game.</t>
+  </si>
+  <si>
+    <t>The web interface of the Join Game page will be written in HTML5.</t>
+  </si>
+  <si>
+    <t>The Join Game program will be compatible with the web browsers Chrome, Firefox, and Safari.</t>
+  </si>
+  <si>
+    <t>The interactive and dynamic functionality within the Join Game component will be written in JavaScript.</t>
+  </si>
+  <si>
+    <t>When the button to play against another player is pressed, the Join Game program will send the player information along with the game mode to the Page Manager component to initalize the pairing up process to begin a game.</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestPlayerMatch(), addToQueue(), Data.js/getGameMode()</t>
+  </si>
+  <si>
+    <t>When the button to play against a bot is pressed, the Join Game program will send the player information along with the game mode to the Page Manager component to intialize the process to start a game against a bot.</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestBotMatch(), addToQueue(), Data.js/getGameMode()</t>
+  </si>
+  <si>
+    <t>When a player(s) requests to join a game, the Join Game page removes their name from the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/remove(), joingame/Data.js/getID()</t>
+  </si>
+  <si>
+    <t>When a player(s) logins successfully, the Join Game page adds their name to the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/add(), joingame/Data.js/getID(), joingame/Data.js/getUsername()</t>
+  </si>
+  <si>
+    <t>The Join Game program will receive and process player information (username and ID) from the Page Manager through a websocket. Once the processing is finished, other components will be notified about player information.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js/handlePlayerData(), Data.js</t>
+  </si>
+  <si>
+    <t>The Join Game program will create a player instance based on the provided data from the Page Manager.</t>
+  </si>
+  <si>
+    <t>The Join Game program will send player information (username and ID) and their selected game mode to the Page Manager through a websocket.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js/sendPlayerAttributes(), Data.js</t>
+  </si>
+  <si>
+    <t>When the button to spectate a game of two bots playing against each other, the Join Game program will send players' username and ID along with the game mode to Page Manager to intialize the process to start the game</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestSpectateBotVsBot(), addToQueue(), Data.js/getGameMode()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2069,27 +2072,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56:C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -2147,7 +2150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="43.15">
+    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="28.9">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="28.9">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.9">
+    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="28.9">
+    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="28.9">
+    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2254,7 +2257,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="28.9">
+    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2282,7 +2285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="28.9">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="28.9">
+    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2324,7 +2327,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2338,7 +2341,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.9">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.9">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.9">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2380,7 +2383,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.9">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.9">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="43.15">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43.15">
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.9">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2450,7 +2453,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.9">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="43.15">
+    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.9">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.9">
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="43.15">
+    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="28.9">
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="43.15">
+    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28.9">
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.9">
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.9">
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>31</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.9">
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>32</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="43.15">
+    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>33</v>
       </c>
@@ -2618,7 +2621,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="43.15">
+    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>34</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="57.6">
+    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>35</v>
       </c>
@@ -2646,7 +2649,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.9">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>36</v>
       </c>
@@ -2660,7 +2663,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.9">
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <v>37</v>
       </c>
@@ -2674,7 +2677,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28.9">
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>38</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>39</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28.9">
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>40</v>
       </c>
@@ -2716,7 +2719,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.9">
+    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>41</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.9">
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>42</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.9">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>43</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="57.6">
+    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>44</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="43.15">
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>45</v>
       </c>
@@ -2786,7 +2789,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="28.9">
+    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>46</v>
       </c>
@@ -2800,7 +2803,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.9">
+    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>47</v>
       </c>
@@ -2814,7 +2817,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.9">
+    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>48</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="28.9">
+    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
         <v>49</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="43.15">
+    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
         <v>50</v>
       </c>
@@ -2850,13 +2853,13 @@
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="28.9">
+    </row>
+    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
         <v>51</v>
       </c>
@@ -2864,13 +2867,13 @@
         <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>104</v>
+        <v>391</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="28.9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <v>52</v>
       </c>
@@ -2878,13 +2881,13 @@
         <v>26</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>106</v>
+        <v>392</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="28.9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <v>53</v>
       </c>
@@ -2892,13 +2895,13 @@
         <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>393</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="28.9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>54</v>
       </c>
@@ -2906,13 +2909,13 @@
         <v>26</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>109</v>
+        <v>394</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>55</v>
       </c>
@@ -2920,13 +2923,13 @@
         <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>111</v>
+        <v>395</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="28.9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>56</v>
       </c>
@@ -2934,13 +2937,13 @@
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>112</v>
+        <v>396</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>57</v>
       </c>
@@ -2948,13 +2951,13 @@
         <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>114</v>
+        <v>397</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="43.15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>58</v>
       </c>
@@ -2962,13 +2965,13 @@
         <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>115</v>
+        <v>398</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="28.9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>59</v>
       </c>
@@ -2976,13 +2979,13 @@
         <v>26</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>399</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="28.9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>60</v>
       </c>
@@ -2990,13 +2993,13 @@
         <v>26</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>117</v>
+        <v>400</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="28.9">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>61</v>
       </c>
@@ -3004,13 +3007,13 @@
         <v>26</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>119</v>
+        <v>401</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="72">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
         <v>62</v>
       </c>
@@ -3018,13 +3021,13 @@
         <v>26</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>121</v>
+        <v>402</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="57.6">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="9">
         <v>63</v>
       </c>
@@ -3032,13 +3035,13 @@
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>123</v>
+        <v>404</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="28.9">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="9">
         <v>64</v>
       </c>
@@ -3046,13 +3049,13 @@
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>125</v>
+        <v>406</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="28.9">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="9">
         <v>65</v>
       </c>
@@ -3060,13 +3063,13 @@
         <v>26</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>127</v>
+        <v>408</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="28.9">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" s="9">
         <v>66</v>
       </c>
@@ -3074,13 +3077,13 @@
         <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>129</v>
+        <v>410</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="28.9">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
         <v>67</v>
       </c>
@@ -3088,13 +3091,13 @@
         <v>26</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>131</v>
+        <v>412</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="43.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="9">
         <v>68</v>
       </c>
@@ -3102,13 +3105,13 @@
         <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>133</v>
+        <v>413</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="57.6">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="9">
         <v>69</v>
       </c>
@@ -3116,13 +3119,13 @@
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>135</v>
+        <v>415</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="28.9">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
         <v>70</v>
       </c>
@@ -3130,13 +3133,13 @@
         <v>35</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="43.15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="9">
         <v>71</v>
       </c>
@@ -3144,13 +3147,13 @@
         <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="9">
         <v>72</v>
       </c>
@@ -3158,13 +3161,13 @@
         <v>35</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="43.15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="9">
         <v>73</v>
       </c>
@@ -3172,13 +3175,13 @@
         <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="43.15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="9">
         <v>74</v>
       </c>
@@ -3186,13 +3189,13 @@
         <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="28.9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
         <v>75</v>
       </c>
@@ -3200,13 +3203,13 @@
         <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="28.9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="9">
         <v>76</v>
       </c>
@@ -3214,13 +3217,13 @@
         <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="28.9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="9">
         <v>77</v>
       </c>
@@ -3228,13 +3231,13 @@
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="28.9">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="9">
         <v>78</v>
       </c>
@@ -3242,13 +3245,13 @@
         <v>35</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="28.9">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
         <v>79</v>
       </c>
@@ -3256,13 +3259,13 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="9">
         <v>80</v>
       </c>
@@ -3270,13 +3273,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="57.6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
         <v>81</v>
       </c>
@@ -3284,13 +3287,13 @@
         <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="43.15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
         <v>82</v>
       </c>
@@ -3298,13 +3301,13 @@
         <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="72">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
         <v>83</v>
       </c>
@@ -3312,13 +3315,13 @@
         <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
         <v>84</v>
       </c>
@@ -3326,13 +3329,13 @@
         <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="28.9">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="9">
         <v>85</v>
       </c>
@@ -3340,13 +3343,13 @@
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="43.15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="9">
         <v>86</v>
       </c>
@@ -3354,13 +3357,13 @@
         <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="28.9">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="9">
         <v>87</v>
       </c>
@@ -3368,13 +3371,13 @@
         <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="28.9">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="9">
         <v>88</v>
       </c>
@@ -3382,13 +3385,13 @@
         <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="28.9">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="9">
         <v>89</v>
       </c>
@@ -3396,13 +3399,13 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="28.9">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="9">
         <v>90</v>
       </c>
@@ -3410,13 +3413,13 @@
         <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="28.9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="9">
         <v>91</v>
       </c>
@@ -3424,13 +3427,13 @@
         <v>27</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="28.9">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="9">
         <v>92</v>
       </c>
@@ -3438,13 +3441,13 @@
         <v>27</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="28.9">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="9">
         <v>93</v>
       </c>
@@ -3452,13 +3455,13 @@
         <v>27</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="43.15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="9">
         <v>94</v>
       </c>
@@ -3466,13 +3469,13 @@
         <v>27</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="28.9">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="9">
         <v>95</v>
       </c>
@@ -3480,13 +3483,13 @@
         <v>27</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="28.9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="9">
         <v>96</v>
       </c>
@@ -3494,13 +3497,13 @@
         <v>27</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="28.9">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="9">
         <v>97</v>
       </c>
@@ -3508,13 +3511,13 @@
         <v>27</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="9">
         <v>98</v>
       </c>
@@ -3522,13 +3525,13 @@
         <v>27</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="28.9">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="9">
         <v>99</v>
       </c>
@@ -3536,13 +3539,13 @@
         <v>36</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="57.6">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="9">
         <v>100</v>
       </c>
@@ -3550,13 +3553,13 @@
         <v>36</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="43.15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="9">
         <v>101</v>
       </c>
@@ -3564,13 +3567,13 @@
         <v>36</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="28.9">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="9">
         <v>102</v>
       </c>
@@ -3578,13 +3581,13 @@
         <v>36</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="43.15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="9">
         <v>103</v>
       </c>
@@ -3592,13 +3595,13 @@
         <v>36</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="28.9">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="9">
         <v>104</v>
       </c>
@@ -3606,13 +3609,13 @@
         <v>36</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="86.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A108" s="9">
         <v>105</v>
       </c>
@@ -3620,13 +3623,13 @@
         <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="28.9">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="9">
         <v>106</v>
       </c>
@@ -3634,13 +3637,13 @@
         <v>36</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="9">
         <v>107</v>
       </c>
@@ -3648,13 +3651,13 @@
         <v>36</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="43.15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="9">
         <v>108</v>
       </c>
@@ -3662,13 +3665,13 @@
         <v>36</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="57.6">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="9">
         <v>109</v>
       </c>
@@ -3676,13 +3679,13 @@
         <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="28.9">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="9">
         <v>110</v>
       </c>
@@ -3690,13 +3693,13 @@
         <v>36</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="9">
         <v>111</v>
       </c>
@@ -3704,13 +3707,13 @@
         <v>36</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="43.15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="9">
         <v>112</v>
       </c>
@@ -3718,13 +3721,13 @@
         <v>36</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="28.9">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="9">
         <v>113</v>
       </c>
@@ -3732,13 +3735,13 @@
         <v>36</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="43.15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="9">
         <v>114</v>
       </c>
@@ -3746,13 +3749,13 @@
         <v>31</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="43.15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="9">
         <v>115</v>
       </c>
@@ -3760,13 +3763,13 @@
         <v>31</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="28.9">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="9">
         <v>116</v>
       </c>
@@ -3774,13 +3777,13 @@
         <v>31</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="43.15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="9">
         <v>117</v>
       </c>
@@ -3788,13 +3791,13 @@
         <v>31</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="43.15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="9">
         <v>118</v>
       </c>
@@ -3802,13 +3805,13 @@
         <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="43.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A122" s="9">
         <v>119</v>
       </c>
@@ -3816,13 +3819,13 @@
         <v>31</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="43.15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="9">
         <v>120</v>
       </c>
@@ -3830,13 +3833,13 @@
         <v>31</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="43.15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="9">
         <v>121</v>
       </c>
@@ -3844,13 +3847,13 @@
         <v>31</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="28.9">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="9">
         <v>122</v>
       </c>
@@ -3858,13 +3861,13 @@
         <v>31</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="72">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A126" s="9">
         <v>123</v>
       </c>
@@ -3872,13 +3875,13 @@
         <v>31</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="D126" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="86.45">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A127" s="9">
         <v>124</v>
       </c>
@@ -3886,13 +3889,13 @@
         <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="D127" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="57.6">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A128" s="9">
         <v>125</v>
       </c>
@@ -3900,13 +3903,13 @@
         <v>31</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" ht="72">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A129" s="9">
         <v>126</v>
       </c>
@@ -3914,13 +3917,13 @@
         <v>31</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="D129" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" ht="43.15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A130" s="9">
         <v>127</v>
       </c>
@@ -3928,13 +3931,13 @@
         <v>31</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="D130" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="28.9">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="9">
         <v>128</v>
       </c>
@@ -3942,13 +3945,13 @@
         <v>30</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" ht="43.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A132" s="9">
         <v>129</v>
       </c>
@@ -3956,13 +3959,13 @@
         <v>30</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="9">
         <v>130</v>
       </c>
@@ -3970,13 +3973,13 @@
         <v>30</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="43.15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A134" s="9">
         <v>131</v>
       </c>
@@ -3984,13 +3987,13 @@
         <v>30</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" ht="43.15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" s="9">
         <v>132</v>
       </c>
@@ -3998,13 +4001,13 @@
         <v>30</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" ht="28.9">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="9">
         <v>133</v>
       </c>
@@ -4012,13 +4015,13 @@
         <v>30</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="43.15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="9">
         <v>134</v>
       </c>
@@ -4026,13 +4029,13 @@
         <v>30</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" ht="28.9">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="9">
         <v>135</v>
       </c>
@@ -4040,13 +4043,13 @@
         <v>30</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" ht="57.6">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A139" s="9">
         <v>136</v>
       </c>
@@ -4054,13 +4057,13 @@
         <v>30</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" ht="57.6">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="9">
         <v>137</v>
       </c>
@@ -4068,13 +4071,13 @@
         <v>30</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" ht="187.15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A141" s="9">
         <v>138</v>
       </c>
@@ -4082,13 +4085,13 @@
         <v>30</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="9">
         <v>139</v>
       </c>
@@ -4096,19 +4099,19 @@
         <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="R142" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" ht="43.15">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A143" s="9">
         <v>140</v>
       </c>
@@ -4116,16 +4119,16 @@
         <v>28</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" ht="28.9">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="9">
         <v>141</v>
       </c>
@@ -4133,13 +4136,13 @@
         <v>28</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="28.9">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="9">
         <v>142</v>
       </c>
@@ -4147,13 +4150,13 @@
         <v>28</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="D145" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="28.9">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="9">
         <v>143</v>
       </c>
@@ -4161,13 +4164,13 @@
         <v>28</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="28.9">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="9">
         <v>144</v>
       </c>
@@ -4175,13 +4178,13 @@
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="28.9">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="9">
         <v>145</v>
       </c>
@@ -4189,13 +4192,13 @@
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="9">
         <v>146</v>
       </c>
@@ -4203,13 +4206,13 @@
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="28.9">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="9">
         <v>147</v>
       </c>
@@ -4217,13 +4220,13 @@
         <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="28.9">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="9">
         <v>148</v>
       </c>
@@ -4231,13 +4234,13 @@
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="72">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A152" s="9">
         <v>149</v>
       </c>
@@ -4245,13 +4248,13 @@
         <v>29</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="57.6">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A153" s="9">
         <v>150</v>
       </c>
@@ -4259,13 +4262,13 @@
         <v>29</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="28.9">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="9">
         <v>151</v>
       </c>
@@ -4273,13 +4276,13 @@
         <v>29</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="43.15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="9">
         <v>152</v>
       </c>
@@ -4287,13 +4290,13 @@
         <v>29</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="43.15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="9">
         <v>153</v>
       </c>
@@ -4301,13 +4304,13 @@
         <v>29</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="43.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="9">
         <v>154</v>
       </c>
@@ -4315,13 +4318,13 @@
         <v>29</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="43.15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="9">
         <v>155</v>
       </c>
@@ -4329,13 +4332,13 @@
         <v>29</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="57.6">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A159" s="9">
         <v>156</v>
       </c>
@@ -4343,13 +4346,13 @@
         <v>29</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="57.6">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A160" s="9">
         <v>157</v>
       </c>
@@ -4357,13 +4360,13 @@
         <v>29</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="43.15">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A161" s="9">
         <v>158</v>
       </c>
@@ -4371,13 +4374,13 @@
         <v>29</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="43.15">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A162" s="9">
         <v>159</v>
       </c>
@@ -4385,13 +4388,13 @@
         <v>29</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="43.15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="9">
         <v>160</v>
       </c>
@@ -4399,13 +4402,13 @@
         <v>29</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="43.15">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A164" s="9">
         <v>161</v>
       </c>
@@ -4413,13 +4416,13 @@
         <v>29</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="28.9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="9">
         <v>162</v>
       </c>
@@ -4427,13 +4430,13 @@
         <v>29</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="43.15">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A166" s="9">
         <v>163</v>
       </c>
@@ -4441,13 +4444,13 @@
         <v>29</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="D166" s="12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="43.15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A167" s="9">
         <v>164</v>
       </c>
@@ -4455,13 +4458,13 @@
         <v>29</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="43.15">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A168" s="9">
         <v>165</v>
       </c>
@@ -4469,13 +4472,13 @@
         <v>29</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="D168" s="12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="28.9">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="9">
         <v>166</v>
       </c>
@@ -4483,13 +4486,13 @@
         <v>29</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="D169" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" ht="43.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="9">
         <v>167</v>
       </c>
@@ -4497,13 +4500,13 @@
         <v>29</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="28.9">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="9">
         <v>168</v>
       </c>
@@ -4511,13 +4514,13 @@
         <v>29</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" ht="28.9">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="9">
         <v>169</v>
       </c>
@@ -4525,13 +4528,13 @@
         <v>32</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="9">
         <v>170</v>
       </c>
@@ -4539,13 +4542,13 @@
         <v>32</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="28.9">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="9">
         <v>171</v>
       </c>
@@ -4553,13 +4556,13 @@
         <v>32</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" ht="28.9">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="9">
         <v>172</v>
       </c>
@@ -4567,13 +4570,13 @@
         <v>32</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="28.9">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="9">
         <v>173</v>
       </c>
@@ -4581,13 +4584,13 @@
         <v>32</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="28.9">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="9">
         <v>174</v>
       </c>
@@ -4595,13 +4598,13 @@
         <v>32</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="28.9">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="9">
         <v>175</v>
       </c>
@@ -4609,13 +4612,13 @@
         <v>32</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="28.9">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="9">
         <v>176</v>
       </c>
@@ -4623,13 +4626,13 @@
         <v>32</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="43.15">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A180" s="9">
         <v>177</v>
       </c>
@@ -4637,13 +4640,13 @@
         <v>32</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="28.9">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="9">
         <v>178</v>
       </c>
@@ -4651,13 +4654,13 @@
         <v>32</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>328</v>
+        <v>302</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="28.9">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="9">
         <v>179</v>
       </c>
@@ -4665,13 +4668,13 @@
         <v>32</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="28.9">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="9">
         <v>180</v>
       </c>
@@ -4679,13 +4682,13 @@
         <v>32</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="28.9">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="9">
         <v>181</v>
       </c>
@@ -4693,13 +4696,13 @@
         <v>32</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="28.9">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="9">
         <v>182</v>
       </c>
@@ -4707,13 +4710,13 @@
         <v>32</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="9">
         <v>183</v>
       </c>
@@ -4721,13 +4724,13 @@
         <v>32</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="28.9">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="9">
         <v>184</v>
       </c>
@@ -4735,13 +4738,13 @@
         <v>32</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="28.9">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="9">
         <v>185</v>
       </c>
@@ -4749,13 +4752,13 @@
         <v>32</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="9">
         <v>186</v>
       </c>
@@ -4763,13 +4766,13 @@
         <v>32</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="28.9">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="9">
         <v>187</v>
       </c>
@@ -4777,13 +4780,13 @@
         <v>32</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="9">
         <v>188</v>
       </c>
@@ -4791,13 +4794,13 @@
         <v>32</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="9">
         <v>189</v>
       </c>
@@ -4805,13 +4808,13 @@
         <v>32</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="D192" s="10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="193" spans="1:18" ht="28.9">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="9">
         <v>190</v>
       </c>
@@ -4819,13 +4822,13 @@
         <v>32</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="194" spans="1:18">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="9">
         <v>191</v>
       </c>
@@ -4833,13 +4836,13 @@
         <v>32</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="195" spans="1:18" ht="28.9">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="9">
         <v>192</v>
       </c>
@@ -4847,16 +4850,16 @@
         <v>32</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" ht="28.9">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="9">
         <v>193</v>
       </c>
@@ -4864,13 +4867,13 @@
         <v>32</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="197" spans="1:18">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="9">
         <v>194</v>
       </c>
@@ -4878,13 +4881,13 @@
         <v>32</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="198" spans="1:18" ht="28.9">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="9">
         <v>195</v>
       </c>
@@ -4892,13 +4895,13 @@
         <v>32</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="199" spans="1:18">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="9">
         <v>196</v>
       </c>
@@ -4906,13 +4909,13 @@
         <v>32</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>363</v>
+        <v>337</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="200" spans="1:18">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="9">
         <v>197</v>
       </c>
@@ -4920,13 +4923,13 @@
         <v>32</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="201" spans="1:18">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="9">
         <v>198</v>
       </c>
@@ -4934,13 +4937,13 @@
         <v>32</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="202" spans="1:18">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="9">
         <v>199</v>
       </c>
@@ -4948,13 +4951,13 @@
         <v>32</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="203" spans="1:18">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="9">
         <v>200</v>
       </c>
@@ -4962,13 +4965,13 @@
         <v>32</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="D203" s="10" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="204" spans="1:18">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="9">
         <v>201</v>
       </c>
@@ -4976,13 +4979,13 @@
         <v>32</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="205" spans="1:18" ht="28.9">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="9">
         <v>202</v>
       </c>
@@ -4990,13 +4993,13 @@
         <v>32</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="D205" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="206" spans="1:18">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="9">
         <v>203</v>
       </c>
@@ -5004,13 +5007,13 @@
         <v>32</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="D206" s="10" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="207" spans="1:18">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="9">
         <v>204</v>
       </c>
@@ -5018,16 +5021,16 @@
         <v>32</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="D207" s="10" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="R207" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="208" spans="1:18" ht="29.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="8">
         <v>205</v>
       </c>
@@ -5035,13 +5038,13 @@
         <v>25</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>381</v>
+        <v>355</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="209" spans="1:18" ht="43.5">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="8">
         <v>206</v>
       </c>
@@ -5049,13 +5052,13 @@
         <v>25</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>383</v>
+        <v>357</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="210" spans="1:18" ht="43.5">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="8">
         <v>207</v>
       </c>
@@ -5063,16 +5066,16 @@
         <v>25</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>386</v>
+        <v>360</v>
       </c>
       <c r="R210" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="211" spans="1:18" ht="43.5">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A211" s="8">
         <v>208</v>
       </c>
@@ -5080,13 +5083,13 @@
         <v>25</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="212" spans="1:18" ht="29.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="8">
         <v>209</v>
       </c>
@@ -5094,13 +5097,13 @@
         <v>25</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="213" spans="1:18" ht="29.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="8">
         <v>210</v>
       </c>
@@ -5108,13 +5111,13 @@
         <v>25</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="214" spans="1:18" ht="29.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="8">
         <v>211</v>
       </c>
@@ -5122,13 +5125,13 @@
         <v>25</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="215" spans="1:18" ht="43.5">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="8">
         <v>212</v>
       </c>
@@ -5136,16 +5139,16 @@
         <v>25</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>391</v>
+        <v>365</v>
       </c>
       <c r="R215" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="216" spans="1:18" ht="29.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="8">
         <v>213</v>
       </c>
@@ -5153,13 +5156,13 @@
         <v>25</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>398</v>
+        <v>372</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="217" spans="1:18" ht="15">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="8">
         <v>214</v>
       </c>
@@ -5167,13 +5170,13 @@
         <v>25</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>400</v>
+        <v>374</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="218" spans="1:18" ht="29.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="8">
         <v>215</v>
       </c>
@@ -5181,13 +5184,13 @@
         <v>25</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="219" spans="1:18" ht="29.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="9">
         <v>216</v>
       </c>
@@ -5195,13 +5198,13 @@
         <v>25</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>403</v>
+        <v>377</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="220" spans="1:18" ht="29.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="9">
         <v>217</v>
       </c>
@@ -5209,13 +5212,13 @@
         <v>25</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>405</v>
+        <v>379</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="221" spans="1:18" ht="29.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="9">
         <v>218</v>
       </c>
@@ -5223,16 +5226,16 @@
         <v>25</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="R221" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="222" spans="1:18" ht="30.75">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="9">
         <v>219</v>
       </c>
@@ -5240,13 +5243,13 @@
         <v>25</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="223" spans="1:18" ht="29.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="9">
         <v>220</v>
       </c>
@@ -5254,13 +5257,13 @@
         <v>25</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="224" spans="1:18" ht="29.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="9">
         <v>221</v>
       </c>
@@ -5268,15 +5271,15 @@
         <v>25</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="230" spans="18:18">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="230" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R230" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5287,6 +5290,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDD0FC4969DCF4449136D2C873E795D1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c6f44795faba901663e8a9bf3a6322e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d2c32087-eb03-4a65-b505-380146e007a4" xmlns:ns4="2f381668-55bb-4cca-a2e9-7746dbcfba3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7caa3c07606457882248d14e3a3261f4" ns3:_="" ns4:_="">
     <xsd:import namespace="d2c32087-eb03-4a65-b505-380146e007a4"/>
@@ -5507,14 +5518,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5525,13 +5528,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
+    <ds:schemaRef ds:uri="2f381668-55bb-4cca-a2e9-7746dbcfba3d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated login requirements- group 25
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/anh7674_mavs_uta_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFE4871-967C-244C-B466-C827EC2CE343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BC9751C-A6C4-4E21-8EB6-DDB8B1DF3622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="416">
   <si>
     <t>Tested By</t>
   </si>
@@ -346,28 +346,106 @@
     <t>BotI.java / isInsideBoard</t>
   </si>
   <si>
+    <t>The program shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined.</t>
+  </si>
+  <si>
     <t>joingame/Waitlist.js/displayWaitlist()</t>
   </si>
   <si>
+    <t>The program shall display a button for a game against another user.</t>
+  </si>
+  <si>
     <t>webapp/index.html</t>
   </si>
   <si>
+    <t>The program shall display a button for a game against a bot.</t>
+  </si>
+  <si>
+    <t>The program shall update the waitlist as players login and join/leave a game.</t>
+  </si>
+  <si>
     <t>joingame/Waitlist.js/add(), joingame/Waitlist.js/remove()</t>
   </si>
   <si>
+    <t>The program shall display a notification with updates to the waitlist.</t>
+  </si>
+  <si>
     <t>joingame/DisplayNotification.js/displayNotification()</t>
   </si>
   <si>
+    <t>The program will display a notification to the user when they are next to join a game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The program shall have display a button to spectate a game of 2 bots playing against each other. </t>
+  </si>
+  <si>
     <t>joingame/MatchMaker.js/requestSpectateBotVsBot()</t>
   </si>
   <si>
+    <t>The program will display players that choose to replay and new players at the bottom of the waitlist.</t>
+  </si>
+  <si>
+    <t>The program will load usernames and IDs in waitlist and display them within 2 seconds of logging in/joining a game.</t>
+  </si>
+  <si>
+    <t>The web interface of the Join Game component will be written in HTML5.</t>
+  </si>
+  <si>
+    <t>The program will be compatible with the web browsers Chrome, Firefox, and Safari.</t>
+  </si>
+  <si>
     <t>joingame</t>
   </si>
   <si>
+    <t>The interactive and dynamic functionality within the component will be written in JavaScript.</t>
+  </si>
+  <si>
     <t>joingame/Communication.js, Data.js, Displaynotification.js, MatchMaking.js, Waitlist.js</t>
   </si>
   <si>
+    <t>When the button to play against another player is pressed, the program will send the player information along with the game mode to the Page Manager component to initalize the pairing up process to begin a game.</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestPlayerMatch()</t>
+  </si>
+  <si>
+    <t>When the button to play against a bot is pressed, the program will send the player information along with the game mode to the Page Manager component to intialize the process to start a game against a bot.</t>
+  </si>
+  <si>
+    <t>joingame/MatchMaker.js/requestBotMatch()</t>
+  </si>
+  <si>
+    <t>When a player(s) requests to join a game, the program removes their name from the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/remove()</t>
+  </si>
+  <si>
+    <t>When a player(s) logins successfully, the program adds their name to the waitlist.</t>
+  </si>
+  <si>
+    <t>joingame/Waitlist.js/add()</t>
+  </si>
+  <si>
+    <t>The program will receive player information (username and ID) from the Page Manager through a websocket.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js/handlePlayerData()</t>
+  </si>
+  <si>
+    <t>The program will create a player instance based on the provided data from the Page Manager.</t>
+  </si>
+  <si>
     <t>joingame/Data.js/constructor()</t>
+  </si>
+  <si>
+    <t>The program will send player information (username and ID) and their selected game mode to the Page Manager through a websocket.</t>
+  </si>
+  <si>
+    <t>joingame/Communication.js/sendPlayerAttributes()</t>
+  </si>
+  <si>
+    <t>When the button to spectate a game of two bots playing against each other, the program will send players' username and ID along with the game mode to Page Manager to intialize the process to start the game</t>
   </si>
   <si>
     <t>After a game concludes, the players go to the end of the line waiting for the new game</t>
@@ -1231,93 +1309,12 @@
   <si>
     <t>summary:</t>
   </si>
-  <si>
-    <t>The join game page shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined.</t>
-  </si>
-  <si>
-    <t>The join game page shall display a button for a game against another user.</t>
-  </si>
-  <si>
-    <t>The join game page shall display a button for a game against a bot.</t>
-  </si>
-  <si>
-    <t>The join game program shall update the waitlist as players login and join/leave a game.</t>
-  </si>
-  <si>
-    <t>The join game page shall display a notification with updates to the waitlist.</t>
-  </si>
-  <si>
-    <t>The join game page will display a notification to the user when they are next to join a game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The join game page shall have display a button to spectate a game of 2 bots playing against each other. </t>
-  </si>
-  <si>
-    <t>The join game page will display players that choose to replay and new players at the bottom of the waitlist.</t>
-  </si>
-  <si>
-    <t>The join game program will load usernames and IDs in waitlist and display them within 2 seconds of logging in/joining a game.</t>
-  </si>
-  <si>
-    <t>The web interface of the Join Game page will be written in HTML5.</t>
-  </si>
-  <si>
-    <t>The Join Game program will be compatible with the web browsers Chrome, Firefox, and Safari.</t>
-  </si>
-  <si>
-    <t>The interactive and dynamic functionality within the Join Game component will be written in JavaScript.</t>
-  </si>
-  <si>
-    <t>When the button to play against another player is pressed, the Join Game program will send the player information along with the game mode to the Page Manager component to initalize the pairing up process to begin a game.</t>
-  </si>
-  <si>
-    <t>joingame/MatchMaker.js/requestPlayerMatch(), addToQueue(), Data.js/getGameMode()</t>
-  </si>
-  <si>
-    <t>When the button to play against a bot is pressed, the Join Game program will send the player information along with the game mode to the Page Manager component to intialize the process to start a game against a bot.</t>
-  </si>
-  <si>
-    <t>joingame/MatchMaker.js/requestBotMatch(), addToQueue(), Data.js/getGameMode()</t>
-  </si>
-  <si>
-    <t>When a player(s) requests to join a game, the Join Game page removes their name from the waitlist.</t>
-  </si>
-  <si>
-    <t>joingame/Waitlist.js/remove(), joingame/Data.js/getID()</t>
-  </si>
-  <si>
-    <t>When a player(s) logins successfully, the Join Game page adds their name to the waitlist.</t>
-  </si>
-  <si>
-    <t>joingame/Waitlist.js/add(), joingame/Data.js/getID(), joingame/Data.js/getUsername()</t>
-  </si>
-  <si>
-    <t>The Join Game program will receive and process player information (username and ID) from the Page Manager through a websocket. Once the processing is finished, other components will be notified about player information.</t>
-  </si>
-  <si>
-    <t>joingame/Communication.js/handlePlayerData(), Data.js</t>
-  </si>
-  <si>
-    <t>The Join Game program will create a player instance based on the provided data from the Page Manager.</t>
-  </si>
-  <si>
-    <t>The Join Game program will send player information (username and ID) and their selected game mode to the Page Manager through a websocket.</t>
-  </si>
-  <si>
-    <t>joingame/Communication.js/sendPlayerAttributes(), Data.js</t>
-  </si>
-  <si>
-    <t>When the button to spectate a game of two bots playing against each other, the Join Game program will send players' username and ID along with the game mode to Page Manager to intialize the process to start the game</t>
-  </si>
-  <si>
-    <t>joingame/MatchMaker.js/requestSpectateBotVsBot(), addToQueue(), Data.js/getGameMode()</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2072,27 +2069,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56:C66"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -2150,7 +2147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="43.15">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2173,7 +2170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="28.9">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2187,7 +2184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="28.9">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2201,7 +2198,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="28.9">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2215,7 +2212,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2229,7 +2226,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="28.9">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2243,7 +2240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="28.9">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2257,7 +2254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="28.9">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2271,7 +2268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2285,7 +2282,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="28.9">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2299,7 +2296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2313,7 +2310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="28.9">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2327,7 +2324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2341,7 +2338,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="28.9">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2355,7 +2352,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="28.9">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2369,7 +2366,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="28.9">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2383,7 +2380,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="28.9">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2397,7 +2394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="28.9">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2411,7 +2408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="43.15">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2425,7 +2422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="43.15">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2439,7 +2436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="28.9">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2453,7 +2450,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="28.9">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2467,7 +2464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="43.15">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2481,7 +2478,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="28.9">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2495,7 +2492,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="28.9">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2509,7 +2506,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="43.15">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2523,7 +2520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="28.9">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2537,7 +2534,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="43.15">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2551,7 +2548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="28.9">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2565,7 +2562,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="28.9">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2579,7 +2576,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="28.9">
       <c r="A34" s="9">
         <v>31</v>
       </c>
@@ -2593,7 +2590,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="28.9">
       <c r="A35" s="9">
         <v>32</v>
       </c>
@@ -2607,7 +2604,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="43.15">
       <c r="A36" s="9">
         <v>33</v>
       </c>
@@ -2621,7 +2618,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="43.15">
       <c r="A37" s="9">
         <v>34</v>
       </c>
@@ -2635,7 +2632,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="57.6">
       <c r="A38" s="9">
         <v>35</v>
       </c>
@@ -2649,7 +2646,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="28.9">
       <c r="A39" s="9">
         <v>36</v>
       </c>
@@ -2663,7 +2660,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="28.9">
       <c r="A40" s="9">
         <v>37</v>
       </c>
@@ -2677,7 +2674,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="28.9">
       <c r="A41" s="9">
         <v>38</v>
       </c>
@@ -2691,7 +2688,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="9">
         <v>39</v>
       </c>
@@ -2705,7 +2702,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="28.9">
       <c r="A43" s="9">
         <v>40</v>
       </c>
@@ -2719,7 +2716,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="28.9">
       <c r="A44" s="9">
         <v>41</v>
       </c>
@@ -2733,7 +2730,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="28.9">
       <c r="A45" s="9">
         <v>42</v>
       </c>
@@ -2747,7 +2744,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="28.9">
       <c r="A46" s="9">
         <v>43</v>
       </c>
@@ -2761,7 +2758,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="57.6">
       <c r="A47" s="9">
         <v>44</v>
       </c>
@@ -2775,7 +2772,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="43.15">
       <c r="A48" s="9">
         <v>45</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="28.9">
       <c r="A49" s="9">
         <v>46</v>
       </c>
@@ -2803,7 +2800,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="28.9">
       <c r="A50" s="9">
         <v>47</v>
       </c>
@@ -2817,7 +2814,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="28.9">
       <c r="A51" s="9">
         <v>48</v>
       </c>
@@ -2831,7 +2828,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="28.9">
       <c r="A52" s="9">
         <v>49</v>
       </c>
@@ -2845,7 +2842,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="43.15">
       <c r="A53" s="9">
         <v>50</v>
       </c>
@@ -2853,13 +2850,13 @@
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>390</v>
+        <v>102</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.9">
       <c r="A54" s="9">
         <v>51</v>
       </c>
@@ -2867,13 +2864,13 @@
         <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>391</v>
+        <v>104</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="28.9">
       <c r="A55" s="9">
         <v>52</v>
       </c>
@@ -2881,13 +2878,13 @@
         <v>26</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>392</v>
+        <v>106</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.9">
       <c r="A56" s="9">
         <v>53</v>
       </c>
@@ -2895,13 +2892,13 @@
         <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>393</v>
+        <v>107</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.9">
       <c r="A57" s="9">
         <v>54</v>
       </c>
@@ -2909,13 +2906,13 @@
         <v>26</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>394</v>
+        <v>109</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.9">
       <c r="A58" s="9">
         <v>55</v>
       </c>
@@ -2923,13 +2920,13 @@
         <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>395</v>
+        <v>111</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.9">
       <c r="A59" s="9">
         <v>56</v>
       </c>
@@ -2937,13 +2934,13 @@
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>396</v>
+        <v>112</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.9">
       <c r="A60" s="9">
         <v>57</v>
       </c>
@@ -2951,13 +2948,13 @@
         <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>397</v>
+        <v>114</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="43.15">
       <c r="A61" s="9">
         <v>58</v>
       </c>
@@ -2965,13 +2962,13 @@
         <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>398</v>
+        <v>115</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="28.9">
       <c r="A62" s="9">
         <v>59</v>
       </c>
@@ -2979,13 +2976,13 @@
         <v>26</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>399</v>
+        <v>116</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28.9">
       <c r="A63" s="9">
         <v>60</v>
       </c>
@@ -2993,13 +2990,13 @@
         <v>26</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>400</v>
+        <v>117</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.9">
       <c r="A64" s="9">
         <v>61</v>
       </c>
@@ -3007,13 +3004,13 @@
         <v>26</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>401</v>
+        <v>119</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="72">
       <c r="A65" s="9">
         <v>62</v>
       </c>
@@ -3021,13 +3018,13 @@
         <v>26</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>402</v>
+        <v>121</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="57.6">
       <c r="A66" s="9">
         <v>63</v>
       </c>
@@ -3035,13 +3032,13 @@
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>404</v>
+        <v>123</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="28.9">
       <c r="A67" s="9">
         <v>64</v>
       </c>
@@ -3049,13 +3046,13 @@
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>406</v>
+        <v>125</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="28.9">
       <c r="A68" s="9">
         <v>65</v>
       </c>
@@ -3063,13 +3060,13 @@
         <v>26</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>408</v>
+        <v>127</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="28.9">
       <c r="A69" s="9">
         <v>66</v>
       </c>
@@ -3077,13 +3074,13 @@
         <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>410</v>
+        <v>129</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="28.9">
       <c r="A70" s="9">
         <v>67</v>
       </c>
@@ -3091,13 +3088,13 @@
         <v>26</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>412</v>
+        <v>131</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="43.15">
       <c r="A71" s="9">
         <v>68</v>
       </c>
@@ -3105,13 +3102,13 @@
         <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>413</v>
+        <v>133</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="57.6">
       <c r="A72" s="9">
         <v>69</v>
       </c>
@@ -3119,13 +3116,13 @@
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>415</v>
+        <v>135</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="28.9">
       <c r="A73" s="9">
         <v>70</v>
       </c>
@@ -3133,13 +3130,13 @@
         <v>35</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="43.15">
       <c r="A74" s="9">
         <v>71</v>
       </c>
@@ -3147,13 +3144,13 @@
         <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="9">
         <v>72</v>
       </c>
@@ -3161,13 +3158,13 @@
         <v>35</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="43.15">
       <c r="A76" s="9">
         <v>73</v>
       </c>
@@ -3175,13 +3172,13 @@
         <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="43.15">
       <c r="A77" s="9">
         <v>74</v>
       </c>
@@ -3189,13 +3186,13 @@
         <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="28.9">
       <c r="A78" s="9">
         <v>75</v>
       </c>
@@ -3203,13 +3200,13 @@
         <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="28.9">
       <c r="A79" s="9">
         <v>76</v>
       </c>
@@ -3217,13 +3214,13 @@
         <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="28.9">
       <c r="A80" s="9">
         <v>77</v>
       </c>
@@ -3231,13 +3228,13 @@
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="28.9">
       <c r="A81" s="9">
         <v>78</v>
       </c>
@@ -3245,13 +3242,13 @@
         <v>35</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="28.9">
       <c r="A82" s="9">
         <v>79</v>
       </c>
@@ -3259,13 +3256,13 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="9">
         <v>80</v>
       </c>
@@ -3273,13 +3270,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="57.6">
       <c r="A84" s="9">
         <v>81</v>
       </c>
@@ -3287,13 +3284,13 @@
         <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="43.15">
       <c r="A85" s="9">
         <v>82</v>
       </c>
@@ -3301,13 +3298,13 @@
         <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="72">
       <c r="A86" s="9">
         <v>83</v>
       </c>
@@ -3315,13 +3312,13 @@
         <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="9">
         <v>84</v>
       </c>
@@ -3329,13 +3326,13 @@
         <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="28.9">
       <c r="A88" s="9">
         <v>85</v>
       </c>
@@ -3343,13 +3340,13 @@
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="43.15">
       <c r="A89" s="9">
         <v>86</v>
       </c>
@@ -3357,13 +3354,13 @@
         <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="28.9">
       <c r="A90" s="9">
         <v>87</v>
       </c>
@@ -3371,13 +3368,13 @@
         <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="28.9">
       <c r="A91" s="9">
         <v>88</v>
       </c>
@@ -3385,13 +3382,13 @@
         <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="28.9">
       <c r="A92" s="9">
         <v>89</v>
       </c>
@@ -3399,13 +3396,13 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="28.9">
       <c r="A93" s="9">
         <v>90</v>
       </c>
@@ -3413,13 +3410,13 @@
         <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="28.9">
       <c r="A94" s="9">
         <v>91</v>
       </c>
@@ -3427,13 +3424,13 @@
         <v>27</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="28.9">
       <c r="A95" s="9">
         <v>92</v>
       </c>
@@ -3441,13 +3438,13 @@
         <v>27</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="28.9">
       <c r="A96" s="9">
         <v>93</v>
       </c>
@@ -3455,13 +3452,13 @@
         <v>27</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="43.15">
       <c r="A97" s="9">
         <v>94</v>
       </c>
@@ -3469,13 +3466,13 @@
         <v>27</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="28.9">
       <c r="A98" s="9">
         <v>95</v>
       </c>
@@ -3483,13 +3480,13 @@
         <v>27</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="28.9">
       <c r="A99" s="9">
         <v>96</v>
       </c>
@@ -3497,13 +3494,13 @@
         <v>27</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="28.9">
       <c r="A100" s="9">
         <v>97</v>
       </c>
@@ -3511,13 +3508,13 @@
         <v>27</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="9">
         <v>98</v>
       </c>
@@ -3525,13 +3522,13 @@
         <v>27</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="28.9">
       <c r="A102" s="9">
         <v>99</v>
       </c>
@@ -3539,13 +3536,13 @@
         <v>36</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="57.6">
       <c r="A103" s="9">
         <v>100</v>
       </c>
@@ -3553,13 +3550,13 @@
         <v>36</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="43.15">
       <c r="A104" s="9">
         <v>101</v>
       </c>
@@ -3567,13 +3564,13 @@
         <v>36</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="28.9">
       <c r="A105" s="9">
         <v>102</v>
       </c>
@@ -3581,13 +3578,13 @@
         <v>36</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="43.15">
       <c r="A106" s="9">
         <v>103</v>
       </c>
@@ -3595,13 +3592,13 @@
         <v>36</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="28.9">
       <c r="A107" s="9">
         <v>104</v>
       </c>
@@ -3609,13 +3606,13 @@
         <v>36</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="86.45">
       <c r="A108" s="9">
         <v>105</v>
       </c>
@@ -3623,13 +3620,13 @@
         <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="28.9">
       <c r="A109" s="9">
         <v>106</v>
       </c>
@@ -3637,13 +3634,13 @@
         <v>36</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="9">
         <v>107</v>
       </c>
@@ -3651,13 +3648,13 @@
         <v>36</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="43.15">
       <c r="A111" s="9">
         <v>108</v>
       </c>
@@ -3665,13 +3662,13 @@
         <v>36</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="57.6">
       <c r="A112" s="9">
         <v>109</v>
       </c>
@@ -3679,13 +3676,13 @@
         <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="28.9">
       <c r="A113" s="9">
         <v>110</v>
       </c>
@@ -3693,13 +3690,13 @@
         <v>36</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="9">
         <v>111</v>
       </c>
@@ -3707,13 +3704,13 @@
         <v>36</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="43.15">
       <c r="A115" s="9">
         <v>112</v>
       </c>
@@ -3721,13 +3718,13 @@
         <v>36</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="28.9">
       <c r="A116" s="9">
         <v>113</v>
       </c>
@@ -3735,13 +3732,13 @@
         <v>36</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="43.15">
       <c r="A117" s="9">
         <v>114</v>
       </c>
@@ -3749,13 +3746,13 @@
         <v>31</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="43.15">
       <c r="A118" s="9">
         <v>115</v>
       </c>
@@ -3763,13 +3760,13 @@
         <v>31</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="28.9">
       <c r="A119" s="9">
         <v>116</v>
       </c>
@@ -3777,13 +3774,13 @@
         <v>31</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="43.15">
       <c r="A120" s="9">
         <v>117</v>
       </c>
@@ -3791,13 +3788,13 @@
         <v>31</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="43.15">
       <c r="A121" s="9">
         <v>118</v>
       </c>
@@ -3805,13 +3802,13 @@
         <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="43.15">
       <c r="A122" s="9">
         <v>119</v>
       </c>
@@ -3819,13 +3816,13 @@
         <v>31</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="43.15">
       <c r="A123" s="9">
         <v>120</v>
       </c>
@@ -3833,13 +3830,13 @@
         <v>31</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="43.15">
       <c r="A124" s="9">
         <v>121</v>
       </c>
@@ -3847,13 +3844,13 @@
         <v>31</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="28.9">
       <c r="A125" s="9">
         <v>122</v>
       </c>
@@ -3861,13 +3858,13 @@
         <v>31</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="72">
       <c r="A126" s="9">
         <v>123</v>
       </c>
@@ -3875,13 +3872,13 @@
         <v>31</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="D126" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="86.45">
       <c r="A127" s="9">
         <v>124</v>
       </c>
@@ -3889,13 +3886,13 @@
         <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
       <c r="D127" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="57.6">
       <c r="A128" s="9">
         <v>125</v>
       </c>
@@ -3903,13 +3900,13 @@
         <v>31</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" ht="72">
       <c r="A129" s="9">
         <v>126</v>
       </c>
@@ -3917,13 +3914,13 @@
         <v>31</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="D129" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" ht="43.15">
       <c r="A130" s="9">
         <v>127</v>
       </c>
@@ -3931,13 +3928,13 @@
         <v>31</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="D130" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="28.9">
       <c r="A131" s="9">
         <v>128</v>
       </c>
@@ -3945,13 +3942,13 @@
         <v>30</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" ht="43.15">
       <c r="A132" s="9">
         <v>129</v>
       </c>
@@ -3959,13 +3956,13 @@
         <v>30</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18">
       <c r="A133" s="9">
         <v>130</v>
       </c>
@@ -3973,13 +3970,13 @@
         <v>30</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" ht="43.15">
       <c r="A134" s="9">
         <v>131</v>
       </c>
@@ -3987,13 +3984,13 @@
         <v>30</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" ht="43.15">
       <c r="A135" s="9">
         <v>132</v>
       </c>
@@ -4001,13 +3998,13 @@
         <v>30</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="28.9">
       <c r="A136" s="9">
         <v>133</v>
       </c>
@@ -4015,13 +4012,13 @@
         <v>30</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="43.15">
       <c r="A137" s="9">
         <v>134</v>
       </c>
@@ -4029,13 +4026,13 @@
         <v>30</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="28.9">
       <c r="A138" s="9">
         <v>135</v>
       </c>
@@ -4043,13 +4040,13 @@
         <v>30</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" ht="57.6">
       <c r="A139" s="9">
         <v>136</v>
       </c>
@@ -4057,13 +4054,13 @@
         <v>30</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" ht="57.6">
       <c r="A140" s="9">
         <v>137</v>
       </c>
@@ -4071,13 +4068,13 @@
         <v>30</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="187.15">
       <c r="A141" s="9">
         <v>138</v>
       </c>
@@ -4085,13 +4082,13 @@
         <v>30</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18">
       <c r="A142" s="9">
         <v>139</v>
       </c>
@@ -4099,19 +4096,19 @@
         <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>231</v>
+        <v>257</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
       <c r="R142" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="43.15">
       <c r="A143" s="9">
         <v>140</v>
       </c>
@@ -4119,16 +4116,16 @@
         <v>28</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" ht="28.9">
       <c r="A144" s="9">
         <v>141</v>
       </c>
@@ -4136,13 +4133,13 @@
         <v>28</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="28.9">
       <c r="A145" s="9">
         <v>142</v>
       </c>
@@ -4150,13 +4147,13 @@
         <v>28</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="D145" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="28.9">
       <c r="A146" s="9">
         <v>143</v>
       </c>
@@ -4164,13 +4161,13 @@
         <v>28</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="28.9">
       <c r="A147" s="9">
         <v>144</v>
       </c>
@@ -4178,13 +4175,13 @@
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="28.9">
       <c r="A148" s="9">
         <v>145</v>
       </c>
@@ -4192,13 +4189,13 @@
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>241</v>
+        <v>267</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="9">
         <v>146</v>
       </c>
@@ -4206,13 +4203,13 @@
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="28.9">
       <c r="A150" s="9">
         <v>147</v>
       </c>
@@ -4220,13 +4217,13 @@
         <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="28.9">
       <c r="A151" s="9">
         <v>148</v>
       </c>
@@ -4234,13 +4231,13 @@
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="72">
       <c r="A152" s="9">
         <v>149</v>
       </c>
@@ -4248,13 +4245,13 @@
         <v>29</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="57.6">
       <c r="A153" s="9">
         <v>150</v>
       </c>
@@ -4262,13 +4259,13 @@
         <v>29</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="28.9">
       <c r="A154" s="9">
         <v>151</v>
       </c>
@@ -4276,13 +4273,13 @@
         <v>29</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="43.15">
       <c r="A155" s="9">
         <v>152</v>
       </c>
@@ -4290,13 +4287,13 @@
         <v>29</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="43.15">
       <c r="A156" s="9">
         <v>153</v>
       </c>
@@ -4304,13 +4301,13 @@
         <v>29</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="43.15">
       <c r="A157" s="9">
         <v>154</v>
       </c>
@@ -4318,13 +4315,13 @@
         <v>29</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="43.15">
       <c r="A158" s="9">
         <v>155</v>
       </c>
@@ -4332,13 +4329,13 @@
         <v>29</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="57.6">
       <c r="A159" s="9">
         <v>156</v>
       </c>
@@ -4346,13 +4343,13 @@
         <v>29</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="57.6">
       <c r="A160" s="9">
         <v>157</v>
       </c>
@@ -4360,13 +4357,13 @@
         <v>29</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="43.15">
       <c r="A161" s="9">
         <v>158</v>
       </c>
@@ -4374,13 +4371,13 @@
         <v>29</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="43.15">
       <c r="A162" s="9">
         <v>159</v>
       </c>
@@ -4388,13 +4385,13 @@
         <v>29</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>265</v>
+        <v>291</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="43.15">
       <c r="A163" s="9">
         <v>160</v>
       </c>
@@ -4402,13 +4399,13 @@
         <v>29</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>267</v>
+        <v>293</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="43.15">
       <c r="A164" s="9">
         <v>161</v>
       </c>
@@ -4416,13 +4413,13 @@
         <v>29</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>269</v>
+        <v>295</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="28.9">
       <c r="A165" s="9">
         <v>162</v>
       </c>
@@ -4430,13 +4427,13 @@
         <v>29</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="43.15">
       <c r="A166" s="9">
         <v>163</v>
       </c>
@@ -4444,13 +4441,13 @@
         <v>29</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c r="D166" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="43.15">
       <c r="A167" s="9">
         <v>164</v>
       </c>
@@ -4458,13 +4455,13 @@
         <v>29</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="43.15">
       <c r="A168" s="9">
         <v>165</v>
       </c>
@@ -4472,13 +4469,13 @@
         <v>29</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="D168" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="28.9">
       <c r="A169" s="9">
         <v>166</v>
       </c>
@@ -4486,13 +4483,13 @@
         <v>29</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="D169" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="43.15">
       <c r="A170" s="9">
         <v>167</v>
       </c>
@@ -4500,13 +4497,13 @@
         <v>29</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="28.9">
       <c r="A171" s="9">
         <v>168</v>
       </c>
@@ -4514,13 +4511,13 @@
         <v>29</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="28.9">
       <c r="A172" s="9">
         <v>169</v>
       </c>
@@ -4528,13 +4525,13 @@
         <v>32</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="9">
         <v>170</v>
       </c>
@@ -4542,13 +4539,13 @@
         <v>32</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="28.9">
       <c r="A174" s="9">
         <v>171</v>
       </c>
@@ -4556,13 +4553,13 @@
         <v>32</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="28.9">
       <c r="A175" s="9">
         <v>172</v>
       </c>
@@ -4570,13 +4567,13 @@
         <v>32</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="28.9">
       <c r="A176" s="9">
         <v>173</v>
       </c>
@@ -4584,13 +4581,13 @@
         <v>32</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="28.9">
       <c r="A177" s="9">
         <v>174</v>
       </c>
@@ -4598,13 +4595,13 @@
         <v>32</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="28.9">
       <c r="A178" s="9">
         <v>175</v>
       </c>
@@ -4612,13 +4609,13 @@
         <v>32</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="28.9">
       <c r="A179" s="9">
         <v>176</v>
       </c>
@@ -4626,13 +4623,13 @@
         <v>32</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="43.15">
       <c r="A180" s="9">
         <v>177</v>
       </c>
@@ -4640,13 +4637,13 @@
         <v>32</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="28.9">
       <c r="A181" s="9">
         <v>178</v>
       </c>
@@ -4654,13 +4651,13 @@
         <v>32</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="28.9">
       <c r="A182" s="9">
         <v>179</v>
       </c>
@@ -4668,13 +4665,13 @@
         <v>32</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>304</v>
+        <v>330</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="28.9">
       <c r="A183" s="9">
         <v>180</v>
       </c>
@@ -4682,13 +4679,13 @@
         <v>32</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="28.9">
       <c r="A184" s="9">
         <v>181</v>
       </c>
@@ -4696,13 +4693,13 @@
         <v>32</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="28.9">
       <c r="A185" s="9">
         <v>182</v>
       </c>
@@ -4710,13 +4707,13 @@
         <v>32</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="9">
         <v>183</v>
       </c>
@@ -4724,13 +4721,13 @@
         <v>32</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="28.9">
       <c r="A187" s="9">
         <v>184</v>
       </c>
@@ -4738,13 +4735,13 @@
         <v>32</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="28.9">
       <c r="A188" s="9">
         <v>185</v>
       </c>
@@ -4752,13 +4749,13 @@
         <v>32</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" s="9">
         <v>186</v>
       </c>
@@ -4766,13 +4763,13 @@
         <v>32</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="28.9">
       <c r="A190" s="9">
         <v>187</v>
       </c>
@@ -4780,13 +4777,13 @@
         <v>32</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" s="9">
         <v>188</v>
       </c>
@@ -4794,13 +4791,13 @@
         <v>32</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192" s="9">
         <v>189</v>
       </c>
@@ -4808,13 +4805,13 @@
         <v>32</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="D192" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="193" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18" ht="28.9">
       <c r="A193" s="9">
         <v>190</v>
       </c>
@@ -4822,13 +4819,13 @@
         <v>32</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="194" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18">
       <c r="A194" s="9">
         <v>191</v>
       </c>
@@ -4836,13 +4833,13 @@
         <v>32</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="195" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18" ht="28.9">
       <c r="A195" s="9">
         <v>192</v>
       </c>
@@ -4850,16 +4847,16 @@
         <v>32</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" ht="28.9">
       <c r="A196" s="9">
         <v>193</v>
       </c>
@@ -4867,13 +4864,13 @@
         <v>32</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18">
       <c r="A197" s="9">
         <v>194</v>
       </c>
@@ -4881,13 +4878,13 @@
         <v>32</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>333</v>
+        <v>359</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="198" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" ht="28.9">
       <c r="A198" s="9">
         <v>195</v>
       </c>
@@ -4895,13 +4892,13 @@
         <v>32</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>335</v>
+        <v>361</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="199" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18">
       <c r="A199" s="9">
         <v>196</v>
       </c>
@@ -4909,13 +4906,13 @@
         <v>32</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>337</v>
+        <v>363</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18">
       <c r="A200" s="9">
         <v>197</v>
       </c>
@@ -4923,13 +4920,13 @@
         <v>32</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>339</v>
+        <v>365</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18">
       <c r="A201" s="9">
         <v>198</v>
       </c>
@@ -4937,13 +4934,13 @@
         <v>32</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18">
       <c r="A202" s="9">
         <v>199</v>
       </c>
@@ -4951,13 +4948,13 @@
         <v>32</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>343</v>
+        <v>369</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18">
       <c r="A203" s="9">
         <v>200</v>
       </c>
@@ -4965,13 +4962,13 @@
         <v>32</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>345</v>
+        <v>371</v>
       </c>
       <c r="D203" s="10" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="204" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18">
       <c r="A204" s="9">
         <v>201</v>
       </c>
@@ -4979,13 +4976,13 @@
         <v>32</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" ht="28.9">
       <c r="A205" s="9">
         <v>202</v>
       </c>
@@ -4993,13 +4990,13 @@
         <v>32</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="D205" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="206" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18">
       <c r="A206" s="9">
         <v>203</v>
       </c>
@@ -5007,13 +5004,13 @@
         <v>32</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>350</v>
+        <v>376</v>
       </c>
       <c r="D206" s="10" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="207" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18">
       <c r="A207" s="9">
         <v>204</v>
       </c>
@@ -5021,16 +5018,16 @@
         <v>32</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="D207" s="10" t="s">
-        <v>353</v>
+        <v>379</v>
       </c>
       <c r="R207" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="208" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" ht="29.25">
       <c r="A208" s="8">
         <v>205</v>
       </c>
@@ -5038,13 +5035,13 @@
         <v>25</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>355</v>
+        <v>381</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="209" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" ht="43.5">
       <c r="A209" s="8">
         <v>206</v>
       </c>
@@ -5052,13 +5049,13 @@
         <v>25</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>357</v>
+        <v>383</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="210" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" ht="43.5">
       <c r="A210" s="8">
         <v>207</v>
       </c>
@@ -5066,16 +5063,16 @@
         <v>25</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>359</v>
+        <v>385</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>360</v>
+        <v>386</v>
       </c>
       <c r="R210" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="211" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" ht="43.5">
       <c r="A211" s="8">
         <v>208</v>
       </c>
@@ -5083,13 +5080,13 @@
         <v>25</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>362</v>
+        <v>388</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="212" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" ht="29.25">
       <c r="A212" s="8">
         <v>209</v>
       </c>
@@ -5097,13 +5094,13 @@
         <v>25</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>364</v>
+        <v>390</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="213" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" ht="29.25">
       <c r="A213" s="8">
         <v>210</v>
       </c>
@@ -5111,13 +5108,13 @@
         <v>25</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>366</v>
+        <v>392</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="214" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" ht="29.25">
       <c r="A214" s="8">
         <v>211</v>
       </c>
@@ -5125,13 +5122,13 @@
         <v>25</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>368</v>
+        <v>394</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="215" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" ht="43.5">
       <c r="A215" s="8">
         <v>212</v>
       </c>
@@ -5139,16 +5136,16 @@
         <v>25</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>370</v>
+        <v>396</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>365</v>
+        <v>391</v>
       </c>
       <c r="R215" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="216" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" ht="29.25">
       <c r="A216" s="8">
         <v>213</v>
       </c>
@@ -5156,13 +5153,13 @@
         <v>25</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>372</v>
+        <v>398</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" ht="15">
       <c r="A217" s="8">
         <v>214</v>
       </c>
@@ -5170,13 +5167,13 @@
         <v>25</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>374</v>
+        <v>400</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="218" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" ht="29.25">
       <c r="A218" s="8">
         <v>215</v>
       </c>
@@ -5184,13 +5181,13 @@
         <v>25</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="219" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" ht="29.25">
       <c r="A219" s="9">
         <v>216</v>
       </c>
@@ -5198,13 +5195,13 @@
         <v>25</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>377</v>
+        <v>403</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="220" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" ht="29.25">
       <c r="A220" s="9">
         <v>217</v>
       </c>
@@ -5212,13 +5209,13 @@
         <v>25</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="221" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" ht="29.25">
       <c r="A221" s="9">
         <v>218</v>
       </c>
@@ -5226,16 +5223,16 @@
         <v>25</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="R221" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="222" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" ht="30.75">
       <c r="A222" s="9">
         <v>219</v>
       </c>
@@ -5243,13 +5240,13 @@
         <v>25</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="223" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" ht="29.25">
       <c r="A223" s="9">
         <v>220</v>
       </c>
@@ -5257,13 +5254,13 @@
         <v>25</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="224" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" ht="29.25">
       <c r="A224" s="9">
         <v>221</v>
       </c>
@@ -5271,15 +5268,15 @@
         <v>25</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="230" spans="18:18" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="230" spans="18:18">
       <c r="R230" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -5290,14 +5287,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDD0FC4969DCF4449136D2C873E795D1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c6f44795faba901663e8a9bf3a6322e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d2c32087-eb03-4a65-b505-380146e007a4" xmlns:ns4="2f381668-55bb-4cca-a2e9-7746dbcfba3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7caa3c07606457882248d14e3a3261f4" ns3:_="" ns4:_="">
     <xsd:import namespace="d2c32087-eb03-4a65-b505-380146e007a4"/>
@@ -5518,6 +5507,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5528,38 +5525,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
-    <ds:schemaRef ds:uri="2f381668-55bb-4cca-a2e9-7746dbcfba3d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}"/>
 </file>
</xml_diff>

<commit_message>
Added UI XREF diagram to the game display reqs
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/anh7674_mavs_uta_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BC9751C-A6C4-4E21-8EB6-DDB8B1DF3622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0D52E4-04C9-42BB-BA42-1AC5434149D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="422">
   <si>
     <t>Tested By</t>
   </si>
@@ -1309,12 +1309,30 @@
   <si>
     <t>summary:</t>
   </si>
+  <si>
+    <t>UI011</t>
+  </si>
+  <si>
+    <t>UI012</t>
+  </si>
+  <si>
+    <t>UI013</t>
+  </si>
+  <si>
+    <t>UI014</t>
+  </si>
+  <si>
+    <t>UI015</t>
+  </si>
+  <si>
+    <t>UI016</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1747,6 +1765,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>381889</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>372271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29CA7573-E112-928C-388C-1FAFFDCA2666}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21040725" y="37909500"/>
+          <a:ext cx="6373114" cy="5706271"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2069,11 +2131,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" topLeftCell="B78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S84" sqref="S84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
@@ -2084,12 +2146,12 @@
     <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2127,7 +2189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -2147,7 +2209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="43.15">
+    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2170,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="28.9">
+    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2184,7 +2246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="28.9">
+    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2198,7 +2260,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.9">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2212,7 +2274,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2226,7 +2288,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="28.9">
+    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2240,7 +2302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="28.9">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2254,7 +2316,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="28.9">
+    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2268,7 +2330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2282,7 +2344,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="28.9">
+    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2296,7 +2358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2310,7 +2372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="28.9">
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2324,7 +2386,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2338,7 +2400,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.9">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2352,7 +2414,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.9">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2366,7 +2428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.9">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2380,7 +2442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.9">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2394,7 +2456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.9">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2408,7 +2470,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="43.15">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2422,7 +2484,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43.15">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2436,7 +2498,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.9">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2450,7 +2512,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.9">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2464,7 +2526,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="43.15">
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2478,7 +2540,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.9">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2492,7 +2554,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.9">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2506,7 +2568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="43.15">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2520,7 +2582,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="28.9">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2534,7 +2596,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="43.15">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2548,7 +2610,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28.9">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2562,7 +2624,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.9">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2576,7 +2638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.9">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>31</v>
       </c>
@@ -2590,7 +2652,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.9">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>32</v>
       </c>
@@ -2604,7 +2666,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="43.15">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>33</v>
       </c>
@@ -2618,7 +2680,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="43.15">
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>34</v>
       </c>
@@ -2632,7 +2694,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="57.6">
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>35</v>
       </c>
@@ -2646,7 +2708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.9">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>36</v>
       </c>
@@ -2660,7 +2722,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.9">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>37</v>
       </c>
@@ -2674,7 +2736,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28.9">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>38</v>
       </c>
@@ -2688,7 +2750,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>39</v>
       </c>
@@ -2702,7 +2764,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28.9">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>40</v>
       </c>
@@ -2716,7 +2778,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.9">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>41</v>
       </c>
@@ -2730,7 +2792,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.9">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>42</v>
       </c>
@@ -2744,7 +2806,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.9">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>43</v>
       </c>
@@ -2758,7 +2820,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="57.6">
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>44</v>
       </c>
@@ -2772,7 +2834,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="43.15">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>45</v>
       </c>
@@ -2786,7 +2848,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="28.9">
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>46</v>
       </c>
@@ -2800,7 +2862,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.9">
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>47</v>
       </c>
@@ -2814,7 +2876,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.9">
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>48</v>
       </c>
@@ -2828,7 +2890,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="28.9">
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>49</v>
       </c>
@@ -2842,7 +2904,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="43.15">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>50</v>
       </c>
@@ -2856,7 +2918,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.9">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>51</v>
       </c>
@@ -2870,7 +2932,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.9">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>52</v>
       </c>
@@ -2884,7 +2946,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="28.9">
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>53</v>
       </c>
@@ -2898,7 +2960,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28.9">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>54</v>
       </c>
@@ -2912,7 +2974,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="28.9">
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>55</v>
       </c>
@@ -2926,7 +2988,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="28.9">
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>56</v>
       </c>
@@ -2940,7 +3002,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.9">
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>57</v>
       </c>
@@ -2954,7 +3016,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="43.15">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>58</v>
       </c>
@@ -2968,7 +3030,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.9">
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>59</v>
       </c>
@@ -2982,7 +3044,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="28.9">
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>60</v>
       </c>
@@ -2996,7 +3058,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="28.9">
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>61</v>
       </c>
@@ -3010,7 +3072,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="72">
+    <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>62</v>
       </c>
@@ -3024,7 +3086,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="57.6">
+    <row r="66" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>63</v>
       </c>
@@ -3038,7 +3100,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="28.9">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>64</v>
       </c>
@@ -3052,7 +3114,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="28.9">
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>65</v>
       </c>
@@ -3066,7 +3128,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="28.9">
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>66</v>
       </c>
@@ -3080,7 +3142,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.9">
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>67</v>
       </c>
@@ -3094,7 +3156,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="43.15">
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>68</v>
       </c>
@@ -3108,7 +3170,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="57.6">
+    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>69</v>
       </c>
@@ -3122,7 +3184,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="28.9">
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>70</v>
       </c>
@@ -3136,7 +3198,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="43.15">
+    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>71</v>
       </c>
@@ -3150,7 +3212,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>72</v>
       </c>
@@ -3164,7 +3226,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="43.15">
+    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>73</v>
       </c>
@@ -3178,7 +3240,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="43.15">
+    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>74</v>
       </c>
@@ -3192,7 +3254,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="28.9">
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>75</v>
       </c>
@@ -3206,7 +3268,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="28.9">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>76</v>
       </c>
@@ -3220,7 +3282,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="28.9">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>77</v>
       </c>
@@ -3234,7 +3296,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="28.9">
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>78</v>
       </c>
@@ -3248,7 +3310,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="28.9">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>79</v>
       </c>
@@ -3262,7 +3324,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>80</v>
       </c>
@@ -3276,7 +3338,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="57.6">
+    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>81</v>
       </c>
@@ -3289,8 +3351,11 @@
       <c r="D84" s="10" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="43.15">
+      <c r="E84" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>82</v>
       </c>
@@ -3303,8 +3368,11 @@
       <c r="D85" s="10" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="72">
+      <c r="E85" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>83</v>
       </c>
@@ -3317,8 +3385,11 @@
       <c r="D86" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>84</v>
       </c>
@@ -3331,8 +3402,11 @@
       <c r="D87" s="10" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="28.9">
+      <c r="E87" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>85</v>
       </c>
@@ -3346,7 +3420,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="43.15">
+    <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>86</v>
       </c>
@@ -3360,7 +3434,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="28.9">
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>87</v>
       </c>
@@ -3373,8 +3447,11 @@
       <c r="D90" s="10" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="28.9">
+      <c r="E90" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>88</v>
       </c>
@@ -3388,7 +3465,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="28.9">
+    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>89</v>
       </c>
@@ -3401,8 +3478,11 @@
       <c r="D92" s="10" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="28.9">
+      <c r="E92" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>90</v>
       </c>
@@ -3416,7 +3496,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="28.9">
+    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>91</v>
       </c>
@@ -3430,7 +3510,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="28.9">
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>92</v>
       </c>
@@ -3444,7 +3524,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="28.9">
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>93</v>
       </c>
@@ -3458,7 +3538,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="43.15">
+    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>94</v>
       </c>
@@ -3472,7 +3552,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="28.9">
+    <row r="98" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>95</v>
       </c>
@@ -3486,7 +3566,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="28.9">
+    <row r="99" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>96</v>
       </c>
@@ -3500,7 +3580,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.9">
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>97</v>
       </c>
@@ -3514,7 +3594,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>98</v>
       </c>
@@ -3528,7 +3608,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="28.9">
+    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>99</v>
       </c>
@@ -3542,7 +3622,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="57.6">
+    <row r="103" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>100</v>
       </c>
@@ -3556,7 +3636,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="43.15">
+    <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>101</v>
       </c>
@@ -3570,7 +3650,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="28.9">
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>102</v>
       </c>
@@ -3584,7 +3664,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="43.15">
+    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>103</v>
       </c>
@@ -3598,7 +3678,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="28.9">
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>104</v>
       </c>
@@ -3612,7 +3692,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="86.45">
+    <row r="108" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>105</v>
       </c>
@@ -3626,7 +3706,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="28.9">
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>106</v>
       </c>
@@ -3640,7 +3720,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <v>107</v>
       </c>
@@ -3654,7 +3734,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="43.15">
+    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="9">
         <v>108</v>
       </c>
@@ -3668,7 +3748,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="57.6">
+    <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <v>109</v>
       </c>
@@ -3682,7 +3762,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="28.9">
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <v>110</v>
       </c>
@@ -3696,7 +3776,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="9">
         <v>111</v>
       </c>
@@ -3710,7 +3790,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="43.15">
+    <row r="115" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="9">
         <v>112</v>
       </c>
@@ -3724,7 +3804,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="28.9">
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <v>113</v>
       </c>
@@ -3738,7 +3818,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="43.15">
+    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <v>114</v>
       </c>
@@ -3752,7 +3832,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="43.15">
+    <row r="118" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>115</v>
       </c>
@@ -3766,7 +3846,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="28.9">
+    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <v>116</v>
       </c>
@@ -3780,7 +3860,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="43.15">
+    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>117</v>
       </c>
@@ -3794,7 +3874,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="43.15">
+    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>118</v>
       </c>
@@ -3808,7 +3888,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="43.15">
+    <row r="122" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" s="9">
         <v>119</v>
       </c>
@@ -3822,7 +3902,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="43.15">
+    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="9">
         <v>120</v>
       </c>
@@ -3836,7 +3916,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="43.15">
+    <row r="124" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="9">
         <v>121</v>
       </c>
@@ -3850,7 +3930,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="28.9">
+    <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>122</v>
       </c>
@@ -3864,7 +3944,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="72">
+    <row r="126" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>123</v>
       </c>
@@ -3878,7 +3958,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="86.45">
+    <row r="127" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>124</v>
       </c>
@@ -3892,7 +3972,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="57.6">
+    <row r="128" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>125</v>
       </c>
@@ -3906,7 +3986,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="72">
+    <row r="129" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <v>126</v>
       </c>
@@ -3920,7 +4000,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="43.15">
+    <row r="130" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>127</v>
       </c>
@@ -3934,7 +4014,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="28.9">
+    <row r="131" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="9">
         <v>128</v>
       </c>
@@ -3948,7 +4028,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="43.15">
+    <row r="132" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <v>129</v>
       </c>
@@ -3962,7 +4042,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="9">
         <v>130</v>
       </c>
@@ -3976,7 +4056,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="43.15">
+    <row r="134" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <v>131</v>
       </c>
@@ -3990,7 +4070,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="43.15">
+    <row r="135" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="9">
         <v>132</v>
       </c>
@@ -4004,7 +4084,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="28.9">
+    <row r="136" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="9">
         <v>133</v>
       </c>
@@ -4018,7 +4098,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="43.15">
+    <row r="137" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="9">
         <v>134</v>
       </c>
@@ -4032,7 +4112,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="28.9">
+    <row r="138" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="9">
         <v>135</v>
       </c>
@@ -4046,7 +4126,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="57.6">
+    <row r="139" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <v>136</v>
       </c>
@@ -4060,7 +4140,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="57.6">
+    <row r="140" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <v>137</v>
       </c>
@@ -4074,7 +4154,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="187.15">
+    <row r="141" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <v>138</v>
       </c>
@@ -4088,7 +4168,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <v>139</v>
       </c>
@@ -4108,7 +4188,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="43.15">
+    <row r="143" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="9">
         <v>140</v>
       </c>
@@ -4125,7 +4205,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="28.9">
+    <row r="144" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="9">
         <v>141</v>
       </c>
@@ -4139,7 +4219,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="28.9">
+    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>142</v>
       </c>
@@ -4153,7 +4233,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="28.9">
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="9">
         <v>143</v>
       </c>
@@ -4167,7 +4247,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="28.9">
+    <row r="147" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <v>144</v>
       </c>
@@ -4181,7 +4261,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="28.9">
+    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="9">
         <v>145</v>
       </c>
@@ -4195,7 +4275,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9">
         <v>146</v>
       </c>
@@ -4209,7 +4289,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="28.9">
+    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="9">
         <v>147</v>
       </c>
@@ -4223,7 +4303,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="28.9">
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="9">
         <v>148</v>
       </c>
@@ -4237,7 +4317,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="72">
+    <row r="152" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A152" s="9">
         <v>149</v>
       </c>
@@ -4251,7 +4331,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="57.6">
+    <row r="153" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="9">
         <v>150</v>
       </c>
@@ -4265,7 +4345,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="28.9">
+    <row r="154" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
         <v>151</v>
       </c>
@@ -4279,7 +4359,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="43.15">
+    <row r="155" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="9">
         <v>152</v>
       </c>
@@ -4293,7 +4373,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="43.15">
+    <row r="156" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <v>153</v>
       </c>
@@ -4307,7 +4387,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="43.15">
+    <row r="157" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="9">
         <v>154</v>
       </c>
@@ -4321,7 +4401,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="43.15">
+    <row r="158" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
         <v>155</v>
       </c>
@@ -4335,7 +4415,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="57.6">
+    <row r="159" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
         <v>156</v>
       </c>
@@ -4349,7 +4429,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="57.6">
+    <row r="160" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" s="9">
         <v>157</v>
       </c>
@@ -4363,7 +4443,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="43.15">
+    <row r="161" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" s="9">
         <v>158</v>
       </c>
@@ -4377,7 +4457,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="43.15">
+    <row r="162" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="9">
         <v>159</v>
       </c>
@@ -4391,7 +4471,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="43.15">
+    <row r="163" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <v>160</v>
       </c>
@@ -4405,7 +4485,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="43.15">
+    <row r="164" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="9">
         <v>161</v>
       </c>
@@ -4419,7 +4499,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="28.9">
+    <row r="165" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="9">
         <v>162</v>
       </c>
@@ -4433,7 +4513,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="43.15">
+    <row r="166" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A166" s="9">
         <v>163</v>
       </c>
@@ -4447,7 +4527,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="43.15">
+    <row r="167" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A167" s="9">
         <v>164</v>
       </c>
@@ -4461,7 +4541,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="43.15">
+    <row r="168" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A168" s="9">
         <v>165</v>
       </c>
@@ -4475,7 +4555,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="28.9">
+    <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="9">
         <v>166</v>
       </c>
@@ -4489,7 +4569,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="43.15">
+    <row r="170" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="9">
         <v>167</v>
       </c>
@@ -4503,7 +4583,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="28.9">
+    <row r="171" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="9">
         <v>168</v>
       </c>
@@ -4517,7 +4597,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="28.9">
+    <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="9">
         <v>169</v>
       </c>
@@ -4531,7 +4611,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="9">
         <v>170</v>
       </c>
@@ -4545,7 +4625,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="28.9">
+    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="9">
         <v>171</v>
       </c>
@@ -4559,7 +4639,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="28.9">
+    <row r="175" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="9">
         <v>172</v>
       </c>
@@ -4573,7 +4653,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="28.9">
+    <row r="176" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="9">
         <v>173</v>
       </c>
@@ -4587,7 +4667,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="28.9">
+    <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="9">
         <v>174</v>
       </c>
@@ -4601,7 +4681,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="28.9">
+    <row r="178" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="9">
         <v>175</v>
       </c>
@@ -4615,7 +4695,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="28.9">
+    <row r="179" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="9">
         <v>176</v>
       </c>
@@ -4629,7 +4709,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="43.15">
+    <row r="180" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="9">
         <v>177</v>
       </c>
@@ -4643,7 +4723,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="28.9">
+    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="9">
         <v>178</v>
       </c>
@@ -4657,7 +4737,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="28.9">
+    <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="9">
         <v>179</v>
       </c>
@@ -4671,7 +4751,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="28.9">
+    <row r="183" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="9">
         <v>180</v>
       </c>
@@ -4685,7 +4765,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="28.9">
+    <row r="184" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="9">
         <v>181</v>
       </c>
@@ -4699,7 +4779,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="28.9">
+    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="9">
         <v>182</v>
       </c>
@@ -4713,7 +4793,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="9">
         <v>183</v>
       </c>
@@ -4727,7 +4807,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="28.9">
+    <row r="187" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="9">
         <v>184</v>
       </c>
@@ -4741,7 +4821,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="28.9">
+    <row r="188" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="9">
         <v>185</v>
       </c>
@@ -4755,7 +4835,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="9">
         <v>186</v>
       </c>
@@ -4769,7 +4849,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="28.9">
+    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="9">
         <v>187</v>
       </c>
@@ -4783,7 +4863,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="9">
         <v>188</v>
       </c>
@@ -4797,7 +4877,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="9">
         <v>189</v>
       </c>
@@ -4811,7 +4891,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="28.9">
+    <row r="193" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="9">
         <v>190</v>
       </c>
@@ -4825,7 +4905,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="9">
         <v>191</v>
       </c>
@@ -4839,7 +4919,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="28.9">
+    <row r="195" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="9">
         <v>192</v>
       </c>
@@ -4856,7 +4936,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="196" spans="1:18" ht="28.9">
+    <row r="196" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="9">
         <v>193</v>
       </c>
@@ -4870,7 +4950,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="197" spans="1:18">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="9">
         <v>194</v>
       </c>
@@ -4884,7 +4964,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="28.9">
+    <row r="198" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="9">
         <v>195</v>
       </c>
@@ -4898,7 +4978,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="199" spans="1:18">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="9">
         <v>196</v>
       </c>
@@ -4912,7 +4992,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="200" spans="1:18">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="9">
         <v>197</v>
       </c>
@@ -4926,7 +5006,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="201" spans="1:18">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="9">
         <v>198</v>
       </c>
@@ -4940,7 +5020,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="202" spans="1:18">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="9">
         <v>199</v>
       </c>
@@ -4954,7 +5034,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="203" spans="1:18">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="9">
         <v>200</v>
       </c>
@@ -4968,7 +5048,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="204" spans="1:18">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="9">
         <v>201</v>
       </c>
@@ -4982,7 +5062,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="28.9">
+    <row r="205" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="9">
         <v>202</v>
       </c>
@@ -4996,7 +5076,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="206" spans="1:18">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="9">
         <v>203</v>
       </c>
@@ -5010,7 +5090,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="207" spans="1:18">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="9">
         <v>204</v>
       </c>
@@ -5027,7 +5107,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="208" spans="1:18" ht="29.25">
+    <row r="208" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="8">
         <v>205</v>
       </c>
@@ -5041,7 +5121,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="209" spans="1:18" ht="43.5">
+    <row r="209" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" s="8">
         <v>206</v>
       </c>
@@ -5055,7 +5135,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="210" spans="1:18" ht="43.5">
+    <row r="210" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="8">
         <v>207</v>
       </c>
@@ -5072,7 +5152,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="43.5">
+    <row r="211" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A211" s="8">
         <v>208</v>
       </c>
@@ -5086,7 +5166,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="29.25">
+    <row r="212" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" s="8">
         <v>209</v>
       </c>
@@ -5100,7 +5180,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="213" spans="1:18" ht="29.25">
+    <row r="213" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="8">
         <v>210</v>
       </c>
@@ -5114,7 +5194,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="29.25">
+    <row r="214" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="8">
         <v>211</v>
       </c>
@@ -5128,7 +5208,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="43.5">
+    <row r="215" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="8">
         <v>212</v>
       </c>
@@ -5145,7 +5225,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="29.25">
+    <row r="216" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="8">
         <v>213</v>
       </c>
@@ -5159,7 +5239,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="217" spans="1:18" ht="15">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="8">
         <v>214</v>
       </c>
@@ -5173,7 +5253,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="218" spans="1:18" ht="29.25">
+    <row r="218" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="8">
         <v>215</v>
       </c>
@@ -5187,7 +5267,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="219" spans="1:18" ht="29.25">
+    <row r="219" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="9">
         <v>216</v>
       </c>
@@ -5201,7 +5281,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="29.25">
+    <row r="220" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="9">
         <v>217</v>
       </c>
@@ -5215,7 +5295,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="29.25">
+    <row r="221" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="9">
         <v>218</v>
       </c>
@@ -5232,7 +5312,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="30.75">
+    <row r="222" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="9">
         <v>219</v>
       </c>
@@ -5246,7 +5326,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="29.25">
+    <row r="223" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="9">
         <v>220</v>
       </c>
@@ -5260,7 +5340,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="224" spans="1:18" ht="29.25">
+    <row r="224" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="9">
         <v>221</v>
       </c>
@@ -5274,7 +5354,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="230" spans="18:18">
+    <row r="230" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R230" t="s">
         <v>415</v>
       </c>
@@ -5287,6 +5367,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDD0FC4969DCF4449136D2C873E795D1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c6f44795faba901663e8a9bf3a6322e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d2c32087-eb03-4a65-b505-380146e007a4" xmlns:ns4="2f381668-55bb-4cca-a2e9-7746dbcfba3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7caa3c07606457882248d14e3a3261f4" ns3:_="" ns4:_="">
     <xsd:import namespace="d2c32087-eb03-4a65-b505-380146e007a4"/>
@@ -5507,31 +5604,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
+    <ds:schemaRef ds:uri="2f381668-55bb-4cca-a2e9-7746dbcfba3d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added join game UI elements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0D52E4-04C9-42BB-BA42-1AC5434149D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904C9C2F-7EE0-7544-BFC0-A5B13BBC8A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="430">
   <si>
     <t>Tested By</t>
   </si>
@@ -1327,12 +1327,36 @@
   <si>
     <t>UI016</t>
   </si>
+  <si>
+    <t>UI-JG-01</t>
+  </si>
+  <si>
+    <t>UI-JG-02</t>
+  </si>
+  <si>
+    <t>UI-JG-03</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>UI-JG-04</t>
+  </si>
+  <si>
+    <t>UI-JG-05</t>
+  </si>
+  <si>
+    <t>UI-JG-06</t>
+  </si>
+  <si>
+    <t>UI-JG-07</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1809,6 +1833,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>147674</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>498549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>371656</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>118139</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{237EAACE-AF7F-5A0E-4162-B64971FD277B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="24248139" y="21320642"/>
+          <a:ext cx="14577936" cy="7889357"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2131,27 +2216,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S84" sqref="S84"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF76" sqref="AF76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2189,7 +2274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="16">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -2209,7 +2294,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="48">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2232,7 +2317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="16">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2246,7 +2331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="16">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2260,7 +2345,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="32">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2274,7 +2359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="16">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2288,7 +2373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="32">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2302,7 +2387,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="32">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2316,7 +2401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="32">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2330,7 +2415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="16">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2344,7 +2429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="16">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2358,7 +2443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="16">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2372,7 +2457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="32">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2386,7 +2471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="16">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2400,7 +2485,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="32">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2414,7 +2499,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="32">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2428,7 +2513,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="32">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2442,7 +2527,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="32">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2456,7 +2541,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2470,7 +2555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="32">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2484,7 +2569,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="48">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2498,7 +2583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="32">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2512,7 +2597,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="32">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2526,7 +2611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="48">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2540,7 +2625,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="32">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2554,7 +2639,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="32">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2568,7 +2653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="48">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2582,7 +2667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="32">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2596,7 +2681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="32">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2610,7 +2695,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="32">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2624,7 +2709,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="32">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2638,7 +2723,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="32">
       <c r="A34" s="9">
         <v>31</v>
       </c>
@@ -2652,7 +2737,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="32">
       <c r="A35" s="9">
         <v>32</v>
       </c>
@@ -2666,7 +2751,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="48">
       <c r="A36" s="9">
         <v>33</v>
       </c>
@@ -2680,7 +2765,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="48">
       <c r="A37" s="9">
         <v>34</v>
       </c>
@@ -2694,7 +2779,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="64">
       <c r="A38" s="9">
         <v>35</v>
       </c>
@@ -2708,7 +2793,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="32">
       <c r="A39" s="9">
         <v>36</v>
       </c>
@@ -2722,7 +2807,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="32">
       <c r="A40" s="9">
         <v>37</v>
       </c>
@@ -2736,7 +2821,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="32">
       <c r="A41" s="9">
         <v>38</v>
       </c>
@@ -2750,7 +2835,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16">
       <c r="A42" s="9">
         <v>39</v>
       </c>
@@ -2764,7 +2849,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="32">
       <c r="A43" s="9">
         <v>40</v>
       </c>
@@ -2778,7 +2863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="32">
       <c r="A44" s="9">
         <v>41</v>
       </c>
@@ -2792,7 +2877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="32">
       <c r="A45" s="9">
         <v>42</v>
       </c>
@@ -2806,7 +2891,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="32">
       <c r="A46" s="9">
         <v>43</v>
       </c>
@@ -2820,7 +2905,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="48">
       <c r="A47" s="9">
         <v>44</v>
       </c>
@@ -2834,7 +2919,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="32">
       <c r="A48" s="9">
         <v>45</v>
       </c>
@@ -2848,7 +2933,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="32">
       <c r="A49" s="9">
         <v>46</v>
       </c>
@@ -2862,7 +2947,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="32">
       <c r="A50" s="9">
         <v>47</v>
       </c>
@@ -2876,7 +2961,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="32">
       <c r="A51" s="9">
         <v>48</v>
       </c>
@@ -2890,7 +2975,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="32">
       <c r="A52" s="9">
         <v>49</v>
       </c>
@@ -2904,7 +2989,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="48">
       <c r="A53" s="9">
         <v>50</v>
       </c>
@@ -2917,8 +3002,11 @@
       <c r="D53" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="32">
       <c r="A54" s="9">
         <v>51</v>
       </c>
@@ -2931,8 +3019,11 @@
       <c r="D54" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16">
       <c r="A55" s="9">
         <v>52</v>
       </c>
@@ -2945,8 +3036,11 @@
       <c r="D55" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="32">
       <c r="A56" s="9">
         <v>53</v>
       </c>
@@ -2959,8 +3053,11 @@
       <c r="D56" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="32">
       <c r="A57" s="9">
         <v>54</v>
       </c>
@@ -2973,8 +3070,11 @@
       <c r="D57" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="32">
       <c r="A58" s="9">
         <v>55</v>
       </c>
@@ -2987,8 +3087,11 @@
       <c r="D58" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="32">
       <c r="A59" s="9">
         <v>56</v>
       </c>
@@ -3001,8 +3104,11 @@
       <c r="D59" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="32">
       <c r="A60" s="9">
         <v>57</v>
       </c>
@@ -3015,8 +3121,11 @@
       <c r="D60" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="32">
       <c r="A61" s="9">
         <v>58</v>
       </c>
@@ -3029,8 +3138,11 @@
       <c r="D61" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="32">
       <c r="A62" s="9">
         <v>59</v>
       </c>
@@ -3043,8 +3155,11 @@
       <c r="D62" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="32">
       <c r="A63" s="9">
         <v>60</v>
       </c>
@@ -3057,8 +3172,11 @@
       <c r="D63" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="32">
       <c r="A64" s="9">
         <v>61</v>
       </c>
@@ -3071,8 +3189,11 @@
       <c r="D64" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="64">
       <c r="A65" s="9">
         <v>62</v>
       </c>
@@ -3085,8 +3206,11 @@
       <c r="D65" s="10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="64">
       <c r="A66" s="9">
         <v>63</v>
       </c>
@@ -3099,8 +3223,11 @@
       <c r="D66" s="10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="32">
       <c r="A67" s="9">
         <v>64</v>
       </c>
@@ -3113,8 +3240,11 @@
       <c r="D67" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="32">
       <c r="A68" s="9">
         <v>65</v>
       </c>
@@ -3127,8 +3257,11 @@
       <c r="D68" s="10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="32">
       <c r="A69" s="9">
         <v>66</v>
       </c>
@@ -3141,8 +3274,11 @@
       <c r="D69" s="10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="32">
       <c r="A70" s="9">
         <v>67</v>
       </c>
@@ -3155,8 +3291,11 @@
       <c r="D70" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="48">
       <c r="A71" s="9">
         <v>68</v>
       </c>
@@ -3169,8 +3308,11 @@
       <c r="D71" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="64">
       <c r="A72" s="9">
         <v>69</v>
       </c>
@@ -3183,8 +3325,11 @@
       <c r="D72" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="32">
       <c r="A73" s="9">
         <v>70</v>
       </c>
@@ -3198,7 +3343,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="48">
       <c r="A74" s="9">
         <v>71</v>
       </c>
@@ -3212,7 +3357,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="16">
       <c r="A75" s="9">
         <v>72</v>
       </c>
@@ -3226,7 +3371,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="48">
       <c r="A76" s="9">
         <v>73</v>
       </c>
@@ -3240,7 +3385,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="48">
       <c r="A77" s="9">
         <v>74</v>
       </c>
@@ -3254,7 +3399,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="32">
       <c r="A78" s="9">
         <v>75</v>
       </c>
@@ -3268,7 +3413,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="32">
       <c r="A79" s="9">
         <v>76</v>
       </c>
@@ -3282,7 +3427,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="32">
       <c r="A80" s="9">
         <v>77</v>
       </c>
@@ -3296,7 +3441,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="32">
       <c r="A81" s="9">
         <v>78</v>
       </c>
@@ -3310,7 +3455,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="32">
       <c r="A82" s="9">
         <v>79</v>
       </c>
@@ -3324,7 +3469,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="16">
       <c r="A83" s="9">
         <v>80</v>
       </c>
@@ -3338,7 +3483,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="48">
       <c r="A84" s="9">
         <v>81</v>
       </c>
@@ -3355,7 +3500,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="48">
       <c r="A85" s="9">
         <v>82</v>
       </c>
@@ -3372,7 +3517,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="80">
       <c r="A86" s="9">
         <v>83</v>
       </c>
@@ -3389,7 +3534,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="16">
       <c r="A87" s="9">
         <v>84</v>
       </c>
@@ -3406,7 +3551,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="32">
       <c r="A88" s="9">
         <v>85</v>
       </c>
@@ -3420,7 +3565,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="48">
       <c r="A89" s="9">
         <v>86</v>
       </c>
@@ -3434,7 +3579,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="32">
       <c r="A90" s="9">
         <v>87</v>
       </c>
@@ -3451,7 +3596,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="16">
       <c r="A91" s="9">
         <v>88</v>
       </c>
@@ -3465,7 +3610,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="32">
       <c r="A92" s="9">
         <v>89</v>
       </c>
@@ -3482,7 +3627,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="32">
       <c r="A93" s="9">
         <v>90</v>
       </c>
@@ -3496,7 +3641,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="32">
       <c r="A94" s="9">
         <v>91</v>
       </c>
@@ -3510,7 +3655,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="32">
       <c r="A95" s="9">
         <v>92</v>
       </c>
@@ -3524,7 +3669,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="32">
       <c r="A96" s="9">
         <v>93</v>
       </c>
@@ -3538,7 +3683,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="32">
       <c r="A97" s="9">
         <v>94</v>
       </c>
@@ -3552,7 +3697,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="32">
       <c r="A98" s="9">
         <v>95</v>
       </c>
@@ -3566,7 +3711,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="32">
       <c r="A99" s="9">
         <v>96</v>
       </c>
@@ -3580,7 +3725,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="32">
       <c r="A100" s="9">
         <v>97</v>
       </c>
@@ -3594,7 +3739,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="16">
       <c r="A101" s="9">
         <v>98</v>
       </c>
@@ -3608,7 +3753,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="32">
       <c r="A102" s="9">
         <v>99</v>
       </c>
@@ -3622,7 +3767,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="48">
       <c r="A103" s="9">
         <v>100</v>
       </c>
@@ -3636,7 +3781,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="48">
       <c r="A104" s="9">
         <v>101</v>
       </c>
@@ -3650,7 +3795,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="32">
       <c r="A105" s="9">
         <v>102</v>
       </c>
@@ -3664,7 +3809,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="48">
       <c r="A106" s="9">
         <v>103</v>
       </c>
@@ -3678,7 +3823,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="32">
       <c r="A107" s="9">
         <v>104</v>
       </c>
@@ -3692,7 +3837,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="96">
       <c r="A108" s="9">
         <v>105</v>
       </c>
@@ -3706,7 +3851,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="32">
       <c r="A109" s="9">
         <v>106</v>
       </c>
@@ -3720,7 +3865,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="16">
       <c r="A110" s="9">
         <v>107</v>
       </c>
@@ -3734,7 +3879,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="32">
       <c r="A111" s="9">
         <v>108</v>
       </c>
@@ -3748,7 +3893,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="48">
       <c r="A112" s="9">
         <v>109</v>
       </c>
@@ -3762,7 +3907,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="32">
       <c r="A113" s="9">
         <v>110</v>
       </c>
@@ -3776,7 +3921,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="16">
       <c r="A114" s="9">
         <v>111</v>
       </c>
@@ -3790,7 +3935,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="32">
       <c r="A115" s="9">
         <v>112</v>
       </c>
@@ -3804,7 +3949,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="32">
       <c r="A116" s="9">
         <v>113</v>
       </c>
@@ -3818,7 +3963,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="48">
       <c r="A117" s="9">
         <v>114</v>
       </c>
@@ -3832,7 +3977,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="32">
       <c r="A118" s="9">
         <v>115</v>
       </c>
@@ -3846,7 +3991,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="32">
       <c r="A119" s="9">
         <v>116</v>
       </c>
@@ -3860,7 +4005,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="48">
       <c r="A120" s="9">
         <v>117</v>
       </c>
@@ -3874,7 +4019,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="48">
       <c r="A121" s="9">
         <v>118</v>
       </c>
@@ -3888,7 +4033,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="48">
       <c r="A122" s="9">
         <v>119</v>
       </c>
@@ -3902,7 +4047,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="32">
       <c r="A123" s="9">
         <v>120</v>
       </c>
@@ -3916,7 +4061,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="48">
       <c r="A124" s="9">
         <v>121</v>
       </c>
@@ -3930,7 +4075,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="32">
       <c r="A125" s="9">
         <v>122</v>
       </c>
@@ -3944,7 +4089,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="80">
       <c r="A126" s="9">
         <v>123</v>
       </c>
@@ -3958,7 +4103,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="80">
       <c r="A127" s="9">
         <v>124</v>
       </c>
@@ -3972,7 +4117,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="48">
       <c r="A128" s="9">
         <v>125</v>
       </c>
@@ -3986,7 +4131,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" ht="80">
       <c r="A129" s="9">
         <v>126</v>
       </c>
@@ -4000,7 +4145,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" ht="48">
       <c r="A130" s="9">
         <v>127</v>
       </c>
@@ -4014,7 +4159,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" ht="32">
       <c r="A131" s="9">
         <v>128</v>
       </c>
@@ -4028,7 +4173,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" ht="48">
       <c r="A132" s="9">
         <v>129</v>
       </c>
@@ -4042,7 +4187,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" ht="16">
       <c r="A133" s="9">
         <v>130</v>
       </c>
@@ -4056,7 +4201,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" ht="48">
       <c r="A134" s="9">
         <v>131</v>
       </c>
@@ -4070,7 +4215,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" ht="48">
       <c r="A135" s="9">
         <v>132</v>
       </c>
@@ -4084,7 +4229,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" ht="32">
       <c r="A136" s="9">
         <v>133</v>
       </c>
@@ -4098,7 +4243,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" ht="48">
       <c r="A137" s="9">
         <v>134</v>
       </c>
@@ -4112,7 +4257,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="32">
       <c r="A138" s="9">
         <v>135</v>
       </c>
@@ -4126,7 +4271,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" ht="48">
       <c r="A139" s="9">
         <v>136</v>
       </c>
@@ -4140,7 +4285,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" ht="48">
       <c r="A140" s="9">
         <v>137</v>
       </c>
@@ -4154,7 +4299,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="195" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" ht="208">
       <c r="A141" s="9">
         <v>138</v>
       </c>
@@ -4168,7 +4313,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" ht="16">
       <c r="A142" s="9">
         <v>139</v>
       </c>
@@ -4188,7 +4333,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="48">
       <c r="A143" s="9">
         <v>140</v>
       </c>
@@ -4205,7 +4350,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" ht="32">
       <c r="A144" s="9">
         <v>141</v>
       </c>
@@ -4219,7 +4364,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="16">
       <c r="A145" s="9">
         <v>142</v>
       </c>
@@ -4233,7 +4378,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="32">
       <c r="A146" s="9">
         <v>143</v>
       </c>
@@ -4247,7 +4392,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="32">
       <c r="A147" s="9">
         <v>144</v>
       </c>
@@ -4261,7 +4406,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="32">
       <c r="A148" s="9">
         <v>145</v>
       </c>
@@ -4275,7 +4420,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="16">
       <c r="A149" s="9">
         <v>146</v>
       </c>
@@ -4289,7 +4434,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="32">
       <c r="A150" s="9">
         <v>147</v>
       </c>
@@ -4303,7 +4448,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="32">
       <c r="A151" s="9">
         <v>148</v>
       </c>
@@ -4317,7 +4462,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="80">
       <c r="A152" s="9">
         <v>149</v>
       </c>
@@ -4331,7 +4476,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="48">
       <c r="A153" s="9">
         <v>150</v>
       </c>
@@ -4345,7 +4490,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="32">
       <c r="A154" s="9">
         <v>151</v>
       </c>
@@ -4359,7 +4504,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="48">
       <c r="A155" s="9">
         <v>152</v>
       </c>
@@ -4373,7 +4518,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="48">
       <c r="A156" s="9">
         <v>153</v>
       </c>
@@ -4387,7 +4532,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="32">
       <c r="A157" s="9">
         <v>154</v>
       </c>
@@ -4401,7 +4546,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="48">
       <c r="A158" s="9">
         <v>155</v>
       </c>
@@ -4415,7 +4560,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="48">
       <c r="A159" s="9">
         <v>156</v>
       </c>
@@ -4429,7 +4574,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="48">
       <c r="A160" s="9">
         <v>157</v>
       </c>
@@ -4443,7 +4588,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" ht="48">
       <c r="A161" s="9">
         <v>158</v>
       </c>
@@ -4457,7 +4602,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" ht="48">
       <c r="A162" s="9">
         <v>159</v>
       </c>
@@ -4471,7 +4616,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="48">
       <c r="A163" s="9">
         <v>160</v>
       </c>
@@ -4485,7 +4630,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" ht="48">
       <c r="A164" s="9">
         <v>161</v>
       </c>
@@ -4499,7 +4644,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="32">
       <c r="A165" s="9">
         <v>162</v>
       </c>
@@ -4513,7 +4658,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="48">
       <c r="A166" s="9">
         <v>163</v>
       </c>
@@ -4527,7 +4672,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="48">
       <c r="A167" s="9">
         <v>164</v>
       </c>
@@ -4541,7 +4686,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="48">
       <c r="A168" s="9">
         <v>165</v>
       </c>
@@ -4555,7 +4700,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="32">
       <c r="A169" s="9">
         <v>166</v>
       </c>
@@ -4569,7 +4714,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="48">
       <c r="A170" s="9">
         <v>167</v>
       </c>
@@ -4583,7 +4728,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="32">
       <c r="A171" s="9">
         <v>168</v>
       </c>
@@ -4597,7 +4742,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="32">
       <c r="A172" s="9">
         <v>169</v>
       </c>
@@ -4611,7 +4756,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="16">
       <c r="A173" s="9">
         <v>170</v>
       </c>
@@ -4625,7 +4770,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="32">
       <c r="A174" s="9">
         <v>171</v>
       </c>
@@ -4639,7 +4784,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="32">
       <c r="A175" s="9">
         <v>172</v>
       </c>
@@ -4653,7 +4798,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="32">
       <c r="A176" s="9">
         <v>173</v>
       </c>
@@ -4667,7 +4812,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="32">
       <c r="A177" s="9">
         <v>174</v>
       </c>
@@ -4681,7 +4826,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="32">
       <c r="A178" s="9">
         <v>175</v>
       </c>
@@ -4695,7 +4840,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" ht="32">
       <c r="A179" s="9">
         <v>176</v>
       </c>
@@ -4709,7 +4854,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" ht="48">
       <c r="A180" s="9">
         <v>177</v>
       </c>
@@ -4723,7 +4868,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="32">
       <c r="A181" s="9">
         <v>178</v>
       </c>
@@ -4737,7 +4882,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" ht="32">
       <c r="A182" s="9">
         <v>179</v>
       </c>
@@ -4751,7 +4896,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" ht="32">
       <c r="A183" s="9">
         <v>180</v>
       </c>
@@ -4765,7 +4910,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="32">
       <c r="A184" s="9">
         <v>181</v>
       </c>
@@ -4779,7 +4924,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="32">
       <c r="A185" s="9">
         <v>182</v>
       </c>
@@ -4793,7 +4938,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="16">
       <c r="A186" s="9">
         <v>183</v>
       </c>
@@ -4807,7 +4952,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" ht="32">
       <c r="A187" s="9">
         <v>184</v>
       </c>
@@ -4821,7 +4966,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="16">
       <c r="A188" s="9">
         <v>185</v>
       </c>
@@ -4835,7 +4980,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" ht="16">
       <c r="A189" s="9">
         <v>186</v>
       </c>
@@ -4849,7 +4994,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="32">
       <c r="A190" s="9">
         <v>187</v>
       </c>
@@ -4863,7 +5008,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" ht="16">
       <c r="A191" s="9">
         <v>188</v>
       </c>
@@ -4877,7 +5022,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="16">
       <c r="A192" s="9">
         <v>189</v>
       </c>
@@ -4891,7 +5036,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:18" ht="32">
       <c r="A193" s="9">
         <v>190</v>
       </c>
@@ -4905,7 +5050,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:18" ht="16">
       <c r="A194" s="9">
         <v>191</v>
       </c>
@@ -4919,7 +5064,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" ht="16">
       <c r="A195" s="9">
         <v>192</v>
       </c>
@@ -4936,7 +5081,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="196" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:18" ht="16">
       <c r="A196" s="9">
         <v>193</v>
       </c>
@@ -4950,7 +5095,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" ht="16">
       <c r="A197" s="9">
         <v>194</v>
       </c>
@@ -4964,7 +5109,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" ht="16">
       <c r="A198" s="9">
         <v>195</v>
       </c>
@@ -4978,7 +5123,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:18" ht="16">
       <c r="A199" s="9">
         <v>196</v>
       </c>
@@ -4992,7 +5137,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" ht="16">
       <c r="A200" s="9">
         <v>197</v>
       </c>
@@ -5006,7 +5151,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" ht="16">
       <c r="A201" s="9">
         <v>198</v>
       </c>
@@ -5020,7 +5165,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:18" ht="16">
       <c r="A202" s="9">
         <v>199</v>
       </c>
@@ -5034,7 +5179,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" ht="16">
       <c r="A203" s="9">
         <v>200</v>
       </c>
@@ -5048,7 +5193,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:18" ht="16">
       <c r="A204" s="9">
         <v>201</v>
       </c>
@@ -5062,7 +5207,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:18" ht="32">
       <c r="A205" s="9">
         <v>202</v>
       </c>
@@ -5076,7 +5221,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" ht="16">
       <c r="A206" s="9">
         <v>203</v>
       </c>
@@ -5090,7 +5235,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:18" ht="16">
       <c r="A207" s="9">
         <v>204</v>
       </c>
@@ -5107,7 +5252,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="208" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:18" ht="32">
       <c r="A208" s="8">
         <v>205</v>
       </c>
@@ -5121,7 +5266,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="209" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" ht="32">
       <c r="A209" s="8">
         <v>206</v>
       </c>
@@ -5135,7 +5280,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="210" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" ht="32">
       <c r="A210" s="8">
         <v>207</v>
       </c>
@@ -5152,7 +5297,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:18" ht="48">
       <c r="A211" s="8">
         <v>208</v>
       </c>
@@ -5166,7 +5311,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:18" ht="32">
       <c r="A212" s="8">
         <v>209</v>
       </c>
@@ -5180,7 +5325,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="213" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:18" ht="32">
       <c r="A213" s="8">
         <v>210</v>
       </c>
@@ -5194,7 +5339,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:18" ht="32">
       <c r="A214" s="8">
         <v>211</v>
       </c>
@@ -5208,7 +5353,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:18" ht="32">
       <c r="A215" s="8">
         <v>212</v>
       </c>
@@ -5225,7 +5370,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:18" ht="32">
       <c r="A216" s="8">
         <v>213</v>
       </c>
@@ -5239,7 +5384,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:18" ht="16">
       <c r="A217" s="8">
         <v>214</v>
       </c>
@@ -5253,7 +5398,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="218" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:18" ht="16">
       <c r="A218" s="8">
         <v>215</v>
       </c>
@@ -5267,7 +5412,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="219" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:18" ht="32">
       <c r="A219" s="9">
         <v>216</v>
       </c>
@@ -5281,7 +5426,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:18" ht="32">
       <c r="A220" s="9">
         <v>217</v>
       </c>
@@ -5295,7 +5440,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:18" ht="32">
       <c r="A221" s="9">
         <v>218</v>
       </c>
@@ -5312,7 +5457,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:18" ht="32">
       <c r="A222" s="9">
         <v>219</v>
       </c>
@@ -5326,7 +5471,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:18" ht="32">
       <c r="A223" s="9">
         <v>220</v>
       </c>
@@ -5340,7 +5485,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="224" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:18" ht="32">
       <c r="A224" s="9">
         <v>221</v>
       </c>
@@ -5354,7 +5499,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="230" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="230" spans="18:18">
       <c r="R230" t="s">
         <v>415</v>
       </c>
@@ -5367,20 +5512,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5605,19 +5750,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Modified UI related requirements for clarity
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904C9C2F-7EE0-7544-BFC0-A5B13BBC8A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF1402B-DF28-EC4E-9381-E7DB09EA358F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,43 +346,22 @@
     <t>BotI.java / isInsideBoard</t>
   </si>
   <si>
-    <t>The program shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined.</t>
-  </si>
-  <si>
     <t>joingame/Waitlist.js/displayWaitlist()</t>
   </si>
   <si>
-    <t>The program shall display a button for a game against another user.</t>
-  </si>
-  <si>
     <t>webapp/index.html</t>
   </si>
   <si>
-    <t>The program shall display a button for a game against a bot.</t>
-  </si>
-  <si>
     <t>The program shall update the waitlist as players login and join/leave a game.</t>
   </si>
   <si>
     <t>joingame/Waitlist.js/add(), joingame/Waitlist.js/remove()</t>
   </si>
   <si>
-    <t>The program shall display a notification with updates to the waitlist.</t>
-  </si>
-  <si>
     <t>joingame/DisplayNotification.js/displayNotification()</t>
   </si>
   <si>
-    <t>The program will display a notification to the user when they are next to join a game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The program shall have display a button to spectate a game of 2 bots playing against each other. </t>
-  </si>
-  <si>
     <t>joingame/MatchMaker.js/requestSpectateBotVsBot()</t>
-  </si>
-  <si>
-    <t>The program will display players that choose to replay and new players at the bottom of the waitlist.</t>
   </si>
   <si>
     <t>The program will load usernames and IDs in waitlist and display them within 2 seconds of logging in/joining a game.</t>
@@ -1351,12 +1330,33 @@
   <si>
     <t>UI-JG-07</t>
   </si>
+  <si>
+    <t>The join game page shall display a waitlist of available players ready to play with their usernames and IDs in the order that the players joined under a section labeled 'Current Waitlist'.</t>
+  </si>
+  <si>
+    <t>The join game page shall display a button for a game against another user under a section labeled 'Choose a Game Mode'.</t>
+  </si>
+  <si>
+    <t>The join game page shall display a button for a game against a bot under a section labeled 'Choose a Game Mode'.</t>
+  </si>
+  <si>
+    <t>The join game page shall display a notification with updates to the waitlist under a section labeled 'Notifications'.</t>
+  </si>
+  <si>
+    <t>The join game page will display a notification indicating that the user is next to join a game under a section labeled 'Notifications'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The join game page shall have display a button to spectate a game of 2 bots playing against each other under a section labeled 'Choose a Game Mode'. </t>
+  </si>
+  <si>
+    <t>The join game page shall display new players and replaying players at the bottom (or start of the waitlist) under a section labeled 'Current Waitlist'.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1565,7 +1565,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>212</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
+      <xdr:rowOff>333376</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1612,7 +1612,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>2038350</xdr:colOff>
       <xdr:row>219</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1659,7 +1659,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>2400300</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1706,7 +1706,7 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1753,7 +1753,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>239</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1843,8 +1843,8 @@
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>371656</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>118139</xdr:rowOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>310564</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2216,11 +2216,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF76" sqref="AF76"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
@@ -2231,12 +2231,12 @@
     <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="48">
+    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32">
+    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="16">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="32">
+    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="32">
+    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="32">
+    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16">
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="32">
+    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16">
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48">
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48">
+    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32">
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="48">
+    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="32">
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="32">
+    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32">
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32">
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32">
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>31</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32">
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>32</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="48">
+    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>33</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="48">
+    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>34</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="64">
+    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>35</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>36</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32">
+    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <v>37</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32">
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>38</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>39</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32">
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>40</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="32">
+    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>41</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="32">
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>42</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32">
+    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>43</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="48">
+    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>44</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="32">
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>45</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="32">
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>46</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="32">
+    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>47</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="32">
+    <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>48</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="32">
+    <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
         <v>49</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="48">
+    <row r="53" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
         <v>50</v>
       </c>
@@ -2997,16 +2997,16 @@
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="E53" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
         <v>51</v>
       </c>
@@ -3014,16 +3014,16 @@
         <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>104</v>
+        <v>424</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="16">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <v>52</v>
       </c>
@@ -3031,16 +3031,16 @@
         <v>26</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>106</v>
+        <v>425</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <v>53</v>
       </c>
@@ -3048,16 +3048,16 @@
         <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>54</v>
       </c>
@@ -3065,16 +3065,16 @@
         <v>26</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>109</v>
+        <v>426</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="32">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>55</v>
       </c>
@@ -3082,16 +3082,16 @@
         <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>111</v>
+        <v>427</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="32">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>56</v>
       </c>
@@ -3099,16 +3099,16 @@
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>112</v>
+        <v>428</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="32">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>57</v>
       </c>
@@ -3116,16 +3116,16 @@
         <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>114</v>
+        <v>429</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="32">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>58</v>
       </c>
@@ -3133,16 +3133,16 @@
         <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>59</v>
       </c>
@@ -3150,16 +3150,16 @@
         <v>26</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>60</v>
       </c>
@@ -3167,16 +3167,16 @@
         <v>26</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>61</v>
       </c>
@@ -3184,16 +3184,16 @@
         <v>26</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="64">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
         <v>62</v>
       </c>
@@ -3201,16 +3201,16 @@
         <v>26</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="64">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="9">
         <v>63</v>
       </c>
@@ -3218,16 +3218,16 @@
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="9">
         <v>64</v>
       </c>
@@ -3235,16 +3235,16 @@
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="9">
         <v>65</v>
       </c>
@@ -3252,16 +3252,16 @@
         <v>26</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="9">
         <v>66</v>
       </c>
@@ -3269,16 +3269,16 @@
         <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
         <v>67</v>
       </c>
@@ -3286,16 +3286,16 @@
         <v>26</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="48">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="9">
         <v>68</v>
       </c>
@@ -3303,16 +3303,16 @@
         <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="64">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="9">
         <v>69</v>
       </c>
@@ -3320,16 +3320,16 @@
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="32">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
         <v>70</v>
       </c>
@@ -3337,13 +3337,13 @@
         <v>35</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="9">
         <v>71</v>
       </c>
@@ -3351,13 +3351,13 @@
         <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="16">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="9">
         <v>72</v>
       </c>
@@ -3365,13 +3365,13 @@
         <v>35</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="9">
         <v>73</v>
       </c>
@@ -3379,13 +3379,13 @@
         <v>35</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="48">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="9">
         <v>74</v>
       </c>
@@ -3393,13 +3393,13 @@
         <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="32">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
         <v>75</v>
       </c>
@@ -3407,13 +3407,13 @@
         <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="32">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="9">
         <v>76</v>
       </c>
@@ -3421,13 +3421,13 @@
         <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="32">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="9">
         <v>77</v>
       </c>
@@ -3435,13 +3435,13 @@
         <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="32">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="9">
         <v>78</v>
       </c>
@@ -3449,13 +3449,13 @@
         <v>35</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="32">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
         <v>79</v>
       </c>
@@ -3463,13 +3463,13 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="16">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="9">
         <v>80</v>
       </c>
@@ -3477,13 +3477,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="48">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
         <v>81</v>
       </c>
@@ -3491,16 +3491,16 @@
         <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="48">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
         <v>82</v>
       </c>
@@ -3508,16 +3508,16 @@
         <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="80">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
         <v>83</v>
       </c>
@@ -3525,16 +3525,16 @@
         <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="16">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
         <v>84</v>
       </c>
@@ -3542,16 +3542,16 @@
         <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="32">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="9">
         <v>85</v>
       </c>
@@ -3559,13 +3559,13 @@
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="48">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="9">
         <v>86</v>
       </c>
@@ -3573,13 +3573,13 @@
         <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="32">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="9">
         <v>87</v>
       </c>
@@ -3587,16 +3587,16 @@
         <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="16">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="9">
         <v>88</v>
       </c>
@@ -3604,13 +3604,13 @@
         <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="32">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="9">
         <v>89</v>
       </c>
@@ -3618,16 +3618,16 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="32">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="9">
         <v>90</v>
       </c>
@@ -3635,13 +3635,13 @@
         <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="32">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="9">
         <v>91</v>
       </c>
@@ -3649,13 +3649,13 @@
         <v>27</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="32">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="9">
         <v>92</v>
       </c>
@@ -3663,13 +3663,13 @@
         <v>27</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="32">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="9">
         <v>93</v>
       </c>
@@ -3677,13 +3677,13 @@
         <v>27</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="32">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="9">
         <v>94</v>
       </c>
@@ -3691,13 +3691,13 @@
         <v>27</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="32">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="9">
         <v>95</v>
       </c>
@@ -3705,13 +3705,13 @@
         <v>27</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="32">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="9">
         <v>96</v>
       </c>
@@ -3719,13 +3719,13 @@
         <v>27</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="32">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="9">
         <v>97</v>
       </c>
@@ -3733,13 +3733,13 @@
         <v>27</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="16">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="9">
         <v>98</v>
       </c>
@@ -3747,13 +3747,13 @@
         <v>27</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="32">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="9">
         <v>99</v>
       </c>
@@ -3761,13 +3761,13 @@
         <v>36</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="48">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="9">
         <v>100</v>
       </c>
@@ -3775,13 +3775,13 @@
         <v>36</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="48">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="9">
         <v>101</v>
       </c>
@@ -3789,13 +3789,13 @@
         <v>36</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="32">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="9">
         <v>102</v>
       </c>
@@ -3803,13 +3803,13 @@
         <v>36</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="48">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="9">
         <v>103</v>
       </c>
@@ -3817,13 +3817,13 @@
         <v>36</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="32">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="9">
         <v>104</v>
       </c>
@@ -3831,13 +3831,13 @@
         <v>36</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="96">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A108" s="9">
         <v>105</v>
       </c>
@@ -3845,13 +3845,13 @@
         <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="32">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="9">
         <v>106</v>
       </c>
@@ -3859,13 +3859,13 @@
         <v>36</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="16">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="9">
         <v>107</v>
       </c>
@@ -3873,13 +3873,13 @@
         <v>36</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="32">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="9">
         <v>108</v>
       </c>
@@ -3887,13 +3887,13 @@
         <v>36</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="48">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="9">
         <v>109</v>
       </c>
@@ -3901,13 +3901,13 @@
         <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="32">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="9">
         <v>110</v>
       </c>
@@ -3915,13 +3915,13 @@
         <v>36</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="16">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="9">
         <v>111</v>
       </c>
@@ -3929,13 +3929,13 @@
         <v>36</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="32">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="9">
         <v>112</v>
       </c>
@@ -3943,13 +3943,13 @@
         <v>36</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="32">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="9">
         <v>113</v>
       </c>
@@ -3957,13 +3957,13 @@
         <v>36</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="48">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="9">
         <v>114</v>
       </c>
@@ -3971,13 +3971,13 @@
         <v>31</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="32">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="9">
         <v>115</v>
       </c>
@@ -3985,13 +3985,13 @@
         <v>31</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="32">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="9">
         <v>116</v>
       </c>
@@ -3999,13 +3999,13 @@
         <v>31</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="48">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="9">
         <v>117</v>
       </c>
@@ -4013,13 +4013,13 @@
         <v>31</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="48">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="9">
         <v>118</v>
       </c>
@@ -4027,13 +4027,13 @@
         <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="48">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A122" s="9">
         <v>119</v>
       </c>
@@ -4041,13 +4041,13 @@
         <v>31</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="32">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="9">
         <v>120</v>
       </c>
@@ -4055,13 +4055,13 @@
         <v>31</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="48">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="9">
         <v>121</v>
       </c>
@@ -4069,13 +4069,13 @@
         <v>31</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="32">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="9">
         <v>122</v>
       </c>
@@ -4083,13 +4083,13 @@
         <v>31</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="80">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A126" s="9">
         <v>123</v>
       </c>
@@ -4097,13 +4097,13 @@
         <v>31</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D126" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="80">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A127" s="9">
         <v>124</v>
       </c>
@@ -4111,13 +4111,13 @@
         <v>31</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D127" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="48">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A128" s="9">
         <v>125</v>
       </c>
@@ -4125,13 +4125,13 @@
         <v>31</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" ht="80">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A129" s="9">
         <v>126</v>
       </c>
@@ -4139,13 +4139,13 @@
         <v>31</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D129" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" ht="48">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A130" s="9">
         <v>127</v>
       </c>
@@ -4153,13 +4153,13 @@
         <v>31</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D130" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="32">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="9">
         <v>128</v>
       </c>
@@ -4167,13 +4167,13 @@
         <v>30</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" ht="48">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A132" s="9">
         <v>129</v>
       </c>
@@ -4181,13 +4181,13 @@
         <v>30</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" ht="16">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="9">
         <v>130</v>
       </c>
@@ -4195,13 +4195,13 @@
         <v>30</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="48">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A134" s="9">
         <v>131</v>
       </c>
@@ -4209,13 +4209,13 @@
         <v>30</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" ht="48">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" s="9">
         <v>132</v>
       </c>
@@ -4223,13 +4223,13 @@
         <v>30</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" ht="32">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="9">
         <v>133</v>
       </c>
@@ -4237,13 +4237,13 @@
         <v>30</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="48">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="9">
         <v>134</v>
       </c>
@@ -4251,13 +4251,13 @@
         <v>30</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" ht="32">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="9">
         <v>135</v>
       </c>
@@ -4265,13 +4265,13 @@
         <v>30</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" ht="48">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A139" s="9">
         <v>136</v>
       </c>
@@ -4279,13 +4279,13 @@
         <v>30</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" ht="48">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="9">
         <v>137</v>
       </c>
@@ -4293,13 +4293,13 @@
         <v>30</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" ht="208">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A141" s="9">
         <v>138</v>
       </c>
@@ -4307,13 +4307,13 @@
         <v>30</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" ht="16">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="9">
         <v>139</v>
       </c>
@@ -4321,19 +4321,19 @@
         <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="R142" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" ht="48">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A143" s="9">
         <v>140</v>
       </c>
@@ -4341,16 +4341,16 @@
         <v>28</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" ht="32">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="9">
         <v>141</v>
       </c>
@@ -4358,13 +4358,13 @@
         <v>28</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="16">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="9">
         <v>142</v>
       </c>
@@ -4372,13 +4372,13 @@
         <v>28</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D145" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="32">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="9">
         <v>143</v>
       </c>
@@ -4386,13 +4386,13 @@
         <v>28</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="9">
         <v>144</v>
       </c>
@@ -4400,13 +4400,13 @@
         <v>28</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="32">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="9">
         <v>145</v>
       </c>
@@ -4414,13 +4414,13 @@
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="16">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="9">
         <v>146</v>
       </c>
@@ -4428,13 +4428,13 @@
         <v>28</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="9">
         <v>147</v>
       </c>
@@ -4442,13 +4442,13 @@
         <v>28</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="32">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="9">
         <v>148</v>
       </c>
@@ -4456,13 +4456,13 @@
         <v>28</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="80">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A152" s="9">
         <v>149</v>
       </c>
@@ -4470,13 +4470,13 @@
         <v>29</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="48">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A153" s="9">
         <v>150</v>
       </c>
@@ -4484,13 +4484,13 @@
         <v>29</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="32">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="9">
         <v>151</v>
       </c>
@@ -4498,13 +4498,13 @@
         <v>29</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="48">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="9">
         <v>152</v>
       </c>
@@ -4512,13 +4512,13 @@
         <v>29</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="48">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="9">
         <v>153</v>
       </c>
@@ -4526,13 +4526,13 @@
         <v>29</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="32">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="9">
         <v>154</v>
       </c>
@@ -4540,13 +4540,13 @@
         <v>29</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="48">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="9">
         <v>155</v>
       </c>
@@ -4554,13 +4554,13 @@
         <v>29</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="48">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A159" s="9">
         <v>156</v>
       </c>
@@ -4568,13 +4568,13 @@
         <v>29</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="48">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A160" s="9">
         <v>157</v>
       </c>
@@ -4582,13 +4582,13 @@
         <v>29</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="48">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A161" s="9">
         <v>158</v>
       </c>
@@ -4596,13 +4596,13 @@
         <v>29</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="48">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A162" s="9">
         <v>159</v>
       </c>
@@ -4610,13 +4610,13 @@
         <v>29</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="48">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="9">
         <v>160</v>
       </c>
@@ -4624,13 +4624,13 @@
         <v>29</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="48">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A164" s="9">
         <v>161</v>
       </c>
@@ -4638,13 +4638,13 @@
         <v>29</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="32">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="9">
         <v>162</v>
       </c>
@@ -4652,13 +4652,13 @@
         <v>29</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="48">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A166" s="9">
         <v>163</v>
       </c>
@@ -4666,13 +4666,13 @@
         <v>29</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D166" s="12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="48">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A167" s="9">
         <v>164</v>
       </c>
@@ -4680,13 +4680,13 @@
         <v>29</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="48">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A168" s="9">
         <v>165</v>
       </c>
@@ -4694,13 +4694,13 @@
         <v>29</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D168" s="12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="32">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="9">
         <v>166</v>
       </c>
@@ -4708,13 +4708,13 @@
         <v>29</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D169" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" ht="48">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="9">
         <v>167</v>
       </c>
@@ -4722,13 +4722,13 @@
         <v>29</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="32">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="9">
         <v>168</v>
       </c>
@@ -4736,13 +4736,13 @@
         <v>29</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" ht="32">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="9">
         <v>169</v>
       </c>
@@ -4750,13 +4750,13 @@
         <v>32</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="16">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="9">
         <v>170</v>
       </c>
@@ -4764,13 +4764,13 @@
         <v>32</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="32">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="9">
         <v>171</v>
       </c>
@@ -4778,13 +4778,13 @@
         <v>32</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" ht="32">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="9">
         <v>172</v>
       </c>
@@ -4792,13 +4792,13 @@
         <v>32</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="32">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="9">
         <v>173</v>
       </c>
@@ -4806,13 +4806,13 @@
         <v>32</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="32">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="9">
         <v>174</v>
       </c>
@@ -4820,13 +4820,13 @@
         <v>32</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="32">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="9">
         <v>175</v>
       </c>
@@ -4834,13 +4834,13 @@
         <v>32</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="32">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="9">
         <v>176</v>
       </c>
@@ -4848,13 +4848,13 @@
         <v>32</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="48">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A180" s="9">
         <v>177</v>
       </c>
@@ -4862,13 +4862,13 @@
         <v>32</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="32">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="9">
         <v>178</v>
       </c>
@@ -4876,13 +4876,13 @@
         <v>32</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="32">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="9">
         <v>179</v>
       </c>
@@ -4890,13 +4890,13 @@
         <v>32</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="32">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="9">
         <v>180</v>
       </c>
@@ -4904,13 +4904,13 @@
         <v>32</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="32">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="9">
         <v>181</v>
       </c>
@@ -4918,13 +4918,13 @@
         <v>32</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="32">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="9">
         <v>182</v>
       </c>
@@ -4932,13 +4932,13 @@
         <v>32</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="16">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="9">
         <v>183</v>
       </c>
@@ -4946,13 +4946,13 @@
         <v>32</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="32">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="9">
         <v>184</v>
       </c>
@@ -4960,13 +4960,13 @@
         <v>32</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="16">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="9">
         <v>185</v>
       </c>
@@ -4974,13 +4974,13 @@
         <v>32</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" ht="16">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="9">
         <v>186</v>
       </c>
@@ -4988,13 +4988,13 @@
         <v>32</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="32">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="9">
         <v>187</v>
       </c>
@@ -5002,13 +5002,13 @@
         <v>32</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="16">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="9">
         <v>188</v>
       </c>
@@ -5016,13 +5016,13 @@
         <v>32</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="16">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="9">
         <v>189</v>
       </c>
@@ -5030,13 +5030,13 @@
         <v>32</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D192" s="10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="193" spans="1:18" ht="32">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="9">
         <v>190</v>
       </c>
@@ -5044,13 +5044,13 @@
         <v>32</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="194" spans="1:18" ht="16">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="9">
         <v>191</v>
       </c>
@@ -5058,13 +5058,13 @@
         <v>32</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="195" spans="1:18" ht="16">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="9">
         <v>192</v>
       </c>
@@ -5072,16 +5072,16 @@
         <v>32</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" ht="16">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="9">
         <v>193</v>
       </c>
@@ -5089,13 +5089,13 @@
         <v>32</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="197" spans="1:18" ht="16">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="9">
         <v>194</v>
       </c>
@@ -5103,13 +5103,13 @@
         <v>32</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="198" spans="1:18" ht="16">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="9">
         <v>195</v>
       </c>
@@ -5117,13 +5117,13 @@
         <v>32</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="199" spans="1:18" ht="16">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="9">
         <v>196</v>
       </c>
@@ -5131,13 +5131,13 @@
         <v>32</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="200" spans="1:18" ht="16">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="9">
         <v>197</v>
       </c>
@@ -5145,13 +5145,13 @@
         <v>32</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="201" spans="1:18" ht="16">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="9">
         <v>198</v>
       </c>
@@ -5159,13 +5159,13 @@
         <v>32</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="202" spans="1:18" ht="16">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="9">
         <v>199</v>
       </c>
@@ -5173,13 +5173,13 @@
         <v>32</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="203" spans="1:18" ht="16">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="9">
         <v>200</v>
       </c>
@@ -5187,13 +5187,13 @@
         <v>32</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D203" s="10" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="204" spans="1:18" ht="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="9">
         <v>201</v>
       </c>
@@ -5201,13 +5201,13 @@
         <v>32</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="205" spans="1:18" ht="32">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="9">
         <v>202</v>
       </c>
@@ -5215,13 +5215,13 @@
         <v>32</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="D205" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="206" spans="1:18" ht="16">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="9">
         <v>203</v>
       </c>
@@ -5229,13 +5229,13 @@
         <v>32</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D206" s="10" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="207" spans="1:18" ht="16">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="9">
         <v>204</v>
       </c>
@@ -5243,16 +5243,16 @@
         <v>32</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D207" s="10" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="R207" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="208" spans="1:18" ht="32">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="8">
         <v>205</v>
       </c>
@@ -5260,13 +5260,13 @@
         <v>25</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="209" spans="1:18" ht="32">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="8">
         <v>206</v>
       </c>
@@ -5274,13 +5274,13 @@
         <v>25</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="210" spans="1:18" ht="32">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="8">
         <v>207</v>
       </c>
@@ -5288,16 +5288,16 @@
         <v>25</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="R210" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="211" spans="1:18" ht="48">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A211" s="8">
         <v>208</v>
       </c>
@@ -5305,13 +5305,13 @@
         <v>25</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="212" spans="1:18" ht="32">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="8">
         <v>209</v>
       </c>
@@ -5319,13 +5319,13 @@
         <v>25</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="213" spans="1:18" ht="32">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="8">
         <v>210</v>
       </c>
@@ -5333,13 +5333,13 @@
         <v>25</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="214" spans="1:18" ht="32">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="8">
         <v>211</v>
       </c>
@@ -5347,13 +5347,13 @@
         <v>25</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="215" spans="1:18" ht="32">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="8">
         <v>212</v>
       </c>
@@ -5361,16 +5361,16 @@
         <v>25</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="R215" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="216" spans="1:18" ht="32">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="8">
         <v>213</v>
       </c>
@@ -5378,13 +5378,13 @@
         <v>25</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="217" spans="1:18" ht="16">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="8">
         <v>214</v>
       </c>
@@ -5392,13 +5392,13 @@
         <v>25</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="218" spans="1:18" ht="16">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="8">
         <v>215</v>
       </c>
@@ -5406,13 +5406,13 @@
         <v>25</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="219" spans="1:18" ht="32">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="9">
         <v>216</v>
       </c>
@@ -5420,13 +5420,13 @@
         <v>25</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="220" spans="1:18" ht="32">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="9">
         <v>217</v>
       </c>
@@ -5434,13 +5434,13 @@
         <v>25</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="221" spans="1:18" ht="32">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="9">
         <v>218</v>
       </c>
@@ -5448,16 +5448,16 @@
         <v>25</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="R221" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="222" spans="1:18" ht="32">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="9">
         <v>219</v>
       </c>
@@ -5465,13 +5465,13 @@
         <v>25</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="223" spans="1:18" ht="32">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="9">
         <v>220</v>
       </c>
@@ -5479,13 +5479,13 @@
         <v>25</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="224" spans="1:18" ht="32">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="9">
         <v>221</v>
       </c>
@@ -5493,15 +5493,15 @@
         <v>25</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="230" spans="18:18">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="230" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R230" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Group 31 Reqs
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDE4DA8-6DF4-0644-8552-0450DFC5B980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A9E6EF-DC70-4C29-817F-88BA2FE883EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="447">
   <si>
     <t>Tested By</t>
   </si>
@@ -1396,6 +1396,9 @@
   </si>
   <si>
     <t>Req. might be too unlcear to test.What does if needed mean?</t>
+  </si>
+  <si>
+    <t>Untestable</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1680,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1771,7 +1774,7 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>224</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1818,7 +1821,7 @@
       <xdr:col>31</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>224</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2176,32 +2179,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G182" sqref="G182"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -2260,7 +2263,7 @@
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:19" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
       <c r="B4" s="8"/>
       <c r="D4" s="10"/>
@@ -2271,7 +2274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>1</v>
       </c>
@@ -2290,6 +2293,9 @@
       <c r="I5" t="s">
         <v>21</v>
       </c>
+      <c r="L5" t="s">
+        <v>446</v>
+      </c>
       <c r="N5" t="s">
         <v>21</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -2316,6 +2322,9 @@
       <c r="I6" t="s">
         <v>21</v>
       </c>
+      <c r="L6" t="s">
+        <v>446</v>
+      </c>
       <c r="N6" t="s">
         <v>21</v>
       </c>
@@ -2323,7 +2332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -2338,7 +2347,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -2353,7 +2362,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>5</v>
       </c>
@@ -2368,7 +2377,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -2383,7 +2392,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -2402,6 +2411,9 @@
       <c r="I11" t="s">
         <v>21</v>
       </c>
+      <c r="L11" t="s">
+        <v>446</v>
+      </c>
       <c r="N11" t="s">
         <v>21</v>
       </c>
@@ -2409,7 +2421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -2428,6 +2440,9 @@
       <c r="I12" t="s">
         <v>21</v>
       </c>
+      <c r="L12" t="s">
+        <v>446</v>
+      </c>
       <c r="N12" t="s">
         <v>21</v>
       </c>
@@ -2435,7 +2450,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>9</v>
       </c>
@@ -2450,7 +2465,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -2465,7 +2480,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -2484,6 +2499,9 @@
       <c r="I15" t="s">
         <v>21</v>
       </c>
+      <c r="L15" t="s">
+        <v>446</v>
+      </c>
       <c r="N15" t="s">
         <v>21</v>
       </c>
@@ -2491,7 +2509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -2510,6 +2528,9 @@
       <c r="I16" t="s">
         <v>21</v>
       </c>
+      <c r="L16" t="s">
+        <v>446</v>
+      </c>
       <c r="N16" t="s">
         <v>21</v>
       </c>
@@ -2517,7 +2538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -2536,6 +2557,9 @@
       <c r="I17" t="s">
         <v>21</v>
       </c>
+      <c r="L17" t="s">
+        <v>446</v>
+      </c>
       <c r="N17" t="s">
         <v>21</v>
       </c>
@@ -2543,7 +2567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -2562,6 +2586,9 @@
       <c r="I18" t="s">
         <v>21</v>
       </c>
+      <c r="L18" t="s">
+        <v>446</v>
+      </c>
       <c r="N18" t="s">
         <v>21</v>
       </c>
@@ -2569,7 +2596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>15</v>
       </c>
@@ -2588,6 +2615,9 @@
       <c r="I19" t="s">
         <v>21</v>
       </c>
+      <c r="L19" t="s">
+        <v>446</v>
+      </c>
       <c r="N19" t="s">
         <v>21</v>
       </c>
@@ -2595,7 +2625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>16</v>
       </c>
@@ -2614,6 +2644,9 @@
       <c r="I20" t="s">
         <v>21</v>
       </c>
+      <c r="L20" t="s">
+        <v>446</v>
+      </c>
       <c r="N20" t="s">
         <v>21</v>
       </c>
@@ -2621,7 +2654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>17</v>
       </c>
@@ -2640,6 +2673,9 @@
       <c r="I21" t="s">
         <v>21</v>
       </c>
+      <c r="L21" t="s">
+        <v>446</v>
+      </c>
       <c r="N21" t="s">
         <v>21</v>
       </c>
@@ -2647,7 +2683,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>18</v>
       </c>
@@ -2666,6 +2702,9 @@
       <c r="I22" t="s">
         <v>21</v>
       </c>
+      <c r="L22" t="s">
+        <v>446</v>
+      </c>
       <c r="N22" t="s">
         <v>21</v>
       </c>
@@ -2673,7 +2712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>19</v>
       </c>
@@ -2692,6 +2731,9 @@
       <c r="I23" t="s">
         <v>21</v>
       </c>
+      <c r="L23" t="s">
+        <v>446</v>
+      </c>
       <c r="N23" t="s">
         <v>21</v>
       </c>
@@ -2699,7 +2741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>20</v>
       </c>
@@ -2716,7 +2758,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>21</v>
       </c>
@@ -2733,7 +2775,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>22</v>
       </c>
@@ -2752,6 +2794,9 @@
       <c r="I26" t="s">
         <v>21</v>
       </c>
+      <c r="L26" t="s">
+        <v>446</v>
+      </c>
       <c r="N26" t="s">
         <v>21</v>
       </c>
@@ -2759,7 +2804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>23</v>
       </c>
@@ -2778,6 +2823,9 @@
       <c r="I27" t="s">
         <v>21</v>
       </c>
+      <c r="L27" t="s">
+        <v>446</v>
+      </c>
       <c r="N27" t="s">
         <v>21</v>
       </c>
@@ -2785,7 +2833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>24</v>
       </c>
@@ -2804,6 +2852,9 @@
       <c r="I28" t="s">
         <v>21</v>
       </c>
+      <c r="L28" t="s">
+        <v>446</v>
+      </c>
       <c r="N28" t="s">
         <v>21</v>
       </c>
@@ -2811,7 +2862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>25</v>
       </c>
@@ -2830,6 +2881,9 @@
       <c r="I29" t="s">
         <v>21</v>
       </c>
+      <c r="L29" t="s">
+        <v>446</v>
+      </c>
       <c r="N29" t="s">
         <v>21</v>
       </c>
@@ -2837,7 +2891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>26</v>
       </c>
@@ -2854,7 +2908,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>27</v>
       </c>
@@ -2873,6 +2927,9 @@
       <c r="I31" t="s">
         <v>21</v>
       </c>
+      <c r="L31" t="s">
+        <v>446</v>
+      </c>
       <c r="N31" t="s">
         <v>21</v>
       </c>
@@ -2880,7 +2937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>28</v>
       </c>
@@ -2899,6 +2956,9 @@
       <c r="I32" t="s">
         <v>21</v>
       </c>
+      <c r="L32" t="s">
+        <v>446</v>
+      </c>
       <c r="N32" t="s">
         <v>21</v>
       </c>
@@ -2906,7 +2966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <v>29</v>
       </c>
@@ -2925,6 +2985,9 @@
       <c r="I33" t="s">
         <v>21</v>
       </c>
+      <c r="L33" t="s">
+        <v>446</v>
+      </c>
       <c r="N33" t="s">
         <v>21</v>
       </c>
@@ -2932,7 +2995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
         <v>30</v>
       </c>
@@ -2947,7 +3010,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
         <v>31</v>
       </c>
@@ -2966,6 +3029,9 @@
       <c r="I35" t="s">
         <v>21</v>
       </c>
+      <c r="L35" t="s">
+        <v>446</v>
+      </c>
       <c r="N35" t="s">
         <v>21</v>
       </c>
@@ -2973,7 +3039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
         <v>32</v>
       </c>
@@ -2992,6 +3058,9 @@
       <c r="I36" t="s">
         <v>21</v>
       </c>
+      <c r="L36" t="s">
+        <v>446</v>
+      </c>
       <c r="N36" t="s">
         <v>21</v>
       </c>
@@ -2999,7 +3068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
         <v>33</v>
       </c>
@@ -3018,6 +3087,9 @@
       <c r="I37" t="s">
         <v>21</v>
       </c>
+      <c r="L37" t="s">
+        <v>446</v>
+      </c>
       <c r="N37" t="s">
         <v>21</v>
       </c>
@@ -3025,7 +3097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
         <v>34</v>
       </c>
@@ -3044,6 +3116,9 @@
       <c r="I38" t="s">
         <v>21</v>
       </c>
+      <c r="L38" t="s">
+        <v>446</v>
+      </c>
       <c r="N38" t="s">
         <v>21</v>
       </c>
@@ -3051,7 +3126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <v>35</v>
       </c>
@@ -3070,6 +3145,9 @@
       <c r="I39" t="s">
         <v>21</v>
       </c>
+      <c r="L39" t="s">
+        <v>446</v>
+      </c>
       <c r="N39" t="s">
         <v>21</v>
       </c>
@@ -3077,7 +3155,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
         <v>36</v>
       </c>
@@ -3092,7 +3170,7 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
         <v>37</v>
       </c>
@@ -3111,6 +3189,9 @@
       <c r="I41" t="s">
         <v>21</v>
       </c>
+      <c r="L41" t="s">
+        <v>446</v>
+      </c>
       <c r="N41" t="s">
         <v>21</v>
       </c>
@@ -3118,7 +3199,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
         <v>38</v>
       </c>
@@ -3137,6 +3218,9 @@
       <c r="I42" t="s">
         <v>21</v>
       </c>
+      <c r="L42" t="s">
+        <v>446</v>
+      </c>
       <c r="N42" t="s">
         <v>21</v>
       </c>
@@ -3144,7 +3228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
         <v>39</v>
       </c>
@@ -3163,6 +3247,9 @@
       <c r="I43" t="s">
         <v>21</v>
       </c>
+      <c r="L43" t="s">
+        <v>446</v>
+      </c>
       <c r="N43" t="s">
         <v>21</v>
       </c>
@@ -3170,7 +3257,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
         <v>40</v>
       </c>
@@ -3187,7 +3274,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
         <v>41</v>
       </c>
@@ -3202,7 +3289,7 @@
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
         <v>42</v>
       </c>
@@ -3221,6 +3308,9 @@
       <c r="I46" t="s">
         <v>21</v>
       </c>
+      <c r="L46" t="s">
+        <v>446</v>
+      </c>
       <c r="N46" t="s">
         <v>21</v>
       </c>
@@ -3228,7 +3318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
         <v>43</v>
       </c>
@@ -3247,6 +3337,9 @@
       <c r="I47" t="s">
         <v>21</v>
       </c>
+      <c r="L47" t="s">
+        <v>446</v>
+      </c>
       <c r="N47" t="s">
         <v>21</v>
       </c>
@@ -3254,7 +3347,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
         <v>44</v>
       </c>
@@ -3273,6 +3366,9 @@
       <c r="I48" t="s">
         <v>21</v>
       </c>
+      <c r="L48" t="s">
+        <v>446</v>
+      </c>
       <c r="N48" t="s">
         <v>21</v>
       </c>
@@ -3280,7 +3376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
         <v>45</v>
       </c>
@@ -3299,6 +3395,9 @@
       <c r="I49" t="s">
         <v>21</v>
       </c>
+      <c r="L49" t="s">
+        <v>446</v>
+      </c>
       <c r="N49" t="s">
         <v>21</v>
       </c>
@@ -3306,7 +3405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <v>46</v>
       </c>
@@ -3325,6 +3424,9 @@
       <c r="I50" t="s">
         <v>21</v>
       </c>
+      <c r="L50" t="s">
+        <v>446</v>
+      </c>
       <c r="N50" t="s">
         <v>21</v>
       </c>
@@ -3332,7 +3434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
         <v>47</v>
       </c>
@@ -3351,6 +3453,9 @@
       <c r="I51" t="s">
         <v>21</v>
       </c>
+      <c r="L51" t="s">
+        <v>446</v>
+      </c>
       <c r="N51" t="s">
         <v>21</v>
       </c>
@@ -3358,7 +3463,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
         <v>48</v>
       </c>
@@ -3373,7 +3478,7 @@
       </c>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
         <v>49</v>
       </c>
@@ -3391,7 +3496,7 @@
       </c>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <v>50</v>
       </c>
@@ -3409,7 +3514,7 @@
       </c>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
         <v>51</v>
       </c>
@@ -3427,7 +3532,7 @@
       </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
         <v>52</v>
       </c>
@@ -3445,7 +3550,7 @@
       </c>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
         <v>53</v>
       </c>
@@ -3463,7 +3568,7 @@
       </c>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
         <v>54</v>
       </c>
@@ -3481,7 +3586,7 @@
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
         <v>55</v>
       </c>
@@ -3499,7 +3604,7 @@
       </c>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <v>56</v>
       </c>
@@ -3517,7 +3622,7 @@
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
         <v>57</v>
       </c>
@@ -3535,7 +3640,7 @@
       </c>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
         <v>58</v>
       </c>
@@ -3557,6 +3662,9 @@
       <c r="I62" t="s">
         <v>21</v>
       </c>
+      <c r="L62" t="s">
+        <v>446</v>
+      </c>
       <c r="N62" t="s">
         <v>21</v>
       </c>
@@ -3564,7 +3672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="9">
         <v>59</v>
       </c>
@@ -3584,6 +3692,9 @@
       <c r="I63" t="s">
         <v>21</v>
       </c>
+      <c r="L63" t="s">
+        <v>446</v>
+      </c>
       <c r="N63" t="s">
         <v>21</v>
       </c>
@@ -3591,7 +3702,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="9">
         <v>60</v>
       </c>
@@ -3613,6 +3724,9 @@
       <c r="I64" t="s">
         <v>21</v>
       </c>
+      <c r="L64" t="s">
+        <v>446</v>
+      </c>
       <c r="N64" t="s">
         <v>21</v>
       </c>
@@ -3620,7 +3734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
         <v>61</v>
       </c>
@@ -3642,6 +3756,9 @@
       <c r="I65" t="s">
         <v>21</v>
       </c>
+      <c r="L65" t="s">
+        <v>446</v>
+      </c>
       <c r="N65" t="s">
         <v>21</v>
       </c>
@@ -3649,7 +3766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="9">
         <v>62</v>
       </c>
@@ -3671,6 +3788,9 @@
       <c r="I66" t="s">
         <v>21</v>
       </c>
+      <c r="L66" t="s">
+        <v>446</v>
+      </c>
       <c r="N66" t="s">
         <v>21</v>
       </c>
@@ -3678,7 +3798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="9">
         <v>63</v>
       </c>
@@ -3696,7 +3816,7 @@
       </c>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="9">
         <v>64</v>
       </c>
@@ -3714,7 +3834,7 @@
       </c>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="9">
         <v>65</v>
       </c>
@@ -3736,6 +3856,9 @@
       <c r="I69" t="s">
         <v>21</v>
       </c>
+      <c r="L69" t="s">
+        <v>446</v>
+      </c>
       <c r="N69" t="s">
         <v>21</v>
       </c>
@@ -3743,7 +3866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="9">
         <v>66</v>
       </c>
@@ -3765,6 +3888,9 @@
       <c r="I70" t="s">
         <v>21</v>
       </c>
+      <c r="L70" t="s">
+        <v>446</v>
+      </c>
       <c r="N70" t="s">
         <v>21</v>
       </c>
@@ -3772,7 +3898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="9">
         <v>67</v>
       </c>
@@ -3794,6 +3920,9 @@
       <c r="I71" t="s">
         <v>21</v>
       </c>
+      <c r="L71" t="s">
+        <v>446</v>
+      </c>
       <c r="N71" t="s">
         <v>21</v>
       </c>
@@ -3801,7 +3930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="9">
         <v>68</v>
       </c>
@@ -3823,6 +3952,9 @@
       <c r="I72" t="s">
         <v>21</v>
       </c>
+      <c r="L72" t="s">
+        <v>446</v>
+      </c>
       <c r="N72" t="s">
         <v>21</v>
       </c>
@@ -3830,7 +3962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="9">
         <v>69</v>
       </c>
@@ -3845,7 +3977,7 @@
       </c>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="9">
         <v>70</v>
       </c>
@@ -3860,7 +3992,7 @@
       </c>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="9">
         <v>71</v>
       </c>
@@ -3875,7 +4007,7 @@
       </c>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="9">
         <v>72</v>
       </c>
@@ -3890,7 +4022,7 @@
       </c>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="9">
         <v>73</v>
       </c>
@@ -3909,6 +4041,9 @@
       <c r="I77" t="s">
         <v>21</v>
       </c>
+      <c r="L77" t="s">
+        <v>446</v>
+      </c>
       <c r="N77" t="s">
         <v>21</v>
       </c>
@@ -3916,7 +4051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="9">
         <v>74</v>
       </c>
@@ -3935,6 +4070,9 @@
       <c r="I78" t="s">
         <v>21</v>
       </c>
+      <c r="L78" t="s">
+        <v>446</v>
+      </c>
       <c r="N78" t="s">
         <v>21</v>
       </c>
@@ -3942,7 +4080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="9">
         <v>75</v>
       </c>
@@ -3961,6 +4099,9 @@
       <c r="I79" t="s">
         <v>21</v>
       </c>
+      <c r="L79" t="s">
+        <v>446</v>
+      </c>
       <c r="N79" t="s">
         <v>21</v>
       </c>
@@ -3968,7 +4109,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="9">
         <v>76</v>
       </c>
@@ -3987,6 +4128,9 @@
       <c r="I80" t="s">
         <v>21</v>
       </c>
+      <c r="L80" t="s">
+        <v>446</v>
+      </c>
       <c r="N80" t="s">
         <v>21</v>
       </c>
@@ -3994,7 +4138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="9">
         <v>77</v>
       </c>
@@ -4013,6 +4157,9 @@
       <c r="I81" t="s">
         <v>21</v>
       </c>
+      <c r="L81" t="s">
+        <v>446</v>
+      </c>
       <c r="N81" t="s">
         <v>21</v>
       </c>
@@ -4020,7 +4167,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="9">
         <v>78</v>
       </c>
@@ -4039,6 +4186,9 @@
       <c r="I82" t="s">
         <v>21</v>
       </c>
+      <c r="L82" t="s">
+        <v>446</v>
+      </c>
       <c r="N82" t="s">
         <v>21</v>
       </c>
@@ -4046,7 +4196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="9">
         <v>79</v>
       </c>
@@ -4061,7 +4211,7 @@
       </c>
       <c r="G83" s="2"/>
     </row>
-    <row r="84" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="9">
         <v>80</v>
       </c>
@@ -4079,7 +4229,7 @@
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="9">
         <v>81</v>
       </c>
@@ -4097,7 +4247,7 @@
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" s="9">
         <v>82</v>
       </c>
@@ -4115,7 +4265,7 @@
       </c>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="9">
         <v>83</v>
       </c>
@@ -4133,7 +4283,7 @@
       </c>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="9">
         <v>84</v>
       </c>
@@ -4152,6 +4302,9 @@
       <c r="I88" t="s">
         <v>21</v>
       </c>
+      <c r="L88" t="s">
+        <v>446</v>
+      </c>
       <c r="N88" t="s">
         <v>21</v>
       </c>
@@ -4159,7 +4312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="9">
         <v>85</v>
       </c>
@@ -4174,7 +4327,7 @@
       </c>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="9">
         <v>86</v>
       </c>
@@ -4192,7 +4345,7 @@
       </c>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="9">
         <v>87</v>
       </c>
@@ -4207,7 +4360,7 @@
       </c>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="9">
         <v>88</v>
       </c>
@@ -4225,7 +4378,7 @@
       </c>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="9">
         <v>89</v>
       </c>
@@ -4244,6 +4397,9 @@
       <c r="I93" t="s">
         <v>21</v>
       </c>
+      <c r="L93" t="s">
+        <v>446</v>
+      </c>
       <c r="N93" t="s">
         <v>21</v>
       </c>
@@ -4251,7 +4407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="9">
         <v>90</v>
       </c>
@@ -4270,6 +4426,9 @@
       <c r="I94" t="s">
         <v>21</v>
       </c>
+      <c r="L94" t="s">
+        <v>446</v>
+      </c>
       <c r="N94" t="s">
         <v>21</v>
       </c>
@@ -4277,7 +4436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="9">
         <v>91</v>
       </c>
@@ -4292,7 +4451,7 @@
       </c>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="9">
         <v>92</v>
       </c>
@@ -4307,7 +4466,7 @@
       </c>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="9">
         <v>93</v>
       </c>
@@ -4326,6 +4485,9 @@
       <c r="I97" t="s">
         <v>21</v>
       </c>
+      <c r="L97" t="s">
+        <v>446</v>
+      </c>
       <c r="N97" t="s">
         <v>21</v>
       </c>
@@ -4333,7 +4495,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="9">
         <v>94</v>
       </c>
@@ -4348,7 +4510,7 @@
       </c>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="9">
         <v>95</v>
       </c>
@@ -4363,7 +4525,7 @@
       </c>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="9">
         <v>96</v>
       </c>
@@ -4378,7 +4540,7 @@
       </c>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="9">
         <v>97</v>
       </c>
@@ -4397,6 +4559,9 @@
       <c r="I101" t="s">
         <v>21</v>
       </c>
+      <c r="L101" t="s">
+        <v>446</v>
+      </c>
       <c r="N101" t="s">
         <v>21</v>
       </c>
@@ -4404,7 +4569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="9">
         <v>98</v>
       </c>
@@ -4423,6 +4588,9 @@
       <c r="I102" t="s">
         <v>21</v>
       </c>
+      <c r="L102" t="s">
+        <v>446</v>
+      </c>
       <c r="N102" t="s">
         <v>21</v>
       </c>
@@ -4430,7 +4598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A103" s="9">
         <v>99</v>
       </c>
@@ -4445,7 +4613,7 @@
       </c>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A104" s="9">
         <v>100</v>
       </c>
@@ -4460,7 +4628,7 @@
       </c>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="9">
         <v>101</v>
       </c>
@@ -4475,7 +4643,7 @@
       </c>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A106" s="9">
         <v>102</v>
       </c>
@@ -4494,6 +4662,9 @@
       <c r="I106" t="s">
         <v>21</v>
       </c>
+      <c r="L106" t="s">
+        <v>446</v>
+      </c>
       <c r="N106" t="s">
         <v>21</v>
       </c>
@@ -4501,7 +4672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="9">
         <v>103</v>
       </c>
@@ -4516,7 +4687,7 @@
       </c>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A108" s="9">
         <v>104</v>
       </c>
@@ -4531,7 +4702,7 @@
       </c>
       <c r="G108" s="2"/>
     </row>
-    <row r="109" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="9">
         <v>105</v>
       </c>
@@ -4546,7 +4717,7 @@
       </c>
       <c r="G109" s="2"/>
     </row>
-    <row r="110" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" s="9">
         <v>106</v>
       </c>
@@ -4561,7 +4732,7 @@
       </c>
       <c r="G110" s="2"/>
     </row>
-    <row r="111" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="9">
         <v>107</v>
       </c>
@@ -4576,7 +4747,7 @@
       </c>
       <c r="G111" s="2"/>
     </row>
-    <row r="112" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A112" s="9">
         <v>108</v>
       </c>
@@ -4591,7 +4762,7 @@
       </c>
       <c r="G112" s="2"/>
     </row>
-    <row r="113" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="9">
         <v>109</v>
       </c>
@@ -4606,7 +4777,7 @@
       </c>
       <c r="G113" s="2"/>
     </row>
-    <row r="114" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="9">
         <v>110</v>
       </c>
@@ -4621,7 +4792,7 @@
       </c>
       <c r="G114" s="2"/>
     </row>
-    <row r="115" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="9">
         <v>111</v>
       </c>
@@ -4636,7 +4807,7 @@
       </c>
       <c r="G115" s="2"/>
     </row>
-    <row r="116" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="9">
         <v>112</v>
       </c>
@@ -4655,6 +4826,9 @@
       <c r="I116" t="s">
         <v>21</v>
       </c>
+      <c r="L116" t="s">
+        <v>446</v>
+      </c>
       <c r="N116" t="s">
         <v>21</v>
       </c>
@@ -4662,7 +4836,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A117" s="9">
         <v>113</v>
       </c>
@@ -4677,7 +4851,7 @@
       </c>
       <c r="G117" s="2"/>
     </row>
-    <row r="118" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="9">
         <v>114</v>
       </c>
@@ -4692,7 +4866,7 @@
       </c>
       <c r="G118" s="2"/>
     </row>
-    <row r="119" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="9">
         <v>115</v>
       </c>
@@ -4707,7 +4881,7 @@
       </c>
       <c r="G119" s="2"/>
     </row>
-    <row r="120" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A120" s="9">
         <v>116</v>
       </c>
@@ -4726,6 +4900,9 @@
       <c r="I120" t="s">
         <v>21</v>
       </c>
+      <c r="L120" t="s">
+        <v>446</v>
+      </c>
       <c r="N120" t="s">
         <v>21</v>
       </c>
@@ -4733,7 +4910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="9">
         <v>117</v>
       </c>
@@ -4752,6 +4929,9 @@
       <c r="I121" t="s">
         <v>21</v>
       </c>
+      <c r="L121" t="s">
+        <v>446</v>
+      </c>
       <c r="N121" t="s">
         <v>21</v>
       </c>
@@ -4759,7 +4939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A122" s="9">
         <v>118</v>
       </c>
@@ -4778,6 +4958,9 @@
       <c r="I122" t="s">
         <v>21</v>
       </c>
+      <c r="L122" t="s">
+        <v>446</v>
+      </c>
       <c r="N122" t="s">
         <v>21</v>
       </c>
@@ -4785,7 +4968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="9">
         <v>119</v>
       </c>
@@ -4804,6 +4987,9 @@
       <c r="I123" t="s">
         <v>21</v>
       </c>
+      <c r="L123" t="s">
+        <v>446</v>
+      </c>
       <c r="N123" t="s">
         <v>21</v>
       </c>
@@ -4811,7 +4997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A124" s="9">
         <v>120</v>
       </c>
@@ -4828,7 +5014,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="9">
         <v>121</v>
       </c>
@@ -4847,6 +5033,9 @@
       <c r="I125" t="s">
         <v>21</v>
       </c>
+      <c r="L125" t="s">
+        <v>446</v>
+      </c>
       <c r="N125" t="s">
         <v>21</v>
       </c>
@@ -4854,7 +5043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A126" s="9">
         <v>122</v>
       </c>
@@ -4873,6 +5062,9 @@
       <c r="I126" t="s">
         <v>21</v>
       </c>
+      <c r="L126" t="s">
+        <v>446</v>
+      </c>
       <c r="N126" t="s">
         <v>21</v>
       </c>
@@ -4880,7 +5072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A127" s="9">
         <v>123</v>
       </c>
@@ -4895,7 +5087,7 @@
       </c>
       <c r="G127" s="2"/>
     </row>
-    <row r="128" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A128" s="9">
         <v>124</v>
       </c>
@@ -4912,7 +5104,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A129" s="9">
         <v>125</v>
       </c>
@@ -4931,6 +5123,9 @@
       <c r="I129" t="s">
         <v>21</v>
       </c>
+      <c r="L129" t="s">
+        <v>446</v>
+      </c>
       <c r="N129" t="s">
         <v>21</v>
       </c>
@@ -4938,7 +5133,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A130" s="9">
         <v>126</v>
       </c>
@@ -4953,7 +5148,7 @@
       </c>
       <c r="G130" s="2"/>
     </row>
-    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="9">
         <v>127</v>
       </c>
@@ -4972,6 +5167,9 @@
       <c r="I131" t="s">
         <v>21</v>
       </c>
+      <c r="L131" t="s">
+        <v>446</v>
+      </c>
       <c r="N131" t="s">
         <v>21</v>
       </c>
@@ -4979,7 +5177,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A132" s="9">
         <v>128</v>
       </c>
@@ -4998,6 +5196,9 @@
       <c r="I132" t="s">
         <v>21</v>
       </c>
+      <c r="L132" t="s">
+        <v>446</v>
+      </c>
       <c r="N132" t="s">
         <v>21</v>
       </c>
@@ -5005,7 +5206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A133" s="9">
         <v>129</v>
       </c>
@@ -5024,6 +5225,9 @@
       <c r="I133" t="s">
         <v>21</v>
       </c>
+      <c r="L133" t="s">
+        <v>446</v>
+      </c>
       <c r="N133" t="s">
         <v>21</v>
       </c>
@@ -5031,7 +5235,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A134" s="9">
         <v>130</v>
       </c>
@@ -5050,6 +5254,9 @@
       <c r="I134" t="s">
         <v>21</v>
       </c>
+      <c r="L134" t="s">
+        <v>446</v>
+      </c>
       <c r="N134" t="s">
         <v>21</v>
       </c>
@@ -5057,7 +5264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A135" s="9">
         <v>131</v>
       </c>
@@ -5072,7 +5279,7 @@
       </c>
       <c r="G135" s="2"/>
     </row>
-    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="9">
         <v>132</v>
       </c>
@@ -5087,7 +5294,7 @@
       </c>
       <c r="G136" s="2"/>
     </row>
-    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A137" s="9">
         <v>133</v>
       </c>
@@ -5106,6 +5313,9 @@
       <c r="I137" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L137" t="s">
+        <v>446</v>
+      </c>
       <c r="N137" s="13" t="s">
         <v>21</v>
       </c>
@@ -5113,7 +5323,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="9">
         <v>134</v>
       </c>
@@ -5132,6 +5342,9 @@
       <c r="I138" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L138" t="s">
+        <v>446</v>
+      </c>
       <c r="N138" s="13" t="s">
         <v>21</v>
       </c>
@@ -5139,7 +5352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A139" s="9">
         <v>135</v>
       </c>
@@ -5154,7 +5367,7 @@
       </c>
       <c r="G139" s="2"/>
     </row>
-    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A140" s="9">
         <v>136</v>
       </c>
@@ -5173,6 +5386,9 @@
       <c r="I140" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L140" t="s">
+        <v>446</v>
+      </c>
       <c r="N140" s="13" t="s">
         <v>21</v>
       </c>
@@ -5180,7 +5396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A141" s="9">
         <v>137</v>
       </c>
@@ -5199,6 +5415,9 @@
       <c r="I141" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L141" t="s">
+        <v>446</v>
+      </c>
       <c r="N141" s="13" t="s">
         <v>21</v>
       </c>
@@ -5206,7 +5425,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A142" s="9">
         <v>138</v>
       </c>
@@ -5227,7 +5446,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A143" s="9">
         <v>139</v>
       </c>
@@ -5249,6 +5468,9 @@
       <c r="I143" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L143" t="s">
+        <v>446</v>
+      </c>
       <c r="N143" s="13" t="s">
         <v>21</v>
       </c>
@@ -5256,7 +5478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="9">
         <v>140</v>
       </c>
@@ -5271,7 +5493,7 @@
       </c>
       <c r="G144" s="2"/>
     </row>
-    <row r="145" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A145" s="9">
         <v>141</v>
       </c>
@@ -5286,7 +5508,7 @@
       </c>
       <c r="G145" s="2"/>
     </row>
-    <row r="146" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="9">
         <v>142</v>
       </c>
@@ -5301,7 +5523,7 @@
       </c>
       <c r="G146" s="2"/>
     </row>
-    <row r="147" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="9">
         <v>143</v>
       </c>
@@ -5316,7 +5538,7 @@
       </c>
       <c r="G147" s="2"/>
     </row>
-    <row r="148" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A148" s="9">
         <v>144</v>
       </c>
@@ -5335,6 +5557,9 @@
       <c r="I148" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L148" t="s">
+        <v>446</v>
+      </c>
       <c r="N148" s="13" t="s">
         <v>21</v>
       </c>
@@ -5342,7 +5567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A149" s="9">
         <v>145</v>
       </c>
@@ -5361,6 +5586,9 @@
       <c r="I149" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L149" t="s">
+        <v>446</v>
+      </c>
       <c r="N149" s="13" t="s">
         <v>21</v>
       </c>
@@ -5368,7 +5596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="9">
         <v>146</v>
       </c>
@@ -5383,7 +5611,7 @@
       </c>
       <c r="G150" s="2"/>
     </row>
-    <row r="151" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A151" s="9">
         <v>147</v>
       </c>
@@ -5398,7 +5626,7 @@
       </c>
       <c r="G151" s="2"/>
     </row>
-    <row r="152" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A152" s="9">
         <v>148</v>
       </c>
@@ -5417,6 +5645,9 @@
       <c r="I152" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L152" t="s">
+        <v>446</v>
+      </c>
       <c r="N152" s="13" t="s">
         <v>21</v>
       </c>
@@ -5424,7 +5655,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A153" s="9">
         <v>149</v>
       </c>
@@ -5443,6 +5674,9 @@
       <c r="I153" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L153" t="s">
+        <v>446</v>
+      </c>
       <c r="N153" s="13" t="s">
         <v>21</v>
       </c>
@@ -5450,7 +5684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A154" s="9">
         <v>150</v>
       </c>
@@ -5467,12 +5701,15 @@
       <c r="I154" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="L154" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="N154" s="1"/>
       <c r="O154" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A155" s="9">
         <v>151</v>
       </c>
@@ -5487,7 +5724,7 @@
       </c>
       <c r="G155" s="2"/>
     </row>
-    <row r="156" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A156" s="9">
         <v>152</v>
       </c>
@@ -5506,6 +5743,9 @@
       <c r="I156" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L156" t="s">
+        <v>446</v>
+      </c>
       <c r="N156" s="13" t="s">
         <v>21</v>
       </c>
@@ -5513,7 +5753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="9">
         <v>153</v>
       </c>
@@ -5532,6 +5772,9 @@
       <c r="I157" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L157" t="s">
+        <v>446</v>
+      </c>
       <c r="N157" s="13" t="s">
         <v>21</v>
       </c>
@@ -5539,7 +5782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A158" s="9">
         <v>154</v>
       </c>
@@ -5558,6 +5801,9 @@
       <c r="I158" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L158" t="s">
+        <v>446</v>
+      </c>
       <c r="N158" s="13" t="s">
         <v>21</v>
       </c>
@@ -5565,7 +5811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A159" s="9">
         <v>155</v>
       </c>
@@ -5584,6 +5830,9 @@
       <c r="I159" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L159" t="s">
+        <v>446</v>
+      </c>
       <c r="N159" s="13" t="s">
         <v>21</v>
       </c>
@@ -5591,7 +5840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A160" s="9">
         <v>156</v>
       </c>
@@ -5610,6 +5859,9 @@
       <c r="I160" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L160" t="s">
+        <v>446</v>
+      </c>
       <c r="N160" s="13" t="s">
         <v>21</v>
       </c>
@@ -5617,7 +5869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A161" s="9">
         <v>157</v>
       </c>
@@ -5636,6 +5888,9 @@
       <c r="I161" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L161" t="s">
+        <v>446</v>
+      </c>
       <c r="N161" s="13" t="s">
         <v>21</v>
       </c>
@@ -5643,7 +5898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A162" s="9">
         <v>158</v>
       </c>
@@ -5658,7 +5913,7 @@
       </c>
       <c r="G162" s="2"/>
     </row>
-    <row r="163" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A163" s="9">
         <v>159</v>
       </c>
@@ -5677,6 +5932,9 @@
       <c r="I163" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L163" t="s">
+        <v>446</v>
+      </c>
       <c r="N163" s="13" t="s">
         <v>21</v>
       </c>
@@ -5684,7 +5942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A164" s="9">
         <v>160</v>
       </c>
@@ -5699,7 +5957,7 @@
       </c>
       <c r="G164" s="2"/>
     </row>
-    <row r="165" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="9">
         <v>161</v>
       </c>
@@ -5714,7 +5972,7 @@
       </c>
       <c r="G165" s="2"/>
     </row>
-    <row r="166" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A166" s="9">
         <v>162</v>
       </c>
@@ -5733,6 +5991,9 @@
       <c r="I166" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L166" t="s">
+        <v>446</v>
+      </c>
       <c r="N166" s="13" t="s">
         <v>21</v>
       </c>
@@ -5740,7 +6001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A167" s="9">
         <v>163</v>
       </c>
@@ -5757,7 +6018,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A168" s="9">
         <v>164</v>
       </c>
@@ -5772,7 +6033,7 @@
       </c>
       <c r="G168" s="2"/>
     </row>
-    <row r="169" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="9">
         <v>165</v>
       </c>
@@ -5791,6 +6052,9 @@
       <c r="I169" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L169" t="s">
+        <v>446</v>
+      </c>
       <c r="N169" s="13" t="s">
         <v>21</v>
       </c>
@@ -5798,7 +6062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A170" s="9">
         <v>166</v>
       </c>
@@ -5817,6 +6081,9 @@
       <c r="I170" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L170" t="s">
+        <v>446</v>
+      </c>
       <c r="N170" s="13" t="s">
         <v>21</v>
       </c>
@@ -5824,7 +6091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="9">
         <v>167</v>
       </c>
@@ -5843,6 +6110,9 @@
       <c r="I171" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L171" t="s">
+        <v>446</v>
+      </c>
       <c r="N171" s="13" t="s">
         <v>21</v>
       </c>
@@ -5850,7 +6120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="9">
         <v>168</v>
       </c>
@@ -5869,6 +6139,9 @@
       <c r="I172" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L172" t="s">
+        <v>446</v>
+      </c>
       <c r="N172" s="13" t="s">
         <v>21</v>
       </c>
@@ -5876,7 +6149,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A173" s="9">
         <v>169</v>
       </c>
@@ -5895,6 +6168,9 @@
       <c r="I173" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L173" t="s">
+        <v>446</v>
+      </c>
       <c r="N173" s="13" t="s">
         <v>21</v>
       </c>
@@ -5902,7 +6178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="9">
         <v>170</v>
       </c>
@@ -5921,6 +6197,9 @@
       <c r="I174" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L174" t="s">
+        <v>446</v>
+      </c>
       <c r="N174" s="13" t="s">
         <v>21</v>
       </c>
@@ -5928,7 +6207,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="9">
         <v>171</v>
       </c>
@@ -5943,7 +6222,7 @@
       </c>
       <c r="G175" s="2"/>
     </row>
-    <row r="176" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="9">
         <v>172</v>
       </c>
@@ -5958,7 +6237,7 @@
       </c>
       <c r="G176" s="2"/>
     </row>
-    <row r="177" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="9">
         <v>173</v>
       </c>
@@ -5975,7 +6254,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="9">
         <v>174</v>
       </c>
@@ -5990,7 +6269,7 @@
       </c>
       <c r="G178" s="2"/>
     </row>
-    <row r="179" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A179" s="9">
         <v>175</v>
       </c>
@@ -6009,6 +6288,9 @@
       <c r="I179" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L179" t="s">
+        <v>446</v>
+      </c>
       <c r="N179" s="13" t="s">
         <v>21</v>
       </c>
@@ -6016,7 +6298,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A180" s="9">
         <v>176</v>
       </c>
@@ -6031,7 +6313,7 @@
       </c>
       <c r="G180" s="2"/>
     </row>
-    <row r="181" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="9">
         <v>177</v>
       </c>
@@ -6046,7 +6328,7 @@
       </c>
       <c r="G181" s="2"/>
     </row>
-    <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="9">
         <v>178</v>
       </c>
@@ -6063,6 +6345,9 @@
       <c r="I182" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L182" t="s">
+        <v>446</v>
+      </c>
       <c r="N182" s="13" t="s">
         <v>21</v>
       </c>
@@ -6070,7 +6355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="9">
         <v>179</v>
       </c>
@@ -6089,6 +6374,9 @@
       <c r="I183" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L183" t="s">
+        <v>446</v>
+      </c>
       <c r="N183" s="13" t="s">
         <v>21</v>
       </c>
@@ -6096,7 +6384,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A184" s="9">
         <v>180</v>
       </c>
@@ -6115,6 +6403,9 @@
       <c r="I184" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L184" t="s">
+        <v>446</v>
+      </c>
       <c r="N184" s="13" t="s">
         <v>21</v>
       </c>
@@ -6122,7 +6413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="9">
         <v>181</v>
       </c>
@@ -6141,6 +6432,9 @@
       <c r="I185" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L185" t="s">
+        <v>446</v>
+      </c>
       <c r="N185" s="13" t="s">
         <v>21</v>
       </c>
@@ -6148,7 +6442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A186" s="9">
         <v>182</v>
       </c>
@@ -6167,6 +6461,9 @@
       <c r="I186" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L186" t="s">
+        <v>446</v>
+      </c>
       <c r="N186" s="13" t="s">
         <v>21</v>
       </c>
@@ -6174,7 +6471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="9">
         <v>183</v>
       </c>
@@ -6193,6 +6490,9 @@
       <c r="I187" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L187" t="s">
+        <v>446</v>
+      </c>
       <c r="N187" s="13" t="s">
         <v>21</v>
       </c>
@@ -6200,7 +6500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A188" s="9">
         <v>184</v>
       </c>
@@ -6219,6 +6519,9 @@
       <c r="I188" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L188" t="s">
+        <v>446</v>
+      </c>
       <c r="N188" s="13" t="s">
         <v>21</v>
       </c>
@@ -6226,7 +6529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A189" s="9">
         <v>185</v>
       </c>
@@ -6245,6 +6548,9 @@
       <c r="I189" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L189" t="s">
+        <v>446</v>
+      </c>
       <c r="N189" s="13" t="s">
         <v>21</v>
       </c>
@@ -6252,7 +6558,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="9">
         <v>186</v>
       </c>
@@ -6271,6 +6577,9 @@
       <c r="I190" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L190" t="s">
+        <v>446</v>
+      </c>
       <c r="N190" s="13" t="s">
         <v>21</v>
       </c>
@@ -6278,7 +6587,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A191" s="9">
         <v>187</v>
       </c>
@@ -6297,6 +6606,9 @@
       <c r="I191" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L191" t="s">
+        <v>446</v>
+      </c>
       <c r="N191" s="13" t="s">
         <v>21</v>
       </c>
@@ -6304,7 +6616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A192" s="9">
         <v>188</v>
       </c>
@@ -6323,6 +6635,9 @@
       <c r="I192" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L192" t="s">
+        <v>446</v>
+      </c>
       <c r="N192" s="13" t="s">
         <v>21</v>
       </c>
@@ -6330,7 +6645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="9">
         <v>189</v>
       </c>
@@ -6349,6 +6664,9 @@
       <c r="I193" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L193" t="s">
+        <v>446</v>
+      </c>
       <c r="N193" s="13" t="s">
         <v>21</v>
       </c>
@@ -6356,7 +6674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A194" s="9">
         <v>190</v>
       </c>
@@ -6375,6 +6693,9 @@
       <c r="I194" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L194" t="s">
+        <v>446</v>
+      </c>
       <c r="N194" s="13" t="s">
         <v>21</v>
       </c>
@@ -6382,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A195" s="9">
         <v>191</v>
       </c>
@@ -6400,7 +6721,7 @@
       </c>
       <c r="G195" s="2"/>
     </row>
-    <row r="196" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A196" s="9">
         <v>192</v>
       </c>
@@ -6419,6 +6740,9 @@
       <c r="I196" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L196" t="s">
+        <v>446</v>
+      </c>
       <c r="N196" s="13" t="s">
         <v>21</v>
       </c>
@@ -6426,7 +6750,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A197" s="9">
         <v>193</v>
       </c>
@@ -6445,6 +6769,9 @@
       <c r="I197" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L197" t="s">
+        <v>446</v>
+      </c>
       <c r="N197" s="13" t="s">
         <v>21</v>
       </c>
@@ -6452,7 +6779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="9">
         <v>194</v>
       </c>
@@ -6471,6 +6798,9 @@
       <c r="I198" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L198" t="s">
+        <v>446</v>
+      </c>
       <c r="N198" s="13" t="s">
         <v>21</v>
       </c>
@@ -6478,7 +6808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A199" s="9">
         <v>195</v>
       </c>
@@ -6497,6 +6827,9 @@
       <c r="I199" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L199" t="s">
+        <v>446</v>
+      </c>
       <c r="N199" s="13" t="s">
         <v>21</v>
       </c>
@@ -6504,7 +6837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A200" s="9">
         <v>196</v>
       </c>
@@ -6523,6 +6856,9 @@
       <c r="I200" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L200" t="s">
+        <v>446</v>
+      </c>
       <c r="N200" s="13" t="s">
         <v>21</v>
       </c>
@@ -6530,7 +6866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A201" s="9">
         <v>197</v>
       </c>
@@ -6549,6 +6885,9 @@
       <c r="I201" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L201" t="s">
+        <v>446</v>
+      </c>
       <c r="N201" s="13" t="s">
         <v>21</v>
       </c>
@@ -6556,7 +6895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A202" s="9">
         <v>198</v>
       </c>
@@ -6575,6 +6914,9 @@
       <c r="I202" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L202" t="s">
+        <v>446</v>
+      </c>
       <c r="N202" s="13" t="s">
         <v>21</v>
       </c>
@@ -6582,7 +6924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A203" s="9">
         <v>199</v>
       </c>
@@ -6601,6 +6943,9 @@
       <c r="I203" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L203" t="s">
+        <v>446</v>
+      </c>
       <c r="N203" s="13" t="s">
         <v>21</v>
       </c>
@@ -6608,7 +6953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="204" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A204" s="9">
         <v>200</v>
       </c>
@@ -6623,7 +6968,7 @@
       </c>
       <c r="G204" s="2"/>
     </row>
-    <row r="205" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A205" s="9">
         <v>201</v>
       </c>
@@ -6642,6 +6987,9 @@
       <c r="I205" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L205" t="s">
+        <v>446</v>
+      </c>
       <c r="N205" s="13" t="s">
         <v>21</v>
       </c>
@@ -6649,7 +6997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A206" s="9">
         <v>202</v>
       </c>
@@ -6668,6 +7016,9 @@
       <c r="I206" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L206" t="s">
+        <v>446</v>
+      </c>
       <c r="N206" s="13" t="s">
         <v>21</v>
       </c>
@@ -6675,7 +7026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A207" s="9">
         <v>203</v>
       </c>
@@ -6694,6 +7045,9 @@
       <c r="I207" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L207" t="s">
+        <v>446</v>
+      </c>
       <c r="N207" s="13" t="s">
         <v>21</v>
       </c>
@@ -6701,7 +7055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A208" s="9">
         <v>204</v>
       </c>
@@ -6719,7 +7073,7 @@
       </c>
       <c r="G208" s="2"/>
     </row>
-    <row r="209" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A209" s="9">
         <v>205</v>
       </c>
@@ -6737,7 +7091,7 @@
       </c>
       <c r="G209" s="2"/>
     </row>
-    <row r="210" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A210" s="9">
         <v>206</v>
       </c>
@@ -6752,7 +7106,7 @@
       </c>
       <c r="G210" s="2"/>
     </row>
-    <row r="211" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A211" s="9">
         <v>207</v>
       </c>
@@ -6767,7 +7121,7 @@
       </c>
       <c r="G211" s="2"/>
     </row>
-    <row r="212" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A212" s="9">
         <v>208</v>
       </c>
@@ -6785,7 +7139,7 @@
       </c>
       <c r="G212" s="2"/>
     </row>
-    <row r="213" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A213" s="9">
         <v>209</v>
       </c>
@@ -6803,7 +7157,7 @@
       </c>
       <c r="G213" s="2"/>
     </row>
-    <row r="214" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A214" s="9">
         <v>210</v>
       </c>
@@ -6821,7 +7175,7 @@
       </c>
       <c r="G214" s="2"/>
     </row>
-    <row r="215" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="9">
         <v>211</v>
       </c>
@@ -6836,7 +7190,7 @@
       </c>
       <c r="G215" s="2"/>
     </row>
-    <row r="216" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A216" s="9">
         <v>212</v>
       </c>
@@ -6855,6 +7209,9 @@
       <c r="I216" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L216" t="s">
+        <v>446</v>
+      </c>
       <c r="N216" s="13" t="s">
         <v>21</v>
       </c>
@@ -6862,7 +7219,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A217" s="9">
         <v>213</v>
       </c>
@@ -6881,6 +7238,9 @@
       <c r="I217" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L217" t="s">
+        <v>446</v>
+      </c>
       <c r="N217" s="13" t="s">
         <v>21</v>
       </c>
@@ -6888,7 +7248,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A218" s="9">
         <v>214</v>
       </c>
@@ -6907,6 +7267,9 @@
       <c r="I218" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="L218" t="s">
+        <v>446</v>
+      </c>
       <c r="N218" s="13" t="s">
         <v>21</v>
       </c>
@@ -6914,7 +7277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="9">
         <v>215</v>
       </c>
@@ -6929,7 +7292,7 @@
       </c>
       <c r="G219" s="2"/>
     </row>
-    <row r="220" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A220" s="9">
         <v>216</v>
       </c>
@@ -6944,7 +7307,7 @@
       </c>
       <c r="G220" s="2"/>
     </row>
-    <row r="221" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A221" s="9">
         <v>217</v>
       </c>
@@ -6962,7 +7325,7 @@
       </c>
       <c r="G221" s="2"/>
     </row>
-    <row r="222" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A222" s="9">
         <v>218</v>
       </c>
@@ -6980,7 +7343,7 @@
       </c>
       <c r="G222" s="2"/>
     </row>
-    <row r="223" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="9">
         <v>219</v>
       </c>
@@ -6998,7 +7361,7 @@
       </c>
       <c r="G223" s="2"/>
     </row>
-    <row r="224" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A224" s="9">
         <v>220</v>
       </c>
@@ -7013,7 +7376,7 @@
       </c>
       <c r="G224" s="2"/>
     </row>
-    <row r="225" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>221</v>
       </c>
@@ -7040,6 +7403,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FDD0FC4969DCF4449136D2C873E795D1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c6f44795faba901663e8a9bf3a6322e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d2c32087-eb03-4a65-b505-380146e007a4" xmlns:ns4="2f381668-55bb-4cca-a2e9-7746dbcfba3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7caa3c07606457882248d14e3a3261f4" ns3:_="" ns4:_="">
     <xsd:import namespace="d2c32087-eb03-4a65-b505-380146e007a4"/>
@@ -7260,24 +7640,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d2c32087-eb03-4a65-b505-380146e007a4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DC07DF-80B7-4F51-9B64-7871291DEDB3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7294,22 +7675,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE93FEC-ED14-4C1A-BA6D-EE805B8918BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d2c32087-eb03-4a65-b505-380146e007a4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A69940-CFF9-46AC-A70F-7FC482219FC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added test for req 59
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlbea\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD55C36E-489D-4573-984E-E737B1D4404E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4E598F-CAEE-6340-8908-6586B2667468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="483">
   <si>
     <t>Tested By</t>
   </si>
@@ -389,9 +389,6 @@
   </si>
   <si>
     <t>The web interface of the Join Game component will be written in HTML5.</t>
-  </si>
-  <si>
-    <t>The program will be compatible with the web browsers Chrome, Firefox, and Safari.</t>
   </si>
   <si>
     <t>joingame</t>
@@ -1487,6 +1484,13 @@
   </si>
   <si>
     <t>Test 3: steps 4-8</t>
+  </si>
+  <si>
+    <t>The program will be compatible with the web browsers Chrome and Firefox.</t>
+  </si>
+  <si>
+    <t>Test 1 Step 3
+Note: This requirement was modified to exclude Safari as this is not on Fedora.</t>
   </si>
 </sst>
 </file>
@@ -1885,33 +1889,33 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F99" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.46484375" style="2" customWidth="1"/>
-    <col min="16" max="17" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" style="2" customWidth="1"/>
+    <col min="16" max="17" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1949,7 +1953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1969,7 +1973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="D4" s="4"/>
@@ -1977,7 +1981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1997,7 +2001,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -2017,7 +2021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -2034,7 +2038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -2048,10 +2052,10 @@
         <v>29</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -2065,10 +2069,10 @@
         <v>31</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -2082,10 +2086,10 @@
         <v>31</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -2105,7 +2109,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -2125,7 +2129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -2139,10 +2143,10 @@
         <v>25</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -2156,10 +2160,10 @@
         <v>31</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -2179,7 +2183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -2199,7 +2203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -2219,7 +2223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -2279,7 +2283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -2299,7 +2303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -2339,7 +2343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -2356,7 +2360,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -2373,7 +2377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -2393,7 +2397,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -2413,7 +2417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -2453,7 +2457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -2467,10 +2471,10 @@
         <v>59</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -2490,7 +2494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -2510,7 +2514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -2544,10 +2548,10 @@
         <v>64</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -2567,7 +2571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -2607,7 +2611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -2627,7 +2631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -2647,7 +2651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -2661,10 +2665,10 @@
         <v>59</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -2684,7 +2688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>38</v>
       </c>
@@ -2704,7 +2708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -2724,7 +2728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -2741,7 +2745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>41</v>
       </c>
@@ -2755,10 +2759,10 @@
         <v>85</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>43</v>
       </c>
@@ -2798,7 +2802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>45</v>
       </c>
@@ -2838,7 +2842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>46</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>47</v>
       </c>
@@ -2878,7 +2882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>48</v>
       </c>
@@ -2892,10 +2896,10 @@
         <v>99</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>49</v>
       </c>
@@ -2912,10 +2916,10 @@
         <v>102</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>50</v>
       </c>
@@ -2932,10 +2936,10 @@
         <v>105</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>51</v>
       </c>
@@ -2952,10 +2956,10 @@
         <v>107</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>52</v>
       </c>
@@ -2972,10 +2976,10 @@
         <v>110</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>53</v>
       </c>
@@ -2992,10 +2996,10 @@
         <v>113</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>54</v>
       </c>
@@ -3012,10 +3016,10 @@
         <v>115</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>55</v>
       </c>
@@ -3032,10 +3036,10 @@
         <v>118</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>56</v>
       </c>
@@ -3052,10 +3056,10 @@
         <v>120</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>57</v>
       </c>
@@ -3072,10 +3076,10 @@
         <v>110</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:15" ht="128" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -3106,14 +3110,17 @@
         <v>26</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G63" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="N63" t="s">
         <v>22</v>
       </c>
@@ -3121,7 +3128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>60</v>
       </c>
@@ -3129,10 +3136,10 @@
         <v>26</v>
       </c>
       <c r="C64" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>110</v>
@@ -3144,7 +3151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -3152,10 +3159,10 @@
         <v>26</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>110</v>
@@ -3167,7 +3174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>62</v>
       </c>
@@ -3175,10 +3182,10 @@
         <v>26</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>110</v>
@@ -3190,7 +3197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>63</v>
       </c>
@@ -3198,19 +3205,19 @@
         <v>26</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>110</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>64</v>
       </c>
@@ -3218,19 +3225,19 @@
         <v>26</v>
       </c>
       <c r="C68" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>110</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -3238,10 +3245,10 @@
         <v>26</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>110</v>
@@ -3253,7 +3260,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>66</v>
       </c>
@@ -3261,10 +3268,10 @@
         <v>26</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>110</v>
@@ -3276,7 +3283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>67</v>
       </c>
@@ -3284,10 +3291,10 @@
         <v>26</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>110</v>
@@ -3299,7 +3306,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>68</v>
       </c>
@@ -3307,7 +3314,7 @@
         <v>26</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>117</v>
@@ -3322,7 +3329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>69</v>
       </c>
@@ -3330,16 +3337,16 @@
         <v>35</v>
       </c>
       <c r="C73" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="O73" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>70</v>
       </c>
@@ -3347,16 +3354,16 @@
         <v>35</v>
       </c>
       <c r="C74" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D74" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="O74" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>71</v>
       </c>
@@ -3364,16 +3371,16 @@
         <v>35</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>72</v>
       </c>
@@ -3381,16 +3388,16 @@
         <v>35</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D76" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="O76" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>73</v>
       </c>
@@ -3398,11 +3405,11 @@
         <v>35</v>
       </c>
       <c r="C77" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D77" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="N77" t="s">
         <v>22</v>
       </c>
@@ -3410,7 +3417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>74</v>
       </c>
@@ -3418,11 +3425,11 @@
         <v>35</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D78" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N78" t="s">
         <v>22</v>
       </c>
@@ -3430,7 +3437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -3438,11 +3445,11 @@
         <v>35</v>
       </c>
       <c r="C79" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D79" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="N79" t="s">
         <v>22</v>
       </c>
@@ -3450,7 +3457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>76</v>
       </c>
@@ -3458,11 +3465,11 @@
         <v>35</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D80" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="N80" t="s">
         <v>22</v>
       </c>
@@ -3470,7 +3477,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>77</v>
       </c>
@@ -3478,11 +3485,11 @@
         <v>35</v>
       </c>
       <c r="C81" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="N81" t="s">
         <v>22</v>
       </c>
@@ -3490,7 +3497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>78</v>
       </c>
@@ -3498,11 +3505,11 @@
         <v>27</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D82" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="N82" t="s">
         <v>22</v>
       </c>
@@ -3510,7 +3517,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>79</v>
       </c>
@@ -3518,16 +3525,16 @@
         <v>27</v>
       </c>
       <c r="C83" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D83" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="O83" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>80</v>
       </c>
@@ -3535,19 +3542,19 @@
         <v>27</v>
       </c>
       <c r="C84" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="E84" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E84" s="4" t="s">
-        <v>165</v>
-      </c>
       <c r="O84" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>81</v>
       </c>
@@ -3555,19 +3562,19 @@
         <v>27</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="E85" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E85" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="O85" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>82</v>
       </c>
@@ -3575,19 +3582,19 @@
         <v>27</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="E86" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E86" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="O86" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>83</v>
       </c>
@@ -3595,19 +3602,19 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E87" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="O87" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>84</v>
       </c>
@@ -3615,11 +3622,11 @@
         <v>27</v>
       </c>
       <c r="C88" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>176</v>
-      </c>
       <c r="N88" t="s">
         <v>22</v>
       </c>
@@ -3627,7 +3634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>85</v>
       </c>
@@ -3635,16 +3642,16 @@
         <v>27</v>
       </c>
       <c r="C89" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="O89" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>86</v>
       </c>
@@ -3652,19 +3659,19 @@
         <v>27</v>
       </c>
       <c r="C90" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E90" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="O90" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>87</v>
       </c>
@@ -3672,16 +3679,16 @@
         <v>27</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="O91" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>88</v>
       </c>
@@ -3689,19 +3696,19 @@
         <v>27</v>
       </c>
       <c r="C92" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E92" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="O92" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -3709,11 +3716,11 @@
         <v>27</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="N93" t="s">
         <v>22</v>
       </c>
@@ -3721,7 +3728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>90</v>
       </c>
@@ -3729,11 +3736,11 @@
         <v>27</v>
       </c>
       <c r="C94" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="N94" t="s">
         <v>22</v>
       </c>
@@ -3741,7 +3748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>91</v>
       </c>
@@ -3749,16 +3756,16 @@
         <v>27</v>
       </c>
       <c r="C95" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="O95" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>92</v>
       </c>
@@ -3766,16 +3773,16 @@
         <v>27</v>
       </c>
       <c r="C96" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="O96" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>93</v>
       </c>
@@ -3783,11 +3790,11 @@
         <v>27</v>
       </c>
       <c r="C97" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D97" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="N97" t="s">
         <v>22</v>
       </c>
@@ -3795,7 +3802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>94</v>
       </c>
@@ -3803,16 +3810,16 @@
         <v>27</v>
       </c>
       <c r="C98" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D98" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="O98" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>95</v>
       </c>
@@ -3820,16 +3827,16 @@
         <v>27</v>
       </c>
       <c r="C99" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D99" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="O99" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>96</v>
       </c>
@@ -3837,16 +3844,16 @@
         <v>27</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D100" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D100" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="O100" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>97</v>
       </c>
@@ -3854,11 +3861,11 @@
         <v>27</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D101" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D101" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="N101" t="s">
         <v>22</v>
       </c>
@@ -3866,7 +3873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>98</v>
       </c>
@@ -3874,11 +3881,11 @@
         <v>36</v>
       </c>
       <c r="C102" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D102" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="N102" t="s">
         <v>22</v>
       </c>
@@ -3886,7 +3893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>99</v>
       </c>
@@ -3894,16 +3901,16 @@
         <v>36</v>
       </c>
       <c r="C103" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>208</v>
-      </c>
       <c r="O103" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>100</v>
       </c>
@@ -3911,16 +3918,16 @@
         <v>36</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>101</v>
       </c>
@@ -3928,16 +3935,16 @@
         <v>36</v>
       </c>
       <c r="C105" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D105" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="O105" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>102</v>
       </c>
@@ -3945,10 +3952,10 @@
         <v>36</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N106" t="s">
         <v>22</v>
@@ -3957,7 +3964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>103</v>
       </c>
@@ -3965,16 +3972,16 @@
         <v>36</v>
       </c>
       <c r="C107" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D107" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D107" s="4" t="s">
-        <v>214</v>
-      </c>
       <c r="O107" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" ht="85.5" x14ac:dyDescent="0.45">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>104</v>
       </c>
@@ -3982,16 +3989,16 @@
         <v>36</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -3999,16 +4006,16 @@
         <v>36</v>
       </c>
       <c r="C109" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>217</v>
-      </c>
       <c r="O109" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -4016,16 +4023,16 @@
         <v>36</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O110" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -4033,16 +4040,16 @@
         <v>36</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O111" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -4050,16 +4057,16 @@
         <v>36</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O112" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -4067,16 +4074,16 @@
         <v>36</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -4084,16 +4091,16 @@
         <v>36</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -4101,16 +4108,16 @@
         <v>36</v>
       </c>
       <c r="C115" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D115" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D115" s="4" t="s">
-        <v>224</v>
-      </c>
       <c r="O115" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>112</v>
       </c>
@@ -4118,11 +4125,11 @@
         <v>36</v>
       </c>
       <c r="C116" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D116" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D116" s="4" t="s">
-        <v>226</v>
-      </c>
       <c r="N116" t="s">
         <v>22</v>
       </c>
@@ -4130,7 +4137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>113</v>
       </c>
@@ -4138,16 +4145,16 @@
         <v>31</v>
       </c>
       <c r="C117" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D117" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D117" s="4" t="s">
-        <v>228</v>
-      </c>
       <c r="O117" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>114</v>
       </c>
@@ -4155,16 +4162,16 @@
         <v>31</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O118" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>115</v>
       </c>
@@ -4172,16 +4179,16 @@
         <v>31</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O119" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>116</v>
       </c>
@@ -4189,11 +4196,11 @@
         <v>31</v>
       </c>
       <c r="C120" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D120" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D120" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="N120" t="s">
         <v>22</v>
       </c>
@@ -4201,7 +4208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>117</v>
       </c>
@@ -4209,11 +4216,11 @@
         <v>31</v>
       </c>
       <c r="C121" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D121" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D121" s="4" t="s">
-        <v>234</v>
-      </c>
       <c r="N121" t="s">
         <v>22</v>
       </c>
@@ -4221,7 +4228,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>118</v>
       </c>
@@ -4229,11 +4236,11 @@
         <v>31</v>
       </c>
       <c r="C122" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D122" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D122" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="N122" t="s">
         <v>22</v>
       </c>
@@ -4241,7 +4248,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>119</v>
       </c>
@@ -4249,10 +4256,10 @@
         <v>31</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N123" t="s">
         <v>22</v>
@@ -4261,7 +4268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>120</v>
       </c>
@@ -4269,16 +4276,16 @@
         <v>31</v>
       </c>
       <c r="C124" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D124" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D124" s="4" t="s">
-        <v>239</v>
-      </c>
       <c r="O124" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>121</v>
       </c>
@@ -4286,11 +4293,11 @@
         <v>31</v>
       </c>
       <c r="C125" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D125" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D125" s="4" t="s">
-        <v>241</v>
-      </c>
       <c r="N125" t="s">
         <v>22</v>
       </c>
@@ -4298,7 +4305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>122</v>
       </c>
@@ -4306,10 +4313,10 @@
         <v>31</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N126" t="s">
         <v>22</v>
@@ -4318,7 +4325,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>123</v>
       </c>
@@ -4326,16 +4333,16 @@
         <v>31</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O127" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>124</v>
       </c>
@@ -4343,16 +4350,16 @@
         <v>31</v>
       </c>
       <c r="C128" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D128" s="4" t="s">
-        <v>245</v>
-      </c>
       <c r="O128" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>125</v>
       </c>
@@ -4360,11 +4367,11 @@
         <v>31</v>
       </c>
       <c r="C129" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D129" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D129" s="4" t="s">
-        <v>247</v>
-      </c>
       <c r="N129" t="s">
         <v>22</v>
       </c>
@@ -4372,7 +4379,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>126</v>
       </c>
@@ -4380,16 +4387,16 @@
         <v>31</v>
       </c>
       <c r="C130" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D130" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="D130" s="4" t="s">
-        <v>249</v>
-      </c>
       <c r="O130" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>127</v>
       </c>
@@ -4397,11 +4404,11 @@
         <v>30</v>
       </c>
       <c r="C131" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D131" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="D131" s="6" t="s">
-        <v>251</v>
-      </c>
       <c r="N131" t="s">
         <v>22</v>
       </c>
@@ -4409,7 +4416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>128</v>
       </c>
@@ -4417,11 +4424,11 @@
         <v>30</v>
       </c>
       <c r="C132" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D132" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D132" s="6" t="s">
-        <v>253</v>
-      </c>
       <c r="N132" t="s">
         <v>22</v>
       </c>
@@ -4429,7 +4436,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>129</v>
       </c>
@@ -4437,11 +4444,11 @@
         <v>30</v>
       </c>
       <c r="C133" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D133" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D133" s="6" t="s">
-        <v>255</v>
-      </c>
       <c r="N133" t="s">
         <v>22</v>
       </c>
@@ -4449,7 +4456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>130</v>
       </c>
@@ -4457,11 +4464,11 @@
         <v>30</v>
       </c>
       <c r="C134" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D134" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D134" s="6" t="s">
-        <v>257</v>
-      </c>
       <c r="N134" t="s">
         <v>22</v>
       </c>
@@ -4469,7 +4476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>131</v>
       </c>
@@ -4477,16 +4484,16 @@
         <v>30</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O135" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>132</v>
       </c>
@@ -4494,16 +4501,16 @@
         <v>30</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O136" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>133</v>
       </c>
@@ -4511,10 +4518,10 @@
         <v>30</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N137" s="8" t="s">
         <v>22</v>
@@ -4523,7 +4530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>134</v>
       </c>
@@ -4531,10 +4538,10 @@
         <v>30</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N138" s="8" t="s">
         <v>22</v>
@@ -4543,7 +4550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="57" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>135</v>
       </c>
@@ -4551,16 +4558,16 @@
         <v>30</v>
       </c>
       <c r="C139" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D139" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="D139" s="6" t="s">
-        <v>263</v>
-      </c>
       <c r="O139" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" ht="57" x14ac:dyDescent="0.45">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>136</v>
       </c>
@@ -4568,11 +4575,11 @@
         <v>30</v>
       </c>
       <c r="C140" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D140" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="D140" s="6" t="s">
-        <v>265</v>
-      </c>
       <c r="N140" s="8" t="s">
         <v>22</v>
       </c>
@@ -4580,7 +4587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>137</v>
       </c>
@@ -4588,11 +4595,11 @@
         <v>30</v>
       </c>
       <c r="C141" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D141" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="D141" s="6" t="s">
-        <v>267</v>
-      </c>
       <c r="N141" s="8" t="s">
         <v>22</v>
       </c>
@@ -4600,7 +4607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>138</v>
       </c>
@@ -4608,22 +4615,22 @@
         <v>28</v>
       </c>
       <c r="C142" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D142" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="E142" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="O142" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="R142" t="s">
         <v>270</v>
       </c>
-      <c r="O142" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="R142" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>139</v>
       </c>
@@ -4631,14 +4638,14 @@
         <v>28</v>
       </c>
       <c r="C143" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D143" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="E143" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E143" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="N143" s="8" t="s">
         <v>22</v>
       </c>
@@ -4646,7 +4653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>140</v>
       </c>
@@ -4654,16 +4661,16 @@
         <v>28</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O144" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="145" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>141</v>
       </c>
@@ -4671,16 +4678,16 @@
         <v>28</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O145" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>142</v>
       </c>
@@ -4688,16 +4695,16 @@
         <v>28</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O146" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="147" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>143</v>
       </c>
@@ -4705,16 +4712,16 @@
         <v>28</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O147" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>144</v>
       </c>
@@ -4722,10 +4729,10 @@
         <v>28</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N148" s="8" t="s">
         <v>22</v>
@@ -4734,7 +4741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>145</v>
       </c>
@@ -4742,10 +4749,10 @@
         <v>28</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N149" s="8" t="s">
         <v>22</v>
@@ -4754,7 +4761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>146</v>
       </c>
@@ -4762,16 +4769,16 @@
         <v>28</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O150" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>147</v>
       </c>
@@ -4779,16 +4786,16 @@
         <v>28</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O151" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="152" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>148</v>
       </c>
@@ -4796,11 +4803,11 @@
         <v>29</v>
       </c>
       <c r="C152" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D152" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="D152" s="4" t="s">
-        <v>284</v>
-      </c>
       <c r="N152" s="8" t="s">
         <v>22</v>
       </c>
@@ -4808,7 +4815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>149</v>
       </c>
@@ -4816,11 +4823,11 @@
         <v>29</v>
       </c>
       <c r="C153" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D153" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="D153" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="N153" s="8" t="s">
         <v>22</v>
       </c>
@@ -4828,7 +4835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>150</v>
       </c>
@@ -4836,17 +4843,17 @@
         <v>29</v>
       </c>
       <c r="C154" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D154" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>288</v>
       </c>
       <c r="N154" s="4"/>
       <c r="O154" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="155" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>151</v>
       </c>
@@ -4854,16 +4861,16 @@
         <v>29</v>
       </c>
       <c r="C155" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D155" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D155" s="4" t="s">
-        <v>291</v>
-      </c>
       <c r="O155" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>152</v>
       </c>
@@ -4871,11 +4878,11 @@
         <v>29</v>
       </c>
       <c r="C156" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D156" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="D156" s="4" t="s">
-        <v>293</v>
-      </c>
       <c r="N156" s="8" t="s">
         <v>22</v>
       </c>
@@ -4883,7 +4890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>153</v>
       </c>
@@ -4891,11 +4898,11 @@
         <v>29</v>
       </c>
       <c r="C157" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D157" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="D157" s="4" t="s">
-        <v>295</v>
-      </c>
       <c r="N157" s="8" t="s">
         <v>22</v>
       </c>
@@ -4903,7 +4910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>154</v>
       </c>
@@ -4911,11 +4918,11 @@
         <v>29</v>
       </c>
       <c r="C158" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D158" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="D158" s="4" t="s">
-        <v>297</v>
-      </c>
       <c r="N158" s="8" t="s">
         <v>22</v>
       </c>
@@ -4923,7 +4930,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>155</v>
       </c>
@@ -4931,11 +4938,11 @@
         <v>29</v>
       </c>
       <c r="C159" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D159" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="D159" s="4" t="s">
-        <v>299</v>
-      </c>
       <c r="N159" s="8" t="s">
         <v>22</v>
       </c>
@@ -4943,7 +4950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>156</v>
       </c>
@@ -4951,11 +4958,11 @@
         <v>29</v>
       </c>
       <c r="C160" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D160" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="D160" s="4" t="s">
-        <v>301</v>
-      </c>
       <c r="N160" s="8" t="s">
         <v>22</v>
       </c>
@@ -4963,7 +4970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>157</v>
       </c>
@@ -4971,11 +4978,11 @@
         <v>29</v>
       </c>
       <c r="C161" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D161" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D161" s="4" t="s">
-        <v>303</v>
-      </c>
       <c r="N161" s="8" t="s">
         <v>22</v>
       </c>
@@ -4983,7 +4990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>158</v>
       </c>
@@ -4991,16 +4998,16 @@
         <v>29</v>
       </c>
       <c r="C162" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D162" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D162" s="4" t="s">
-        <v>305</v>
-      </c>
       <c r="O162" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>159</v>
       </c>
@@ -5008,11 +5015,11 @@
         <v>29</v>
       </c>
       <c r="C163" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D163" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="D163" s="4" t="s">
-        <v>307</v>
-      </c>
       <c r="N163" s="8" t="s">
         <v>22</v>
       </c>
@@ -5020,7 +5027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>160</v>
       </c>
@@ -5028,16 +5035,16 @@
         <v>29</v>
       </c>
       <c r="C164" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D164" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="D164" s="4" t="s">
-        <v>309</v>
-      </c>
       <c r="O164" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>161</v>
       </c>
@@ -5045,16 +5052,16 @@
         <v>29</v>
       </c>
       <c r="C165" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D165" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="D165" s="4" t="s">
-        <v>311</v>
-      </c>
       <c r="O165" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>162</v>
       </c>
@@ -5062,11 +5069,11 @@
         <v>29</v>
       </c>
       <c r="C166" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D166" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="D166" s="4" t="s">
-        <v>313</v>
-      </c>
       <c r="N166" s="8" t="s">
         <v>22</v>
       </c>
@@ -5074,7 +5081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>163</v>
       </c>
@@ -5082,16 +5089,16 @@
         <v>29</v>
       </c>
       <c r="C167" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D167" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="D167" s="4" t="s">
-        <v>315</v>
-      </c>
       <c r="O167" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>164</v>
       </c>
@@ -5099,16 +5106,16 @@
         <v>29</v>
       </c>
       <c r="C168" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D168" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D168" s="4" t="s">
-        <v>317</v>
-      </c>
       <c r="O168" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>165</v>
       </c>
@@ -5116,11 +5123,11 @@
         <v>29</v>
       </c>
       <c r="C169" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D169" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="D169" s="4" t="s">
-        <v>319</v>
-      </c>
       <c r="N169" s="8" t="s">
         <v>22</v>
       </c>
@@ -5128,7 +5135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>166</v>
       </c>
@@ -5136,10 +5143,10 @@
         <v>29</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N170" s="8" t="s">
         <v>22</v>
@@ -5148,7 +5155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>167</v>
       </c>
@@ -5156,11 +5163,11 @@
         <v>29</v>
       </c>
       <c r="C171" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D171" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D171" s="4" t="s">
-        <v>322</v>
-      </c>
       <c r="N171" s="8" t="s">
         <v>22</v>
       </c>
@@ -5168,7 +5175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="3">
         <v>168</v>
       </c>
@@ -5176,11 +5183,11 @@
         <v>32</v>
       </c>
       <c r="C172" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D172" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="D172" s="4" t="s">
-        <v>324</v>
-      </c>
       <c r="N172" s="8" t="s">
         <v>22</v>
       </c>
@@ -5188,7 +5195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>169</v>
       </c>
@@ -5196,11 +5203,11 @@
         <v>32</v>
       </c>
       <c r="C173" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D173" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D173" s="4" t="s">
-        <v>326</v>
-      </c>
       <c r="N173" s="8" t="s">
         <v>22</v>
       </c>
@@ -5208,7 +5215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>170</v>
       </c>
@@ -5216,11 +5223,11 @@
         <v>32</v>
       </c>
       <c r="C174" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D174" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D174" s="4" t="s">
-        <v>328</v>
-      </c>
       <c r="N174" s="8" t="s">
         <v>22</v>
       </c>
@@ -5228,7 +5235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>171</v>
       </c>
@@ -5236,16 +5243,16 @@
         <v>32</v>
       </c>
       <c r="C175" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D175" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="D175" s="4" t="s">
-        <v>330</v>
-      </c>
       <c r="O175" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="176" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="3">
         <v>172</v>
       </c>
@@ -5253,16 +5260,16 @@
         <v>32</v>
       </c>
       <c r="C176" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D176" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="D176" s="4" t="s">
-        <v>332</v>
-      </c>
       <c r="O176" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="177" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>173</v>
       </c>
@@ -5270,16 +5277,16 @@
         <v>32</v>
       </c>
       <c r="C177" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D177" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D177" s="4" t="s">
-        <v>334</v>
-      </c>
       <c r="O177" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="178" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>174</v>
       </c>
@@ -5287,16 +5294,16 @@
         <v>32</v>
       </c>
       <c r="C178" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D178" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="D178" s="4" t="s">
-        <v>336</v>
-      </c>
       <c r="O178" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>175</v>
       </c>
@@ -5304,11 +5311,11 @@
         <v>32</v>
       </c>
       <c r="C179" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D179" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D179" s="4" t="s">
-        <v>338</v>
-      </c>
       <c r="N179" s="8" t="s">
         <v>22</v>
       </c>
@@ -5316,7 +5323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A180" s="3">
         <v>176</v>
       </c>
@@ -5324,16 +5331,16 @@
         <v>32</v>
       </c>
       <c r="C180" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D180" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="D180" s="4" t="s">
-        <v>340</v>
-      </c>
       <c r="O180" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="181" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>177</v>
       </c>
@@ -5341,13 +5348,13 @@
         <v>32</v>
       </c>
       <c r="C181" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D181" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D181" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="182" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>178</v>
       </c>
@@ -5355,11 +5362,11 @@
         <v>32</v>
       </c>
       <c r="C182" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D182" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="D182" s="4" t="s">
-        <v>344</v>
-      </c>
       <c r="N182" s="8" t="s">
         <v>22</v>
       </c>
@@ -5367,7 +5374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>179</v>
       </c>
@@ -5375,11 +5382,11 @@
         <v>32</v>
       </c>
       <c r="C183" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D183" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="D183" s="4" t="s">
-        <v>346</v>
-      </c>
       <c r="N183" s="8" t="s">
         <v>22</v>
       </c>
@@ -5387,7 +5394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
         <v>180</v>
       </c>
@@ -5395,11 +5402,11 @@
         <v>32</v>
       </c>
       <c r="C184" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D184" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="D184" s="4" t="s">
-        <v>348</v>
-      </c>
       <c r="N184" s="8" t="s">
         <v>22</v>
       </c>
@@ -5407,7 +5414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>181</v>
       </c>
@@ -5415,11 +5422,11 @@
         <v>32</v>
       </c>
       <c r="C185" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D185" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="D185" s="4" t="s">
-        <v>350</v>
-      </c>
       <c r="N185" s="8" t="s">
         <v>22</v>
       </c>
@@ -5427,7 +5434,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>182</v>
       </c>
@@ -5435,11 +5442,11 @@
         <v>32</v>
       </c>
       <c r="C186" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D186" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="D186" s="4" t="s">
-        <v>352</v>
-      </c>
       <c r="N186" s="8" t="s">
         <v>22</v>
       </c>
@@ -5447,7 +5454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>183</v>
       </c>
@@ -5455,11 +5462,11 @@
         <v>32</v>
       </c>
       <c r="C187" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D187" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D187" s="4" t="s">
-        <v>354</v>
-      </c>
       <c r="N187" s="8" t="s">
         <v>22</v>
       </c>
@@ -5467,7 +5474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>184</v>
       </c>
@@ -5475,11 +5482,11 @@
         <v>32</v>
       </c>
       <c r="C188" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D188" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="D188" s="4" t="s">
-        <v>356</v>
-      </c>
       <c r="N188" s="8" t="s">
         <v>22</v>
       </c>
@@ -5487,7 +5494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>185</v>
       </c>
@@ -5495,10 +5502,10 @@
         <v>32</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N189" s="8" t="s">
         <v>22</v>
@@ -5507,7 +5514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
         <v>186</v>
       </c>
@@ -5515,10 +5522,10 @@
         <v>32</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N190" s="8" t="s">
         <v>22</v>
@@ -5527,7 +5534,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>187</v>
       </c>
@@ -5535,11 +5542,11 @@
         <v>32</v>
       </c>
       <c r="C191" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D191" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="D191" s="4" t="s">
-        <v>360</v>
-      </c>
       <c r="N191" s="8" t="s">
         <v>22</v>
       </c>
@@ -5547,7 +5554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>188</v>
       </c>
@@ -5555,11 +5562,11 @@
         <v>32</v>
       </c>
       <c r="C192" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D192" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="D192" s="4" t="s">
-        <v>362</v>
-      </c>
       <c r="N192" s="8" t="s">
         <v>22</v>
       </c>
@@ -5567,7 +5574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>189</v>
       </c>
@@ -5575,11 +5582,11 @@
         <v>32</v>
       </c>
       <c r="C193" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D193" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="D193" s="4" t="s">
-        <v>364</v>
-      </c>
       <c r="N193" s="8" t="s">
         <v>22</v>
       </c>
@@ -5587,7 +5594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
         <v>190</v>
       </c>
@@ -5595,11 +5602,11 @@
         <v>32</v>
       </c>
       <c r="C194" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D194" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="D194" s="4" t="s">
-        <v>366</v>
-      </c>
       <c r="N194" s="8" t="s">
         <v>22</v>
       </c>
@@ -5607,7 +5614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>191</v>
       </c>
@@ -5615,19 +5622,19 @@
         <v>32</v>
       </c>
       <c r="C195" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D195" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="D195" s="4" t="s">
+      <c r="E195" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="E195" s="4" t="s">
-        <v>369</v>
-      </c>
       <c r="O195" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>192</v>
       </c>
@@ -5635,11 +5642,11 @@
         <v>32</v>
       </c>
       <c r="C196" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D196" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="D196" s="4" t="s">
-        <v>371</v>
-      </c>
       <c r="N196" s="8" t="s">
         <v>22</v>
       </c>
@@ -5647,7 +5654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>193</v>
       </c>
@@ -5655,11 +5662,11 @@
         <v>32</v>
       </c>
       <c r="C197" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D197" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>373</v>
-      </c>
       <c r="N197" s="8" t="s">
         <v>22</v>
       </c>
@@ -5667,7 +5674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>194</v>
       </c>
@@ -5675,11 +5682,11 @@
         <v>32</v>
       </c>
       <c r="C198" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D198" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="D198" s="4" t="s">
-        <v>375</v>
-      </c>
       <c r="N198" s="8" t="s">
         <v>22</v>
       </c>
@@ -5687,7 +5694,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>195</v>
       </c>
@@ -5695,11 +5702,11 @@
         <v>32</v>
       </c>
       <c r="C199" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D199" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="D199" s="4" t="s">
-        <v>377</v>
-      </c>
       <c r="N199" s="8" t="s">
         <v>22</v>
       </c>
@@ -5707,7 +5714,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>196</v>
       </c>
@@ -5715,11 +5722,11 @@
         <v>32</v>
       </c>
       <c r="C200" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D200" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="D200" s="4" t="s">
-        <v>379</v>
-      </c>
       <c r="N200" s="8" t="s">
         <v>22</v>
       </c>
@@ -5727,7 +5734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>197</v>
       </c>
@@ -5735,11 +5742,11 @@
         <v>32</v>
       </c>
       <c r="C201" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D201" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="D201" s="4" t="s">
-        <v>381</v>
-      </c>
       <c r="N201" s="8" t="s">
         <v>22</v>
       </c>
@@ -5747,7 +5754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>198</v>
       </c>
@@ -5755,11 +5762,11 @@
         <v>32</v>
       </c>
       <c r="C202" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D202" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="D202" s="4" t="s">
-        <v>383</v>
-      </c>
       <c r="N202" s="8" t="s">
         <v>22</v>
       </c>
@@ -5767,7 +5774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>199</v>
       </c>
@@ -5775,11 +5782,11 @@
         <v>32</v>
       </c>
       <c r="C203" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D203" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="D203" s="4" t="s">
-        <v>385</v>
-      </c>
       <c r="N203" s="8" t="s">
         <v>22</v>
       </c>
@@ -5787,7 +5794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>200</v>
       </c>
@@ -5795,16 +5802,16 @@
         <v>32</v>
       </c>
       <c r="C204" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D204" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="D204" s="4" t="s">
-        <v>387</v>
-      </c>
       <c r="O204" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="205" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>201</v>
       </c>
@@ -5812,10 +5819,10 @@
         <v>32</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N205" s="8" t="s">
         <v>22</v>
@@ -5824,7 +5831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>202</v>
       </c>
@@ -5832,11 +5839,11 @@
         <v>32</v>
       </c>
       <c r="C206" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D206" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D206" s="4" t="s">
-        <v>390</v>
-      </c>
       <c r="N206" s="8" t="s">
         <v>22</v>
       </c>
@@ -5844,7 +5851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>203</v>
       </c>
@@ -5852,22 +5859,22 @@
         <v>32</v>
       </c>
       <c r="C207" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D207" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="D207" s="4" t="s">
+      <c r="N207" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O207" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R207" t="s">
         <v>392</v>
       </c>
-      <c r="N207" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="O207" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R207" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="208" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="208" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>204</v>
       </c>
@@ -5875,19 +5882,19 @@
         <v>25</v>
       </c>
       <c r="C208" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D208" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="D208" s="4" t="s">
+      <c r="E208" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="E208" s="4" t="s">
-        <v>396</v>
-      </c>
       <c r="O208" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="209" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>205</v>
       </c>
@@ -5895,19 +5902,19 @@
         <v>25</v>
       </c>
       <c r="C209" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D209" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="D209" s="4" t="s">
+      <c r="E209" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="E209" s="4" t="s">
-        <v>399</v>
-      </c>
       <c r="O209" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="210" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>206</v>
       </c>
@@ -5915,19 +5922,19 @@
         <v>25</v>
       </c>
       <c r="C210" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D210" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="D210" s="4" t="s">
+      <c r="O210" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R210" t="s">
         <v>401</v>
       </c>
-      <c r="O210" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R210" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="211" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="211" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>207</v>
       </c>
@@ -5935,16 +5942,16 @@
         <v>25</v>
       </c>
       <c r="C211" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D211" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="D211" s="4" t="s">
-        <v>404</v>
-      </c>
       <c r="O211" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="212" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>208</v>
       </c>
@@ -5952,19 +5959,19 @@
         <v>25</v>
       </c>
       <c r="C212" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D212" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="D212" s="4" t="s">
+      <c r="E212" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E212" s="4" t="s">
-        <v>407</v>
-      </c>
       <c r="O212" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="213" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>209</v>
       </c>
@@ -5972,19 +5979,19 @@
         <v>25</v>
       </c>
       <c r="C213" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D213" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="D213" s="4" t="s">
+      <c r="E213" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="E213" s="4" t="s">
-        <v>410</v>
-      </c>
       <c r="O213" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="214" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>210</v>
       </c>
@@ -5992,19 +5999,19 @@
         <v>25</v>
       </c>
       <c r="C214" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="D214" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="D214" s="4" t="s">
+      <c r="E214" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E214" s="4" t="s">
-        <v>413</v>
-      </c>
       <c r="O214" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="215" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>211</v>
       </c>
@@ -6012,19 +6019,19 @@
         <v>25</v>
       </c>
       <c r="C215" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="O215" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="R215" t="s">
         <v>414</v>
       </c>
-      <c r="D215" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="O215" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="R215" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="216" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="216" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>212</v>
       </c>
@@ -6032,11 +6039,11 @@
         <v>25</v>
       </c>
       <c r="C216" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D216" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="D216" s="4" t="s">
-        <v>417</v>
-      </c>
       <c r="N216" s="8" t="s">
         <v>22</v>
       </c>
@@ -6044,7 +6051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>213</v>
       </c>
@@ -6052,10 +6059,10 @@
         <v>25</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N217" s="8" t="s">
         <v>22</v>
@@ -6064,7 +6071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>214</v>
       </c>
@@ -6072,11 +6079,11 @@
         <v>25</v>
       </c>
       <c r="C218" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D218" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="D218" s="4" t="s">
-        <v>420</v>
-      </c>
       <c r="N218" s="8" t="s">
         <v>22</v>
       </c>
@@ -6084,7 +6091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>215</v>
       </c>
@@ -6092,16 +6099,16 @@
         <v>25</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O219" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="220" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>216</v>
       </c>
@@ -6109,16 +6116,16 @@
         <v>25</v>
       </c>
       <c r="C220" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="D220" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="D220" s="4" t="s">
-        <v>423</v>
-      </c>
       <c r="O220" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="221" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>217</v>
       </c>
@@ -6126,22 +6133,22 @@
         <v>25</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D221" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="E221" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="E221" s="4" t="s">
+      <c r="O221" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="R221" t="s">
         <v>425</v>
       </c>
-      <c r="O221" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="R221" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="222" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="222" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>218</v>
       </c>
@@ -6149,19 +6156,19 @@
         <v>25</v>
       </c>
       <c r="C222" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D222" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="D222" s="4" t="s">
+      <c r="E222" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="E222" s="4" t="s">
-        <v>429</v>
-      </c>
       <c r="O222" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="223" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>219</v>
       </c>
@@ -6169,19 +6176,19 @@
         <v>25</v>
       </c>
       <c r="C223" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D223" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="E223" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="D223" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="E223" s="4" t="s">
-        <v>431</v>
-      </c>
       <c r="O223" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="224" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>220</v>
       </c>
@@ -6189,23 +6196,23 @@
         <v>25</v>
       </c>
       <c r="C224" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D224" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="D224" s="4" t="s">
+      <c r="O224" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R230" t="s">
         <v>433</v>
-      </c>
-      <c r="O224" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="R230" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for reqs 204 and 209
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4E598F-CAEE-6340-8908-6586B2667468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE62D027-D264-5849-B536-2AF57E552421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="484">
   <si>
     <t>Tested By</t>
   </si>
@@ -1491,6 +1491,9 @@
   <si>
     <t>Test 1 Step 3
 Note: This requirement was modified to exclude Safari as this is not on Fedora.</t>
+  </si>
+  <si>
+    <t>Test 1: Step 4</t>
   </si>
 </sst>
 </file>
@@ -1558,7 +1561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1581,6 +1584,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1889,8 +1895,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H217" sqref="H217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5890,6 +5896,9 @@
       <c r="E208" s="4" t="s">
         <v>395</v>
       </c>
+      <c r="G208" s="9" t="s">
+        <v>483</v>
+      </c>
       <c r="O208" s="2" t="s">
         <v>446</v>
       </c>
@@ -5986,6 +5995,9 @@
       </c>
       <c r="E213" s="4" t="s">
         <v>409</v>
+      </c>
+      <c r="G213" s="9" t="s">
+        <v>483</v>
       </c>
       <c r="O213" s="2" t="s">
         <v>448</v>

</xml_diff>

<commit_message>
Previous untestable comments were removed. Readded.
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE62D027-D264-5849-B536-2AF57E552421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCADCF5-3AAF-9148-972A-34551A7ECBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="497">
   <si>
     <t>Tested By</t>
   </si>
@@ -1489,11 +1489,49 @@
     <t>The program will be compatible with the web browsers Chrome and Firefox.</t>
   </si>
   <si>
-    <t>Test 1 Step 3
-Note: This requirement was modified to exclude Safari as this is not on Fedora.</t>
-  </si>
-  <si>
     <t>Test 1: Step 4</t>
+  </si>
+  <si>
+    <t>Unable to test</t>
+  </si>
+  <si>
+    <t>Partially testable - may be observed by playing several games but full verfication would require code inspection</t>
+  </si>
+  <si>
+    <t>Unable to test - move evaluation is likely internal</t>
+  </si>
+  <si>
+    <t>Req might be too unclear to test.</t>
+  </si>
+  <si>
+    <t>Req might be too unclear as "fixed strategy" is not fully defined/</t>
+  </si>
+  <si>
+    <t>Req might be too unclear to test as "aggressively" is subjective.</t>
+  </si>
+  <si>
+    <t>Req might be too unclear to test. "Cautiously" is not precisely defined.</t>
+  </si>
+  <si>
+    <t>Test 1: Step 3</t>
+  </si>
+  <si>
+    <t>Note: This requirement was modified to remove Safari as this is not on Fedora.</t>
+  </si>
+  <si>
+    <t>Unable to tsst</t>
+  </si>
+  <si>
+    <t>Will need multiple games to verify</t>
+  </si>
+  <si>
+    <t>Req. might be too unlcear to test. What is the state of the board?</t>
+  </si>
+  <si>
+    <t>Depends if the active game count is displayed</t>
+  </si>
+  <si>
+    <t>Req. might be too unlcear to test.What does if needed mean?</t>
   </si>
 </sst>
 </file>
@@ -1561,7 +1599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1584,9 +1622,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1895,8 +1930,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H217" sqref="H217"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2000,6 +2035,9 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N5" t="s">
         <v>22</v>
       </c>
@@ -2020,6 +2058,9 @@
       <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N6" t="s">
         <v>22</v>
       </c>
@@ -2027,7 +2068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -2039,6 +2080,9 @@
       </c>
       <c r="D7" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>484</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>23</v>
@@ -2057,6 +2101,7 @@
       <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="G8" s="2"/>
       <c r="O8" s="2" t="s">
         <v>479</v>
       </c>
@@ -2074,6 +2119,7 @@
       <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G9" s="2"/>
       <c r="O9" s="2" t="s">
         <v>479</v>
       </c>
@@ -2091,6 +2137,7 @@
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G10" s="2"/>
       <c r="O10" s="2" t="s">
         <v>479</v>
       </c>
@@ -2108,6 +2155,9 @@
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N11" t="s">
         <v>22</v>
       </c>
@@ -2128,6 +2178,9 @@
       <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>485</v>
+      </c>
       <c r="N12" t="s">
         <v>22</v>
       </c>
@@ -2148,6 +2201,7 @@
       <c r="D13" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G13" s="2"/>
       <c r="O13" s="2" t="s">
         <v>480</v>
       </c>
@@ -2165,6 +2219,7 @@
       <c r="D14" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G14" s="2"/>
       <c r="O14" s="2" t="s">
         <v>479</v>
       </c>
@@ -2182,6 +2237,9 @@
       <c r="D15" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N15" t="s">
         <v>22</v>
       </c>
@@ -2202,6 +2260,9 @@
       <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N16" t="s">
         <v>22</v>
       </c>
@@ -2222,6 +2283,9 @@
       <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="G17" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N17" t="s">
         <v>22</v>
       </c>
@@ -2242,6 +2306,9 @@
       <c r="D18" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N18" t="s">
         <v>22</v>
       </c>
@@ -2262,6 +2329,9 @@
       <c r="D19" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="G19" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N19" t="s">
         <v>22</v>
       </c>
@@ -2282,6 +2352,9 @@
       <c r="D20" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N20" t="s">
         <v>22</v>
       </c>
@@ -2302,6 +2375,9 @@
       <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N21" t="s">
         <v>22</v>
       </c>
@@ -2322,6 +2398,9 @@
       <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N22" t="s">
         <v>22</v>
       </c>
@@ -2342,6 +2421,9 @@
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N23" t="s">
         <v>22</v>
       </c>
@@ -2362,6 +2444,9 @@
       <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="O24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2379,6 +2464,9 @@
       <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="O25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2396,6 +2484,9 @@
       <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N26" t="s">
         <v>22</v>
       </c>
@@ -2415,6 +2506,9 @@
       </c>
       <c r="D27" s="4" t="s">
         <v>55</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>483</v>
       </c>
       <c r="N27" t="s">
         <v>22</v>
@@ -2436,6 +2530,9 @@
       <c r="D28" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N28" t="s">
         <v>22</v>
       </c>
@@ -2456,6 +2553,9 @@
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G29" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N29" t="s">
         <v>22</v>
       </c>
@@ -2463,7 +2563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -2475,6 +2575,9 @@
       </c>
       <c r="D30" s="4" t="s">
         <v>59</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>487</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>479</v>
@@ -2493,6 +2596,9 @@
       <c r="D31" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="G31" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N31" t="s">
         <v>22</v>
       </c>
@@ -2513,6 +2619,9 @@
       <c r="D32" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="G32" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N32" t="s">
         <v>22</v>
       </c>
@@ -2533,6 +2642,9 @@
       <c r="D33" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N33" t="s">
         <v>22</v>
       </c>
@@ -2553,6 +2665,7 @@
       <c r="D34" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G34" s="2"/>
       <c r="O34" s="2" t="s">
         <v>479</v>
       </c>
@@ -2570,6 +2683,9 @@
       <c r="D35" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="G35" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N35" t="s">
         <v>22</v>
       </c>
@@ -2590,6 +2706,9 @@
       <c r="D36" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="G36" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N36" t="s">
         <v>22</v>
       </c>
@@ -2610,6 +2729,9 @@
       <c r="D37" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="G37" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N37" t="s">
         <v>22</v>
       </c>
@@ -2630,6 +2752,9 @@
       <c r="D38" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="G38" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N38" t="s">
         <v>22</v>
       </c>
@@ -2650,6 +2775,9 @@
       <c r="D39" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="G39" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N39" t="s">
         <v>22</v>
       </c>
@@ -2670,6 +2798,7 @@
       <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="G40" s="2"/>
       <c r="O40" s="2" t="s">
         <v>479</v>
       </c>
@@ -2687,6 +2816,9 @@
       <c r="D41" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="G41" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N41" t="s">
         <v>22</v>
       </c>
@@ -2707,6 +2839,9 @@
       <c r="D42" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="G42" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N42" t="s">
         <v>22</v>
       </c>
@@ -2714,7 +2849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -2727,6 +2862,9 @@
       <c r="D43" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="G43" s="2" t="s">
+        <v>488</v>
+      </c>
       <c r="N43" t="s">
         <v>22</v>
       </c>
@@ -2734,7 +2872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -2746,6 +2884,9 @@
       </c>
       <c r="D44" s="4" t="s">
         <v>83</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>489</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>23</v>
@@ -2764,6 +2905,7 @@
       <c r="D45" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="G45" s="2"/>
       <c r="O45" s="2" t="s">
         <v>479</v>
       </c>
@@ -2781,6 +2923,9 @@
       <c r="D46" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="G46" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N46" t="s">
         <v>22</v>
       </c>
@@ -2801,6 +2946,9 @@
       <c r="D47" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="G47" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N47" t="s">
         <v>22</v>
       </c>
@@ -2821,6 +2969,9 @@
       <c r="D48" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N48" t="s">
         <v>22</v>
       </c>
@@ -2841,6 +2992,9 @@
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="G49" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N49" t="s">
         <v>22</v>
       </c>
@@ -2861,6 +3015,9 @@
       <c r="D50" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="G50" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N50" t="s">
         <v>22</v>
       </c>
@@ -2881,6 +3038,9 @@
       <c r="D51" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="G51" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N51" t="s">
         <v>22</v>
       </c>
@@ -2901,6 +3061,7 @@
       <c r="D52" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="G52" s="2"/>
       <c r="O52" s="2" t="s">
         <v>479</v>
       </c>
@@ -2921,6 +3082,7 @@
       <c r="E53" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="G53" s="2"/>
       <c r="O53" s="2" t="s">
         <v>451</v>
       </c>
@@ -2941,6 +3103,7 @@
       <c r="E54" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="G54" s="2"/>
       <c r="O54" s="2" t="s">
         <v>452</v>
       </c>
@@ -2961,6 +3124,7 @@
       <c r="E55" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="G55" s="2"/>
       <c r="O55" s="2" t="s">
         <v>452</v>
       </c>
@@ -2981,6 +3145,7 @@
       <c r="E56" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G56" s="2"/>
       <c r="O56" s="2" t="s">
         <v>451</v>
       </c>
@@ -3001,6 +3166,7 @@
       <c r="E57" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="G57" s="2"/>
       <c r="O57" s="2" t="s">
         <v>451</v>
       </c>
@@ -3021,6 +3187,7 @@
       <c r="E58" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="G58" s="2"/>
       <c r="O58" s="2" t="s">
         <v>443</v>
       </c>
@@ -3041,6 +3208,7 @@
       <c r="E59" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="G59" s="2"/>
       <c r="O59" s="2" t="s">
         <v>437</v>
       </c>
@@ -3061,6 +3229,7 @@
       <c r="E60" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="G60" s="2"/>
       <c r="O60" s="2" t="s">
         <v>451</v>
       </c>
@@ -3081,6 +3250,7 @@
       <c r="E61" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G61" s="2"/>
       <c r="O61" s="2" t="s">
         <v>451</v>
       </c>
@@ -3101,6 +3271,9 @@
       <c r="E62" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G62" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N62" t="s">
         <v>22</v>
       </c>
@@ -3108,7 +3281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -3125,7 +3298,7 @@
         <v>110</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="N63" t="s">
         <v>22</v>
@@ -3150,6 +3323,7 @@
       <c r="E64" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G64" s="2"/>
       <c r="N64" t="s">
         <v>22</v>
       </c>
@@ -3157,7 +3331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -3172,6 +3346,9 @@
       </c>
       <c r="E65" s="4" t="s">
         <v>110</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>491</v>
       </c>
       <c r="N65" t="s">
         <v>22</v>
@@ -3196,6 +3373,9 @@
       <c r="E66" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G66" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N66" t="s">
         <v>22</v>
       </c>
@@ -3219,6 +3399,9 @@
       <c r="E67" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G67" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O67" s="2" t="s">
         <v>434</v>
       </c>
@@ -3239,6 +3422,9 @@
       <c r="E68" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G68" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O68" s="2" t="s">
         <v>453</v>
       </c>
@@ -3259,6 +3445,7 @@
       <c r="E69" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G69" s="2"/>
       <c r="N69" t="s">
         <v>22</v>
       </c>
@@ -3282,6 +3469,7 @@
       <c r="E70" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G70" s="2"/>
       <c r="N70" t="s">
         <v>22</v>
       </c>
@@ -3305,6 +3493,9 @@
       <c r="E71" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G71" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N71" t="s">
         <v>22</v>
       </c>
@@ -3328,6 +3519,9 @@
       <c r="E72" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G72" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N72" t="s">
         <v>22</v>
       </c>
@@ -3348,6 +3542,9 @@
       <c r="D73" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="G73" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O73" s="2" t="s">
         <v>454</v>
       </c>
@@ -3365,6 +3562,9 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="G74" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O74" s="2" t="s">
         <v>23</v>
       </c>
@@ -3382,6 +3582,7 @@
       <c r="D75" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="G75" s="2"/>
       <c r="O75" s="2" t="s">
         <v>456</v>
       </c>
@@ -3399,6 +3600,7 @@
       <c r="D76" s="4" t="s">
         <v>147</v>
       </c>
+      <c r="G76" s="2"/>
       <c r="O76" s="2" t="s">
         <v>455</v>
       </c>
@@ -3416,6 +3618,7 @@
       <c r="D77" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="G77" s="2"/>
       <c r="N77" t="s">
         <v>22</v>
       </c>
@@ -3436,6 +3639,7 @@
       <c r="D78" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="G78" s="2"/>
       <c r="N78" t="s">
         <v>22</v>
       </c>
@@ -3456,6 +3660,9 @@
       <c r="D79" s="4" t="s">
         <v>153</v>
       </c>
+      <c r="G79" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N79" t="s">
         <v>22</v>
       </c>
@@ -3476,6 +3683,9 @@
       <c r="D80" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="G80" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N80" t="s">
         <v>22</v>
       </c>
@@ -3496,6 +3706,9 @@
       <c r="D81" s="4" t="s">
         <v>157</v>
       </c>
+      <c r="G81" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N81" t="s">
         <v>22</v>
       </c>
@@ -3516,6 +3729,9 @@
       <c r="D82" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="G82" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N82" t="s">
         <v>22</v>
       </c>
@@ -3536,6 +3752,9 @@
       <c r="D83" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="G83" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O83" s="2" t="s">
         <v>455</v>
       </c>
@@ -3556,6 +3775,9 @@
       <c r="E84" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="G84" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O84" s="2" t="s">
         <v>458</v>
       </c>
@@ -3576,6 +3798,7 @@
       <c r="E85" s="4" t="s">
         <v>167</v>
       </c>
+      <c r="G85" s="2"/>
       <c r="O85" s="2" t="s">
         <v>457</v>
       </c>
@@ -3596,6 +3819,7 @@
       <c r="E86" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="G86" s="2"/>
       <c r="O86" s="2" t="s">
         <v>459</v>
       </c>
@@ -3616,6 +3840,7 @@
       <c r="E87" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="G87" s="2"/>
       <c r="O87" s="2" t="s">
         <v>460</v>
       </c>
@@ -3633,6 +3858,7 @@
       <c r="D88" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="G88" s="2"/>
       <c r="N88" t="s">
         <v>22</v>
       </c>
@@ -3653,6 +3879,7 @@
       <c r="D89" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="G89" s="2"/>
       <c r="O89" s="2" t="s">
         <v>435</v>
       </c>
@@ -3673,6 +3900,9 @@
       <c r="E90" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="G90" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O90" s="2" t="s">
         <v>436</v>
       </c>
@@ -3690,6 +3920,7 @@
       <c r="D91" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="G91" s="2"/>
       <c r="O91" s="2" t="s">
         <v>437</v>
       </c>
@@ -3710,6 +3941,7 @@
       <c r="E92" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="G92" s="2"/>
       <c r="O92" s="2" t="s">
         <v>438</v>
       </c>
@@ -3727,6 +3959,7 @@
       <c r="D93" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="G93" s="2"/>
       <c r="N93" t="s">
         <v>22</v>
       </c>
@@ -3747,6 +3980,7 @@
       <c r="D94" s="4" t="s">
         <v>189</v>
       </c>
+      <c r="G94" s="2"/>
       <c r="N94" t="s">
         <v>22</v>
       </c>
@@ -3767,6 +4001,9 @@
       <c r="D95" s="4" t="s">
         <v>191</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O95" s="2" t="s">
         <v>457</v>
       </c>
@@ -3784,6 +4021,9 @@
       <c r="D96" s="4" t="s">
         <v>193</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O96" s="2" t="s">
         <v>439</v>
       </c>
@@ -3801,6 +4041,7 @@
       <c r="D97" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="G97" s="2"/>
       <c r="N97" t="s">
         <v>22</v>
       </c>
@@ -3821,6 +4062,7 @@
       <c r="D98" s="4" t="s">
         <v>197</v>
       </c>
+      <c r="G98" s="2"/>
       <c r="O98" s="2" t="s">
         <v>440</v>
       </c>
@@ -3838,6 +4080,9 @@
       <c r="D99" s="4" t="s">
         <v>199</v>
       </c>
+      <c r="G99" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O99" s="2" t="s">
         <v>441</v>
       </c>
@@ -3855,6 +4100,7 @@
       <c r="D100" s="4" t="s">
         <v>201</v>
       </c>
+      <c r="G100" s="2"/>
       <c r="O100" s="2" t="s">
         <v>441</v>
       </c>
@@ -3872,6 +4118,7 @@
       <c r="D101" s="4" t="s">
         <v>203</v>
       </c>
+      <c r="G101" s="2"/>
       <c r="N101" t="s">
         <v>22</v>
       </c>
@@ -3892,6 +4139,7 @@
       <c r="D102" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G102" s="2"/>
       <c r="N102" t="s">
         <v>22</v>
       </c>
@@ -3912,6 +4160,9 @@
       <c r="D103" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G103" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O103" s="2" t="s">
         <v>442</v>
       </c>
@@ -3929,6 +4180,9 @@
       <c r="D104" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G104" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O104" s="2" t="s">
         <v>461</v>
       </c>
@@ -3946,6 +4200,7 @@
       <c r="D105" s="4" t="s">
         <v>210</v>
       </c>
+      <c r="G105" s="2"/>
       <c r="O105" s="2" t="s">
         <v>461</v>
       </c>
@@ -3963,6 +4218,7 @@
       <c r="D106" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G106" s="2"/>
       <c r="N106" t="s">
         <v>22</v>
       </c>
@@ -3983,6 +4239,7 @@
       <c r="D107" s="4" t="s">
         <v>213</v>
       </c>
+      <c r="G107" s="2"/>
       <c r="O107" s="2" t="s">
         <v>462</v>
       </c>
@@ -4000,6 +4257,9 @@
       <c r="D108" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G108" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O108" s="2" t="s">
         <v>463</v>
       </c>
@@ -4017,6 +4277,7 @@
       <c r="D109" s="4" t="s">
         <v>216</v>
       </c>
+      <c r="G109" s="2"/>
       <c r="O109" s="2" t="s">
         <v>23</v>
       </c>
@@ -4034,6 +4295,7 @@
       <c r="D110" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G110" s="2"/>
       <c r="O110" s="2" t="s">
         <v>443</v>
       </c>
@@ -4051,6 +4313,7 @@
       <c r="D111" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G111" s="2"/>
       <c r="O111" s="2" t="s">
         <v>464</v>
       </c>
@@ -4068,6 +4331,7 @@
       <c r="D112" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G112" s="2"/>
       <c r="O112" s="2" t="s">
         <v>463</v>
       </c>
@@ -4085,6 +4349,7 @@
       <c r="D113" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G113" s="2"/>
       <c r="O113" s="2" t="s">
         <v>23</v>
       </c>
@@ -4102,6 +4367,7 @@
       <c r="D114" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G114" s="2"/>
       <c r="O114" s="2" t="s">
         <v>465</v>
       </c>
@@ -4119,6 +4385,7 @@
       <c r="D115" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="G115" s="2"/>
       <c r="O115" s="2" t="s">
         <v>466</v>
       </c>
@@ -4136,6 +4403,7 @@
       <c r="D116" s="4" t="s">
         <v>225</v>
       </c>
+      <c r="G116" s="2"/>
       <c r="N116" t="s">
         <v>22</v>
       </c>
@@ -4156,6 +4424,7 @@
       <c r="D117" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G117" s="2"/>
       <c r="O117" s="2" t="s">
         <v>467</v>
       </c>
@@ -4173,6 +4442,9 @@
       <c r="D118" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G118" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O118" s="2" t="s">
         <v>444</v>
       </c>
@@ -4190,6 +4462,7 @@
       <c r="D119" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G119" s="2"/>
       <c r="O119" s="2" t="s">
         <v>468</v>
       </c>
@@ -4207,6 +4480,7 @@
       <c r="D120" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="G120" s="2"/>
       <c r="N120" t="s">
         <v>22</v>
       </c>
@@ -4227,6 +4501,7 @@
       <c r="D121" s="4" t="s">
         <v>233</v>
       </c>
+      <c r="G121" s="2"/>
       <c r="N121" t="s">
         <v>22</v>
       </c>
@@ -4247,6 +4522,9 @@
       <c r="D122" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="G122" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N122" t="s">
         <v>22</v>
       </c>
@@ -4267,6 +4545,9 @@
       <c r="D123" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G123" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N123" t="s">
         <v>22</v>
       </c>
@@ -4287,6 +4568,9 @@
       <c r="D124" s="4" t="s">
         <v>238</v>
       </c>
+      <c r="G124" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O124" s="2" t="s">
         <v>23</v>
       </c>
@@ -4304,6 +4588,9 @@
       <c r="D125" s="4" t="s">
         <v>240</v>
       </c>
+      <c r="G125" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N125" t="s">
         <v>22</v>
       </c>
@@ -4324,6 +4611,9 @@
       <c r="D126" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="G126" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N126" t="s">
         <v>22</v>
       </c>
@@ -4344,6 +4634,9 @@
       <c r="D127" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="G127" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O127" s="2" t="s">
         <v>23</v>
       </c>
@@ -4361,6 +4654,9 @@
       <c r="D128" s="4" t="s">
         <v>244</v>
       </c>
+      <c r="G128" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O128" s="2" t="s">
         <v>23</v>
       </c>
@@ -4378,6 +4674,7 @@
       <c r="D129" s="4" t="s">
         <v>246</v>
       </c>
+      <c r="G129" s="2"/>
       <c r="N129" t="s">
         <v>22</v>
       </c>
@@ -4398,6 +4695,9 @@
       <c r="D130" s="4" t="s">
         <v>248</v>
       </c>
+      <c r="G130" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O130" s="2" t="s">
         <v>469</v>
       </c>
@@ -4415,6 +4715,9 @@
       <c r="D131" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G131" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N131" t="s">
         <v>22</v>
       </c>
@@ -4435,6 +4738,7 @@
       <c r="D132" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="G132" s="2"/>
       <c r="N132" t="s">
         <v>22</v>
       </c>
@@ -4455,6 +4759,9 @@
       <c r="D133" s="6" t="s">
         <v>254</v>
       </c>
+      <c r="G133" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N133" t="s">
         <v>22</v>
       </c>
@@ -4475,6 +4782,9 @@
       <c r="D134" s="6" t="s">
         <v>256</v>
       </c>
+      <c r="G134" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N134" t="s">
         <v>22</v>
       </c>
@@ -4495,6 +4805,9 @@
       <c r="D135" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="G135" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="O135" s="2" t="s">
         <v>456</v>
       </c>
@@ -4512,6 +4825,9 @@
       <c r="D136" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="G136" s="2" t="s">
+        <v>493</v>
+      </c>
       <c r="O136" s="2" t="s">
         <v>470</v>
       </c>
@@ -4529,6 +4845,7 @@
       <c r="D137" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G137" s="2"/>
       <c r="N137" s="8" t="s">
         <v>22</v>
       </c>
@@ -4549,6 +4866,7 @@
       <c r="D138" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G138" s="2"/>
       <c r="N138" s="8" t="s">
         <v>22</v>
       </c>
@@ -4569,6 +4887,9 @@
       <c r="D139" s="6" t="s">
         <v>262</v>
       </c>
+      <c r="G139" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O139" s="2" t="s">
         <v>439</v>
       </c>
@@ -4586,6 +4907,9 @@
       <c r="D140" s="6" t="s">
         <v>264</v>
       </c>
+      <c r="G140" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N140" s="8" t="s">
         <v>22</v>
       </c>
@@ -4606,6 +4930,7 @@
       <c r="D141" s="6" t="s">
         <v>266</v>
       </c>
+      <c r="G141" s="2"/>
       <c r="N141" s="8" t="s">
         <v>22</v>
       </c>
@@ -4629,6 +4954,9 @@
       <c r="E142" s="4" t="s">
         <v>269</v>
       </c>
+      <c r="G142" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O142" s="2" t="s">
         <v>470</v>
       </c>
@@ -4652,6 +4980,9 @@
       <c r="E143" s="4" t="s">
         <v>273</v>
       </c>
+      <c r="G143" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N143" s="8" t="s">
         <v>22</v>
       </c>
@@ -4672,6 +5003,7 @@
       <c r="D144" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G144" s="2"/>
       <c r="O144" s="2" t="s">
         <v>470</v>
       </c>
@@ -4689,6 +5021,9 @@
       <c r="D145" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G145" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O145" s="2" t="s">
         <v>470</v>
       </c>
@@ -4706,6 +5041,7 @@
       <c r="D146" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G146" s="2"/>
       <c r="O146" s="2" t="s">
         <v>470</v>
       </c>
@@ -4723,6 +5059,7 @@
       <c r="D147" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G147" s="2"/>
       <c r="O147" s="2" t="s">
         <v>470</v>
       </c>
@@ -4740,6 +5077,7 @@
       <c r="D148" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G148" s="2"/>
       <c r="N148" s="8" t="s">
         <v>22</v>
       </c>
@@ -4760,6 +5098,7 @@
       <c r="D149" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G149" s="2"/>
       <c r="N149" s="8" t="s">
         <v>22</v>
       </c>
@@ -4780,6 +5119,9 @@
       <c r="D150" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G150" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O150" s="2" t="s">
         <v>470</v>
       </c>
@@ -4797,6 +5139,9 @@
       <c r="D151" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G151" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O151" s="2" t="s">
         <v>471</v>
       </c>
@@ -4814,6 +5159,7 @@
       <c r="D152" s="4" t="s">
         <v>283</v>
       </c>
+      <c r="G152" s="2"/>
       <c r="N152" s="8" t="s">
         <v>22</v>
       </c>
@@ -4834,6 +5180,7 @@
       <c r="D153" s="4" t="s">
         <v>285</v>
       </c>
+      <c r="G153" s="2"/>
       <c r="N153" s="8" t="s">
         <v>22</v>
       </c>
@@ -4854,6 +5201,9 @@
       <c r="D154" s="4" t="s">
         <v>287</v>
       </c>
+      <c r="G154" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N154" s="4"/>
       <c r="O154" s="4" t="s">
         <v>288</v>
@@ -4872,6 +5222,9 @@
       <c r="D155" s="4" t="s">
         <v>290</v>
       </c>
+      <c r="G155" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O155" s="2" t="s">
         <v>472</v>
       </c>
@@ -4889,6 +5242,7 @@
       <c r="D156" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="G156" s="2"/>
       <c r="N156" s="8" t="s">
         <v>22</v>
       </c>
@@ -4909,6 +5263,7 @@
       <c r="D157" s="4" t="s">
         <v>294</v>
       </c>
+      <c r="G157" s="2"/>
       <c r="N157" s="8" t="s">
         <v>22</v>
       </c>
@@ -4929,6 +5284,9 @@
       <c r="D158" s="4" t="s">
         <v>296</v>
       </c>
+      <c r="G158" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N158" s="8" t="s">
         <v>22</v>
       </c>
@@ -4949,6 +5307,9 @@
       <c r="D159" s="4" t="s">
         <v>298</v>
       </c>
+      <c r="G159" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N159" s="8" t="s">
         <v>22</v>
       </c>
@@ -4969,6 +5330,9 @@
       <c r="D160" s="4" t="s">
         <v>300</v>
       </c>
+      <c r="G160" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N160" s="8" t="s">
         <v>22</v>
       </c>
@@ -4989,6 +5353,9 @@
       <c r="D161" s="4" t="s">
         <v>302</v>
       </c>
+      <c r="G161" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N161" s="8" t="s">
         <v>22</v>
       </c>
@@ -5009,6 +5376,9 @@
       <c r="D162" s="4" t="s">
         <v>304</v>
       </c>
+      <c r="G162" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O162" s="2" t="s">
         <v>473</v>
       </c>
@@ -5026,6 +5396,9 @@
       <c r="D163" s="4" t="s">
         <v>306</v>
       </c>
+      <c r="G163" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N163" s="8" t="s">
         <v>22</v>
       </c>
@@ -5046,6 +5419,7 @@
       <c r="D164" s="4" t="s">
         <v>308</v>
       </c>
+      <c r="G164" s="2"/>
       <c r="O164" s="2" t="s">
         <v>23</v>
       </c>
@@ -5063,6 +5437,9 @@
       <c r="D165" s="4" t="s">
         <v>310</v>
       </c>
+      <c r="G165" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O165" s="2" t="s">
         <v>23</v>
       </c>
@@ -5080,6 +5457,7 @@
       <c r="D166" s="4" t="s">
         <v>312</v>
       </c>
+      <c r="G166" s="2"/>
       <c r="N166" s="8" t="s">
         <v>22</v>
       </c>
@@ -5100,6 +5478,7 @@
       <c r="D167" s="4" t="s">
         <v>314</v>
       </c>
+      <c r="G167" s="2"/>
       <c r="O167" s="2" t="s">
         <v>23</v>
       </c>
@@ -5117,6 +5496,9 @@
       <c r="D168" s="4" t="s">
         <v>316</v>
       </c>
+      <c r="G168" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O168" s="2" t="s">
         <v>23</v>
       </c>
@@ -5134,6 +5516,9 @@
       <c r="D169" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="G169" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N169" s="8" t="s">
         <v>22</v>
       </c>
@@ -5154,6 +5539,7 @@
       <c r="D170" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="G170" s="2"/>
       <c r="N170" s="8" t="s">
         <v>22</v>
       </c>
@@ -5174,6 +5560,9 @@
       <c r="D171" s="4" t="s">
         <v>321</v>
       </c>
+      <c r="G171" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N171" s="8" t="s">
         <v>22</v>
       </c>
@@ -5194,6 +5583,9 @@
       <c r="D172" s="4" t="s">
         <v>323</v>
       </c>
+      <c r="G172" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N172" s="8" t="s">
         <v>22</v>
       </c>
@@ -5214,6 +5606,9 @@
       <c r="D173" s="4" t="s">
         <v>325</v>
       </c>
+      <c r="G173" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N173" s="8" t="s">
         <v>22</v>
       </c>
@@ -5234,6 +5629,9 @@
       <c r="D174" s="4" t="s">
         <v>327</v>
       </c>
+      <c r="G174" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N174" s="8" t="s">
         <v>22</v>
       </c>
@@ -5254,6 +5652,9 @@
       <c r="D175" s="4" t="s">
         <v>329</v>
       </c>
+      <c r="G175" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O175" s="2" t="s">
         <v>474</v>
       </c>
@@ -5271,6 +5672,9 @@
       <c r="D176" s="4" t="s">
         <v>331</v>
       </c>
+      <c r="G176" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O176" s="2" t="s">
         <v>474</v>
       </c>
@@ -5288,6 +5692,7 @@
       <c r="D177" s="4" t="s">
         <v>333</v>
       </c>
+      <c r="G177" s="2"/>
       <c r="O177" s="2" t="s">
         <v>474</v>
       </c>
@@ -5305,6 +5710,7 @@
       <c r="D178" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="G178" s="2"/>
       <c r="O178" s="2" t="s">
         <v>23</v>
       </c>
@@ -5322,6 +5728,9 @@
       <c r="D179" s="4" t="s">
         <v>337</v>
       </c>
+      <c r="G179" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N179" s="8" t="s">
         <v>22</v>
       </c>
@@ -5342,6 +5751,7 @@
       <c r="D180" s="4" t="s">
         <v>339</v>
       </c>
+      <c r="G180" s="2"/>
       <c r="O180" s="2" t="s">
         <v>474</v>
       </c>
@@ -5359,6 +5769,9 @@
       <c r="D181" s="4" t="s">
         <v>341</v>
       </c>
+      <c r="G181" s="2" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
@@ -5373,6 +5786,7 @@
       <c r="D182" s="4" t="s">
         <v>343</v>
       </c>
+      <c r="G182" s="2"/>
       <c r="N182" s="8" t="s">
         <v>22</v>
       </c>
@@ -5393,6 +5807,7 @@
       <c r="D183" s="4" t="s">
         <v>345</v>
       </c>
+      <c r="G183" s="2"/>
       <c r="N183" s="8" t="s">
         <v>22</v>
       </c>
@@ -5413,6 +5828,7 @@
       <c r="D184" s="4" t="s">
         <v>347</v>
       </c>
+      <c r="G184" s="2"/>
       <c r="N184" s="8" t="s">
         <v>22</v>
       </c>
@@ -5433,6 +5849,9 @@
       <c r="D185" s="4" t="s">
         <v>349</v>
       </c>
+      <c r="G185" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N185" s="8" t="s">
         <v>22</v>
       </c>
@@ -5453,6 +5872,9 @@
       <c r="D186" s="4" t="s">
         <v>351</v>
       </c>
+      <c r="G186" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N186" s="8" t="s">
         <v>22</v>
       </c>
@@ -5473,6 +5895,9 @@
       <c r="D187" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="G187" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N187" s="8" t="s">
         <v>22</v>
       </c>
@@ -5493,6 +5918,9 @@
       <c r="D188" s="4" t="s">
         <v>355</v>
       </c>
+      <c r="G188" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N188" s="8" t="s">
         <v>22</v>
       </c>
@@ -5513,6 +5941,9 @@
       <c r="D189" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="G189" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N189" s="8" t="s">
         <v>22</v>
       </c>
@@ -5533,6 +5964,9 @@
       <c r="D190" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="G190" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N190" s="8" t="s">
         <v>22</v>
       </c>
@@ -5553,6 +5987,9 @@
       <c r="D191" s="4" t="s">
         <v>359</v>
       </c>
+      <c r="G191" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N191" s="8" t="s">
         <v>22</v>
       </c>
@@ -5573,6 +6010,9 @@
       <c r="D192" s="4" t="s">
         <v>361</v>
       </c>
+      <c r="G192" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N192" s="8" t="s">
         <v>22</v>
       </c>
@@ -5593,6 +6033,9 @@
       <c r="D193" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="G193" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N193" s="8" t="s">
         <v>22</v>
       </c>
@@ -5613,6 +6056,9 @@
       <c r="D194" s="4" t="s">
         <v>365</v>
       </c>
+      <c r="G194" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N194" s="8" t="s">
         <v>22</v>
       </c>
@@ -5636,6 +6082,9 @@
       <c r="E195" s="4" t="s">
         <v>368</v>
       </c>
+      <c r="G195" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O195" s="2" t="s">
         <v>475</v>
       </c>
@@ -5653,6 +6102,9 @@
       <c r="D196" s="4" t="s">
         <v>370</v>
       </c>
+      <c r="G196" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N196" s="8" t="s">
         <v>22</v>
       </c>
@@ -5673,6 +6125,7 @@
       <c r="D197" s="4" t="s">
         <v>372</v>
       </c>
+      <c r="G197" s="2"/>
       <c r="N197" s="8" t="s">
         <v>22</v>
       </c>
@@ -5693,6 +6146,9 @@
       <c r="D198" s="4" t="s">
         <v>374</v>
       </c>
+      <c r="G198" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N198" s="8" t="s">
         <v>22</v>
       </c>
@@ -5713,6 +6169,9 @@
       <c r="D199" s="4" t="s">
         <v>376</v>
       </c>
+      <c r="G199" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N199" s="8" t="s">
         <v>22</v>
       </c>
@@ -5733,6 +6192,9 @@
       <c r="D200" s="4" t="s">
         <v>378</v>
       </c>
+      <c r="G200" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N200" s="8" t="s">
         <v>22</v>
       </c>
@@ -5740,7 +6202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>197</v>
       </c>
@@ -5752,6 +6214,9 @@
       </c>
       <c r="D201" s="4" t="s">
         <v>380</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>494</v>
       </c>
       <c r="N201" s="8" t="s">
         <v>22</v>
@@ -5773,6 +6238,9 @@
       <c r="D202" s="4" t="s">
         <v>382</v>
       </c>
+      <c r="G202" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N202" s="8" t="s">
         <v>22</v>
       </c>
@@ -5793,6 +6261,9 @@
       <c r="D203" s="4" t="s">
         <v>384</v>
       </c>
+      <c r="G203" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N203" s="8" t="s">
         <v>22</v>
       </c>
@@ -5800,7 +6271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>200</v>
       </c>
@@ -5813,11 +6284,14 @@
       <c r="D204" s="4" t="s">
         <v>386</v>
       </c>
+      <c r="G204" s="2" t="s">
+        <v>495</v>
+      </c>
       <c r="O204" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>201</v>
       </c>
@@ -5829,6 +6303,9 @@
       </c>
       <c r="D205" s="4" t="s">
         <v>353</v>
+      </c>
+      <c r="G205" s="2" t="s">
+        <v>496</v>
       </c>
       <c r="N205" s="8" t="s">
         <v>22</v>
@@ -5850,6 +6327,7 @@
       <c r="D206" s="4" t="s">
         <v>389</v>
       </c>
+      <c r="G206" s="2"/>
       <c r="N206" s="8" t="s">
         <v>22</v>
       </c>
@@ -5870,6 +6348,9 @@
       <c r="D207" s="4" t="s">
         <v>391</v>
       </c>
+      <c r="G207" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N207" s="8" t="s">
         <v>22</v>
       </c>
@@ -5896,7 +6377,7 @@
       <c r="E208" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="G208" s="9" t="s">
+      <c r="G208" s="4" t="s">
         <v>483</v>
       </c>
       <c r="O208" s="2" t="s">
@@ -5919,6 +6400,9 @@
       <c r="E209" s="4" t="s">
         <v>398</v>
       </c>
+      <c r="G209" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O209" s="2" t="s">
         <v>447</v>
       </c>
@@ -5936,6 +6420,9 @@
       <c r="D210" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="G210" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="O210" s="2" t="s">
         <v>23</v>
       </c>
@@ -5956,6 +6443,7 @@
       <c r="D211" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="G211" s="2"/>
       <c r="O211" s="2" t="s">
         <v>445</v>
       </c>
@@ -5976,6 +6464,7 @@
       <c r="E212" s="4" t="s">
         <v>406</v>
       </c>
+      <c r="G212" s="2"/>
       <c r="O212" s="2" t="s">
         <v>447</v>
       </c>
@@ -5996,9 +6485,7 @@
       <c r="E213" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="G213" s="9" t="s">
-        <v>483</v>
-      </c>
+      <c r="G213" s="4"/>
       <c r="O213" s="2" t="s">
         <v>448</v>
       </c>
@@ -6019,6 +6506,7 @@
       <c r="E214" s="4" t="s">
         <v>412</v>
       </c>
+      <c r="G214" s="2"/>
       <c r="O214" s="2" t="s">
         <v>448</v>
       </c>
@@ -6036,6 +6524,9 @@
       <c r="D215" s="4" t="s">
         <v>405</v>
       </c>
+      <c r="G215" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="O215" s="2" t="s">
         <v>447</v>
       </c>
@@ -6056,6 +6547,7 @@
       <c r="D216" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="G216" s="2"/>
       <c r="N216" s="8" t="s">
         <v>22</v>
       </c>
@@ -6076,6 +6568,7 @@
       <c r="D217" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="G217" s="2"/>
       <c r="N217" s="8" t="s">
         <v>22</v>
       </c>
@@ -6096,6 +6589,9 @@
       <c r="D218" s="4" t="s">
         <v>419</v>
       </c>
+      <c r="G218" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="N218" s="8" t="s">
         <v>22</v>
       </c>
@@ -6116,6 +6612,9 @@
       <c r="D219" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="G219" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O219" s="2" t="s">
         <v>449</v>
       </c>
@@ -6133,6 +6632,9 @@
       <c r="D220" s="4" t="s">
         <v>422</v>
       </c>
+      <c r="G220" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="O220" s="2" t="s">
         <v>450</v>
       </c>
@@ -6153,6 +6655,7 @@
       <c r="E221" s="4" t="s">
         <v>424</v>
       </c>
+      <c r="G221" s="2"/>
       <c r="O221" s="2" t="s">
         <v>445</v>
       </c>
@@ -6176,6 +6679,7 @@
       <c r="E222" s="4" t="s">
         <v>428</v>
       </c>
+      <c r="G222" s="2"/>
       <c r="O222" s="2" t="s">
         <v>448</v>
       </c>
@@ -6196,6 +6700,7 @@
       <c r="E223" s="4" t="s">
         <v>430</v>
       </c>
+      <c r="G223" s="2"/>
       <c r="O223" s="2" t="s">
         <v>477</v>
       </c>
@@ -6213,6 +6718,7 @@
       <c r="D224" s="4" t="s">
         <v>432</v>
       </c>
+      <c r="G224" s="2"/>
       <c r="O224" s="2" t="s">
         <v>439</v>
       </c>

</xml_diff>

<commit_message>
Tested req 45 to 88
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samridhsingh/Documents/cse3310-sp25-002-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA529746-D51B-2C42-B1A7-21667C82A392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BF040A-B432-C342-83EC-BE3D326AA56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="6520" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="487">
   <si>
     <t>Tested By</t>
   </si>
@@ -1494,6 +1494,15 @@
   </si>
   <si>
     <t>Test 1: Step 4</t>
+  </si>
+  <si>
+    <t>Test Working</t>
+  </si>
+  <si>
+    <t>Test working</t>
+  </si>
+  <si>
+    <t>Uable to Test</t>
   </si>
 </sst>
 </file>
@@ -1892,8 +1901,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G212" sqref="G212"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1997,6 +2006,9 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
       <c r="N5" t="s">
         <v>22</v>
       </c>
@@ -2017,6 +2029,9 @@
       <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
       <c r="N6" t="s">
         <v>22</v>
       </c>
@@ -2105,6 +2120,9 @@
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
       <c r="N11" t="s">
         <v>22</v>
       </c>
@@ -2125,6 +2143,9 @@
       <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
       <c r="N12" t="s">
         <v>22</v>
       </c>
@@ -2179,6 +2200,9 @@
       <c r="D15" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
       <c r="N15" t="s">
         <v>22</v>
       </c>
@@ -2199,6 +2223,9 @@
       <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
       <c r="N16" t="s">
         <v>22</v>
       </c>
@@ -2219,6 +2246,9 @@
       <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
       <c r="N17" t="s">
         <v>22</v>
       </c>
@@ -2239,6 +2269,9 @@
       <c r="D18" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
       <c r="N18" t="s">
         <v>22</v>
       </c>
@@ -2259,6 +2292,9 @@
       <c r="D19" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
       <c r="N19" t="s">
         <v>22</v>
       </c>
@@ -2279,6 +2315,9 @@
       <c r="D20" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
       <c r="N20" t="s">
         <v>22</v>
       </c>
@@ -2299,6 +2338,9 @@
       <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
       <c r="N21" t="s">
         <v>22</v>
       </c>
@@ -2319,6 +2361,9 @@
       <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
       <c r="N22" t="s">
         <v>22</v>
       </c>
@@ -2339,6 +2384,9 @@
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
       <c r="N23" t="s">
         <v>22</v>
       </c>
@@ -2393,6 +2441,9 @@
       <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
       <c r="N26" t="s">
         <v>22</v>
       </c>
@@ -2412,6 +2463,9 @@
       </c>
       <c r="D27" s="4" t="s">
         <v>55</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
       </c>
       <c r="N27" t="s">
         <v>22</v>
@@ -2433,6 +2487,9 @@
       <c r="D28" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
       <c r="N28" t="s">
         <v>22</v>
       </c>
@@ -2453,6 +2510,9 @@
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
       <c r="N29" t="s">
         <v>22</v>
       </c>
@@ -2490,6 +2550,9 @@
       <c r="D31" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
       <c r="N31" t="s">
         <v>22</v>
       </c>
@@ -2510,6 +2573,9 @@
       <c r="D32" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
       <c r="N32" t="s">
         <v>22</v>
       </c>
@@ -2530,6 +2596,9 @@
       <c r="D33" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="I33" t="s">
+        <v>22</v>
+      </c>
       <c r="N33" t="s">
         <v>22</v>
       </c>
@@ -2567,6 +2636,9 @@
       <c r="D35" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="I35" t="s">
+        <v>22</v>
+      </c>
       <c r="N35" t="s">
         <v>22</v>
       </c>
@@ -2587,6 +2659,9 @@
       <c r="D36" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
       <c r="N36" t="s">
         <v>22</v>
       </c>
@@ -2607,6 +2682,9 @@
       <c r="D37" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
       <c r="N37" t="s">
         <v>22</v>
       </c>
@@ -2627,6 +2705,9 @@
       <c r="D38" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
       <c r="N38" t="s">
         <v>22</v>
       </c>
@@ -2647,6 +2728,9 @@
       <c r="D39" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="I39" t="s">
+        <v>22</v>
+      </c>
       <c r="N39" t="s">
         <v>22</v>
       </c>
@@ -2684,6 +2768,9 @@
       <c r="D41" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="I41" t="s">
+        <v>22</v>
+      </c>
       <c r="N41" t="s">
         <v>22</v>
       </c>
@@ -2704,6 +2791,9 @@
       <c r="D42" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="I42" t="s">
+        <v>22</v>
+      </c>
       <c r="N42" t="s">
         <v>22</v>
       </c>
@@ -2724,6 +2814,9 @@
       <c r="D43" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="I43" t="s">
+        <v>22</v>
+      </c>
       <c r="N43" t="s">
         <v>22</v>
       </c>
@@ -2778,6 +2871,9 @@
       <c r="D46" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="I46" t="s">
+        <v>22</v>
+      </c>
       <c r="N46" t="s">
         <v>22</v>
       </c>
@@ -2798,6 +2894,9 @@
       <c r="D47" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="I47" t="s">
+        <v>22</v>
+      </c>
       <c r="N47" t="s">
         <v>22</v>
       </c>
@@ -2818,6 +2917,9 @@
       <c r="D48" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="I48" t="s">
+        <v>22</v>
+      </c>
       <c r="N48" t="s">
         <v>22</v>
       </c>
@@ -2838,6 +2940,9 @@
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="I49" t="s">
+        <v>22</v>
+      </c>
       <c r="N49" t="s">
         <v>22</v>
       </c>
@@ -2858,6 +2963,9 @@
       <c r="D50" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="I50" t="s">
+        <v>22</v>
+      </c>
       <c r="N50" t="s">
         <v>22</v>
       </c>
@@ -2878,6 +2986,9 @@
       <c r="D51" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="I51" t="s">
+        <v>22</v>
+      </c>
       <c r="N51" t="s">
         <v>22</v>
       </c>
@@ -2898,6 +3009,9 @@
       <c r="D52" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="I52" t="s">
+        <v>22</v>
+      </c>
       <c r="O52" s="2" t="s">
         <v>479</v>
       </c>
@@ -2918,6 +3032,9 @@
       <c r="E53" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="I53" t="s">
+        <v>484</v>
+      </c>
       <c r="O53" s="2" t="s">
         <v>451</v>
       </c>
@@ -2938,6 +3055,9 @@
       <c r="E54" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="I54" t="s">
+        <v>485</v>
+      </c>
       <c r="O54" s="2" t="s">
         <v>452</v>
       </c>
@@ -2958,6 +3078,9 @@
       <c r="E55" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="I55" t="s">
+        <v>485</v>
+      </c>
       <c r="O55" s="2" t="s">
         <v>452</v>
       </c>
@@ -2978,6 +3101,9 @@
       <c r="E56" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I56" t="s">
+        <v>484</v>
+      </c>
       <c r="O56" s="2" t="s">
         <v>451</v>
       </c>
@@ -2998,6 +3124,9 @@
       <c r="E57" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="I57" t="s">
+        <v>484</v>
+      </c>
       <c r="O57" s="2" t="s">
         <v>451</v>
       </c>
@@ -3018,6 +3147,9 @@
       <c r="E58" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="I58" t="s">
+        <v>22</v>
+      </c>
       <c r="O58" s="2" t="s">
         <v>443</v>
       </c>
@@ -3038,6 +3170,9 @@
       <c r="E59" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="I59" t="s">
+        <v>484</v>
+      </c>
       <c r="O59" s="2" t="s">
         <v>437</v>
       </c>
@@ -3058,6 +3193,9 @@
       <c r="E60" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="I60" t="s">
+        <v>486</v>
+      </c>
       <c r="O60" s="2" t="s">
         <v>451</v>
       </c>
@@ -3078,6 +3216,9 @@
       <c r="E61" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I61" t="s">
+        <v>484</v>
+      </c>
       <c r="O61" s="2" t="s">
         <v>451</v>
       </c>
@@ -3098,6 +3239,9 @@
       <c r="E62" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I62" t="s">
+        <v>22</v>
+      </c>
       <c r="N62" t="s">
         <v>22</v>
       </c>
@@ -3124,6 +3268,9 @@
       <c r="G63" s="2" t="s">
         <v>482</v>
       </c>
+      <c r="I63" t="s">
+        <v>22</v>
+      </c>
       <c r="N63" t="s">
         <v>22</v>
       </c>
@@ -3147,6 +3294,9 @@
       <c r="E64" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I64" t="s">
+        <v>22</v>
+      </c>
       <c r="N64" t="s">
         <v>22</v>
       </c>
@@ -3170,6 +3320,9 @@
       <c r="E65" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I65" t="s">
+        <v>22</v>
+      </c>
       <c r="N65" t="s">
         <v>22</v>
       </c>
@@ -3193,6 +3346,9 @@
       <c r="E66" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I66" t="s">
+        <v>22</v>
+      </c>
       <c r="N66" t="s">
         <v>22</v>
       </c>
@@ -3216,6 +3372,9 @@
       <c r="E67" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I67" t="s">
+        <v>484</v>
+      </c>
       <c r="O67" s="2" t="s">
         <v>434</v>
       </c>
@@ -3236,6 +3395,9 @@
       <c r="E68" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I68" t="s">
+        <v>484</v>
+      </c>
       <c r="O68" s="2" t="s">
         <v>453</v>
       </c>
@@ -3256,6 +3418,9 @@
       <c r="E69" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I69" t="s">
+        <v>22</v>
+      </c>
       <c r="N69" t="s">
         <v>22</v>
       </c>
@@ -3279,6 +3444,9 @@
       <c r="E70" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I70" t="s">
+        <v>22</v>
+      </c>
       <c r="N70" t="s">
         <v>22</v>
       </c>
@@ -3302,6 +3470,9 @@
       <c r="E71" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I71" t="s">
+        <v>22</v>
+      </c>
       <c r="N71" t="s">
         <v>22</v>
       </c>
@@ -3325,6 +3496,9 @@
       <c r="E72" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="I72" t="s">
+        <v>22</v>
+      </c>
       <c r="N72" t="s">
         <v>22</v>
       </c>
@@ -3345,6 +3519,9 @@
       <c r="D73" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="I73" t="s">
+        <v>22</v>
+      </c>
       <c r="O73" s="2" t="s">
         <v>454</v>
       </c>
@@ -3362,6 +3539,9 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="I74" t="s">
+        <v>22</v>
+      </c>
       <c r="O74" s="2" t="s">
         <v>23</v>
       </c>
@@ -3379,6 +3559,9 @@
       <c r="D75" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="I75" t="s">
+        <v>486</v>
+      </c>
       <c r="O75" s="2" t="s">
         <v>456</v>
       </c>
@@ -3396,6 +3579,9 @@
       <c r="D76" s="4" t="s">
         <v>147</v>
       </c>
+      <c r="I76" t="s">
+        <v>484</v>
+      </c>
       <c r="O76" s="2" t="s">
         <v>455</v>
       </c>
@@ -3413,6 +3599,9 @@
       <c r="D77" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="I77" t="s">
+        <v>22</v>
+      </c>
       <c r="N77" t="s">
         <v>22</v>
       </c>
@@ -3433,6 +3622,9 @@
       <c r="D78" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="I78" t="s">
+        <v>22</v>
+      </c>
       <c r="N78" t="s">
         <v>22</v>
       </c>
@@ -3453,6 +3645,9 @@
       <c r="D79" s="4" t="s">
         <v>153</v>
       </c>
+      <c r="I79" t="s">
+        <v>22</v>
+      </c>
       <c r="N79" t="s">
         <v>22</v>
       </c>
@@ -3473,6 +3668,9 @@
       <c r="D80" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="I80" t="s">
+        <v>22</v>
+      </c>
       <c r="N80" t="s">
         <v>22</v>
       </c>
@@ -3493,6 +3691,9 @@
       <c r="D81" s="4" t="s">
         <v>157</v>
       </c>
+      <c r="I81" t="s">
+        <v>22</v>
+      </c>
       <c r="N81" t="s">
         <v>22</v>
       </c>
@@ -3513,6 +3714,9 @@
       <c r="D82" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="I82" t="s">
+        <v>22</v>
+      </c>
       <c r="N82" t="s">
         <v>22</v>
       </c>
@@ -3533,6 +3737,9 @@
       <c r="D83" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="I83" t="s">
+        <v>22</v>
+      </c>
       <c r="O83" s="2" t="s">
         <v>455</v>
       </c>
@@ -3553,6 +3760,9 @@
       <c r="E84" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="I84" t="s">
+        <v>484</v>
+      </c>
       <c r="O84" s="2" t="s">
         <v>458</v>
       </c>
@@ -3573,6 +3783,9 @@
       <c r="E85" s="4" t="s">
         <v>167</v>
       </c>
+      <c r="I85" t="s">
+        <v>484</v>
+      </c>
       <c r="O85" s="2" t="s">
         <v>457</v>
       </c>
@@ -3593,6 +3806,9 @@
       <c r="E86" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="I86" t="s">
+        <v>486</v>
+      </c>
       <c r="O86" s="2" t="s">
         <v>459</v>
       </c>
@@ -3613,6 +3829,9 @@
       <c r="E87" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="I87" t="s">
+        <v>22</v>
+      </c>
       <c r="O87" s="2" t="s">
         <v>460</v>
       </c>
@@ -3630,6 +3849,9 @@
       <c r="D88" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="I88" t="s">
+        <v>22</v>
+      </c>
       <c r="N88" t="s">
         <v>22</v>
       </c>
@@ -3650,6 +3872,9 @@
       <c r="D89" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="I89" t="s">
+        <v>484</v>
+      </c>
       <c r="O89" s="2" t="s">
         <v>435</v>
       </c>
@@ -3670,6 +3895,9 @@
       <c r="E90" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="I90" t="s">
+        <v>486</v>
+      </c>
       <c r="O90" s="2" t="s">
         <v>436</v>
       </c>
@@ -3687,6 +3915,9 @@
       <c r="D91" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="I91" t="s">
+        <v>484</v>
+      </c>
       <c r="O91" s="2" t="s">
         <v>437</v>
       </c>
@@ -3707,6 +3938,9 @@
       <c r="E92" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="I92" t="s">
+        <v>484</v>
+      </c>
       <c r="O92" s="2" t="s">
         <v>438</v>
       </c>
@@ -3724,6 +3958,9 @@
       <c r="D93" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="I93" t="s">
+        <v>22</v>
+      </c>
       <c r="N93" t="s">
         <v>22</v>
       </c>
@@ -3743,6 +3980,9 @@
       </c>
       <c r="D94" s="4" t="s">
         <v>189</v>
+      </c>
+      <c r="I94" t="s">
+        <v>22</v>
       </c>
       <c r="N94" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Readded group 26 tests
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samridhsingh/Documents/cse3310-sp25-002-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BF040A-B432-C342-83EC-BE3D326AA56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E52164-2403-BE4F-B260-F4E6DE8A21CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="6520" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="1080" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="499">
   <si>
     <t>Tested By</t>
   </si>
@@ -1489,10 +1489,6 @@
     <t>The program will be compatible with the web browsers Chrome and Firefox.</t>
   </si>
   <si>
-    <t>Test 1 Step 3
-Note: This requirement was modified to exclude Safari as this is not on Fedora.</t>
-  </si>
-  <si>
     <t>Test 1: Step 4</t>
   </si>
   <si>
@@ -1503,6 +1499,46 @@
   </si>
   <si>
     <t>Uable to Test</t>
+  </si>
+  <si>
+    <t>Unable to test</t>
+  </si>
+  <si>
+    <t>Partially testable - may be observed by playing several games but full verfication would require code inspection</t>
+  </si>
+  <si>
+    <t>Unable to test - move evaluation is likely internal</t>
+  </si>
+  <si>
+    <t>Req might be too unclear to test.</t>
+  </si>
+  <si>
+    <t>Req might be too unclear as "fixed strategy" is not fully defined/</t>
+  </si>
+  <si>
+    <t>Req might be too unclear to test as "aggressively" is subjective.</t>
+  </si>
+  <si>
+    <t>Req might be too unclear to test. "Cautiously" is not precisely defined.</t>
+  </si>
+  <si>
+    <t>Test 1: Step 3
+Note: This requirement was modified to remove Safari as this is not on Fedora.</t>
+  </si>
+  <si>
+    <t>Unable to tsst</t>
+  </si>
+  <si>
+    <t>Will need multiple games to verify</t>
+  </si>
+  <si>
+    <t>Req. might be too unlcear to test. What is the state of the board?</t>
+  </si>
+  <si>
+    <t>Depends if the active game count is displayed</t>
+  </si>
+  <si>
+    <t>Req. might be too unlcear to test.What does if needed mean?</t>
   </si>
 </sst>
 </file>
@@ -1901,8 +1937,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2006,6 +2042,9 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
@@ -2029,6 +2068,9 @@
       <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I6" t="s">
         <v>22</v>
       </c>
@@ -2039,7 +2081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -2051,6 +2093,9 @@
       </c>
       <c r="D7" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>487</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>23</v>
@@ -2069,6 +2114,7 @@
       <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="G8" s="2"/>
       <c r="O8" s="2" t="s">
         <v>479</v>
       </c>
@@ -2086,6 +2132,7 @@
       <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G9" s="2"/>
       <c r="O9" s="2" t="s">
         <v>479</v>
       </c>
@@ -2103,6 +2150,7 @@
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G10" s="2"/>
       <c r="O10" s="2" t="s">
         <v>479</v>
       </c>
@@ -2120,6 +2168,9 @@
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I11" t="s">
         <v>22</v>
       </c>
@@ -2143,6 +2194,9 @@
       <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>488</v>
+      </c>
       <c r="I12" t="s">
         <v>22</v>
       </c>
@@ -2166,6 +2220,7 @@
       <c r="D13" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G13" s="2"/>
       <c r="O13" s="2" t="s">
         <v>480</v>
       </c>
@@ -2183,6 +2238,7 @@
       <c r="D14" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G14" s="2"/>
       <c r="O14" s="2" t="s">
         <v>479</v>
       </c>
@@ -2200,6 +2256,9 @@
       <c r="D15" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I15" t="s">
         <v>22</v>
       </c>
@@ -2223,6 +2282,9 @@
       <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I16" t="s">
         <v>22</v>
       </c>
@@ -2246,6 +2308,9 @@
       <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="G17" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I17" t="s">
         <v>22</v>
       </c>
@@ -2269,6 +2334,9 @@
       <c r="D18" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I18" t="s">
         <v>22</v>
       </c>
@@ -2292,6 +2360,9 @@
       <c r="D19" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="G19" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I19" t="s">
         <v>22</v>
       </c>
@@ -2315,6 +2386,9 @@
       <c r="D20" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I20" t="s">
         <v>22</v>
       </c>
@@ -2338,6 +2412,9 @@
       <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
@@ -2361,6 +2438,9 @@
       <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I22" t="s">
         <v>22</v>
       </c>
@@ -2384,6 +2464,9 @@
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I23" t="s">
         <v>22</v>
       </c>
@@ -2407,6 +2490,9 @@
       <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>489</v>
+      </c>
       <c r="O24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2424,6 +2510,9 @@
       <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>489</v>
+      </c>
       <c r="O25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2441,6 +2530,9 @@
       <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I26" t="s">
         <v>22</v>
       </c>
@@ -2463,6 +2555,9 @@
       </c>
       <c r="D27" s="4" t="s">
         <v>55</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>486</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -2487,6 +2582,9 @@
       <c r="D28" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I28" t="s">
         <v>22</v>
       </c>
@@ -2510,6 +2608,9 @@
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G29" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I29" t="s">
         <v>22</v>
       </c>
@@ -2520,7 +2621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -2532,6 +2633,9 @@
       </c>
       <c r="D30" s="4" t="s">
         <v>59</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>490</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>479</v>
@@ -2550,6 +2654,9 @@
       <c r="D31" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="G31" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I31" t="s">
         <v>22</v>
       </c>
@@ -2573,6 +2680,9 @@
       <c r="D32" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="G32" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I32" t="s">
         <v>22</v>
       </c>
@@ -2596,6 +2706,9 @@
       <c r="D33" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I33" t="s">
         <v>22</v>
       </c>
@@ -2619,6 +2732,7 @@
       <c r="D34" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G34" s="2"/>
       <c r="O34" s="2" t="s">
         <v>479</v>
       </c>
@@ -2636,6 +2750,9 @@
       <c r="D35" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="G35" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I35" t="s">
         <v>22</v>
       </c>
@@ -2659,6 +2776,9 @@
       <c r="D36" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="G36" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I36" t="s">
         <v>22</v>
       </c>
@@ -2682,6 +2802,9 @@
       <c r="D37" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="G37" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I37" t="s">
         <v>22</v>
       </c>
@@ -2705,6 +2828,9 @@
       <c r="D38" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="G38" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I38" t="s">
         <v>22</v>
       </c>
@@ -2728,6 +2854,9 @@
       <c r="D39" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="G39" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I39" t="s">
         <v>22</v>
       </c>
@@ -2751,6 +2880,7 @@
       <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="G40" s="2"/>
       <c r="O40" s="2" t="s">
         <v>479</v>
       </c>
@@ -2768,6 +2898,9 @@
       <c r="D41" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="G41" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I41" t="s">
         <v>22</v>
       </c>
@@ -2791,6 +2924,9 @@
       <c r="D42" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="G42" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I42" t="s">
         <v>22</v>
       </c>
@@ -2801,7 +2937,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -2814,6 +2950,9 @@
       <c r="D43" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="G43" s="2" t="s">
+        <v>491</v>
+      </c>
       <c r="I43" t="s">
         <v>22</v>
       </c>
@@ -2824,7 +2963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -2836,6 +2975,9 @@
       </c>
       <c r="D44" s="4" t="s">
         <v>83</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>492</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>23</v>
@@ -2854,6 +2996,7 @@
       <c r="D45" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="G45" s="2"/>
       <c r="O45" s="2" t="s">
         <v>479</v>
       </c>
@@ -2871,6 +3014,9 @@
       <c r="D46" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="G46" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I46" t="s">
         <v>22</v>
       </c>
@@ -2894,6 +3040,9 @@
       <c r="D47" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="G47" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I47" t="s">
         <v>22</v>
       </c>
@@ -2917,6 +3066,9 @@
       <c r="D48" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I48" t="s">
         <v>22</v>
       </c>
@@ -2940,6 +3092,9 @@
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="G49" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I49" t="s">
         <v>22</v>
       </c>
@@ -2963,6 +3118,9 @@
       <c r="D50" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="G50" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I50" t="s">
         <v>22</v>
       </c>
@@ -2986,6 +3144,9 @@
       <c r="D51" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="G51" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I51" t="s">
         <v>22</v>
       </c>
@@ -3009,6 +3170,7 @@
       <c r="D52" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="G52" s="2"/>
       <c r="I52" t="s">
         <v>22</v>
       </c>
@@ -3032,8 +3194,9 @@
       <c r="E53" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="G53" s="2"/>
       <c r="I53" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>451</v>
@@ -3055,8 +3218,9 @@
       <c r="E54" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="G54" s="2"/>
       <c r="I54" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>452</v>
@@ -3078,8 +3242,9 @@
       <c r="E55" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="G55" s="2"/>
       <c r="I55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>452</v>
@@ -3101,8 +3266,9 @@
       <c r="E56" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G56" s="2"/>
       <c r="I56" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>451</v>
@@ -3124,8 +3290,9 @@
       <c r="E57" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="G57" s="2"/>
       <c r="I57" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>451</v>
@@ -3147,6 +3314,7 @@
       <c r="E58" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="G58" s="2"/>
       <c r="I58" t="s">
         <v>22</v>
       </c>
@@ -3170,8 +3338,9 @@
       <c r="E59" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="G59" s="2"/>
       <c r="I59" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>437</v>
@@ -3193,8 +3362,9 @@
       <c r="E60" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="G60" s="2"/>
       <c r="I60" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>451</v>
@@ -3216,8 +3386,9 @@
       <c r="E61" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G61" s="2"/>
       <c r="I61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>451</v>
@@ -3239,6 +3410,9 @@
       <c r="E62" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G62" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I62" t="s">
         <v>22</v>
       </c>
@@ -3266,7 +3440,7 @@
         <v>110</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>482</v>
+        <v>493</v>
       </c>
       <c r="I63" t="s">
         <v>22</v>
@@ -3294,6 +3468,9 @@
       <c r="E64" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G64" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I64" t="s">
         <v>22</v>
       </c>
@@ -3320,6 +3497,9 @@
       <c r="E65" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G65" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I65" t="s">
         <v>22</v>
       </c>
@@ -3346,6 +3526,9 @@
       <c r="E66" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G66" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I66" t="s">
         <v>22</v>
       </c>
@@ -3372,8 +3555,9 @@
       <c r="E67" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G67" s="2"/>
       <c r="I67" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>434</v>
@@ -3395,8 +3579,9 @@
       <c r="E68" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G68" s="2"/>
       <c r="I68" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O68" s="2" t="s">
         <v>453</v>
@@ -3418,6 +3603,9 @@
       <c r="E69" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G69" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I69" t="s">
         <v>22</v>
       </c>
@@ -3444,6 +3632,9 @@
       <c r="E70" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G70" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I70" t="s">
         <v>22</v>
       </c>
@@ -3470,6 +3661,9 @@
       <c r="E71" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G71" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I71" t="s">
         <v>22</v>
       </c>
@@ -3496,6 +3690,9 @@
       <c r="E72" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G72" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I72" t="s">
         <v>22</v>
       </c>
@@ -3519,6 +3716,7 @@
       <c r="D73" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="G73" s="2"/>
       <c r="I73" t="s">
         <v>22</v>
       </c>
@@ -3539,6 +3737,7 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="G74" s="2"/>
       <c r="I74" t="s">
         <v>22</v>
       </c>
@@ -3559,8 +3758,9 @@
       <c r="D75" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="G75" s="2"/>
       <c r="I75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>456</v>
@@ -3579,8 +3779,9 @@
       <c r="D76" s="4" t="s">
         <v>147</v>
       </c>
+      <c r="G76" s="2"/>
       <c r="I76" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O76" s="2" t="s">
         <v>455</v>
@@ -3599,6 +3800,9 @@
       <c r="D77" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="G77" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I77" t="s">
         <v>22</v>
       </c>
@@ -3622,6 +3826,9 @@
       <c r="D78" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="G78" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I78" t="s">
         <v>22</v>
       </c>
@@ -3645,6 +3852,9 @@
       <c r="D79" s="4" t="s">
         <v>153</v>
       </c>
+      <c r="G79" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I79" t="s">
         <v>22</v>
       </c>
@@ -3668,6 +3878,9 @@
       <c r="D80" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="G80" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I80" t="s">
         <v>22</v>
       </c>
@@ -3691,6 +3904,9 @@
       <c r="D81" s="4" t="s">
         <v>157</v>
       </c>
+      <c r="G81" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I81" t="s">
         <v>22</v>
       </c>
@@ -3714,6 +3930,9 @@
       <c r="D82" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="G82" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I82" t="s">
         <v>22</v>
       </c>
@@ -3737,6 +3956,7 @@
       <c r="D83" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="G83" s="2"/>
       <c r="I83" t="s">
         <v>22</v>
       </c>
@@ -3760,8 +3980,9 @@
       <c r="E84" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="G84" s="2"/>
       <c r="I84" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>458</v>
@@ -3783,8 +4004,9 @@
       <c r="E85" s="4" t="s">
         <v>167</v>
       </c>
+      <c r="G85" s="2"/>
       <c r="I85" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>457</v>
@@ -3806,8 +4028,9 @@
       <c r="E86" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="G86" s="2"/>
       <c r="I86" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>459</v>
@@ -3829,6 +4052,7 @@
       <c r="E87" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="G87" s="2"/>
       <c r="I87" t="s">
         <v>22</v>
       </c>
@@ -3849,6 +4073,9 @@
       <c r="D88" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="G88" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I88" t="s">
         <v>22</v>
       </c>
@@ -3872,8 +4099,9 @@
       <c r="D89" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="G89" s="2"/>
       <c r="I89" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>435</v>
@@ -3895,8 +4123,9 @@
       <c r="E90" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="G90" s="2"/>
       <c r="I90" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>436</v>
@@ -3915,8 +4144,9 @@
       <c r="D91" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="G91" s="2"/>
       <c r="I91" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>437</v>
@@ -3938,8 +4168,9 @@
       <c r="E92" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="G92" s="2"/>
       <c r="I92" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>438</v>
@@ -3958,6 +4189,9 @@
       <c r="D93" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="G93" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I93" t="s">
         <v>22</v>
       </c>
@@ -3981,6 +4215,9 @@
       <c r="D94" s="4" t="s">
         <v>189</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="I94" t="s">
         <v>22</v>
       </c>
@@ -4004,6 +4241,7 @@
       <c r="D95" s="4" t="s">
         <v>191</v>
       </c>
+      <c r="G95" s="2"/>
       <c r="O95" s="2" t="s">
         <v>457</v>
       </c>
@@ -4021,6 +4259,7 @@
       <c r="D96" s="4" t="s">
         <v>193</v>
       </c>
+      <c r="G96" s="2"/>
       <c r="O96" s="2" t="s">
         <v>439</v>
       </c>
@@ -4038,6 +4277,9 @@
       <c r="D97" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="G97" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N97" t="s">
         <v>22</v>
       </c>
@@ -4058,6 +4300,7 @@
       <c r="D98" s="4" t="s">
         <v>197</v>
       </c>
+      <c r="G98" s="2"/>
       <c r="O98" s="2" t="s">
         <v>440</v>
       </c>
@@ -4075,6 +4318,7 @@
       <c r="D99" s="4" t="s">
         <v>199</v>
       </c>
+      <c r="G99" s="2"/>
       <c r="O99" s="2" t="s">
         <v>441</v>
       </c>
@@ -4092,6 +4336,7 @@
       <c r="D100" s="4" t="s">
         <v>201</v>
       </c>
+      <c r="G100" s="2"/>
       <c r="O100" s="2" t="s">
         <v>441</v>
       </c>
@@ -4109,6 +4354,9 @@
       <c r="D101" s="4" t="s">
         <v>203</v>
       </c>
+      <c r="G101" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N101" t="s">
         <v>22</v>
       </c>
@@ -4129,6 +4377,9 @@
       <c r="D102" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G102" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N102" t="s">
         <v>22</v>
       </c>
@@ -4149,6 +4400,7 @@
       <c r="D103" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G103" s="2"/>
       <c r="O103" s="2" t="s">
         <v>442</v>
       </c>
@@ -4166,6 +4418,7 @@
       <c r="D104" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G104" s="2"/>
       <c r="O104" s="2" t="s">
         <v>461</v>
       </c>
@@ -4183,6 +4436,7 @@
       <c r="D105" s="4" t="s">
         <v>210</v>
       </c>
+      <c r="G105" s="2"/>
       <c r="O105" s="2" t="s">
         <v>461</v>
       </c>
@@ -4200,6 +4454,9 @@
       <c r="D106" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G106" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N106" t="s">
         <v>22</v>
       </c>
@@ -4220,6 +4477,7 @@
       <c r="D107" s="4" t="s">
         <v>213</v>
       </c>
+      <c r="G107" s="2"/>
       <c r="O107" s="2" t="s">
         <v>462</v>
       </c>
@@ -4237,6 +4495,7 @@
       <c r="D108" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G108" s="2"/>
       <c r="O108" s="2" t="s">
         <v>463</v>
       </c>
@@ -4254,6 +4513,7 @@
       <c r="D109" s="4" t="s">
         <v>216</v>
       </c>
+      <c r="G109" s="2"/>
       <c r="O109" s="2" t="s">
         <v>23</v>
       </c>
@@ -4271,6 +4531,7 @@
       <c r="D110" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G110" s="2"/>
       <c r="O110" s="2" t="s">
         <v>443</v>
       </c>
@@ -4288,6 +4549,7 @@
       <c r="D111" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G111" s="2"/>
       <c r="O111" s="2" t="s">
         <v>464</v>
       </c>
@@ -4305,6 +4567,7 @@
       <c r="D112" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G112" s="2"/>
       <c r="O112" s="2" t="s">
         <v>463</v>
       </c>
@@ -4322,6 +4585,7 @@
       <c r="D113" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G113" s="2"/>
       <c r="O113" s="2" t="s">
         <v>23</v>
       </c>
@@ -4339,6 +4603,7 @@
       <c r="D114" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="G114" s="2"/>
       <c r="O114" s="2" t="s">
         <v>465</v>
       </c>
@@ -4356,6 +4621,7 @@
       <c r="D115" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="G115" s="2"/>
       <c r="O115" s="2" t="s">
         <v>466</v>
       </c>
@@ -4373,6 +4639,9 @@
       <c r="D116" s="4" t="s">
         <v>225</v>
       </c>
+      <c r="G116" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N116" t="s">
         <v>22</v>
       </c>
@@ -4393,6 +4662,7 @@
       <c r="D117" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G117" s="2"/>
       <c r="O117" s="2" t="s">
         <v>467</v>
       </c>
@@ -4410,6 +4680,7 @@
       <c r="D118" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G118" s="2"/>
       <c r="O118" s="2" t="s">
         <v>444</v>
       </c>
@@ -4427,6 +4698,7 @@
       <c r="D119" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G119" s="2"/>
       <c r="O119" s="2" t="s">
         <v>468</v>
       </c>
@@ -4444,6 +4716,9 @@
       <c r="D120" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="G120" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N120" t="s">
         <v>22</v>
       </c>
@@ -4464,6 +4739,9 @@
       <c r="D121" s="4" t="s">
         <v>233</v>
       </c>
+      <c r="G121" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N121" t="s">
         <v>22</v>
       </c>
@@ -4484,6 +4762,9 @@
       <c r="D122" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="G122" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N122" t="s">
         <v>22</v>
       </c>
@@ -4504,6 +4785,9 @@
       <c r="D123" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="G123" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N123" t="s">
         <v>22</v>
       </c>
@@ -4524,6 +4808,9 @@
       <c r="D124" s="4" t="s">
         <v>238</v>
       </c>
+      <c r="G124" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="O124" s="2" t="s">
         <v>23</v>
       </c>
@@ -4541,6 +4828,9 @@
       <c r="D125" s="4" t="s">
         <v>240</v>
       </c>
+      <c r="G125" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N125" t="s">
         <v>22</v>
       </c>
@@ -4561,6 +4851,9 @@
       <c r="D126" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="G126" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N126" t="s">
         <v>22</v>
       </c>
@@ -4581,6 +4874,7 @@
       <c r="D127" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="G127" s="2"/>
       <c r="O127" s="2" t="s">
         <v>23</v>
       </c>
@@ -4598,6 +4892,9 @@
       <c r="D128" s="4" t="s">
         <v>244</v>
       </c>
+      <c r="G128" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="O128" s="2" t="s">
         <v>23</v>
       </c>
@@ -4615,6 +4912,9 @@
       <c r="D129" s="4" t="s">
         <v>246</v>
       </c>
+      <c r="G129" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N129" t="s">
         <v>22</v>
       </c>
@@ -4635,6 +4935,7 @@
       <c r="D130" s="4" t="s">
         <v>248</v>
       </c>
+      <c r="G130" s="2"/>
       <c r="O130" s="2" t="s">
         <v>469</v>
       </c>
@@ -4652,6 +4953,9 @@
       <c r="D131" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G131" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N131" t="s">
         <v>22</v>
       </c>
@@ -4672,6 +4976,9 @@
       <c r="D132" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="G132" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N132" t="s">
         <v>22</v>
       </c>
@@ -4692,6 +4999,9 @@
       <c r="D133" s="6" t="s">
         <v>254</v>
       </c>
+      <c r="G133" s="2" t="s">
+        <v>494</v>
+      </c>
       <c r="N133" t="s">
         <v>22</v>
       </c>
@@ -4712,6 +5022,9 @@
       <c r="D134" s="6" t="s">
         <v>256</v>
       </c>
+      <c r="G134" s="2" t="s">
+        <v>495</v>
+      </c>
       <c r="N134" t="s">
         <v>22</v>
       </c>
@@ -4732,6 +5045,7 @@
       <c r="D135" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="G135" s="2"/>
       <c r="O135" s="2" t="s">
         <v>456</v>
       </c>
@@ -4749,6 +5063,7 @@
       <c r="D136" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="G136" s="2"/>
       <c r="O136" s="2" t="s">
         <v>470</v>
       </c>
@@ -4766,6 +5081,9 @@
       <c r="D137" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G137" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N137" s="8" t="s">
         <v>22</v>
       </c>
@@ -4786,6 +5104,9 @@
       <c r="D138" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="G138" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N138" s="8" t="s">
         <v>22</v>
       </c>
@@ -4806,6 +5127,7 @@
       <c r="D139" s="6" t="s">
         <v>262</v>
       </c>
+      <c r="G139" s="2"/>
       <c r="O139" s="2" t="s">
         <v>439</v>
       </c>
@@ -4823,6 +5145,9 @@
       <c r="D140" s="6" t="s">
         <v>264</v>
       </c>
+      <c r="G140" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N140" s="8" t="s">
         <v>22</v>
       </c>
@@ -4843,6 +5168,9 @@
       <c r="D141" s="6" t="s">
         <v>266</v>
       </c>
+      <c r="G141" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N141" s="8" t="s">
         <v>22</v>
       </c>
@@ -4866,6 +5194,7 @@
       <c r="E142" s="4" t="s">
         <v>269</v>
       </c>
+      <c r="G142" s="2"/>
       <c r="O142" s="2" t="s">
         <v>470</v>
       </c>
@@ -4889,6 +5218,9 @@
       <c r="E143" s="4" t="s">
         <v>273</v>
       </c>
+      <c r="G143" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N143" s="8" t="s">
         <v>22</v>
       </c>
@@ -4909,6 +5241,7 @@
       <c r="D144" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G144" s="2"/>
       <c r="O144" s="2" t="s">
         <v>470</v>
       </c>
@@ -4926,6 +5259,7 @@
       <c r="D145" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G145" s="2"/>
       <c r="O145" s="2" t="s">
         <v>470</v>
       </c>
@@ -4943,6 +5277,7 @@
       <c r="D146" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G146" s="2"/>
       <c r="O146" s="2" t="s">
         <v>470</v>
       </c>
@@ -4960,6 +5295,7 @@
       <c r="D147" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G147" s="2"/>
       <c r="O147" s="2" t="s">
         <v>470</v>
       </c>
@@ -4977,6 +5313,9 @@
       <c r="D148" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G148" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N148" s="8" t="s">
         <v>22</v>
       </c>
@@ -4997,6 +5336,9 @@
       <c r="D149" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G149" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N149" s="8" t="s">
         <v>22</v>
       </c>
@@ -5017,6 +5359,7 @@
       <c r="D150" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="G150" s="2"/>
       <c r="O150" s="2" t="s">
         <v>470</v>
       </c>
@@ -5034,6 +5377,7 @@
       <c r="D151" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="G151" s="2"/>
       <c r="O151" s="2" t="s">
         <v>471</v>
       </c>
@@ -5051,6 +5395,9 @@
       <c r="D152" s="4" t="s">
         <v>283</v>
       </c>
+      <c r="G152" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N152" s="8" t="s">
         <v>22</v>
       </c>
@@ -5071,6 +5418,9 @@
       <c r="D153" s="4" t="s">
         <v>285</v>
       </c>
+      <c r="G153" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N153" s="8" t="s">
         <v>22</v>
       </c>
@@ -5091,6 +5441,7 @@
       <c r="D154" s="4" t="s">
         <v>287</v>
       </c>
+      <c r="G154" s="2"/>
       <c r="N154" s="4"/>
       <c r="O154" s="4" t="s">
         <v>288</v>
@@ -5109,6 +5460,7 @@
       <c r="D155" s="4" t="s">
         <v>290</v>
       </c>
+      <c r="G155" s="2"/>
       <c r="O155" s="2" t="s">
         <v>472</v>
       </c>
@@ -5126,6 +5478,9 @@
       <c r="D156" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="G156" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N156" s="8" t="s">
         <v>22</v>
       </c>
@@ -5146,6 +5501,9 @@
       <c r="D157" s="4" t="s">
         <v>294</v>
       </c>
+      <c r="G157" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N157" s="8" t="s">
         <v>22</v>
       </c>
@@ -5166,6 +5524,9 @@
       <c r="D158" s="4" t="s">
         <v>296</v>
       </c>
+      <c r="G158" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N158" s="8" t="s">
         <v>22</v>
       </c>
@@ -5186,6 +5547,9 @@
       <c r="D159" s="4" t="s">
         <v>298</v>
       </c>
+      <c r="G159" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N159" s="8" t="s">
         <v>22</v>
       </c>
@@ -5206,6 +5570,9 @@
       <c r="D160" s="4" t="s">
         <v>300</v>
       </c>
+      <c r="G160" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N160" s="8" t="s">
         <v>22</v>
       </c>
@@ -5226,6 +5593,9 @@
       <c r="D161" s="4" t="s">
         <v>302</v>
       </c>
+      <c r="G161" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N161" s="8" t="s">
         <v>22</v>
       </c>
@@ -5246,6 +5616,7 @@
       <c r="D162" s="4" t="s">
         <v>304</v>
       </c>
+      <c r="G162" s="2"/>
       <c r="O162" s="2" t="s">
         <v>473</v>
       </c>
@@ -5263,6 +5634,9 @@
       <c r="D163" s="4" t="s">
         <v>306</v>
       </c>
+      <c r="G163" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N163" s="8" t="s">
         <v>22</v>
       </c>
@@ -5283,6 +5657,7 @@
       <c r="D164" s="4" t="s">
         <v>308</v>
       </c>
+      <c r="G164" s="2"/>
       <c r="O164" s="2" t="s">
         <v>23</v>
       </c>
@@ -5300,6 +5675,7 @@
       <c r="D165" s="4" t="s">
         <v>310</v>
       </c>
+      <c r="G165" s="2"/>
       <c r="O165" s="2" t="s">
         <v>23</v>
       </c>
@@ -5317,6 +5693,9 @@
       <c r="D166" s="4" t="s">
         <v>312</v>
       </c>
+      <c r="G166" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N166" s="8" t="s">
         <v>22</v>
       </c>
@@ -5337,6 +5716,9 @@
       <c r="D167" s="4" t="s">
         <v>314</v>
       </c>
+      <c r="G167" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="O167" s="2" t="s">
         <v>23</v>
       </c>
@@ -5354,6 +5736,7 @@
       <c r="D168" s="4" t="s">
         <v>316</v>
       </c>
+      <c r="G168" s="2"/>
       <c r="O168" s="2" t="s">
         <v>23</v>
       </c>
@@ -5371,6 +5754,9 @@
       <c r="D169" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="G169" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N169" s="8" t="s">
         <v>22</v>
       </c>
@@ -5391,6 +5777,9 @@
       <c r="D170" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="G170" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N170" s="8" t="s">
         <v>22</v>
       </c>
@@ -5411,6 +5800,9 @@
       <c r="D171" s="4" t="s">
         <v>321</v>
       </c>
+      <c r="G171" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N171" s="8" t="s">
         <v>22</v>
       </c>
@@ -5431,6 +5823,9 @@
       <c r="D172" s="4" t="s">
         <v>323</v>
       </c>
+      <c r="G172" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N172" s="8" t="s">
         <v>22</v>
       </c>
@@ -5451,6 +5846,9 @@
       <c r="D173" s="4" t="s">
         <v>325</v>
       </c>
+      <c r="G173" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N173" s="8" t="s">
         <v>22</v>
       </c>
@@ -5471,6 +5869,9 @@
       <c r="D174" s="4" t="s">
         <v>327</v>
       </c>
+      <c r="G174" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N174" s="8" t="s">
         <v>22</v>
       </c>
@@ -5491,6 +5892,7 @@
       <c r="D175" s="4" t="s">
         <v>329</v>
       </c>
+      <c r="G175" s="2"/>
       <c r="O175" s="2" t="s">
         <v>474</v>
       </c>
@@ -5508,6 +5910,7 @@
       <c r="D176" s="4" t="s">
         <v>331</v>
       </c>
+      <c r="G176" s="2"/>
       <c r="O176" s="2" t="s">
         <v>474</v>
       </c>
@@ -5525,6 +5928,7 @@
       <c r="D177" s="4" t="s">
         <v>333</v>
       </c>
+      <c r="G177" s="2"/>
       <c r="O177" s="2" t="s">
         <v>474</v>
       </c>
@@ -5542,6 +5946,7 @@
       <c r="D178" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="G178" s="2"/>
       <c r="O178" s="2" t="s">
         <v>23</v>
       </c>
@@ -5559,6 +5964,9 @@
       <c r="D179" s="4" t="s">
         <v>337</v>
       </c>
+      <c r="G179" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N179" s="8" t="s">
         <v>22</v>
       </c>
@@ -5579,6 +5987,7 @@
       <c r="D180" s="4" t="s">
         <v>339</v>
       </c>
+      <c r="G180" s="2"/>
       <c r="O180" s="2" t="s">
         <v>474</v>
       </c>
@@ -5596,6 +6005,9 @@
       <c r="D181" s="4" t="s">
         <v>341</v>
       </c>
+      <c r="G181" s="2" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
@@ -5610,6 +6022,9 @@
       <c r="D182" s="4" t="s">
         <v>343</v>
       </c>
+      <c r="G182" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N182" s="8" t="s">
         <v>22</v>
       </c>
@@ -5630,6 +6045,9 @@
       <c r="D183" s="4" t="s">
         <v>345</v>
       </c>
+      <c r="G183" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N183" s="8" t="s">
         <v>22</v>
       </c>
@@ -5650,6 +6068,9 @@
       <c r="D184" s="4" t="s">
         <v>347</v>
       </c>
+      <c r="G184" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N184" s="8" t="s">
         <v>22</v>
       </c>
@@ -5670,6 +6091,9 @@
       <c r="D185" s="4" t="s">
         <v>349</v>
       </c>
+      <c r="G185" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N185" s="8" t="s">
         <v>22</v>
       </c>
@@ -5690,6 +6114,9 @@
       <c r="D186" s="4" t="s">
         <v>351</v>
       </c>
+      <c r="G186" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N186" s="8" t="s">
         <v>22</v>
       </c>
@@ -5710,6 +6137,9 @@
       <c r="D187" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="G187" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N187" s="8" t="s">
         <v>22</v>
       </c>
@@ -5730,6 +6160,9 @@
       <c r="D188" s="4" t="s">
         <v>355</v>
       </c>
+      <c r="G188" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N188" s="8" t="s">
         <v>22</v>
       </c>
@@ -5750,6 +6183,9 @@
       <c r="D189" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="G189" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N189" s="8" t="s">
         <v>22</v>
       </c>
@@ -5770,6 +6206,9 @@
       <c r="D190" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="G190" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N190" s="8" t="s">
         <v>22</v>
       </c>
@@ -5790,6 +6229,9 @@
       <c r="D191" s="4" t="s">
         <v>359</v>
       </c>
+      <c r="G191" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N191" s="8" t="s">
         <v>22</v>
       </c>
@@ -5810,6 +6252,9 @@
       <c r="D192" s="4" t="s">
         <v>361</v>
       </c>
+      <c r="G192" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N192" s="8" t="s">
         <v>22</v>
       </c>
@@ -5830,6 +6275,9 @@
       <c r="D193" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="G193" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N193" s="8" t="s">
         <v>22</v>
       </c>
@@ -5850,6 +6298,9 @@
       <c r="D194" s="4" t="s">
         <v>365</v>
       </c>
+      <c r="G194" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N194" s="8" t="s">
         <v>22</v>
       </c>
@@ -5873,6 +6324,7 @@
       <c r="E195" s="4" t="s">
         <v>368</v>
       </c>
+      <c r="G195" s="2"/>
       <c r="O195" s="2" t="s">
         <v>475</v>
       </c>
@@ -5890,6 +6342,9 @@
       <c r="D196" s="4" t="s">
         <v>370</v>
       </c>
+      <c r="G196" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N196" s="8" t="s">
         <v>22</v>
       </c>
@@ -5910,6 +6365,9 @@
       <c r="D197" s="4" t="s">
         <v>372</v>
       </c>
+      <c r="G197" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N197" s="8" t="s">
         <v>22</v>
       </c>
@@ -5930,6 +6388,9 @@
       <c r="D198" s="4" t="s">
         <v>374</v>
       </c>
+      <c r="G198" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N198" s="8" t="s">
         <v>22</v>
       </c>
@@ -5937,7 +6398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>195</v>
       </c>
@@ -5949,6 +6410,9 @@
       </c>
       <c r="D199" s="4" t="s">
         <v>376</v>
+      </c>
+      <c r="G199" s="2" t="s">
+        <v>496</v>
       </c>
       <c r="N199" s="8" t="s">
         <v>22</v>
@@ -5970,6 +6434,9 @@
       <c r="D200" s="4" t="s">
         <v>378</v>
       </c>
+      <c r="G200" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N200" s="8" t="s">
         <v>22</v>
       </c>
@@ -5990,6 +6457,9 @@
       <c r="D201" s="4" t="s">
         <v>380</v>
       </c>
+      <c r="G201" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N201" s="8" t="s">
         <v>22</v>
       </c>
@@ -5997,7 +6467,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>198</v>
       </c>
@@ -6010,6 +6480,9 @@
       <c r="D202" s="4" t="s">
         <v>382</v>
       </c>
+      <c r="G202" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="N202" s="8" t="s">
         <v>22</v>
       </c>
@@ -6017,7 +6490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>199</v>
       </c>
@@ -6029,6 +6502,9 @@
       </c>
       <c r="D203" s="4" t="s">
         <v>384</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>498</v>
       </c>
       <c r="N203" s="8" t="s">
         <v>22</v>
@@ -6050,6 +6526,7 @@
       <c r="D204" s="4" t="s">
         <v>386</v>
       </c>
+      <c r="G204" s="2"/>
       <c r="O204" s="2" t="s">
         <v>476</v>
       </c>
@@ -6067,6 +6544,9 @@
       <c r="D205" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="G205" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N205" s="8" t="s">
         <v>22</v>
       </c>
@@ -6087,6 +6567,9 @@
       <c r="D206" s="4" t="s">
         <v>389</v>
       </c>
+      <c r="G206" s="4" t="s">
+        <v>486</v>
+      </c>
       <c r="N206" s="8" t="s">
         <v>22</v>
       </c>
@@ -6107,6 +6590,9 @@
       <c r="D207" s="4" t="s">
         <v>391</v>
       </c>
+      <c r="G207" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N207" s="8" t="s">
         <v>22</v>
       </c>
@@ -6133,8 +6619,8 @@
       <c r="E208" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="G208" s="4" t="s">
-        <v>483</v>
+      <c r="G208" s="2" t="s">
+        <v>482</v>
       </c>
       <c r="O208" s="2" t="s">
         <v>446</v>
@@ -6156,6 +6642,7 @@
       <c r="E209" s="4" t="s">
         <v>398</v>
       </c>
+      <c r="G209" s="2"/>
       <c r="O209" s="2" t="s">
         <v>447</v>
       </c>
@@ -6173,6 +6660,7 @@
       <c r="D210" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="G210" s="2"/>
       <c r="O210" s="2" t="s">
         <v>23</v>
       </c>
@@ -6193,6 +6681,7 @@
       <c r="D211" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="G211" s="4"/>
       <c r="O211" s="2" t="s">
         <v>445</v>
       </c>
@@ -6213,6 +6702,7 @@
       <c r="E212" s="4" t="s">
         <v>406</v>
       </c>
+      <c r="G212" s="2"/>
       <c r="O212" s="2" t="s">
         <v>447</v>
       </c>
@@ -6233,8 +6723,8 @@
       <c r="E213" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="G213" s="4" t="s">
-        <v>483</v>
+      <c r="G213" s="2" t="s">
+        <v>482</v>
       </c>
       <c r="O213" s="2" t="s">
         <v>448</v>
@@ -6256,6 +6746,7 @@
       <c r="E214" s="4" t="s">
         <v>412</v>
       </c>
+      <c r="G214" s="2"/>
       <c r="O214" s="2" t="s">
         <v>448</v>
       </c>
@@ -6273,6 +6764,7 @@
       <c r="D215" s="4" t="s">
         <v>405</v>
       </c>
+      <c r="G215" s="2"/>
       <c r="O215" s="2" t="s">
         <v>447</v>
       </c>
@@ -6293,6 +6785,9 @@
       <c r="D216" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="G216" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N216" s="8" t="s">
         <v>22</v>
       </c>
@@ -6313,6 +6808,9 @@
       <c r="D217" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="G217" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N217" s="8" t="s">
         <v>22</v>
       </c>
@@ -6333,6 +6831,9 @@
       <c r="D218" s="4" t="s">
         <v>419</v>
       </c>
+      <c r="G218" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="N218" s="8" t="s">
         <v>22</v>
       </c>
@@ -6390,6 +6891,7 @@
       <c r="E221" s="4" t="s">
         <v>424</v>
       </c>
+      <c r="G221" s="2"/>
       <c r="O221" s="2" t="s">
         <v>445</v>
       </c>
@@ -6413,6 +6915,7 @@
       <c r="E222" s="4" t="s">
         <v>428</v>
       </c>
+      <c r="G222" s="2"/>
       <c r="O222" s="2" t="s">
         <v>448</v>
       </c>
@@ -6433,6 +6936,7 @@
       <c r="E223" s="4" t="s">
         <v>430</v>
       </c>
+      <c r="G223" s="2"/>
       <c r="O223" s="2" t="s">
         <v>477</v>
       </c>
@@ -6450,6 +6954,7 @@
       <c r="D224" s="4" t="s">
         <v>432</v>
       </c>
+      <c r="G224" s="2"/>
       <c r="O224" s="2" t="s">
         <v>439</v>
       </c>

</xml_diff>

<commit_message>
Added tests for requirements 177-220 (group 28)
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondtian/Documents/UTA/Spring 2025/CSE 3310/cse3310-sp25-002/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caden/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E52164-2403-BE4F-B260-F4E6DE8A21CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894AA35-6E1A-8F4A-93E9-170DE07822B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="1080" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="940" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="510">
   <si>
     <t>Tested By</t>
   </si>
@@ -1539,6 +1539,39 @@
   </si>
   <si>
     <t>Req. might be too unlcear to test.What does if needed mean?</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 15)</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 3)</t>
+  </si>
+  <si>
+    <t>Success (Test1: Step 3&amp;4)</t>
+  </si>
+  <si>
+    <t>Success (based off code)</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 5&amp;6)</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 3&amp;4)</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 8)</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 2&amp;3)</t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defect </t>
+  </si>
+  <si>
+    <t>Success (Test 1: Step 11)</t>
   </si>
 </sst>
 </file>
@@ -1937,8 +1970,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95:I224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4280,6 +4313,9 @@
       <c r="G97" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I97" t="s">
+        <v>22</v>
+      </c>
       <c r="N97" t="s">
         <v>22</v>
       </c>
@@ -4357,6 +4393,9 @@
       <c r="G101" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I101" t="s">
+        <v>22</v>
+      </c>
       <c r="N101" t="s">
         <v>22</v>
       </c>
@@ -4380,6 +4419,9 @@
       <c r="G102" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I102" t="s">
+        <v>22</v>
+      </c>
       <c r="N102" t="s">
         <v>22</v>
       </c>
@@ -4457,6 +4499,9 @@
       <c r="G106" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I106" t="s">
+        <v>22</v>
+      </c>
       <c r="N106" t="s">
         <v>22</v>
       </c>
@@ -4642,6 +4687,9 @@
       <c r="G116" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I116" t="s">
+        <v>22</v>
+      </c>
       <c r="N116" t="s">
         <v>22</v>
       </c>
@@ -4719,6 +4767,9 @@
       <c r="G120" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I120" t="s">
+        <v>22</v>
+      </c>
       <c r="N120" t="s">
         <v>22</v>
       </c>
@@ -4742,6 +4793,9 @@
       <c r="G121" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I121" t="s">
+        <v>22</v>
+      </c>
       <c r="N121" t="s">
         <v>22</v>
       </c>
@@ -4765,6 +4819,9 @@
       <c r="G122" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I122" t="s">
+        <v>22</v>
+      </c>
       <c r="N122" t="s">
         <v>22</v>
       </c>
@@ -4788,6 +4845,9 @@
       <c r="G123" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I123" t="s">
+        <v>22</v>
+      </c>
       <c r="N123" t="s">
         <v>22</v>
       </c>
@@ -4831,6 +4891,9 @@
       <c r="G125" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I125" t="s">
+        <v>22</v>
+      </c>
       <c r="N125" t="s">
         <v>22</v>
       </c>
@@ -4854,6 +4917,9 @@
       <c r="G126" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I126" t="s">
+        <v>22</v>
+      </c>
       <c r="N126" t="s">
         <v>22</v>
       </c>
@@ -4915,6 +4981,9 @@
       <c r="G129" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I129" t="s">
+        <v>22</v>
+      </c>
       <c r="N129" t="s">
         <v>22</v>
       </c>
@@ -4956,6 +5025,9 @@
       <c r="G131" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I131" t="s">
+        <v>22</v>
+      </c>
       <c r="N131" t="s">
         <v>22</v>
       </c>
@@ -4979,6 +5051,9 @@
       <c r="G132" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I132" t="s">
+        <v>22</v>
+      </c>
       <c r="N132" t="s">
         <v>22</v>
       </c>
@@ -5002,6 +5077,9 @@
       <c r="G133" s="2" t="s">
         <v>494</v>
       </c>
+      <c r="I133" t="s">
+        <v>22</v>
+      </c>
       <c r="N133" t="s">
         <v>22</v>
       </c>
@@ -5025,6 +5103,9 @@
       <c r="G134" s="2" t="s">
         <v>495</v>
       </c>
+      <c r="I134" t="s">
+        <v>22</v>
+      </c>
       <c r="N134" t="s">
         <v>22</v>
       </c>
@@ -5084,6 +5165,9 @@
       <c r="G137" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I137" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N137" s="8" t="s">
         <v>22</v>
       </c>
@@ -5107,6 +5191,9 @@
       <c r="G138" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I138" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N138" s="8" t="s">
         <v>22</v>
       </c>
@@ -5148,6 +5235,9 @@
       <c r="G140" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I140" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N140" s="8" t="s">
         <v>22</v>
       </c>
@@ -5171,6 +5261,9 @@
       <c r="G141" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I141" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N141" s="8" t="s">
         <v>22</v>
       </c>
@@ -5221,6 +5314,9 @@
       <c r="G143" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I143" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N143" s="8" t="s">
         <v>22</v>
       </c>
@@ -5316,6 +5412,9 @@
       <c r="G148" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I148" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N148" s="8" t="s">
         <v>22</v>
       </c>
@@ -5339,6 +5438,9 @@
       <c r="G149" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I149" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N149" s="8" t="s">
         <v>22</v>
       </c>
@@ -5398,6 +5500,9 @@
       <c r="G152" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I152" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N152" s="8" t="s">
         <v>22</v>
       </c>
@@ -5421,6 +5526,9 @@
       <c r="G153" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I153" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N153" s="8" t="s">
         <v>22</v>
       </c>
@@ -5442,6 +5550,7 @@
         <v>287</v>
       </c>
       <c r="G154" s="2"/>
+      <c r="I154" s="4"/>
       <c r="N154" s="4"/>
       <c r="O154" s="4" t="s">
         <v>288</v>
@@ -5481,6 +5590,9 @@
       <c r="G156" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I156" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N156" s="8" t="s">
         <v>22</v>
       </c>
@@ -5504,6 +5616,9 @@
       <c r="G157" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I157" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N157" s="8" t="s">
         <v>22</v>
       </c>
@@ -5527,6 +5642,9 @@
       <c r="G158" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I158" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N158" s="8" t="s">
         <v>22</v>
       </c>
@@ -5550,6 +5668,9 @@
       <c r="G159" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I159" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N159" s="8" t="s">
         <v>22</v>
       </c>
@@ -5573,6 +5694,9 @@
       <c r="G160" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I160" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N160" s="8" t="s">
         <v>22</v>
       </c>
@@ -5596,6 +5720,9 @@
       <c r="G161" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I161" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N161" s="8" t="s">
         <v>22</v>
       </c>
@@ -5637,6 +5764,9 @@
       <c r="G163" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I163" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N163" s="8" t="s">
         <v>22</v>
       </c>
@@ -5696,6 +5826,9 @@
       <c r="G166" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I166" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N166" s="8" t="s">
         <v>22</v>
       </c>
@@ -5757,6 +5890,9 @@
       <c r="G169" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I169" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N169" s="8" t="s">
         <v>22</v>
       </c>
@@ -5780,6 +5916,9 @@
       <c r="G170" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I170" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N170" s="8" t="s">
         <v>22</v>
       </c>
@@ -5803,6 +5942,9 @@
       <c r="G171" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I171" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N171" s="8" t="s">
         <v>22</v>
       </c>
@@ -5826,6 +5968,9 @@
       <c r="G172" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I172" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N172" s="8" t="s">
         <v>22</v>
       </c>
@@ -5849,6 +5994,9 @@
       <c r="G173" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I173" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N173" s="8" t="s">
         <v>22</v>
       </c>
@@ -5872,6 +6020,9 @@
       <c r="G174" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I174" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N174" s="8" t="s">
         <v>22</v>
       </c>
@@ -5967,6 +6118,9 @@
       <c r="G179" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I179" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N179" s="8" t="s">
         <v>22</v>
       </c>
@@ -6008,6 +6162,9 @@
       <c r="G181" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I181" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
@@ -6025,6 +6182,9 @@
       <c r="G182" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I182" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N182" s="8" t="s">
         <v>22</v>
       </c>
@@ -6048,6 +6208,9 @@
       <c r="G183" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I183" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N183" s="8" t="s">
         <v>22</v>
       </c>
@@ -6071,6 +6234,9 @@
       <c r="G184" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I184" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N184" s="8" t="s">
         <v>22</v>
       </c>
@@ -6094,6 +6260,9 @@
       <c r="G185" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I185" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N185" s="8" t="s">
         <v>22</v>
       </c>
@@ -6117,6 +6286,9 @@
       <c r="G186" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I186" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N186" s="8" t="s">
         <v>22</v>
       </c>
@@ -6140,6 +6312,9 @@
       <c r="G187" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I187" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N187" s="8" t="s">
         <v>22</v>
       </c>
@@ -6163,6 +6338,9 @@
       <c r="G188" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I188" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N188" s="8" t="s">
         <v>22</v>
       </c>
@@ -6186,6 +6364,9 @@
       <c r="G189" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I189" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N189" s="8" t="s">
         <v>22</v>
       </c>
@@ -6209,6 +6390,9 @@
       <c r="G190" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I190" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N190" s="8" t="s">
         <v>22</v>
       </c>
@@ -6232,6 +6416,9 @@
       <c r="G191" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I191" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N191" s="8" t="s">
         <v>22</v>
       </c>
@@ -6255,6 +6442,9 @@
       <c r="G192" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I192" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N192" s="8" t="s">
         <v>22</v>
       </c>
@@ -6278,6 +6468,9 @@
       <c r="G193" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I193" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N193" s="8" t="s">
         <v>22</v>
       </c>
@@ -6301,6 +6494,9 @@
       <c r="G194" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I194" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N194" s="8" t="s">
         <v>22</v>
       </c>
@@ -6325,6 +6521,9 @@
         <v>368</v>
       </c>
       <c r="G195" s="2"/>
+      <c r="I195" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="O195" s="2" t="s">
         <v>475</v>
       </c>
@@ -6345,6 +6544,9 @@
       <c r="G196" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I196" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N196" s="8" t="s">
         <v>22</v>
       </c>
@@ -6368,6 +6570,9 @@
       <c r="G197" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I197" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N197" s="8" t="s">
         <v>22</v>
       </c>
@@ -6391,6 +6596,9 @@
       <c r="G198" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I198" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N198" s="8" t="s">
         <v>22</v>
       </c>
@@ -6414,6 +6622,9 @@
       <c r="G199" s="2" t="s">
         <v>496</v>
       </c>
+      <c r="I199" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N199" s="8" t="s">
         <v>22</v>
       </c>
@@ -6437,6 +6648,9 @@
       <c r="G200" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I200" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N200" s="8" t="s">
         <v>22</v>
       </c>
@@ -6460,6 +6674,9 @@
       <c r="G201" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I201" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N201" s="8" t="s">
         <v>22</v>
       </c>
@@ -6483,6 +6700,9 @@
       <c r="G202" s="2" t="s">
         <v>497</v>
       </c>
+      <c r="I202" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N202" s="8" t="s">
         <v>22</v>
       </c>
@@ -6506,6 +6726,9 @@
       <c r="G203" s="2" t="s">
         <v>498</v>
       </c>
+      <c r="I203" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N203" s="8" t="s">
         <v>22</v>
       </c>
@@ -6527,6 +6750,9 @@
         <v>386</v>
       </c>
       <c r="G204" s="2"/>
+      <c r="I204" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="O204" s="2" t="s">
         <v>476</v>
       </c>
@@ -6547,6 +6773,9 @@
       <c r="G205" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I205" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N205" s="8" t="s">
         <v>22</v>
       </c>
@@ -6570,6 +6799,9 @@
       <c r="G206" s="4" t="s">
         <v>486</v>
       </c>
+      <c r="I206" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N206" s="8" t="s">
         <v>22</v>
       </c>
@@ -6593,6 +6825,9 @@
       <c r="G207" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I207" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N207" s="8" t="s">
         <v>22</v>
       </c>
@@ -6622,6 +6857,9 @@
       <c r="G208" s="2" t="s">
         <v>482</v>
       </c>
+      <c r="I208" s="8" t="s">
+        <v>500</v>
+      </c>
       <c r="O208" s="2" t="s">
         <v>446</v>
       </c>
@@ -6643,6 +6881,9 @@
         <v>398</v>
       </c>
       <c r="G209" s="2"/>
+      <c r="I209" s="8" t="s">
+        <v>501</v>
+      </c>
       <c r="O209" s="2" t="s">
         <v>447</v>
       </c>
@@ -6661,6 +6902,9 @@
         <v>400</v>
       </c>
       <c r="G210" s="2"/>
+      <c r="I210" s="8" t="s">
+        <v>502</v>
+      </c>
       <c r="O210" s="2" t="s">
         <v>23</v>
       </c>
@@ -6682,6 +6926,9 @@
         <v>403</v>
       </c>
       <c r="G211" s="4"/>
+      <c r="I211" s="8" t="s">
+        <v>503</v>
+      </c>
       <c r="O211" s="2" t="s">
         <v>445</v>
       </c>
@@ -6703,6 +6950,9 @@
         <v>406</v>
       </c>
       <c r="G212" s="2"/>
+      <c r="I212" s="8" t="s">
+        <v>504</v>
+      </c>
       <c r="O212" s="2" t="s">
         <v>447</v>
       </c>
@@ -6726,6 +6976,9 @@
       <c r="G213" s="2" t="s">
         <v>482</v>
       </c>
+      <c r="I213" s="8" t="s">
+        <v>505</v>
+      </c>
       <c r="O213" s="2" t="s">
         <v>448</v>
       </c>
@@ -6747,6 +7000,9 @@
         <v>412</v>
       </c>
       <c r="G214" s="2"/>
+      <c r="I214" s="8" t="s">
+        <v>505</v>
+      </c>
       <c r="O214" s="2" t="s">
         <v>448</v>
       </c>
@@ -6788,6 +7044,9 @@
       <c r="G216" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I216" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N216" s="8" t="s">
         <v>22</v>
       </c>
@@ -6811,6 +7070,9 @@
       <c r="G217" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I217" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N217" s="8" t="s">
         <v>22</v>
       </c>
@@ -6834,6 +7096,9 @@
       <c r="G218" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="I218" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="N218" s="8" t="s">
         <v>22</v>
       </c>
@@ -6854,6 +7119,9 @@
       <c r="D219" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="I219" s="8" t="s">
+        <v>500</v>
+      </c>
       <c r="O219" s="2" t="s">
         <v>449</v>
       </c>
@@ -6871,6 +7139,9 @@
       <c r="D220" s="4" t="s">
         <v>422</v>
       </c>
+      <c r="I220" s="8" t="s">
+        <v>506</v>
+      </c>
       <c r="O220" s="2" t="s">
         <v>450</v>
       </c>
@@ -6892,6 +7163,9 @@
         <v>424</v>
       </c>
       <c r="G221" s="2"/>
+      <c r="I221" s="8" t="s">
+        <v>507</v>
+      </c>
       <c r="O221" s="2" t="s">
         <v>445</v>
       </c>
@@ -6916,6 +7190,9 @@
         <v>428</v>
       </c>
       <c r="G222" s="2"/>
+      <c r="I222" s="8" t="s">
+        <v>500</v>
+      </c>
       <c r="O222" s="2" t="s">
         <v>448</v>
       </c>
@@ -6937,6 +7214,9 @@
         <v>430</v>
       </c>
       <c r="G223" s="2"/>
+      <c r="I223" s="8" t="s">
+        <v>508</v>
+      </c>
       <c r="O223" s="2" t="s">
         <v>477</v>
       </c>
@@ -6955,6 +7235,9 @@
         <v>432</v>
       </c>
       <c r="G224" s="2"/>
+      <c r="I224" s="8" t="s">
+        <v>509</v>
+      </c>
       <c r="O224" s="2" t="s">
         <v>439</v>
       </c>

</xml_diff>

<commit_message>
Added Test for reqs 177-220
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caden/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894AA35-6E1A-8F4A-93E9-170DE07822B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A6762A-45D7-D243-9776-8497ADF41A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="940" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1970,7 +1970,7 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I95" sqref="I95:I224"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated testing location for some requirements for Group 34
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caden/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlbea\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A6762A-45D7-D243-9776-8497ADF41A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF92A82-1CB2-41FE-B388-9B04AC3D54AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="940" windowWidth="25800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="4140" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1414,9 +1414,6 @@
     <t>Test 2 step 10</t>
   </si>
   <si>
-    <t>Test 2 Step 6-10</t>
-  </si>
-  <si>
     <t>Tests 2 Step 6-10</t>
   </si>
   <si>
@@ -1426,9 +1423,6 @@
     <t>Test 1/2 Step 6-10</t>
   </si>
   <si>
-    <t>Test 2 step 6-10</t>
-  </si>
-  <si>
     <t>Test 4 Step 12</t>
   </si>
   <si>
@@ -1438,12 +1432,6 @@
     <t>Test 2 Step 11</t>
   </si>
   <si>
-    <t>Test 2 Step 6-10 &amp; 12</t>
-  </si>
-  <si>
-    <t>Test 2 Step 6-10 &amp; 13</t>
-  </si>
-  <si>
     <t>Test 2 Step 5</t>
   </si>
   <si>
@@ -1478,9 +1466,6 @@
   </si>
   <si>
     <t>Instruction is hidden, when pointer is not in the input box</t>
-  </si>
-  <si>
-    <t>Test 1: steps 6-12, Test 3: steps 4-8</t>
   </si>
   <si>
     <t>Test 3: steps 4-8</t>
@@ -1572,6 +1557,21 @@
   </si>
   <si>
     <t>Success (Test 1: Step 11)</t>
+  </si>
+  <si>
+    <t>Test 1: steps 6-13, Test 3: steps 4-8</t>
+  </si>
+  <si>
+    <t>Test 2 step 6-12</t>
+  </si>
+  <si>
+    <t>Test 2 Step 6-12</t>
+  </si>
+  <si>
+    <t>Test 2 step 6-10 &amp; 12</t>
+  </si>
+  <si>
+    <t>Test 2 step 6-10 &amp; 13</t>
   </si>
 </sst>
 </file>
@@ -1970,11 +1970,11 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95:I224"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1982,21 +1982,21 @@
     <col min="4" max="4" width="81" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5" style="2" customWidth="1"/>
-    <col min="16" max="17" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.46484375" style="2" customWidth="1"/>
+    <col min="16" max="17" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="D4" s="4"/>
@@ -2062,7 +2062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
@@ -2088,7 +2088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -2114,7 +2114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -2128,13 +2128,13 @@
         <v>27</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -2149,10 +2149,10 @@
       </c>
       <c r="G8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -2167,10 +2167,10 @@
       </c>
       <c r="G9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -2185,10 +2185,10 @@
       </c>
       <c r="G10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I11" t="s">
         <v>22</v>
@@ -2214,7 +2214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>31</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="I12" t="s">
         <v>22</v>
@@ -2240,7 +2240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -2255,10 +2255,10 @@
       </c>
       <c r="G13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -2273,10 +2273,10 @@
       </c>
       <c r="G14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>31</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
@@ -2302,7 +2302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I16" t="s">
         <v>22</v>
@@ -2328,7 +2328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I17" t="s">
         <v>22</v>
@@ -2354,7 +2354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>39</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I18" t="s">
         <v>22</v>
@@ -2380,7 +2380,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>44</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I19" t="s">
         <v>22</v>
@@ -2406,7 +2406,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>31</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I20" t="s">
         <v>22</v>
@@ -2432,7 +2432,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>31</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
@@ -2458,7 +2458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I22" t="s">
         <v>22</v>
@@ -2484,7 +2484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
@@ -2510,7 +2510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -2524,13 +2524,13 @@
         <v>50</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="O24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -2544,13 +2544,13 @@
         <v>50</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>53</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I26" t="s">
         <v>22</v>
@@ -2576,7 +2576,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>55</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -2602,7 +2602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>25</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I28" t="s">
         <v>22</v>
@@ -2628,7 +2628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>31</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I29" t="s">
         <v>22</v>
@@ -2654,7 +2654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -2668,13 +2668,13 @@
         <v>59</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>59</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I31" t="s">
         <v>22</v>
@@ -2700,7 +2700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>62</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I32" t="s">
         <v>22</v>
@@ -2726,7 +2726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>64</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I33" t="s">
         <v>22</v>
@@ -2752,7 +2752,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -2767,10 +2767,10 @@
       </c>
       <c r="G34" s="2"/>
       <c r="O34" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>67</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I35" t="s">
         <v>22</v>
@@ -2796,7 +2796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>69</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I36" t="s">
         <v>22</v>
@@ -2822,7 +2822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>71</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I37" t="s">
         <v>22</v>
@@ -2848,7 +2848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>73</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I38" t="s">
         <v>22</v>
@@ -2874,7 +2874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>62</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I39" t="s">
         <v>22</v>
@@ -2900,7 +2900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -2915,10 +2915,10 @@
       </c>
       <c r="G40" s="2"/>
       <c r="O40" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>77</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I41" t="s">
         <v>22</v>
@@ -2944,7 +2944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="3">
         <v>38</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>79</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I42" t="s">
         <v>22</v>
@@ -2970,7 +2970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>81</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="I43" t="s">
         <v>22</v>
@@ -2996,7 +2996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -3010,13 +3010,13 @@
         <v>83</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="3">
         <v>41</v>
       </c>
@@ -3031,10 +3031,10 @@
       </c>
       <c r="G45" s="2"/>
       <c r="O45" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>87</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I46" t="s">
         <v>22</v>
@@ -3060,7 +3060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A47" s="3">
         <v>43</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>89</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I47" t="s">
         <v>22</v>
@@ -3086,7 +3086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>91</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I48" t="s">
         <v>22</v>
@@ -3112,7 +3112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49" s="3">
         <v>45</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>93</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I49" t="s">
         <v>22</v>
@@ -3138,7 +3138,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="3">
         <v>46</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>95</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I50" t="s">
         <v>22</v>
@@ -3164,7 +3164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="3">
         <v>47</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>97</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I51" t="s">
         <v>22</v>
@@ -3190,7 +3190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="3">
         <v>48</v>
       </c>
@@ -3208,10 +3208,10 @@
         <v>22</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A53" s="3">
         <v>49</v>
       </c>
@@ -3229,13 +3229,13 @@
       </c>
       <c r="G53" s="2"/>
       <c r="I53" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A54" s="3">
         <v>50</v>
       </c>
@@ -3253,13 +3253,13 @@
       </c>
       <c r="G54" s="2"/>
       <c r="I54" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" s="3">
         <v>51</v>
       </c>
@@ -3277,13 +3277,13 @@
       </c>
       <c r="G55" s="2"/>
       <c r="I55" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A56" s="3">
         <v>52</v>
       </c>
@@ -3301,13 +3301,13 @@
       </c>
       <c r="G56" s="2"/>
       <c r="I56" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A57" s="3">
         <v>53</v>
       </c>
@@ -3325,13 +3325,13 @@
       </c>
       <c r="G57" s="2"/>
       <c r="I57" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A58" s="3">
         <v>54</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>55</v>
       </c>
@@ -3373,13 +3373,13 @@
       </c>
       <c r="G59" s="2"/>
       <c r="I59" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>56</v>
       </c>
@@ -3397,13 +3397,13 @@
       </c>
       <c r="G60" s="2"/>
       <c r="I60" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>57</v>
       </c>
@@ -3421,13 +3421,13 @@
       </c>
       <c r="G61" s="2"/>
       <c r="I61" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>110</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I62" t="s">
         <v>22</v>
@@ -3456,7 +3456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="114" x14ac:dyDescent="0.45">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>26</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>123</v>
@@ -3473,7 +3473,7 @@
         <v>110</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="I63" t="s">
         <v>22</v>
@@ -3485,7 +3485,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="3">
         <v>60</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>110</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I64" t="s">
         <v>22</v>
@@ -3514,7 +3514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>110</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I65" t="s">
         <v>22</v>
@@ -3543,7 +3543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A66" s="3">
         <v>62</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>110</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I66" t="s">
         <v>22</v>
@@ -3572,7 +3572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A67" s="3">
         <v>63</v>
       </c>
@@ -3590,13 +3590,13 @@
       </c>
       <c r="G67" s="2"/>
       <c r="I67" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="3">
         <v>64</v>
       </c>
@@ -3614,13 +3614,13 @@
       </c>
       <c r="G68" s="2"/>
       <c r="I68" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O68" s="2" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>110</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I69" t="s">
         <v>22</v>
@@ -3649,7 +3649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A70" s="3">
         <v>66</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>110</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I70" t="s">
         <v>22</v>
@@ -3678,7 +3678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A71" s="3">
         <v>67</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>110</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I71" t="s">
         <v>22</v>
@@ -3707,7 +3707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A72" s="3">
         <v>68</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>110</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I72" t="s">
         <v>22</v>
@@ -3736,7 +3736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A73" s="3">
         <v>69</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A74" s="3">
         <v>70</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A75" s="3">
         <v>71</v>
       </c>
@@ -3793,13 +3793,13 @@
       </c>
       <c r="G75" s="2"/>
       <c r="I75" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A76" s="3">
         <v>72</v>
       </c>
@@ -3814,13 +3814,13 @@
       </c>
       <c r="G76" s="2"/>
       <c r="I76" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O76" s="2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A77" s="3">
         <v>73</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>149</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I77" t="s">
         <v>22</v>
@@ -3846,7 +3846,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A78" s="3">
         <v>74</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>151</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I78" t="s">
         <v>22</v>
@@ -3872,7 +3872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>153</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I79" t="s">
         <v>22</v>
@@ -3898,7 +3898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A80" s="3">
         <v>76</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>155</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I80" t="s">
         <v>22</v>
@@ -3924,7 +3924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A81" s="3">
         <v>77</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>157</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I81" t="s">
         <v>22</v>
@@ -3950,7 +3950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A82" s="3">
         <v>78</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>159</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I82" t="s">
         <v>22</v>
@@ -3976,7 +3976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A83" s="3">
         <v>79</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A84" s="3">
         <v>80</v>
       </c>
@@ -4015,13 +4015,13 @@
       </c>
       <c r="G84" s="2"/>
       <c r="I84" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A85" s="3">
         <v>81</v>
       </c>
@@ -4039,13 +4039,13 @@
       </c>
       <c r="G85" s="2"/>
       <c r="I85" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A86" s="3">
         <v>82</v>
       </c>
@@ -4063,13 +4063,13 @@
       </c>
       <c r="G86" s="2"/>
       <c r="I86" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A87" s="3">
         <v>83</v>
       </c>
@@ -4090,10 +4090,10 @@
         <v>22</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A88" s="3">
         <v>84</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>175</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I88" t="s">
         <v>22</v>
@@ -4119,7 +4119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A89" s="3">
         <v>85</v>
       </c>
@@ -4134,13 +4134,13 @@
       </c>
       <c r="G89" s="2"/>
       <c r="I89" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A90" s="3">
         <v>86</v>
       </c>
@@ -4158,13 +4158,13 @@
       </c>
       <c r="G90" s="2"/>
       <c r="I90" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A91" s="3">
         <v>87</v>
       </c>
@@ -4179,13 +4179,13 @@
       </c>
       <c r="G91" s="2"/>
       <c r="I91" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A92" s="3">
         <v>88</v>
       </c>
@@ -4203,13 +4203,13 @@
       </c>
       <c r="G92" s="2"/>
       <c r="I92" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>187</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I93" t="s">
         <v>22</v>
@@ -4235,7 +4235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A94" s="3">
         <v>90</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>189</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I94" t="s">
         <v>22</v>
@@ -4261,7 +4261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A95" s="3">
         <v>91</v>
       </c>
@@ -4276,10 +4276,10 @@
       </c>
       <c r="G95" s="2"/>
       <c r="O95" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A96" s="3">
         <v>92</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A97" s="3">
         <v>93</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>195</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I97" t="s">
         <v>22</v>
@@ -4323,7 +4323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A98" s="3">
         <v>94</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A99" s="3">
         <v>95</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A100" s="3">
         <v>96</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A101" s="3">
         <v>97</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>203</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I101" t="s">
         <v>22</v>
@@ -4403,7 +4403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A102" s="3">
         <v>98</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>205</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I102" t="s">
         <v>22</v>
@@ -4429,7 +4429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A103" s="3">
         <v>99</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A104" s="3">
         <v>100</v>
       </c>
@@ -4462,10 +4462,10 @@
       </c>
       <c r="G104" s="2"/>
       <c r="O104" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A105" s="3">
         <v>101</v>
       </c>
@@ -4480,10 +4480,10 @@
       </c>
       <c r="G105" s="2"/>
       <c r="O105" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A106" s="3">
         <v>102</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>205</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I106" t="s">
         <v>22</v>
@@ -4509,7 +4509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A107" s="3">
         <v>103</v>
       </c>
@@ -4524,10 +4524,10 @@
       </c>
       <c r="G107" s="2"/>
       <c r="O107" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A108" s="3">
         <v>104</v>
       </c>
@@ -4542,10 +4542,10 @@
       </c>
       <c r="G108" s="2"/>
       <c r="O108" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -4596,10 +4596,10 @@
       </c>
       <c r="G111" s="2"/>
       <c r="O111" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -4614,10 +4614,10 @@
       </c>
       <c r="G112" s="2"/>
       <c r="O112" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -4650,10 +4650,10 @@
       </c>
       <c r="G114" s="2"/>
       <c r="O114" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -4668,10 +4668,10 @@
       </c>
       <c r="G115" s="2"/>
       <c r="O115" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A116" s="3">
         <v>112</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>225</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I116" t="s">
         <v>22</v>
@@ -4697,7 +4697,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A117" s="3">
         <v>113</v>
       </c>
@@ -4712,10 +4712,10 @@
       </c>
       <c r="G117" s="2"/>
       <c r="O117" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A118" s="3">
         <v>114</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A119" s="3">
         <v>115</v>
       </c>
@@ -4748,10 +4748,10 @@
       </c>
       <c r="G119" s="2"/>
       <c r="O119" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A120" s="3">
         <v>116</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>231</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I120" t="s">
         <v>22</v>
@@ -4777,7 +4777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A121" s="3">
         <v>117</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>233</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I121" t="s">
         <v>22</v>
@@ -4803,7 +4803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A122" s="3">
         <v>118</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>235</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I122" t="s">
         <v>22</v>
@@ -4829,7 +4829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A123" s="3">
         <v>119</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>227</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I123" t="s">
         <v>22</v>
@@ -4855,7 +4855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A124" s="3">
         <v>120</v>
       </c>
@@ -4869,13 +4869,13 @@
         <v>238</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="O124" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A125" s="3">
         <v>121</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>240</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I125" t="s">
         <v>22</v>
@@ -4901,7 +4901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A126" s="3">
         <v>122</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>231</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I126" t="s">
         <v>22</v>
@@ -4927,7 +4927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A127" s="3">
         <v>123</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A128" s="3">
         <v>124</v>
       </c>
@@ -4959,13 +4959,13 @@
         <v>244</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="O128" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A129" s="3">
         <v>125</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>246</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I129" t="s">
         <v>22</v>
@@ -4991,7 +4991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A130" s="3">
         <v>126</v>
       </c>
@@ -5006,10 +5006,10 @@
       </c>
       <c r="G130" s="2"/>
       <c r="O130" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A131" s="3">
         <v>127</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>250</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I131" t="s">
         <v>22</v>
@@ -5035,7 +5035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A132" s="3">
         <v>128</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>252</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I132" t="s">
         <v>22</v>
@@ -5061,7 +5061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A133" s="3">
         <v>129</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>254</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="I133" t="s">
         <v>22</v>
@@ -5087,7 +5087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A134" s="3">
         <v>130</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>256</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="I134" t="s">
         <v>22</v>
@@ -5113,7 +5113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A135" s="3">
         <v>131</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A136" s="3">
         <v>132</v>
       </c>
@@ -5146,10 +5146,10 @@
       </c>
       <c r="G136" s="2"/>
       <c r="O136" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A137" s="3">
         <v>133</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>250</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I137" s="8" t="s">
         <v>22</v>
@@ -5175,7 +5175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A138" s="3">
         <v>134</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>250</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I138" s="8" t="s">
         <v>22</v>
@@ -5201,7 +5201,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A139" s="3">
         <v>135</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A140" s="3">
         <v>136</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>264</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I140" s="8" t="s">
         <v>22</v>
@@ -5245,7 +5245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" ht="185.25" x14ac:dyDescent="0.45">
       <c r="A141" s="3">
         <v>137</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>266</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I141" s="8" t="s">
         <v>22</v>
@@ -5271,7 +5271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A142" s="3">
         <v>138</v>
       </c>
@@ -5289,13 +5289,13 @@
       </c>
       <c r="G142" s="2"/>
       <c r="O142" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="R142" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A143" s="3">
         <v>139</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>273</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I143" s="8" t="s">
         <v>22</v>
@@ -5324,7 +5324,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A144" s="3">
         <v>140</v>
       </c>
@@ -5339,10 +5339,10 @@
       </c>
       <c r="G144" s="2"/>
       <c r="O144" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="145" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A145" s="3">
         <v>141</v>
       </c>
@@ -5357,10 +5357,10 @@
       </c>
       <c r="G145" s="2"/>
       <c r="O145" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A146" s="3">
         <v>142</v>
       </c>
@@ -5375,10 +5375,10 @@
       </c>
       <c r="G146" s="2"/>
       <c r="O146" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="147" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A147" s="3">
         <v>143</v>
       </c>
@@ -5393,10 +5393,10 @@
       </c>
       <c r="G147" s="2"/>
       <c r="O147" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A148" s="3">
         <v>144</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>272</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I148" s="8" t="s">
         <v>22</v>
@@ -5422,7 +5422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A149" s="3">
         <v>145</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>268</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I149" s="8" t="s">
         <v>22</v>
@@ -5448,7 +5448,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A150" s="3">
         <v>146</v>
       </c>
@@ -5463,10 +5463,10 @@
       </c>
       <c r="G150" s="2"/>
       <c r="O150" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A151" s="3">
         <v>147</v>
       </c>
@@ -5481,10 +5481,10 @@
       </c>
       <c r="G151" s="2"/>
       <c r="O151" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="152" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A152" s="3">
         <v>148</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>283</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I152" s="8" t="s">
         <v>22</v>
@@ -5510,7 +5510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A153" s="3">
         <v>149</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>285</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I153" s="8" t="s">
         <v>22</v>
@@ -5536,7 +5536,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A154" s="3">
         <v>150</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A155" s="3">
         <v>151</v>
       </c>
@@ -5571,10 +5571,10 @@
       </c>
       <c r="G155" s="2"/>
       <c r="O155" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A156" s="3">
         <v>152</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>292</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I156" s="8" t="s">
         <v>22</v>
@@ -5600,7 +5600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A157" s="3">
         <v>153</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>294</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I157" s="8" t="s">
         <v>22</v>
@@ -5626,7 +5626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A158" s="3">
         <v>154</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>296</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I158" s="8" t="s">
         <v>22</v>
@@ -5652,7 +5652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A159" s="3">
         <v>155</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>298</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I159" s="8" t="s">
         <v>22</v>
@@ -5678,7 +5678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A160" s="3">
         <v>156</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>300</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I160" s="8" t="s">
         <v>22</v>
@@ -5704,7 +5704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A161" s="3">
         <v>157</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>302</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I161" s="8" t="s">
         <v>22</v>
@@ -5730,7 +5730,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A162" s="3">
         <v>158</v>
       </c>
@@ -5745,10 +5745,10 @@
       </c>
       <c r="G162" s="2"/>
       <c r="O162" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A163" s="3">
         <v>159</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>306</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I163" s="8" t="s">
         <v>22</v>
@@ -5774,7 +5774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A164" s="3">
         <v>160</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A165" s="3">
         <v>161</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A166" s="3">
         <v>162</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>312</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I166" s="8" t="s">
         <v>22</v>
@@ -5836,7 +5836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A167" s="3">
         <v>163</v>
       </c>
@@ -5850,13 +5850,13 @@
         <v>314</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="O167" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A168" s="3">
         <v>164</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A169" s="3">
         <v>165</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>318</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I169" s="8" t="s">
         <v>22</v>
@@ -5900,7 +5900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A170" s="3">
         <v>166</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>318</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I170" s="8" t="s">
         <v>22</v>
@@ -5926,7 +5926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A171" s="3">
         <v>167</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>321</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I171" s="8" t="s">
         <v>22</v>
@@ -5952,7 +5952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A172" s="3">
         <v>168</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>323</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I172" s="8" t="s">
         <v>22</v>
@@ -5978,7 +5978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A173" s="3">
         <v>169</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>325</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I173" s="8" t="s">
         <v>22</v>
@@ -6004,7 +6004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A174" s="3">
         <v>170</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>327</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I174" s="8" t="s">
         <v>22</v>
@@ -6030,7 +6030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A175" s="3">
         <v>171</v>
       </c>
@@ -6045,10 +6045,10 @@
       </c>
       <c r="G175" s="2"/>
       <c r="O175" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="176" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A176" s="3">
         <v>172</v>
       </c>
@@ -6063,10 +6063,10 @@
       </c>
       <c r="G176" s="2"/>
       <c r="O176" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="177" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A177" s="3">
         <v>173</v>
       </c>
@@ -6081,10 +6081,10 @@
       </c>
       <c r="G177" s="2"/>
       <c r="O177" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="178" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A178" s="3">
         <v>174</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A179" s="3">
         <v>175</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>337</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I179" s="8" t="s">
         <v>22</v>
@@ -6128,7 +6128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A180" s="3">
         <v>176</v>
       </c>
@@ -6143,10 +6143,10 @@
       </c>
       <c r="G180" s="2"/>
       <c r="O180" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="181" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A181" s="3">
         <v>177</v>
       </c>
@@ -6160,13 +6160,13 @@
         <v>341</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I181" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="182" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A182" s="3">
         <v>178</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>343</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I182" s="8" t="s">
         <v>22</v>
@@ -6192,7 +6192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A183" s="3">
         <v>179</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>345</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I183" s="8" t="s">
         <v>22</v>
@@ -6218,7 +6218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A184" s="3">
         <v>180</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>347</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I184" s="8" t="s">
         <v>22</v>
@@ -6244,7 +6244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A185" s="3">
         <v>181</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>349</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I185" s="8" t="s">
         <v>22</v>
@@ -6270,7 +6270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A186" s="3">
         <v>182</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>351</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I186" s="8" t="s">
         <v>22</v>
@@ -6296,7 +6296,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A187" s="3">
         <v>183</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>353</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I187" s="8" t="s">
         <v>22</v>
@@ -6322,7 +6322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A188" s="3">
         <v>184</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>355</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I188" s="8" t="s">
         <v>22</v>
@@ -6348,7 +6348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A189" s="3">
         <v>185</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>353</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I189" s="8" t="s">
         <v>22</v>
@@ -6374,7 +6374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A190" s="3">
         <v>186</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>335</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I190" s="8" t="s">
         <v>22</v>
@@ -6400,7 +6400,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A191" s="3">
         <v>187</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>359</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I191" s="8" t="s">
         <v>22</v>
@@ -6426,7 +6426,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A192" s="3">
         <v>188</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>361</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I192" s="8" t="s">
         <v>22</v>
@@ -6452,7 +6452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A193" s="3">
         <v>189</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>363</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I193" s="8" t="s">
         <v>22</v>
@@ -6478,7 +6478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A194" s="3">
         <v>190</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>365</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I194" s="8" t="s">
         <v>22</v>
@@ -6504,7 +6504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A195" s="3">
         <v>191</v>
       </c>
@@ -6525,10 +6525,10 @@
         <v>22</v>
       </c>
       <c r="O195" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A196" s="3">
         <v>192</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>370</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I196" s="8" t="s">
         <v>22</v>
@@ -6554,7 +6554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A197" s="3">
         <v>193</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>372</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I197" s="8" t="s">
         <v>22</v>
@@ -6580,7 +6580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A198" s="3">
         <v>194</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>374</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I198" s="8" t="s">
         <v>22</v>
@@ -6606,7 +6606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A199" s="3">
         <v>195</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>376</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="I199" s="8" t="s">
         <v>22</v>
@@ -6632,7 +6632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A200" s="3">
         <v>196</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>378</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I200" s="8" t="s">
         <v>22</v>
@@ -6658,7 +6658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A201" s="3">
         <v>197</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>380</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I201" s="8" t="s">
         <v>22</v>
@@ -6684,7 +6684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A202" s="3">
         <v>198</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>382</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="I202" s="8" t="s">
         <v>22</v>
@@ -6710,7 +6710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A203" s="3">
         <v>199</v>
       </c>
@@ -6724,7 +6724,7 @@
         <v>384</v>
       </c>
       <c r="G203" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="I203" s="8" t="s">
         <v>22</v>
@@ -6736,7 +6736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A204" s="3">
         <v>200</v>
       </c>
@@ -6754,10 +6754,10 @@
         <v>22</v>
       </c>
       <c r="O204" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A205" s="3">
         <v>201</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>353</v>
       </c>
       <c r="G205" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I205" s="8" t="s">
         <v>22</v>
@@ -6783,7 +6783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A206" s="3">
         <v>202</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>389</v>
       </c>
       <c r="G206" s="4" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I206" s="8" t="s">
         <v>22</v>
@@ -6809,7 +6809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A207" s="3">
         <v>203</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>391</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I207" s="8" t="s">
         <v>22</v>
@@ -6838,7 +6838,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="208" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A208" s="3">
         <v>204</v>
       </c>
@@ -6855,16 +6855,16 @@
         <v>395</v>
       </c>
       <c r="G208" s="2" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="I208" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="O208" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="209" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A209" s="3">
         <v>205</v>
       </c>
@@ -6882,13 +6882,13 @@
       </c>
       <c r="G209" s="2"/>
       <c r="I209" s="8" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="O209" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="210" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A210" s="3">
         <v>206</v>
       </c>
@@ -6903,7 +6903,7 @@
       </c>
       <c r="G210" s="2"/>
       <c r="I210" s="8" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="O210" s="2" t="s">
         <v>23</v>
@@ -6912,7 +6912,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A211" s="3">
         <v>207</v>
       </c>
@@ -6927,13 +6927,13 @@
       </c>
       <c r="G211" s="4"/>
       <c r="I211" s="8" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="O211" s="2" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A212" s="3">
         <v>208</v>
       </c>
@@ -6951,13 +6951,13 @@
       </c>
       <c r="G212" s="2"/>
       <c r="I212" s="8" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="O212" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="213" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A213" s="3">
         <v>209</v>
       </c>
@@ -6974,16 +6974,16 @@
         <v>409</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="I213" s="8" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="O213" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A214" s="3">
         <v>210</v>
       </c>
@@ -7001,13 +7001,13 @@
       </c>
       <c r="G214" s="2"/>
       <c r="I214" s="8" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="O214" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A215" s="3">
         <v>211</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A216" s="3">
         <v>212</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>416</v>
       </c>
       <c r="G216" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I216" s="8" t="s">
         <v>22</v>
@@ -7054,7 +7054,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A217" s="3">
         <v>213</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>416</v>
       </c>
       <c r="G217" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I217" s="8" t="s">
         <v>22</v>
@@ -7080,7 +7080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A218" s="3">
         <v>214</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>419</v>
       </c>
       <c r="G218" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I218" s="8" t="s">
         <v>22</v>
@@ -7106,7 +7106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A219" s="3">
         <v>215</v>
       </c>
@@ -7120,13 +7120,13 @@
         <v>400</v>
       </c>
       <c r="I219" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="O219" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A220" s="3">
         <v>216</v>
       </c>
@@ -7140,13 +7140,13 @@
         <v>422</v>
       </c>
       <c r="I220" s="8" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="O220" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A221" s="3">
         <v>217</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>25</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D221" s="4" t="s">
         <v>423</v>
@@ -7164,7 +7164,7 @@
       </c>
       <c r="G221" s="2"/>
       <c r="I221" s="8" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="O221" s="2" t="s">
         <v>445</v>
@@ -7173,7 +7173,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A222" s="3">
         <v>218</v>
       </c>
@@ -7191,13 +7191,13 @@
       </c>
       <c r="G222" s="2"/>
       <c r="I222" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="O222" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A223" s="3">
         <v>219</v>
       </c>
@@ -7215,13 +7215,13 @@
       </c>
       <c r="G223" s="2"/>
       <c r="I223" s="8" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="O223" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="224" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A224" s="3">
         <v>220</v>
       </c>
@@ -7236,18 +7236,18 @@
       </c>
       <c r="G224" s="2"/>
       <c r="I224" s="8" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="O224" s="2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R230" t="s">
         <v>433</v>
       </c>

</xml_diff>

<commit_message>
Adding Group 25 untestables
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fergie/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mryanpatterson/Documents/CSE3310/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D226B3-CCC6-6C45-B4E5-8708E624622B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D831A5D-B122-1B43-966C-C6A2DF31DB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29920" yWindow="-43680" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="503">
   <si>
     <t>Tested By</t>
   </si>
@@ -1949,8 +1949,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K227" sqref="K227"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F225" sqref="F225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2054,6 +2054,9 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
@@ -2080,6 +2083,9 @@
       <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
       <c r="I6" t="s">
         <v>22</v>
       </c>
@@ -2106,6 +2112,9 @@
       <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
       <c r="K7" t="s">
         <v>487</v>
       </c>
@@ -2186,6 +2195,9 @@
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
       <c r="I11" t="s">
         <v>22</v>
       </c>
@@ -2212,6 +2224,9 @@
       <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" t="s">
         <v>22</v>
       </c>
@@ -2278,6 +2293,9 @@
       <c r="D15" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
       <c r="I15" t="s">
         <v>22</v>
       </c>
@@ -2304,6 +2322,9 @@
       <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
       <c r="I16" t="s">
         <v>22</v>
       </c>
@@ -2330,6 +2351,9 @@
       <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
       <c r="I17" t="s">
         <v>22</v>
       </c>
@@ -2356,6 +2380,9 @@
       <c r="D18" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
       <c r="I18" t="s">
         <v>22</v>
       </c>
@@ -2382,6 +2409,9 @@
       <c r="D19" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
       <c r="I19" t="s">
         <v>22</v>
       </c>
@@ -2408,6 +2438,9 @@
       <c r="D20" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
       <c r="I20" t="s">
         <v>22</v>
       </c>
@@ -2434,6 +2467,9 @@
       <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
@@ -2460,6 +2496,9 @@
       <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
       <c r="I22" t="s">
         <v>22</v>
       </c>
@@ -2486,6 +2525,9 @@
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
       <c r="I23" t="s">
         <v>22</v>
       </c>
@@ -2512,6 +2554,9 @@
       <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
       <c r="K24" t="s">
         <v>487</v>
       </c>
@@ -2532,6 +2577,9 @@
       <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
       <c r="K25" t="s">
         <v>487</v>
       </c>
@@ -2552,6 +2600,9 @@
       <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
       <c r="I26" t="s">
         <v>22</v>
       </c>
@@ -2577,6 +2628,9 @@
       </c>
       <c r="D27" s="4" t="s">
         <v>55</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -2604,6 +2658,9 @@
       <c r="D28" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
       <c r="I28" t="s">
         <v>22</v>
       </c>
@@ -2630,6 +2687,9 @@
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
       <c r="I29" t="s">
         <v>22</v>
       </c>
@@ -2676,6 +2736,9 @@
       <c r="D31" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
       <c r="I31" t="s">
         <v>22</v>
       </c>
@@ -2702,6 +2765,9 @@
       <c r="D32" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
       <c r="I32" t="s">
         <v>22</v>
       </c>
@@ -2728,6 +2794,9 @@
       <c r="D33" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
       <c r="I33" t="s">
         <v>22</v>
       </c>
@@ -2774,6 +2843,9 @@
       <c r="D35" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
       <c r="I35" t="s">
         <v>22</v>
       </c>
@@ -2800,6 +2872,9 @@
       <c r="D36" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
       <c r="I36" t="s">
         <v>22</v>
       </c>
@@ -2826,6 +2901,9 @@
       <c r="D37" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
       <c r="I37" t="s">
         <v>22</v>
       </c>
@@ -2852,6 +2930,9 @@
       <c r="D38" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
       <c r="I38" t="s">
         <v>22</v>
       </c>
@@ -2878,6 +2959,9 @@
       <c r="D39" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
       <c r="I39" t="s">
         <v>22</v>
       </c>
@@ -2924,6 +3008,9 @@
       <c r="D41" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
       <c r="I41" t="s">
         <v>22</v>
       </c>
@@ -2950,6 +3037,9 @@
       <c r="D42" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
       <c r="I42" t="s">
         <v>22</v>
       </c>
@@ -2976,6 +3066,9 @@
       <c r="D43" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
       <c r="I43" t="s">
         <v>22</v>
       </c>
@@ -3042,6 +3135,9 @@
       <c r="D46" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
       <c r="I46" t="s">
         <v>22</v>
       </c>
@@ -3068,6 +3164,9 @@
       <c r="D47" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
       <c r="I47" t="s">
         <v>22</v>
       </c>
@@ -3094,6 +3193,9 @@
       <c r="D48" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
       <c r="I48" t="s">
         <v>22</v>
       </c>
@@ -3120,6 +3222,9 @@
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
       <c r="I49" t="s">
         <v>22</v>
       </c>
@@ -3146,6 +3251,9 @@
       <c r="D50" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
       <c r="I50" t="s">
         <v>22</v>
       </c>
@@ -3172,6 +3280,9 @@
       <c r="D51" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
       <c r="I51" t="s">
         <v>22</v>
       </c>
@@ -3198,6 +3309,9 @@
       <c r="D52" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
       <c r="I52" t="s">
         <v>22</v>
       </c>
@@ -3354,6 +3468,9 @@
       <c r="E58" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="F58" t="s">
+        <v>22</v>
+      </c>
       <c r="I58" t="s">
         <v>22</v>
       </c>
@@ -3406,6 +3523,9 @@
       <c r="E60" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="F60" t="s">
+        <v>22</v>
+      </c>
       <c r="I60" t="s">
         <v>486</v>
       </c>
@@ -3458,6 +3578,9 @@
       <c r="E62" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F62" t="s">
+        <v>22</v>
+      </c>
       <c r="I62" t="s">
         <v>22</v>
       </c>
@@ -3487,6 +3610,9 @@
       <c r="E63" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F63" t="s">
+        <v>22</v>
+      </c>
       <c r="G63" s="2" t="s">
         <v>482</v>
       </c>
@@ -3519,6 +3645,9 @@
       <c r="E64" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F64" t="s">
+        <v>22</v>
+      </c>
       <c r="I64" t="s">
         <v>22</v>
       </c>
@@ -3548,6 +3677,9 @@
       <c r="E65" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F65" t="s">
+        <v>22</v>
+      </c>
       <c r="I65" t="s">
         <v>22</v>
       </c>
@@ -3577,6 +3709,9 @@
       <c r="E66" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F66" t="s">
+        <v>22</v>
+      </c>
       <c r="I66" t="s">
         <v>22</v>
       </c>
@@ -3655,6 +3790,9 @@
       <c r="E69" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F69" t="s">
+        <v>22</v>
+      </c>
       <c r="I69" t="s">
         <v>22</v>
       </c>
@@ -3684,6 +3822,9 @@
       <c r="E70" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F70" t="s">
+        <v>22</v>
+      </c>
       <c r="I70" t="s">
         <v>22</v>
       </c>
@@ -3713,6 +3854,9 @@
       <c r="E71" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F71" t="s">
+        <v>22</v>
+      </c>
       <c r="I71" t="s">
         <v>22</v>
       </c>
@@ -3742,6 +3886,9 @@
       <c r="E72" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F72" t="s">
+        <v>22</v>
+      </c>
       <c r="I72" t="s">
         <v>22</v>
       </c>
@@ -3768,6 +3915,9 @@
       <c r="D73" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="F73" t="s">
+        <v>22</v>
+      </c>
       <c r="I73" t="s">
         <v>22</v>
       </c>
@@ -3791,6 +3941,9 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="F74" t="s">
+        <v>22</v>
+      </c>
       <c r="I74" t="s">
         <v>22</v>
       </c>
@@ -3814,6 +3967,9 @@
       <c r="D75" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="F75" t="s">
+        <v>22</v>
+      </c>
       <c r="I75" t="s">
         <v>486</v>
       </c>
@@ -3860,6 +4016,9 @@
       <c r="D77" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="F77" t="s">
+        <v>22</v>
+      </c>
       <c r="I77" t="s">
         <v>22</v>
       </c>
@@ -3886,6 +4045,9 @@
       <c r="D78" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="F78" t="s">
+        <v>22</v>
+      </c>
       <c r="I78" t="s">
         <v>22</v>
       </c>
@@ -3912,6 +4074,9 @@
       <c r="D79" s="4" t="s">
         <v>153</v>
       </c>
+      <c r="F79" t="s">
+        <v>22</v>
+      </c>
       <c r="I79" t="s">
         <v>22</v>
       </c>
@@ -3938,6 +4103,9 @@
       <c r="D80" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="F80" t="s">
+        <v>22</v>
+      </c>
       <c r="I80" t="s">
         <v>22</v>
       </c>
@@ -3964,6 +4132,9 @@
       <c r="D81" s="4" t="s">
         <v>157</v>
       </c>
+      <c r="F81" t="s">
+        <v>22</v>
+      </c>
       <c r="I81" t="s">
         <v>22</v>
       </c>
@@ -3990,6 +4161,9 @@
       <c r="D82" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="F82" t="s">
+        <v>22</v>
+      </c>
       <c r="I82" t="s">
         <v>22</v>
       </c>
@@ -4016,6 +4190,9 @@
       <c r="D83" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="F83" t="s">
+        <v>22</v>
+      </c>
       <c r="I83" t="s">
         <v>22</v>
       </c>
@@ -4094,6 +4271,9 @@
       <c r="E86" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="F86" t="s">
+        <v>22</v>
+      </c>
       <c r="I86" t="s">
         <v>486</v>
       </c>
@@ -4120,6 +4300,9 @@
       <c r="E87" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="F87" t="s">
+        <v>22</v>
+      </c>
       <c r="I87" t="s">
         <v>22</v>
       </c>
@@ -4143,6 +4326,9 @@
       <c r="D88" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="F88" t="s">
+        <v>22</v>
+      </c>
       <c r="I88" t="s">
         <v>22</v>
       </c>
@@ -4195,6 +4381,9 @@
       <c r="E90" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="F90" t="s">
+        <v>22</v>
+      </c>
       <c r="I90" t="s">
         <v>486</v>
       </c>
@@ -4267,6 +4456,9 @@
       <c r="D93" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="F93" t="s">
+        <v>22</v>
+      </c>
       <c r="I93" t="s">
         <v>22</v>
       </c>
@@ -4293,6 +4485,9 @@
       <c r="D94" s="4" t="s">
         <v>189</v>
       </c>
+      <c r="F94" t="s">
+        <v>22</v>
+      </c>
       <c r="I94" t="s">
         <v>22</v>
       </c>
@@ -4359,6 +4554,9 @@
       <c r="D97" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="F97" t="s">
+        <v>22</v>
+      </c>
       <c r="K97" t="s">
         <v>487</v>
       </c>
@@ -4442,6 +4640,9 @@
       <c r="D101" s="4" t="s">
         <v>203</v>
       </c>
+      <c r="F101" t="s">
+        <v>22</v>
+      </c>
       <c r="K101" t="s">
         <v>487</v>
       </c>
@@ -4465,6 +4666,9 @@
       <c r="D102" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="F102" t="s">
+        <v>22</v>
+      </c>
       <c r="K102" t="s">
         <v>487</v>
       </c>
@@ -4548,6 +4752,9 @@
       <c r="D106" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="F106" t="s">
+        <v>22</v>
+      </c>
       <c r="K106" t="s">
         <v>487</v>
       </c>
@@ -4611,6 +4818,9 @@
       <c r="D109" s="4" t="s">
         <v>216</v>
       </c>
+      <c r="F109" t="s">
+        <v>22</v>
+      </c>
       <c r="K109" t="s">
         <v>487</v>
       </c>
@@ -4631,6 +4841,9 @@
       <c r="D110" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="F110" t="s">
+        <v>22</v>
+      </c>
       <c r="K110" t="s">
         <v>487</v>
       </c>
@@ -4691,6 +4904,9 @@
       <c r="D113" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F113" t="s">
+        <v>22</v>
+      </c>
       <c r="K113" t="s">
         <v>487</v>
       </c>
@@ -4751,6 +4967,9 @@
       <c r="D116" s="4" t="s">
         <v>225</v>
       </c>
+      <c r="F116" t="s">
+        <v>22</v>
+      </c>
       <c r="K116" t="s">
         <v>487</v>
       </c>
@@ -4834,6 +5053,9 @@
       <c r="D120" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="F120" t="s">
+        <v>22</v>
+      </c>
       <c r="K120" t="s">
         <v>487</v>
       </c>
@@ -4857,6 +5079,9 @@
       <c r="D121" s="4" t="s">
         <v>233</v>
       </c>
+      <c r="F121" t="s">
+        <v>22</v>
+      </c>
       <c r="K121" t="s">
         <v>487</v>
       </c>
@@ -4880,6 +5105,9 @@
       <c r="D122" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="F122" t="s">
+        <v>22</v>
+      </c>
       <c r="K122" t="s">
         <v>487</v>
       </c>
@@ -4903,6 +5131,9 @@
       <c r="D123" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="F123" t="s">
+        <v>22</v>
+      </c>
       <c r="K123" t="s">
         <v>487</v>
       </c>
@@ -4926,6 +5157,9 @@
       <c r="D124" s="4" t="s">
         <v>238</v>
       </c>
+      <c r="F124" t="s">
+        <v>22</v>
+      </c>
       <c r="K124" t="s">
         <v>487</v>
       </c>
@@ -4946,6 +5180,9 @@
       <c r="D125" s="4" t="s">
         <v>240</v>
       </c>
+      <c r="F125" t="s">
+        <v>22</v>
+      </c>
       <c r="K125" t="s">
         <v>487</v>
       </c>
@@ -4969,6 +5206,9 @@
       <c r="D126" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="F126" t="s">
+        <v>22</v>
+      </c>
       <c r="K126" t="s">
         <v>487</v>
       </c>
@@ -4992,6 +5232,9 @@
       <c r="D127" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="F127" t="s">
+        <v>22</v>
+      </c>
       <c r="K127" t="s">
         <v>487</v>
       </c>
@@ -5012,6 +5255,9 @@
       <c r="D128" s="4" t="s">
         <v>244</v>
       </c>
+      <c r="F128" t="s">
+        <v>22</v>
+      </c>
       <c r="K128" t="s">
         <v>487</v>
       </c>
@@ -5032,6 +5278,9 @@
       <c r="D129" s="4" t="s">
         <v>246</v>
       </c>
+      <c r="F129" t="s">
+        <v>22</v>
+      </c>
       <c r="K129" t="s">
         <v>487</v>
       </c>
@@ -5072,6 +5321,9 @@
       <c r="D131" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="F131" t="s">
+        <v>22</v>
+      </c>
       <c r="K131" t="s">
         <v>487</v>
       </c>
@@ -5095,6 +5347,9 @@
       <c r="D132" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="F132" t="s">
+        <v>22</v>
+      </c>
       <c r="K132" t="s">
         <v>487</v>
       </c>
@@ -5118,6 +5373,9 @@
       <c r="D133" s="6" t="s">
         <v>254</v>
       </c>
+      <c r="F133" t="s">
+        <v>22</v>
+      </c>
       <c r="K133" t="s">
         <v>487</v>
       </c>
@@ -5141,6 +5399,9 @@
       <c r="D134" s="6" t="s">
         <v>256</v>
       </c>
+      <c r="F134" t="s">
+        <v>22</v>
+      </c>
       <c r="K134" t="s">
         <v>487</v>
       </c>
@@ -5204,6 +5465,9 @@
       <c r="D137" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="F137" t="s">
+        <v>22</v>
+      </c>
       <c r="K137" t="s">
         <v>487</v>
       </c>
@@ -5227,6 +5491,9 @@
       <c r="D138" s="6" t="s">
         <v>250</v>
       </c>
+      <c r="F138" t="s">
+        <v>22</v>
+      </c>
       <c r="K138" t="s">
         <v>487</v>
       </c>
@@ -5270,6 +5537,9 @@
       <c r="D140" s="6" t="s">
         <v>264</v>
       </c>
+      <c r="F140" t="s">
+        <v>22</v>
+      </c>
       <c r="K140" t="s">
         <v>487</v>
       </c>
@@ -5293,6 +5563,9 @@
       <c r="D141" s="6" t="s">
         <v>266</v>
       </c>
+      <c r="F141" t="s">
+        <v>22</v>
+      </c>
       <c r="K141" t="s">
         <v>487</v>
       </c>
@@ -5345,6 +5618,9 @@
       <c r="E143" s="4" t="s">
         <v>273</v>
       </c>
+      <c r="F143" t="s">
+        <v>22</v>
+      </c>
       <c r="K143" t="s">
         <v>487</v>
       </c>
@@ -5448,6 +5724,9 @@
       <c r="D148" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F148" t="s">
+        <v>22</v>
+      </c>
       <c r="K148" t="s">
         <v>487</v>
       </c>
@@ -5471,6 +5750,9 @@
       <c r="D149" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="F149" t="s">
+        <v>22</v>
+      </c>
       <c r="K149" t="s">
         <v>487</v>
       </c>
@@ -5534,6 +5816,9 @@
       <c r="D152" s="4" t="s">
         <v>283</v>
       </c>
+      <c r="F152" t="s">
+        <v>22</v>
+      </c>
       <c r="K152" t="s">
         <v>487</v>
       </c>
@@ -5557,6 +5842,9 @@
       <c r="D153" s="4" t="s">
         <v>285</v>
       </c>
+      <c r="F153" t="s">
+        <v>22</v>
+      </c>
       <c r="K153" t="s">
         <v>487</v>
       </c>
@@ -5621,6 +5909,9 @@
       <c r="D156" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="F156" t="s">
+        <v>22</v>
+      </c>
       <c r="K156" t="s">
         <v>487</v>
       </c>
@@ -5644,6 +5935,9 @@
       <c r="D157" s="4" t="s">
         <v>294</v>
       </c>
+      <c r="F157" t="s">
+        <v>22</v>
+      </c>
       <c r="K157" t="s">
         <v>487</v>
       </c>
@@ -5667,6 +5961,9 @@
       <c r="D158" s="4" t="s">
         <v>296</v>
       </c>
+      <c r="F158" t="s">
+        <v>22</v>
+      </c>
       <c r="K158" t="s">
         <v>487</v>
       </c>
@@ -5690,6 +5987,9 @@
       <c r="D159" s="4" t="s">
         <v>298</v>
       </c>
+      <c r="F159" t="s">
+        <v>22</v>
+      </c>
       <c r="K159" t="s">
         <v>487</v>
       </c>
@@ -5713,6 +6013,9 @@
       <c r="D160" s="4" t="s">
         <v>300</v>
       </c>
+      <c r="F160" t="s">
+        <v>22</v>
+      </c>
       <c r="K160" t="s">
         <v>487</v>
       </c>
@@ -5736,6 +6039,9 @@
       <c r="D161" s="4" t="s">
         <v>302</v>
       </c>
+      <c r="F161" t="s">
+        <v>22</v>
+      </c>
       <c r="K161" t="s">
         <v>487</v>
       </c>
@@ -5779,6 +6085,9 @@
       <c r="D163" s="4" t="s">
         <v>306</v>
       </c>
+      <c r="F163" t="s">
+        <v>22</v>
+      </c>
       <c r="K163" t="s">
         <v>487</v>
       </c>
@@ -5802,6 +6111,9 @@
       <c r="D164" s="4" t="s">
         <v>308</v>
       </c>
+      <c r="F164" t="s">
+        <v>22</v>
+      </c>
       <c r="K164" t="s">
         <v>487</v>
       </c>
@@ -5822,6 +6134,9 @@
       <c r="D165" s="4" t="s">
         <v>310</v>
       </c>
+      <c r="F165" t="s">
+        <v>22</v>
+      </c>
       <c r="K165" t="s">
         <v>487</v>
       </c>
@@ -5842,6 +6157,9 @@
       <c r="D166" s="4" t="s">
         <v>312</v>
       </c>
+      <c r="F166" t="s">
+        <v>22</v>
+      </c>
       <c r="K166" t="s">
         <v>487</v>
       </c>
@@ -5865,6 +6183,9 @@
       <c r="D167" s="4" t="s">
         <v>314</v>
       </c>
+      <c r="F167" t="s">
+        <v>22</v>
+      </c>
       <c r="K167" t="s">
         <v>487</v>
       </c>
@@ -5885,6 +6206,9 @@
       <c r="D168" s="4" t="s">
         <v>316</v>
       </c>
+      <c r="F168" t="s">
+        <v>22</v>
+      </c>
       <c r="K168" t="s">
         <v>487</v>
       </c>
@@ -5905,6 +6229,9 @@
       <c r="D169" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="F169" t="s">
+        <v>22</v>
+      </c>
       <c r="K169" t="s">
         <v>487</v>
       </c>
@@ -5928,6 +6255,9 @@
       <c r="D170" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="F170" t="s">
+        <v>22</v>
+      </c>
       <c r="K170" t="s">
         <v>487</v>
       </c>
@@ -5951,6 +6281,9 @@
       <c r="D171" s="4" t="s">
         <v>321</v>
       </c>
+      <c r="F171" t="s">
+        <v>22</v>
+      </c>
       <c r="K171" t="s">
         <v>487</v>
       </c>
@@ -5974,6 +6307,9 @@
       <c r="D172" s="4" t="s">
         <v>323</v>
       </c>
+      <c r="F172" t="s">
+        <v>22</v>
+      </c>
       <c r="K172" t="s">
         <v>487</v>
       </c>
@@ -5997,6 +6333,9 @@
       <c r="D173" s="4" t="s">
         <v>325</v>
       </c>
+      <c r="F173" t="s">
+        <v>22</v>
+      </c>
       <c r="K173" t="s">
         <v>487</v>
       </c>
@@ -6020,6 +6359,9 @@
       <c r="D174" s="4" t="s">
         <v>327</v>
       </c>
+      <c r="F174" t="s">
+        <v>22</v>
+      </c>
       <c r="K174" t="s">
         <v>487</v>
       </c>
@@ -6123,6 +6465,9 @@
       <c r="D179" s="4" t="s">
         <v>337</v>
       </c>
+      <c r="F179" t="s">
+        <v>22</v>
+      </c>
       <c r="K179" t="s">
         <v>487</v>
       </c>
@@ -6183,6 +6528,9 @@
       <c r="D182" s="4" t="s">
         <v>343</v>
       </c>
+      <c r="F182" t="s">
+        <v>22</v>
+      </c>
       <c r="K182" t="s">
         <v>487</v>
       </c>
@@ -6206,6 +6554,9 @@
       <c r="D183" s="4" t="s">
         <v>345</v>
       </c>
+      <c r="F183" t="s">
+        <v>22</v>
+      </c>
       <c r="K183" t="s">
         <v>487</v>
       </c>
@@ -6229,6 +6580,9 @@
       <c r="D184" s="4" t="s">
         <v>347</v>
       </c>
+      <c r="F184" t="s">
+        <v>22</v>
+      </c>
       <c r="K184" t="s">
         <v>487</v>
       </c>
@@ -6252,6 +6606,9 @@
       <c r="D185" s="4" t="s">
         <v>349</v>
       </c>
+      <c r="F185" t="s">
+        <v>22</v>
+      </c>
       <c r="K185" t="s">
         <v>487</v>
       </c>
@@ -6275,6 +6632,9 @@
       <c r="D186" s="4" t="s">
         <v>351</v>
       </c>
+      <c r="F186" t="s">
+        <v>22</v>
+      </c>
       <c r="K186" t="s">
         <v>487</v>
       </c>
@@ -6298,6 +6658,9 @@
       <c r="D187" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="F187" t="s">
+        <v>22</v>
+      </c>
       <c r="K187" t="s">
         <v>487</v>
       </c>
@@ -6321,6 +6684,9 @@
       <c r="D188" s="4" t="s">
         <v>355</v>
       </c>
+      <c r="F188" t="s">
+        <v>22</v>
+      </c>
       <c r="K188" t="s">
         <v>487</v>
       </c>
@@ -6344,6 +6710,9 @@
       <c r="D189" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="F189" t="s">
+        <v>22</v>
+      </c>
       <c r="K189" t="s">
         <v>487</v>
       </c>
@@ -6367,6 +6736,9 @@
       <c r="D190" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="F190" t="s">
+        <v>22</v>
+      </c>
       <c r="K190" t="s">
         <v>487</v>
       </c>
@@ -6390,6 +6762,9 @@
       <c r="D191" s="4" t="s">
         <v>359</v>
       </c>
+      <c r="F191" t="s">
+        <v>22</v>
+      </c>
       <c r="K191" t="s">
         <v>487</v>
       </c>
@@ -6413,6 +6788,9 @@
       <c r="D192" s="4" t="s">
         <v>361</v>
       </c>
+      <c r="F192" t="s">
+        <v>22</v>
+      </c>
       <c r="K192" t="s">
         <v>487</v>
       </c>
@@ -6436,6 +6814,9 @@
       <c r="D193" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="F193" t="s">
+        <v>22</v>
+      </c>
       <c r="K193" t="s">
         <v>487</v>
       </c>
@@ -6459,6 +6840,9 @@
       <c r="D194" s="4" t="s">
         <v>365</v>
       </c>
+      <c r="F194" t="s">
+        <v>22</v>
+      </c>
       <c r="K194" t="s">
         <v>487</v>
       </c>
@@ -6505,6 +6889,9 @@
       <c r="D196" s="4" t="s">
         <v>370</v>
       </c>
+      <c r="F196" t="s">
+        <v>22</v>
+      </c>
       <c r="K196" t="s">
         <v>487</v>
       </c>
@@ -6528,6 +6915,9 @@
       <c r="D197" s="4" t="s">
         <v>372</v>
       </c>
+      <c r="F197" t="s">
+        <v>22</v>
+      </c>
       <c r="K197" t="s">
         <v>487</v>
       </c>
@@ -6551,6 +6941,9 @@
       <c r="D198" s="4" t="s">
         <v>374</v>
       </c>
+      <c r="F198" t="s">
+        <v>22</v>
+      </c>
       <c r="K198" t="s">
         <v>487</v>
       </c>
@@ -6574,6 +6967,9 @@
       <c r="D199" s="4" t="s">
         <v>376</v>
       </c>
+      <c r="F199" t="s">
+        <v>22</v>
+      </c>
       <c r="K199" t="s">
         <v>487</v>
       </c>
@@ -6597,6 +6993,9 @@
       <c r="D200" s="4" t="s">
         <v>378</v>
       </c>
+      <c r="F200" t="s">
+        <v>22</v>
+      </c>
       <c r="K200" t="s">
         <v>487</v>
       </c>
@@ -6620,6 +7019,9 @@
       <c r="D201" s="4" t="s">
         <v>380</v>
       </c>
+      <c r="F201" t="s">
+        <v>22</v>
+      </c>
       <c r="K201" t="s">
         <v>487</v>
       </c>
@@ -6643,6 +7045,9 @@
       <c r="D202" s="4" t="s">
         <v>382</v>
       </c>
+      <c r="F202" t="s">
+        <v>22</v>
+      </c>
       <c r="K202" t="s">
         <v>487</v>
       </c>
@@ -6666,6 +7071,9 @@
       <c r="D203" s="4" t="s">
         <v>384</v>
       </c>
+      <c r="F203" t="s">
+        <v>22</v>
+      </c>
       <c r="K203" t="s">
         <v>487</v>
       </c>
@@ -6709,6 +7117,9 @@
       <c r="D205" s="4" t="s">
         <v>353</v>
       </c>
+      <c r="F205" t="s">
+        <v>22</v>
+      </c>
       <c r="K205" t="s">
         <v>487</v>
       </c>
@@ -6732,6 +7143,9 @@
       <c r="D206" s="4" t="s">
         <v>389</v>
       </c>
+      <c r="F206" t="s">
+        <v>22</v>
+      </c>
       <c r="K206" t="s">
         <v>487</v>
       </c>
@@ -6755,6 +7169,9 @@
       <c r="D207" s="4" t="s">
         <v>391</v>
       </c>
+      <c r="F207" t="s">
+        <v>22</v>
+      </c>
       <c r="K207" t="s">
         <v>487</v>
       </c>
@@ -6830,6 +7247,9 @@
       <c r="D210" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="F210" t="s">
+        <v>22</v>
+      </c>
       <c r="K210" t="s">
         <v>487</v>
       </c>
@@ -6968,6 +7388,9 @@
       <c r="D216" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="F216" t="s">
+        <v>22</v>
+      </c>
       <c r="K216" t="s">
         <v>487</v>
       </c>
@@ -6991,6 +7414,9 @@
       <c r="D217" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="F217" t="s">
+        <v>22</v>
+      </c>
       <c r="K217" t="s">
         <v>487</v>
       </c>
@@ -7013,6 +7439,9 @@
       </c>
       <c r="D218" s="4" t="s">
         <v>419</v>
+      </c>
+      <c r="F218" t="s">
+        <v>22</v>
       </c>
       <c r="K218" t="s">
         <v>487</v>

</xml_diff>

<commit_message>
Adjust Group 25 testables
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mryanpatterson/Documents/CSE3310/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mryanpatterson/Documents/CSE3310/cse3310-sp25-002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D831A5D-B122-1B43-966C-C6A2DF31DB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C684A21-AEAD-9B42-9548-BFB4FF8932B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29920" yWindow="-43680" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="506">
   <si>
     <t>Tested By</t>
   </si>
@@ -1551,6 +1551,15 @@
   </si>
   <si>
     <t>work in progress</t>
+  </si>
+  <si>
+    <t>Test Not Working</t>
+  </si>
+  <si>
+    <t>Untestable</t>
+  </si>
+  <si>
+    <t>Test Not FULLY Working</t>
   </si>
 </sst>
 </file>
@@ -1618,7 +1627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1641,6 +1650,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1949,8 +1961,8 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F225" sqref="F225"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F228" sqref="F228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2135,6 +2147,9 @@
       <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="F8" t="s">
+        <v>484</v>
+      </c>
       <c r="K8" t="s">
         <v>502</v>
       </c>
@@ -2155,6 +2170,9 @@
       <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F9" t="s">
+        <v>484</v>
+      </c>
       <c r="K9" t="s">
         <v>502</v>
       </c>
@@ -2175,6 +2193,9 @@
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F10" t="s">
+        <v>484</v>
+      </c>
       <c r="K10" t="s">
         <v>502</v>
       </c>
@@ -2253,6 +2274,9 @@
       <c r="D13" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="F13" t="s">
+        <v>503</v>
+      </c>
       <c r="K13" t="s">
         <v>502</v>
       </c>
@@ -2273,6 +2297,9 @@
       <c r="D14" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F14" t="s">
+        <v>484</v>
+      </c>
       <c r="K14" t="s">
         <v>502</v>
       </c>
@@ -2555,7 +2582,7 @@
         <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="K24" t="s">
         <v>487</v>
@@ -2578,7 +2605,7 @@
         <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="K25" t="s">
         <v>487</v>
@@ -2716,6 +2743,9 @@
       <c r="D30" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="F30" t="s">
+        <v>503</v>
+      </c>
       <c r="K30" t="s">
         <v>502</v>
       </c>
@@ -2823,6 +2853,9 @@
       <c r="D34" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="F34" t="s">
+        <v>503</v>
+      </c>
       <c r="K34" t="s">
         <v>501</v>
       </c>
@@ -2988,6 +3021,9 @@
       <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="F40" t="s">
+        <v>484</v>
+      </c>
       <c r="K40" t="s">
         <v>502</v>
       </c>
@@ -3095,6 +3131,9 @@
       <c r="D44" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="F44" t="s">
+        <v>503</v>
+      </c>
       <c r="K44" t="s">
         <v>502</v>
       </c>
@@ -3115,6 +3154,9 @@
       <c r="D45" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="F45" t="s">
+        <v>484</v>
+      </c>
       <c r="K45" t="s">
         <v>502</v>
       </c>
@@ -3310,7 +3352,7 @@
         <v>99</v>
       </c>
       <c r="F52" t="s">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="I52" t="s">
         <v>22</v>
@@ -3338,6 +3380,9 @@
       <c r="E53" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="F53" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I53" t="s">
         <v>484</v>
       </c>
@@ -3364,6 +3409,9 @@
       <c r="E54" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="F54" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I54" t="s">
         <v>485</v>
       </c>
@@ -3390,6 +3438,9 @@
       <c r="E55" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="F55" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I55" t="s">
         <v>485</v>
       </c>
@@ -3416,6 +3467,9 @@
       <c r="E56" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F56" s="9" t="s">
+        <v>503</v>
+      </c>
       <c r="I56" t="s">
         <v>484</v>
       </c>
@@ -3442,6 +3496,9 @@
       <c r="E57" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="F57" s="9" t="s">
+        <v>503</v>
+      </c>
       <c r="I57" t="s">
         <v>484</v>
       </c>
@@ -3469,7 +3526,7 @@
         <v>115</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="I58" t="s">
         <v>22</v>
@@ -3497,6 +3554,9 @@
       <c r="E59" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="F59" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I59" t="s">
         <v>484</v>
       </c>
@@ -3524,7 +3584,7 @@
         <v>120</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="I60" t="s">
         <v>486</v>
@@ -3552,6 +3612,9 @@
       <c r="E61" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F61" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I61" t="s">
         <v>484</v>
       </c>
@@ -3741,6 +3804,9 @@
       <c r="E67" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F67" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I67" t="s">
         <v>484</v>
       </c>
@@ -3764,6 +3830,9 @@
       <c r="E68" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="F68" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I68" t="s">
         <v>484</v>
       </c>
@@ -3916,7 +3985,7 @@
         <v>142</v>
       </c>
       <c r="F73" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="I73" t="s">
         <v>22</v>
@@ -3942,7 +4011,7 @@
         <v>144</v>
       </c>
       <c r="F74" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="I74" t="s">
         <v>22</v>
@@ -3968,7 +4037,7 @@
         <v>142</v>
       </c>
       <c r="F75" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="I75" t="s">
         <v>486</v>
@@ -3993,6 +4062,9 @@
       <c r="D76" s="4" t="s">
         <v>147</v>
       </c>
+      <c r="F76" t="s">
+        <v>503</v>
+      </c>
       <c r="I76" t="s">
         <v>484</v>
       </c>
@@ -4191,7 +4263,7 @@
         <v>161</v>
       </c>
       <c r="F83" t="s">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="I83" t="s">
         <v>22</v>
@@ -4219,6 +4291,9 @@
       <c r="E84" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="F84" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I84" t="s">
         <v>484</v>
       </c>
@@ -4245,6 +4320,9 @@
       <c r="E85" s="4" t="s">
         <v>167</v>
       </c>
+      <c r="F85" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I85" t="s">
         <v>484</v>
       </c>
@@ -4271,9 +4349,6 @@
       <c r="E86" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F86" t="s">
-        <v>22</v>
-      </c>
       <c r="I86" t="s">
         <v>486</v>
       </c>
@@ -4300,9 +4375,6 @@
       <c r="E87" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F87" t="s">
-        <v>22</v>
-      </c>
       <c r="I87" t="s">
         <v>22</v>
       </c>
@@ -4381,9 +4453,6 @@
       <c r="E90" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F90" t="s">
-        <v>22</v>
-      </c>
       <c r="I90" t="s">
         <v>486</v>
       </c>
@@ -4620,6 +4689,9 @@
       <c r="D100" s="4" t="s">
         <v>201</v>
       </c>
+      <c r="F100" t="s">
+        <v>484</v>
+      </c>
       <c r="K100" t="s">
         <v>502</v>
       </c>
@@ -4692,6 +4764,9 @@
       <c r="D103" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F103" t="s">
+        <v>484</v>
+      </c>
       <c r="K103" t="s">
         <v>502</v>
       </c>
@@ -4712,6 +4787,9 @@
       <c r="D104" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F104" t="s">
+        <v>484</v>
+      </c>
       <c r="K104" t="s">
         <v>502</v>
       </c>
@@ -4732,6 +4810,9 @@
       <c r="D105" s="4" t="s">
         <v>210</v>
       </c>
+      <c r="F105" t="s">
+        <v>484</v>
+      </c>
       <c r="K105" t="s">
         <v>502</v>
       </c>
@@ -4778,6 +4859,9 @@
       <c r="D107" s="4" t="s">
         <v>213</v>
       </c>
+      <c r="F107" t="s">
+        <v>484</v>
+      </c>
       <c r="K107" t="s">
         <v>502</v>
       </c>
@@ -4798,6 +4882,9 @@
       <c r="D108" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F108" t="s">
+        <v>504</v>
+      </c>
       <c r="K108" t="s">
         <v>502</v>
       </c>
@@ -4819,7 +4906,7 @@
         <v>216</v>
       </c>
       <c r="F109" t="s">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="K109" t="s">
         <v>487</v>
@@ -4842,7 +4929,7 @@
         <v>205</v>
       </c>
       <c r="F110" t="s">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="K110" t="s">
         <v>487</v>
@@ -4864,6 +4951,9 @@
       <c r="D111" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F111" t="s">
+        <v>484</v>
+      </c>
       <c r="K111" t="s">
         <v>502</v>
       </c>
@@ -4884,6 +4974,9 @@
       <c r="D112" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F112" t="s">
+        <v>484</v>
+      </c>
       <c r="K112" t="s">
         <v>502</v>
       </c>
@@ -4905,7 +4998,7 @@
         <v>207</v>
       </c>
       <c r="F113" t="s">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="K113" t="s">
         <v>487</v>
@@ -4927,6 +5020,9 @@
       <c r="D114" s="4" t="s">
         <v>207</v>
       </c>
+      <c r="F114" t="s">
+        <v>484</v>
+      </c>
       <c r="K114" t="s">
         <v>502</v>
       </c>
@@ -4947,6 +5043,9 @@
       <c r="D115" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="F115" t="s">
+        <v>484</v>
+      </c>
       <c r="K115" t="s">
         <v>502</v>
       </c>
@@ -4993,6 +5092,9 @@
       <c r="D117" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="F117" t="s">
+        <v>484</v>
+      </c>
       <c r="K117" t="s">
         <v>502</v>
       </c>
@@ -5013,6 +5115,9 @@
       <c r="D118" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="F118" t="s">
+        <v>484</v>
+      </c>
       <c r="K118" t="s">
         <v>502</v>
       </c>
@@ -5033,6 +5138,9 @@
       <c r="D119" s="4" t="s">
         <v>227</v>
       </c>
+      <c r="F119" t="s">
+        <v>484</v>
+      </c>
       <c r="K119" t="s">
         <v>502</v>
       </c>
@@ -5158,7 +5266,7 @@
         <v>238</v>
       </c>
       <c r="F124" t="s">
-        <v>22</v>
+        <v>504</v>
       </c>
       <c r="K124" t="s">
         <v>487</v>
@@ -5256,7 +5364,7 @@
         <v>244</v>
       </c>
       <c r="F128" t="s">
-        <v>22</v>
+        <v>504</v>
       </c>
       <c r="K128" t="s">
         <v>487</v>
@@ -5304,6 +5412,9 @@
       <c r="D130" s="4" t="s">
         <v>248</v>
       </c>
+      <c r="F130" t="s">
+        <v>504</v>
+      </c>
       <c r="O130" s="2" t="s">
         <v>469</v>
       </c>
@@ -5425,6 +5536,9 @@
       <c r="D135" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="F135" t="s">
+        <v>503</v>
+      </c>
       <c r="K135" t="s">
         <v>502</v>
       </c>
@@ -5445,6 +5559,9 @@
       <c r="D136" s="6" t="s">
         <v>252</v>
       </c>
+      <c r="F136" t="s">
+        <v>503</v>
+      </c>
       <c r="K136" t="s">
         <v>502</v>
       </c>
@@ -5517,6 +5634,9 @@
       <c r="D139" s="6" t="s">
         <v>262</v>
       </c>
+      <c r="F139" t="s">
+        <v>484</v>
+      </c>
       <c r="K139" t="s">
         <v>502</v>
       </c>
@@ -5592,6 +5712,9 @@
       <c r="E142" s="4" t="s">
         <v>269</v>
       </c>
+      <c r="F142" s="9" t="s">
+        <v>503</v>
+      </c>
       <c r="K142" t="s">
         <v>502</v>
       </c>
@@ -5644,6 +5767,9 @@
       <c r="D144" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="F144" t="s">
+        <v>503</v>
+      </c>
       <c r="K144" t="s">
         <v>502</v>
       </c>
@@ -5664,6 +5790,9 @@
       <c r="D145" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F145" t="s">
+        <v>503</v>
+      </c>
       <c r="K145" t="s">
         <v>502</v>
       </c>
@@ -5684,6 +5813,9 @@
       <c r="D146" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="F146" t="s">
+        <v>503</v>
+      </c>
       <c r="K146" t="s">
         <v>502</v>
       </c>
@@ -5704,6 +5836,9 @@
       <c r="D147" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F147" t="s">
+        <v>503</v>
+      </c>
       <c r="K147" t="s">
         <v>502</v>
       </c>
@@ -5776,6 +5911,9 @@
       <c r="D150" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F150" t="s">
+        <v>503</v>
+      </c>
       <c r="K150" t="s">
         <v>502</v>
       </c>
@@ -5796,6 +5934,9 @@
       <c r="D151" s="4" t="s">
         <v>268</v>
       </c>
+      <c r="F151" t="s">
+        <v>503</v>
+      </c>
       <c r="K151" t="s">
         <v>502</v>
       </c>
@@ -5868,6 +6009,9 @@
       <c r="D154" s="4" t="s">
         <v>287</v>
       </c>
+      <c r="F154" t="s">
+        <v>504</v>
+      </c>
       <c r="K154" t="s">
         <v>502</v>
       </c>
@@ -5889,6 +6033,9 @@
       <c r="D155" s="4" t="s">
         <v>290</v>
       </c>
+      <c r="F155" t="s">
+        <v>484</v>
+      </c>
       <c r="K155" t="s">
         <v>502</v>
       </c>
@@ -6065,6 +6212,9 @@
       <c r="D162" s="4" t="s">
         <v>304</v>
       </c>
+      <c r="F162" t="s">
+        <v>484</v>
+      </c>
       <c r="K162" t="s">
         <v>502</v>
       </c>
@@ -6111,8 +6261,8 @@
       <c r="D164" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="F164" t="s">
-        <v>22</v>
+      <c r="F164" s="2" t="s">
+        <v>505</v>
       </c>
       <c r="K164" t="s">
         <v>487</v>
@@ -6135,7 +6285,7 @@
         <v>310</v>
       </c>
       <c r="F165" t="s">
-        <v>22</v>
+        <v>503</v>
       </c>
       <c r="K165" t="s">
         <v>487</v>
@@ -6385,6 +6535,9 @@
       <c r="D175" s="4" t="s">
         <v>329</v>
       </c>
+      <c r="F175" t="s">
+        <v>484</v>
+      </c>
       <c r="K175" t="s">
         <v>502</v>
       </c>
@@ -6405,6 +6558,9 @@
       <c r="D176" s="4" t="s">
         <v>331</v>
       </c>
+      <c r="F176" t="s">
+        <v>484</v>
+      </c>
       <c r="K176" t="s">
         <v>491</v>
       </c>
@@ -6425,6 +6581,9 @@
       <c r="D177" s="4" t="s">
         <v>333</v>
       </c>
+      <c r="F177" t="s">
+        <v>484</v>
+      </c>
       <c r="K177" t="s">
         <v>491</v>
       </c>
@@ -6445,6 +6604,9 @@
       <c r="D178" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="F178" t="s">
+        <v>504</v>
+      </c>
       <c r="K178" t="s">
         <v>502</v>
       </c>
@@ -6491,6 +6653,9 @@
       <c r="D180" s="4" t="s">
         <v>339</v>
       </c>
+      <c r="F180" t="s">
+        <v>484</v>
+      </c>
       <c r="K180" t="s">
         <v>502</v>
       </c>
@@ -6511,6 +6676,9 @@
       <c r="D181" s="4" t="s">
         <v>341</v>
       </c>
+      <c r="F181" t="s">
+        <v>503</v>
+      </c>
       <c r="K181" t="s">
         <v>502</v>
       </c>
@@ -6869,6 +7037,9 @@
       <c r="E195" s="4" t="s">
         <v>368</v>
       </c>
+      <c r="F195" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="K195" t="s">
         <v>502</v>
       </c>
@@ -7097,6 +7268,9 @@
       <c r="D204" s="4" t="s">
         <v>386</v>
       </c>
+      <c r="F204" t="s">
+        <v>484</v>
+      </c>
       <c r="K204" t="s">
         <v>502</v>
       </c>
@@ -7201,6 +7375,9 @@
       <c r="E208" s="4" t="s">
         <v>395</v>
       </c>
+      <c r="F208" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="G208" s="4" t="s">
         <v>483</v>
       </c>
@@ -7227,6 +7404,9 @@
       <c r="E209" s="4" t="s">
         <v>398</v>
       </c>
+      <c r="F209" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K209" t="s">
         <v>494</v>
       </c>
@@ -7248,7 +7428,7 @@
         <v>400</v>
       </c>
       <c r="F210" t="s">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="K210" t="s">
         <v>487</v>
@@ -7273,6 +7453,9 @@
       <c r="D211" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="F211" t="s">
+        <v>484</v>
+      </c>
       <c r="K211" t="s">
         <v>494</v>
       </c>
@@ -7296,6 +7479,9 @@
       <c r="E212" s="4" t="s">
         <v>406</v>
       </c>
+      <c r="F212" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K212" t="s">
         <v>495</v>
       </c>
@@ -7319,6 +7505,9 @@
       <c r="E213" s="4" t="s">
         <v>409</v>
       </c>
+      <c r="F213" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="G213" s="4" t="s">
         <v>483</v>
       </c>
@@ -7345,6 +7534,9 @@
       <c r="E214" s="4" t="s">
         <v>412</v>
       </c>
+      <c r="F214" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K214" t="s">
         <v>496</v>
       </c>
@@ -7365,6 +7557,9 @@
       <c r="D215" s="4" t="s">
         <v>405</v>
       </c>
+      <c r="F215" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K215" t="s">
         <v>499</v>
       </c>
@@ -7466,6 +7661,9 @@
       <c r="D219" s="4" t="s">
         <v>400</v>
       </c>
+      <c r="F219" t="s">
+        <v>484</v>
+      </c>
       <c r="K219" t="s">
         <v>497</v>
       </c>
@@ -7486,6 +7684,9 @@
       <c r="D220" s="4" t="s">
         <v>422</v>
       </c>
+      <c r="F220" t="s">
+        <v>484</v>
+      </c>
       <c r="K220" t="s">
         <v>497</v>
       </c>
@@ -7509,6 +7710,9 @@
       <c r="E221" s="4" t="s">
         <v>424</v>
       </c>
+      <c r="F221" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K221" t="s">
         <v>498</v>
       </c>
@@ -7535,6 +7739,9 @@
       <c r="E222" s="4" t="s">
         <v>428</v>
       </c>
+      <c r="F222" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K222" t="s">
         <v>497</v>
       </c>
@@ -7558,6 +7765,9 @@
       <c r="E223" s="4" t="s">
         <v>430</v>
       </c>
+      <c r="F223" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="K223" t="s">
         <v>489</v>
       </c>
@@ -7577,6 +7787,9 @@
       </c>
       <c r="D224" s="4" t="s">
         <v>432</v>
+      </c>
+      <c r="F224" s="9" t="s">
+        <v>484</v>
       </c>
       <c r="K224" t="s">
         <v>500</v>

</xml_diff>

<commit_message>
Adding Group 25 Tests again
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9654E9DC5D3F9864/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mryanpatterson/Documents/CSE3310/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9284F97A-C645-4937-95B4-CECC6F0423A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13A4A8AB-52C8-B94D-87E0-E63EFD6528BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29920" yWindow="-43680" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="576">
   <si>
     <t>Tested By</t>
   </si>
@@ -1993,6 +1993,15 @@
   </si>
   <si>
     <t>summary:</t>
+  </si>
+  <si>
+    <t>Test Not Working</t>
+  </si>
+  <si>
+    <t>Untestable</t>
+  </si>
+  <si>
+    <t>Test PARTIALLY Working</t>
   </si>
 </sst>
 </file>
@@ -2036,7 +2045,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2066,7 +2074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2095,6 +2103,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2403,28 +2414,28 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F225" sqref="F225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.453125" style="2" customWidth="1"/>
-    <col min="16" max="17" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" style="2" customWidth="1"/>
+    <col min="16" max="17" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
@@ -2432,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>2</v>
       </c>
@@ -2470,7 +2481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2490,7 +2501,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="D4" s="4"/>
@@ -2498,7 +2509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -2530,7 +2541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -2562,7 +2573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -2588,7 +2599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -2601,6 +2612,9 @@
       <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
       <c r="K8" t="s">
         <v>33</v>
       </c>
@@ -2611,7 +2625,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -2624,6 +2638,9 @@
       <c r="D9" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="F9" t="s">
+        <v>118</v>
+      </c>
       <c r="K9" t="s">
         <v>33</v>
       </c>
@@ -2634,7 +2651,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -2647,6 +2664,9 @@
       <c r="D10" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
       <c r="K10" t="s">
         <v>33</v>
       </c>
@@ -2657,7 +2677,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -2689,7 +2709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -2721,7 +2741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -2734,6 +2754,9 @@
       <c r="D13" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="F13" t="s">
+        <v>573</v>
+      </c>
       <c r="K13" t="s">
         <v>33</v>
       </c>
@@ -2744,7 +2767,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -2757,6 +2780,9 @@
       <c r="D14" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="F14" t="s">
+        <v>118</v>
+      </c>
       <c r="K14" t="s">
         <v>33</v>
       </c>
@@ -2767,7 +2793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -2799,7 +2825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -2831,7 +2857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -2863,7 +2889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -2895,7 +2921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -2927,7 +2953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -2959,7 +2985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -2991,7 +3017,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -3023,7 +3049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -3055,7 +3081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -3069,7 +3095,7 @@
         <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="K24" t="s">
         <v>24</v>
@@ -3081,7 +3107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -3095,7 +3121,7 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="K25" t="s">
         <v>24</v>
@@ -3107,7 +3133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -3139,7 +3165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -3171,7 +3197,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -3203,7 +3229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -3235,7 +3261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -3248,6 +3274,9 @@
       <c r="D30" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="F30" t="s">
+        <v>574</v>
+      </c>
       <c r="K30" t="s">
         <v>33</v>
       </c>
@@ -3258,7 +3287,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -3290,7 +3319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -3322,7 +3351,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -3354,7 +3383,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -3367,6 +3396,9 @@
       <c r="D34" s="4" t="s">
         <v>75</v>
       </c>
+      <c r="F34" t="s">
+        <v>573</v>
+      </c>
       <c r="K34" t="s">
         <v>77</v>
       </c>
@@ -3377,7 +3409,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -3409,7 +3441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -3441,7 +3473,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -3473,7 +3505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -3505,7 +3537,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -3537,7 +3569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -3550,6 +3582,9 @@
       <c r="D40" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="F40" t="s">
+        <v>118</v>
+      </c>
       <c r="K40" t="s">
         <v>33</v>
       </c>
@@ -3560,7 +3595,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -3592,7 +3627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>38</v>
       </c>
@@ -3624,7 +3659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -3656,7 +3691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -3669,6 +3704,9 @@
       <c r="D44" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="F44" t="s">
+        <v>574</v>
+      </c>
       <c r="K44" t="s">
         <v>33</v>
       </c>
@@ -3679,7 +3717,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>41</v>
       </c>
@@ -3692,6 +3730,9 @@
       <c r="D45" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="F45" t="s">
+        <v>118</v>
+      </c>
       <c r="K45" t="s">
         <v>33</v>
       </c>
@@ -3702,7 +3743,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -3734,7 +3775,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>43</v>
       </c>
@@ -3766,7 +3807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -3798,7 +3839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>45</v>
       </c>
@@ -3830,7 +3871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>46</v>
       </c>
@@ -3862,7 +3903,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>47</v>
       </c>
@@ -3894,7 +3935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>48</v>
       </c>
@@ -3908,7 +3949,7 @@
         <v>113</v>
       </c>
       <c r="F52" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="I52" t="s">
         <v>23</v>
@@ -3923,7 +3964,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="208" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>49</v>
       </c>
@@ -3939,6 +3980,9 @@
       <c r="E53" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="F53" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I53" t="s">
         <v>118</v>
       </c>
@@ -3952,7 +3996,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="145" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>50</v>
       </c>
@@ -3968,6 +4012,9 @@
       <c r="E54" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="F54" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I54" t="s">
         <v>125</v>
       </c>
@@ -3981,7 +4028,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="145" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>51</v>
       </c>
@@ -3997,6 +4044,9 @@
       <c r="E55" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="F55" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I55" t="s">
         <v>125</v>
       </c>
@@ -4010,7 +4060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="208" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>52</v>
       </c>
@@ -4026,6 +4076,9 @@
       <c r="E56" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="F56" s="11" t="s">
+        <v>573</v>
+      </c>
       <c r="I56" t="s">
         <v>118</v>
       </c>
@@ -4039,7 +4092,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="145" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>53</v>
       </c>
@@ -4055,6 +4108,9 @@
       <c r="E57" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="F57" s="11" t="s">
+        <v>573</v>
+      </c>
       <c r="I57" t="s">
         <v>118</v>
       </c>
@@ -4068,7 +4124,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="174" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="192" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>54</v>
       </c>
@@ -4085,7 +4141,7 @@
         <v>137</v>
       </c>
       <c r="F58" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I58" t="s">
         <v>23</v>
@@ -4100,7 +4156,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="208" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>55</v>
       </c>
@@ -4116,6 +4172,9 @@
       <c r="E59" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="F59" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I59" t="s">
         <v>118</v>
       </c>
@@ -4129,7 +4188,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" ht="208" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>56</v>
       </c>
@@ -4146,7 +4205,7 @@
         <v>146</v>
       </c>
       <c r="F60" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I60" t="s">
         <v>147</v>
@@ -4161,7 +4220,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>57</v>
       </c>
@@ -4177,6 +4236,9 @@
       <c r="E61" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="F61" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I61" t="s">
         <v>118</v>
       </c>
@@ -4190,7 +4252,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -4225,7 +4287,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" ht="350" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -4263,7 +4325,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>60</v>
       </c>
@@ -4298,7 +4360,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -4333,7 +4395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="348" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>62</v>
       </c>
@@ -4368,7 +4430,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" ht="320" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>63</v>
       </c>
@@ -4384,6 +4446,9 @@
       <c r="E67" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="F67" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I67" t="s">
         <v>118</v>
       </c>
@@ -4394,7 +4459,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" ht="256" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>64</v>
       </c>
@@ -4410,6 +4475,9 @@
       <c r="E68" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="F68" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I68" t="s">
         <v>118</v>
       </c>
@@ -4423,7 +4491,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -4458,7 +4526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>66</v>
       </c>
@@ -4493,7 +4561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="377" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" ht="365" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>67</v>
       </c>
@@ -4528,7 +4596,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>68</v>
       </c>
@@ -4563,7 +4631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>69</v>
       </c>
@@ -4577,7 +4645,7 @@
         <v>179</v>
       </c>
       <c r="F73" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I73" t="s">
         <v>23</v>
@@ -4592,7 +4660,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>70</v>
       </c>
@@ -4606,7 +4674,7 @@
         <v>183</v>
       </c>
       <c r="F74" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I74" t="s">
         <v>23</v>
@@ -4621,7 +4689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" ht="365" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>71</v>
       </c>
@@ -4635,7 +4703,7 @@
         <v>179</v>
       </c>
       <c r="F75" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I75" t="s">
         <v>147</v>
@@ -4650,7 +4718,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>72</v>
       </c>
@@ -4663,6 +4731,9 @@
       <c r="D76" s="4" t="s">
         <v>188</v>
       </c>
+      <c r="F76" t="s">
+        <v>573</v>
+      </c>
       <c r="I76" t="s">
         <v>118</v>
       </c>
@@ -4676,7 +4747,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>73</v>
       </c>
@@ -4708,7 +4779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>74</v>
       </c>
@@ -4740,7 +4811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -4772,7 +4843,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>76</v>
       </c>
@@ -4804,7 +4875,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>77</v>
       </c>
@@ -4836,7 +4907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>78</v>
       </c>
@@ -4868,7 +4939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="203" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" ht="224" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>79</v>
       </c>
@@ -4882,7 +4953,7 @@
         <v>203</v>
       </c>
       <c r="F83" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="I83" t="s">
         <v>23</v>
@@ -4897,7 +4968,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" ht="176" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>80</v>
       </c>
@@ -4913,6 +4984,9 @@
       <c r="E84" s="4" t="s">
         <v>208</v>
       </c>
+      <c r="F84" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I84" t="s">
         <v>118</v>
       </c>
@@ -4926,7 +5000,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" ht="240" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>81</v>
       </c>
@@ -4942,6 +5016,9 @@
       <c r="E85" s="4" t="s">
         <v>213</v>
       </c>
+      <c r="F85" s="11" t="s">
+        <v>573</v>
+      </c>
       <c r="I85" t="s">
         <v>118</v>
       </c>
@@ -4955,7 +5032,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>82</v>
       </c>
@@ -4972,7 +5049,7 @@
         <v>218</v>
       </c>
       <c r="F86" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I86" t="s">
         <v>147</v>
@@ -4987,7 +5064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" ht="320" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>83</v>
       </c>
@@ -5004,7 +5081,7 @@
         <v>223</v>
       </c>
       <c r="F87" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="I87" t="s">
         <v>23</v>
@@ -5019,7 +5096,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>84</v>
       </c>
@@ -5051,7 +5128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" ht="395" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>85</v>
       </c>
@@ -5064,6 +5141,9 @@
       <c r="D89" s="4" t="s">
         <v>229</v>
       </c>
+      <c r="F89" t="s">
+        <v>118</v>
+      </c>
       <c r="I89" t="s">
         <v>118</v>
       </c>
@@ -5077,7 +5157,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" ht="288" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>86</v>
       </c>
@@ -5094,7 +5174,7 @@
         <v>234</v>
       </c>
       <c r="F90" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="I90" t="s">
         <v>147</v>
@@ -5109,7 +5189,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>87</v>
       </c>
@@ -5122,6 +5202,9 @@
       <c r="D91" s="4" t="s">
         <v>238</v>
       </c>
+      <c r="F91" t="s">
+        <v>573</v>
+      </c>
       <c r="I91" t="s">
         <v>118</v>
       </c>
@@ -5135,7 +5218,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>88</v>
       </c>
@@ -5151,6 +5234,9 @@
       <c r="E92" s="4" t="s">
         <v>242</v>
       </c>
+      <c r="F92" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="I92" t="s">
         <v>118</v>
       </c>
@@ -5164,7 +5250,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -5196,7 +5282,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>90</v>
       </c>
@@ -5228,7 +5314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>91</v>
       </c>
@@ -5241,6 +5327,9 @@
       <c r="D95" s="4" t="s">
         <v>250</v>
       </c>
+      <c r="F95" t="s">
+        <v>573</v>
+      </c>
       <c r="K95" t="s">
         <v>33</v>
       </c>
@@ -5251,7 +5340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>92</v>
       </c>
@@ -5264,6 +5353,9 @@
       <c r="D96" s="4" t="s">
         <v>252</v>
       </c>
+      <c r="F96" t="s">
+        <v>573</v>
+      </c>
       <c r="K96" t="s">
         <v>33</v>
       </c>
@@ -5274,7 +5366,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>93</v>
       </c>
@@ -5303,7 +5395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="145" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>94</v>
       </c>
@@ -5316,6 +5408,9 @@
       <c r="D98" s="4" t="s">
         <v>257</v>
       </c>
+      <c r="F98" t="s">
+        <v>118</v>
+      </c>
       <c r="K98" t="s">
         <v>33</v>
       </c>
@@ -5326,7 +5421,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="174" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" ht="176" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>95</v>
       </c>
@@ -5339,6 +5434,9 @@
       <c r="D99" s="4" t="s">
         <v>261</v>
       </c>
+      <c r="F99" t="s">
+        <v>118</v>
+      </c>
       <c r="K99" t="s">
         <v>33</v>
       </c>
@@ -5349,7 +5447,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" ht="128" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>96</v>
       </c>
@@ -5362,6 +5460,9 @@
       <c r="D100" s="4" t="s">
         <v>265</v>
       </c>
+      <c r="F100" t="s">
+        <v>118</v>
+      </c>
       <c r="K100" t="s">
         <v>33</v>
       </c>
@@ -5372,7 +5473,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>97</v>
       </c>
@@ -5401,7 +5502,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>98</v>
       </c>
@@ -5430,7 +5531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" ht="256" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>99</v>
       </c>
@@ -5443,6 +5544,9 @@
       <c r="D103" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F103" t="s">
+        <v>118</v>
+      </c>
       <c r="K103" t="s">
         <v>33</v>
       </c>
@@ -5453,7 +5557,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>100</v>
       </c>
@@ -5466,6 +5570,9 @@
       <c r="D104" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F104" t="s">
+        <v>118</v>
+      </c>
       <c r="K104" t="s">
         <v>33</v>
       </c>
@@ -5476,7 +5583,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>101</v>
       </c>
@@ -5489,6 +5596,9 @@
       <c r="D105" s="4" t="s">
         <v>279</v>
       </c>
+      <c r="F105" t="s">
+        <v>118</v>
+      </c>
       <c r="K105" t="s">
         <v>33</v>
       </c>
@@ -5499,7 +5609,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>102</v>
       </c>
@@ -5528,7 +5638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>103</v>
       </c>
@@ -5541,6 +5651,9 @@
       <c r="D107" s="4" t="s">
         <v>283</v>
       </c>
+      <c r="F107" t="s">
+        <v>118</v>
+      </c>
       <c r="K107" t="s">
         <v>33</v>
       </c>
@@ -5551,7 +5664,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>104</v>
       </c>
@@ -5564,6 +5677,9 @@
       <c r="D108" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F108" t="s">
+        <v>574</v>
+      </c>
       <c r="K108" t="s">
         <v>33</v>
       </c>
@@ -5574,7 +5690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" ht="380" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -5588,7 +5704,7 @@
         <v>289</v>
       </c>
       <c r="F109" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="K109" t="s">
         <v>24</v>
@@ -5600,7 +5716,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="203" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" ht="224" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -5614,7 +5730,7 @@
         <v>270</v>
       </c>
       <c r="F110" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="K110" t="s">
         <v>24</v>
@@ -5626,7 +5742,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" ht="304" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -5639,6 +5755,9 @@
       <c r="D111" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F111" t="s">
+        <v>118</v>
+      </c>
       <c r="K111" t="s">
         <v>33</v>
       </c>
@@ -5649,7 +5768,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -5662,6 +5781,9 @@
       <c r="D112" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F112" t="s">
+        <v>118</v>
+      </c>
       <c r="K112" t="s">
         <v>33</v>
       </c>
@@ -5672,7 +5794,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="406" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -5686,7 +5808,7 @@
         <v>272</v>
       </c>
       <c r="F113" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="K113" t="s">
         <v>24</v>
@@ -5698,7 +5820,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="406" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" ht="395" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -5711,6 +5833,9 @@
       <c r="D114" s="4" t="s">
         <v>272</v>
       </c>
+      <c r="F114" t="s">
+        <v>118</v>
+      </c>
       <c r="K114" t="s">
         <v>33</v>
       </c>
@@ -5721,7 +5846,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -5734,6 +5859,9 @@
       <c r="D115" s="4" t="s">
         <v>303</v>
       </c>
+      <c r="F115" t="s">
+        <v>118</v>
+      </c>
       <c r="K115" t="s">
         <v>33</v>
       </c>
@@ -5742,7 +5870,7 @@
       </c>
       <c r="Q115" s="9"/>
     </row>
-    <row r="116" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>112</v>
       </c>
@@ -5769,7 +5897,7 @@
       </c>
       <c r="Q116" s="9"/>
     </row>
-    <row r="117" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" ht="304" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>113</v>
       </c>
@@ -5782,6 +5910,9 @@
       <c r="D117" s="4" t="s">
         <v>308</v>
       </c>
+      <c r="F117" t="s">
+        <v>118</v>
+      </c>
       <c r="K117" t="s">
         <v>33</v>
       </c>
@@ -5792,7 +5923,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="232" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" ht="240" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>114</v>
       </c>
@@ -5805,6 +5936,9 @@
       <c r="D118" s="4" t="s">
         <v>308</v>
       </c>
+      <c r="F118" t="s">
+        <v>118</v>
+      </c>
       <c r="K118" t="s">
         <v>33</v>
       </c>
@@ -5815,7 +5949,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" ht="256" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>115</v>
       </c>
@@ -5828,6 +5962,9 @@
       <c r="D119" s="4" t="s">
         <v>308</v>
       </c>
+      <c r="F119" t="s">
+        <v>118</v>
+      </c>
       <c r="K119" t="s">
         <v>33</v>
       </c>
@@ -5838,7 +5975,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>116</v>
       </c>
@@ -5867,7 +6004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>117</v>
       </c>
@@ -5896,7 +6033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>118</v>
       </c>
@@ -5925,7 +6062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>119</v>
       </c>
@@ -5954,7 +6091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>120</v>
       </c>
@@ -5968,7 +6105,7 @@
         <v>325</v>
       </c>
       <c r="F124" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="K124" t="s">
         <v>24</v>
@@ -5980,7 +6117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>121</v>
       </c>
@@ -6009,7 +6146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>122</v>
       </c>
@@ -6038,7 +6175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>123</v>
       </c>
@@ -6052,7 +6189,7 @@
         <v>318</v>
       </c>
       <c r="F127" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="K127" t="s">
         <v>24</v>
@@ -6064,7 +6201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>124</v>
       </c>
@@ -6078,7 +6215,7 @@
         <v>331</v>
       </c>
       <c r="F128" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="K128" t="s">
         <v>24</v>
@@ -6090,7 +6227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="87" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>125</v>
       </c>
@@ -6119,7 +6256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>126</v>
       </c>
@@ -6132,6 +6269,9 @@
       <c r="D130" s="4" t="s">
         <v>335</v>
       </c>
+      <c r="F130" t="s">
+        <v>574</v>
+      </c>
       <c r="O130" s="2" t="s">
         <v>336</v>
       </c>
@@ -6139,7 +6279,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>127</v>
       </c>
@@ -6168,7 +6308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>128</v>
       </c>
@@ -6197,7 +6337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>129</v>
       </c>
@@ -6226,7 +6366,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>130</v>
       </c>
@@ -6255,7 +6395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>131</v>
       </c>
@@ -6268,6 +6408,9 @@
       <c r="D135" s="6" t="s">
         <v>341</v>
       </c>
+      <c r="F135" t="s">
+        <v>574</v>
+      </c>
       <c r="K135" t="s">
         <v>33</v>
       </c>
@@ -6278,7 +6421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>132</v>
       </c>
@@ -6291,6 +6434,9 @@
       <c r="D136" s="6" t="s">
         <v>341</v>
       </c>
+      <c r="F136" t="s">
+        <v>574</v>
+      </c>
       <c r="K136" t="s">
         <v>33</v>
       </c>
@@ -6301,7 +6447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>133</v>
       </c>
@@ -6330,7 +6476,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>134</v>
       </c>
@@ -6359,7 +6505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:18" ht="288" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>135</v>
       </c>
@@ -6372,6 +6518,9 @@
       <c r="D139" s="6" t="s">
         <v>352</v>
       </c>
+      <c r="F139" t="s">
+        <v>118</v>
+      </c>
       <c r="K139" t="s">
         <v>33</v>
       </c>
@@ -6382,7 +6531,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>136</v>
       </c>
@@ -6411,7 +6560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>137</v>
       </c>
@@ -6440,7 +6589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="319" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:18" ht="335" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>138</v>
       </c>
@@ -6456,6 +6605,9 @@
       <c r="E142" s="4" t="s">
         <v>360</v>
       </c>
+      <c r="F142" s="11" t="s">
+        <v>573</v>
+      </c>
       <c r="K142" t="s">
         <v>33</v>
       </c>
@@ -6469,7 +6621,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>139</v>
       </c>
@@ -6499,7 +6651,7 @@
       </c>
       <c r="Q143" s="9"/>
     </row>
-    <row r="144" spans="1:18" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:18" ht="395" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>140</v>
       </c>
@@ -6512,6 +6664,9 @@
       <c r="D144" s="4" t="s">
         <v>359</v>
       </c>
+      <c r="F144" t="s">
+        <v>573</v>
+      </c>
       <c r="K144" t="s">
         <v>33</v>
       </c>
@@ -6522,7 +6677,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>141</v>
       </c>
@@ -6535,6 +6690,9 @@
       <c r="D145" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="F145" t="s">
+        <v>573</v>
+      </c>
       <c r="K145" t="s">
         <v>33</v>
       </c>
@@ -6545,7 +6703,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>142</v>
       </c>
@@ -6558,6 +6716,9 @@
       <c r="D146" s="4" t="s">
         <v>359</v>
       </c>
+      <c r="F146" t="s">
+        <v>573</v>
+      </c>
       <c r="K146" t="s">
         <v>33</v>
       </c>
@@ -6568,7 +6729,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>143</v>
       </c>
@@ -6581,6 +6742,9 @@
       <c r="D147" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="F147" t="s">
+        <v>573</v>
+      </c>
       <c r="K147" t="s">
         <v>33</v>
       </c>
@@ -6591,7 +6755,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>144</v>
       </c>
@@ -6620,7 +6784,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>145</v>
       </c>
@@ -6649,7 +6813,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>146</v>
       </c>
@@ -6662,6 +6826,9 @@
       <c r="D150" s="4" t="s">
         <v>363</v>
       </c>
+      <c r="F150" t="s">
+        <v>573</v>
+      </c>
       <c r="K150" t="s">
         <v>33</v>
       </c>
@@ -6672,7 +6839,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="377" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="395" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>147</v>
       </c>
@@ -6685,6 +6852,9 @@
       <c r="D151" s="4" t="s">
         <v>359</v>
       </c>
+      <c r="F151" t="s">
+        <v>573</v>
+      </c>
       <c r="K151" t="s">
         <v>33</v>
       </c>
@@ -6695,7 +6865,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>148</v>
       </c>
@@ -6724,7 +6894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>149</v>
       </c>
@@ -6753,7 +6923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="319" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" ht="335" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>150</v>
       </c>
@@ -6777,7 +6947,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>151</v>
       </c>
@@ -6790,6 +6960,9 @@
       <c r="D155" s="4" t="s">
         <v>384</v>
       </c>
+      <c r="F155" t="s">
+        <v>118</v>
+      </c>
       <c r="K155" t="s">
         <v>33</v>
       </c>
@@ -6800,7 +6973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>152</v>
       </c>
@@ -6829,7 +7002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>153</v>
       </c>
@@ -6858,7 +7031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>154</v>
       </c>
@@ -6887,7 +7060,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>155</v>
       </c>
@@ -6916,7 +7089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" ht="320" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>156</v>
       </c>
@@ -6945,7 +7118,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" ht="176" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>157</v>
       </c>
@@ -6974,7 +7147,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" ht="192" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>158</v>
       </c>
@@ -6987,6 +7160,9 @@
       <c r="D162" s="4" t="s">
         <v>401</v>
       </c>
+      <c r="F162" t="s">
+        <v>118</v>
+      </c>
       <c r="K162" t="s">
         <v>33</v>
       </c>
@@ -6997,7 +7173,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>159</v>
       </c>
@@ -7026,7 +7202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>160</v>
       </c>
@@ -7039,8 +7215,8 @@
       <c r="D164" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="F164" t="s">
-        <v>23</v>
+      <c r="F164" s="2" t="s">
+        <v>575</v>
       </c>
       <c r="K164" t="s">
         <v>24</v>
@@ -7052,7 +7228,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>161</v>
       </c>
@@ -7066,7 +7242,7 @@
         <v>409</v>
       </c>
       <c r="F165" t="s">
-        <v>23</v>
+        <v>573</v>
       </c>
       <c r="K165" t="s">
         <v>24</v>
@@ -7078,7 +7254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>162</v>
       </c>
@@ -7107,7 +7283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>163</v>
       </c>
@@ -7133,7 +7309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>164</v>
       </c>
@@ -7159,7 +7335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>165</v>
       </c>
@@ -7188,7 +7364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>166</v>
       </c>
@@ -7217,7 +7393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>167</v>
       </c>
@@ -7246,7 +7422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="3">
         <v>168</v>
       </c>
@@ -7275,7 +7451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>169</v>
       </c>
@@ -7304,7 +7480,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>170</v>
       </c>
@@ -7333,7 +7509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>171</v>
       </c>
@@ -7346,6 +7522,9 @@
       <c r="D175" s="4" t="s">
         <v>428</v>
       </c>
+      <c r="F175" t="s">
+        <v>118</v>
+      </c>
       <c r="K175" t="s">
         <v>33</v>
       </c>
@@ -7356,7 +7535,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="3">
         <v>172</v>
       </c>
@@ -7369,6 +7548,9 @@
       <c r="D176" s="4" t="s">
         <v>431</v>
       </c>
+      <c r="F176" t="s">
+        <v>118</v>
+      </c>
       <c r="K176" t="s">
         <v>204</v>
       </c>
@@ -7379,7 +7561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>173</v>
       </c>
@@ -7392,6 +7574,9 @@
       <c r="D177" s="4" t="s">
         <v>433</v>
       </c>
+      <c r="F177" t="s">
+        <v>118</v>
+      </c>
       <c r="K177" t="s">
         <v>204</v>
       </c>
@@ -7402,7 +7587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>174</v>
       </c>
@@ -7415,6 +7600,9 @@
       <c r="D178" s="4" t="s">
         <v>435</v>
       </c>
+      <c r="F178" t="s">
+        <v>23</v>
+      </c>
       <c r="K178" t="s">
         <v>33</v>
       </c>
@@ -7425,7 +7613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>175</v>
       </c>
@@ -7454,7 +7642,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="232" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="240" x14ac:dyDescent="0.2">
       <c r="A180" s="3">
         <v>176</v>
       </c>
@@ -7467,6 +7655,9 @@
       <c r="D180" s="4" t="s">
         <v>439</v>
       </c>
+      <c r="F180" t="s">
+        <v>118</v>
+      </c>
       <c r="K180" t="s">
         <v>33</v>
       </c>
@@ -7477,7 +7668,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" ht="380" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>177</v>
       </c>
@@ -7490,6 +7681,9 @@
       <c r="D181" s="4" t="s">
         <v>441</v>
       </c>
+      <c r="F181" t="s">
+        <v>573</v>
+      </c>
       <c r="K181" t="s">
         <v>33</v>
       </c>
@@ -7497,7 +7691,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>178</v>
       </c>
@@ -7526,7 +7720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>179</v>
       </c>
@@ -7555,7 +7749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
         <v>180</v>
       </c>
@@ -7584,7 +7778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>181</v>
       </c>
@@ -7613,7 +7807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>182</v>
       </c>
@@ -7642,7 +7836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>183</v>
       </c>
@@ -7671,7 +7865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>184</v>
       </c>
@@ -7700,7 +7894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>185</v>
       </c>
@@ -7729,7 +7923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
         <v>186</v>
       </c>
@@ -7758,7 +7952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>187</v>
       </c>
@@ -7787,7 +7981,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>188</v>
       </c>
@@ -7816,7 +8010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>189</v>
       </c>
@@ -7845,7 +8039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
         <v>190</v>
       </c>
@@ -7874,7 +8068,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:18" ht="272" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>191</v>
       </c>
@@ -7890,6 +8084,9 @@
       <c r="E195" s="4" t="s">
         <v>469</v>
       </c>
+      <c r="F195" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="K195" t="s">
         <v>33</v>
       </c>
@@ -7900,7 +8097,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="196" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>192</v>
       </c>
@@ -7929,7 +8126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>193</v>
       </c>
@@ -7958,7 +8155,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>194</v>
       </c>
@@ -7987,7 +8184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:18" ht="256" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>195</v>
       </c>
@@ -8016,7 +8213,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>196</v>
       </c>
@@ -8045,7 +8242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>197</v>
       </c>
@@ -8074,7 +8271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>198</v>
       </c>
@@ -8103,7 +8300,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>199</v>
       </c>
@@ -8132,7 +8329,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="204" spans="1:18" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:18" ht="288" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>200</v>
       </c>
@@ -8145,6 +8342,9 @@
       <c r="D204" s="4" t="s">
         <v>490</v>
       </c>
+      <c r="F204" t="s">
+        <v>118</v>
+      </c>
       <c r="K204" t="s">
         <v>33</v>
       </c>
@@ -8155,7 +8355,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>201</v>
       </c>
@@ -8184,7 +8384,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:18" ht="290" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:18" ht="304" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>202</v>
       </c>
@@ -8213,7 +8413,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="207" spans="1:18" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:18" ht="380" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>203</v>
       </c>
@@ -8245,7 +8445,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="208" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:18" ht="176" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>204</v>
       </c>
@@ -8261,6 +8461,9 @@
       <c r="E208" s="4" t="s">
         <v>503</v>
       </c>
+      <c r="F208" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="G208" s="4" t="s">
         <v>504</v>
       </c>
@@ -8274,7 +8477,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="209" spans="1:18" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>205</v>
       </c>
@@ -8290,6 +8493,9 @@
       <c r="E209" s="4" t="s">
         <v>510</v>
       </c>
+      <c r="F209" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K209" t="s">
         <v>511</v>
       </c>
@@ -8300,7 +8506,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="210" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:18" ht="160" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>206</v>
       </c>
@@ -8314,7 +8520,7 @@
         <v>515</v>
       </c>
       <c r="F210" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="K210" t="s">
         <v>24</v>
@@ -8329,7 +8535,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="203" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>207</v>
       </c>
@@ -8342,6 +8548,9 @@
       <c r="D211" s="4" t="s">
         <v>519</v>
       </c>
+      <c r="F211" t="s">
+        <v>118</v>
+      </c>
       <c r="K211" t="s">
         <v>511</v>
       </c>
@@ -8352,7 +8561,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>208</v>
       </c>
@@ -8368,6 +8577,9 @@
       <c r="E212" s="4" t="s">
         <v>524</v>
       </c>
+      <c r="F212" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K212" t="s">
         <v>525</v>
       </c>
@@ -8378,7 +8590,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="213" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:18" ht="112" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>209</v>
       </c>
@@ -8394,6 +8606,9 @@
       <c r="E213" s="4" t="s">
         <v>529</v>
       </c>
+      <c r="F213" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="G213" s="4" t="s">
         <v>504</v>
       </c>
@@ -8407,7 +8622,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" ht="144" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>210</v>
       </c>
@@ -8423,6 +8638,9 @@
       <c r="E214" s="4" t="s">
         <v>535</v>
       </c>
+      <c r="F214" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K214" t="s">
         <v>536</v>
       </c>
@@ -8433,7 +8651,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="203" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>211</v>
       </c>
@@ -8446,6 +8664,9 @@
       <c r="D215" s="4" t="s">
         <v>523</v>
       </c>
+      <c r="F215" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K215" t="s">
         <v>539</v>
       </c>
@@ -8459,7 +8680,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>212</v>
       </c>
@@ -8486,7 +8707,7 @@
       </c>
       <c r="Q216" s="9"/>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>213</v>
       </c>
@@ -8513,7 +8734,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>214</v>
       </c>
@@ -8540,7 +8761,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:18" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:18" ht="224" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>215</v>
       </c>
@@ -8553,6 +8774,9 @@
       <c r="D219" s="4" t="s">
         <v>515</v>
       </c>
+      <c r="F219" t="s">
+        <v>118</v>
+      </c>
       <c r="K219" t="s">
         <v>548</v>
       </c>
@@ -8563,7 +8787,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="87" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:18" ht="96" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>216</v>
       </c>
@@ -8576,6 +8800,9 @@
       <c r="D220" s="4" t="s">
         <v>552</v>
       </c>
+      <c r="F220" t="s">
+        <v>118</v>
+      </c>
       <c r="K220" t="s">
         <v>548</v>
       </c>
@@ -8586,7 +8813,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" ht="144" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>217</v>
       </c>
@@ -8602,6 +8829,9 @@
       <c r="E221" s="4" t="s">
         <v>557</v>
       </c>
+      <c r="F221" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K221" t="s">
         <v>558</v>
       </c>
@@ -8615,7 +8845,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:18" ht="224" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>218</v>
       </c>
@@ -8631,6 +8861,9 @@
       <c r="E222" s="4" t="s">
         <v>563</v>
       </c>
+      <c r="F222" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K222" t="s">
         <v>548</v>
       </c>
@@ -8641,7 +8874,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="203" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:18" ht="208" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>219</v>
       </c>
@@ -8657,6 +8890,9 @@
       <c r="E223" s="4" t="s">
         <v>565</v>
       </c>
+      <c r="F223" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K223" t="s">
         <v>566</v>
       </c>
@@ -8667,7 +8903,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="224" spans="1:18" ht="290" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:18" ht="288" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>220</v>
       </c>
@@ -8680,6 +8916,9 @@
       <c r="D224" s="4" t="s">
         <v>569</v>
       </c>
+      <c r="F224" t="s">
+        <v>118</v>
+      </c>
       <c r="K224" t="s">
         <v>570</v>
       </c>
@@ -8690,12 +8929,12 @@
         <v>571</v>
       </c>
     </row>
-    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R230" t="s">
         <v>572</v>
       </c>

</xml_diff>

<commit_message>
somebody deleted our work so adding it again
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\backup\software development\PROJECT\cse3310-sp25-002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF2ECC0-8674-4DE8-B900-A3F425CDD244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990DD406-2D69-486F-9CB8-A111D0AEAC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="844">
   <si>
     <t>Tested By</t>
   </si>
@@ -2673,12 +2673,144 @@
   <si>
     <t>Fail</t>
   </si>
+  <si>
+    <t>TP-0056</t>
+  </si>
+  <si>
+    <t>TP-0014</t>
+  </si>
+  <si>
+    <t>TP-0026 &amp; TP-0027</t>
+  </si>
+  <si>
+    <t>TP-0059</t>
+  </si>
+  <si>
+    <t>TP-0066</t>
+  </si>
+  <si>
+    <t>TP-0060</t>
+  </si>
+  <si>
+    <t>TP-0061</t>
+  </si>
+  <si>
+    <t>TP-0062</t>
+  </si>
+  <si>
+    <t>TP-0018</t>
+  </si>
+  <si>
+    <t>TP-0064</t>
+  </si>
+  <si>
+    <t>TP-0065</t>
+  </si>
+  <si>
+    <t>TP-0067</t>
+  </si>
+  <si>
+    <t>TP-0068</t>
+  </si>
+  <si>
+    <t>TP-0070</t>
+  </si>
+  <si>
+    <t>TP-0071</t>
+  </si>
+  <si>
+    <t>TP-0072</t>
+  </si>
+  <si>
+    <t>TP-0073</t>
+  </si>
+  <si>
+    <t>TP-0074</t>
+  </si>
+  <si>
+    <t>TP-0077</t>
+  </si>
+  <si>
+    <t>TP-0078</t>
+  </si>
+  <si>
+    <t>TP-0079</t>
+  </si>
+  <si>
+    <t>TP-0080</t>
+  </si>
+  <si>
+    <t>TP-0036</t>
+  </si>
+  <si>
+    <t>TP-0081</t>
+  </si>
+  <si>
+    <t>TP-0003</t>
+  </si>
+  <si>
+    <t>TP-0005</t>
+  </si>
+  <si>
+    <t>TP-0037</t>
+  </si>
+  <si>
+    <t>TP-0052, TP-0053</t>
+  </si>
+  <si>
+    <t>This is not used. N/A</t>
+  </si>
+  <si>
+    <t>TP-0042,TP-0079</t>
+  </si>
+  <si>
+    <t>TP-0005,TP-0036</t>
+  </si>
+  <si>
+    <t>TP-0047, TP-0048, TP-0049</t>
+  </si>
+  <si>
+    <t>TP-0082</t>
+  </si>
+  <si>
+    <t>TP-0048</t>
+  </si>
+  <si>
+    <t>TP-0083</t>
+  </si>
+  <si>
+    <t>TP-0019, TP-0040</t>
+  </si>
+  <si>
+    <t>TP-0058</t>
+  </si>
+  <si>
+    <t>TP-0041</t>
+  </si>
+  <si>
+    <t>TP-0069</t>
+  </si>
+  <si>
+    <t>unable to test</t>
+  </si>
+  <si>
+    <t>TP-0021 - TP-0022</t>
+  </si>
+  <si>
+    <t>TP-0025</t>
+  </si>
+  <si>
+    <t>TP-0002</t>
+  </si>
+  <si>
+    <t>TP-0022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2739,6 +2871,48 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2801,10 +2975,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2861,9 +3036,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{F88945C0-A42E-4E03-813D-E3743885B48E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3168,32 +3355,33 @@
   </sheetPr>
   <dimension ref="A1:S230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="18.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" customWidth="1"/>
-    <col min="10" max="10" width="18.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.26953125" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="20.21875" style="2" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="20.453125" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" customWidth="1"/>
+    <col min="18" max="18" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.77734375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3210,14 +3398,14 @@
       <c r="P1" s="19"/>
       <c r="Q1" s="19"/>
     </row>
-    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -3248,7 +3436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -3268,7 +3456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="D4" s="4"/>
@@ -3276,7 +3464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -3292,6 +3480,9 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
@@ -3317,7 +3508,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -3333,6 +3524,9 @@
       <c r="F6" t="s">
         <v>22</v>
       </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
       <c r="I6" t="s">
         <v>22</v>
       </c>
@@ -3358,7 +3552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="203.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -3374,6 +3568,9 @@
       <c r="F7" t="s">
         <v>22</v>
       </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
       <c r="K7" t="s">
         <v>23</v>
       </c>
@@ -3393,7 +3590,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -3409,6 +3606,9 @@
       <c r="F8" t="s">
         <v>117</v>
       </c>
+      <c r="H8" t="s">
+        <v>800</v>
+      </c>
       <c r="K8" t="s">
         <v>32</v>
       </c>
@@ -3425,7 +3625,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -3441,6 +3641,9 @@
       <c r="F9" t="s">
         <v>117</v>
       </c>
+      <c r="H9" t="s">
+        <v>801</v>
+      </c>
       <c r="K9" t="s">
         <v>32</v>
       </c>
@@ -3460,7 +3663,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -3476,6 +3679,9 @@
       <c r="F10" t="s">
         <v>117</v>
       </c>
+      <c r="H10" s="20" t="s">
+        <v>802</v>
+      </c>
       <c r="K10" t="s">
         <v>32</v>
       </c>
@@ -3492,7 +3698,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -3508,6 +3714,9 @@
       <c r="F11" t="s">
         <v>22</v>
       </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
       <c r="I11" t="s">
         <v>22</v>
       </c>
@@ -3533,7 +3742,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -3549,6 +3758,9 @@
       <c r="F12" t="s">
         <v>22</v>
       </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
       <c r="I12" t="s">
         <v>22</v>
       </c>
@@ -3574,7 +3786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -3590,6 +3802,9 @@
       <c r="F13" t="s">
         <v>572</v>
       </c>
+      <c r="H13" s="20" t="s">
+        <v>803</v>
+      </c>
       <c r="K13" t="s">
         <v>32</v>
       </c>
@@ -3609,7 +3824,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -3625,6 +3840,9 @@
       <c r="F14" t="s">
         <v>117</v>
       </c>
+      <c r="H14" s="21" t="s">
+        <v>804</v>
+      </c>
       <c r="K14" t="s">
         <v>32</v>
       </c>
@@ -3641,7 +3859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -3657,6 +3875,9 @@
       <c r="F15" t="s">
         <v>22</v>
       </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
       <c r="I15" t="s">
         <v>22</v>
       </c>
@@ -3682,7 +3903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -3698,6 +3919,9 @@
       <c r="F16" t="s">
         <v>22</v>
       </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
       <c r="I16" t="s">
         <v>22</v>
       </c>
@@ -3723,7 +3947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -3739,6 +3963,9 @@
       <c r="F17" t="s">
         <v>22</v>
       </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
       <c r="I17" t="s">
         <v>22</v>
       </c>
@@ -3764,7 +3991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -3780,6 +4007,9 @@
       <c r="F18" t="s">
         <v>22</v>
       </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
       <c r="I18" t="s">
         <v>22</v>
       </c>
@@ -3805,7 +4035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -3821,6 +4051,9 @@
       <c r="F19" t="s">
         <v>22</v>
       </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
       <c r="I19" t="s">
         <v>22</v>
       </c>
@@ -3846,7 +4079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -3862,6 +4095,9 @@
       <c r="F20" t="s">
         <v>22</v>
       </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
       <c r="I20" t="s">
         <v>22</v>
       </c>
@@ -3887,7 +4123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -3903,6 +4139,9 @@
       <c r="F21" t="s">
         <v>22</v>
       </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
@@ -3928,7 +4167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -3944,6 +4183,9 @@
       <c r="F22" t="s">
         <v>22</v>
       </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
       <c r="I22" t="s">
         <v>22</v>
       </c>
@@ -3969,7 +4211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -3985,6 +4227,9 @@
       <c r="F23" t="s">
         <v>22</v>
       </c>
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
       <c r="I23" t="s">
         <v>22</v>
       </c>
@@ -4010,7 +4255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -4026,6 +4271,9 @@
       <c r="F24" t="s">
         <v>573</v>
       </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
       <c r="K24" t="s">
         <v>23</v>
       </c>
@@ -4045,7 +4293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -4061,6 +4309,9 @@
       <c r="F25" t="s">
         <v>573</v>
       </c>
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
       <c r="K25" t="s">
         <v>23</v>
       </c>
@@ -4080,7 +4331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -4096,6 +4347,9 @@
       <c r="F26" t="s">
         <v>22</v>
       </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
       <c r="I26" t="s">
         <v>22</v>
       </c>
@@ -4121,7 +4375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -4137,6 +4391,9 @@
       <c r="F27" t="s">
         <v>22</v>
       </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
       <c r="I27" t="s">
         <v>22</v>
       </c>
@@ -4162,7 +4419,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -4178,6 +4435,9 @@
       <c r="F28" t="s">
         <v>22</v>
       </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
       <c r="I28" t="s">
         <v>22</v>
       </c>
@@ -4203,7 +4463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -4219,6 +4479,9 @@
       <c r="F29" t="s">
         <v>22</v>
       </c>
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
       <c r="I29" t="s">
         <v>22</v>
       </c>
@@ -4244,7 +4507,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="203.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -4260,6 +4523,9 @@
       <c r="F30" t="s">
         <v>573</v>
       </c>
+      <c r="H30" s="21" t="s">
+        <v>805</v>
+      </c>
       <c r="K30" t="s">
         <v>32</v>
       </c>
@@ -4279,7 +4545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -4295,6 +4561,9 @@
       <c r="F31" t="s">
         <v>22</v>
       </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
       <c r="I31" t="s">
         <v>22</v>
       </c>
@@ -4320,7 +4589,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -4336,6 +4605,9 @@
       <c r="F32" t="s">
         <v>22</v>
       </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
       <c r="I32" t="s">
         <v>22</v>
       </c>
@@ -4361,7 +4633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -4377,6 +4649,9 @@
       <c r="F33" t="s">
         <v>22</v>
       </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
       <c r="I33" t="s">
         <v>22</v>
       </c>
@@ -4402,7 +4677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="102" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -4418,6 +4693,9 @@
       <c r="F34" t="s">
         <v>572</v>
       </c>
+      <c r="H34" s="20" t="s">
+        <v>803</v>
+      </c>
       <c r="K34" t="s">
         <v>76</v>
       </c>
@@ -4437,7 +4715,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -4453,6 +4731,9 @@
       <c r="F35" t="s">
         <v>22</v>
       </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
       <c r="I35" t="s">
         <v>22</v>
       </c>
@@ -4478,7 +4759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -4494,6 +4775,9 @@
       <c r="F36" t="s">
         <v>22</v>
       </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
       <c r="I36" t="s">
         <v>22</v>
       </c>
@@ -4519,7 +4803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -4535,6 +4819,9 @@
       <c r="F37" t="s">
         <v>22</v>
       </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
       <c r="I37" t="s">
         <v>22</v>
       </c>
@@ -4560,7 +4847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -4576,6 +4863,9 @@
       <c r="F38" t="s">
         <v>22</v>
       </c>
+      <c r="H38" t="s">
+        <v>25</v>
+      </c>
       <c r="I38" t="s">
         <v>22</v>
       </c>
@@ -4601,7 +4891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -4617,6 +4907,9 @@
       <c r="F39" t="s">
         <v>22</v>
       </c>
+      <c r="H39" t="s">
+        <v>25</v>
+      </c>
       <c r="I39" t="s">
         <v>22</v>
       </c>
@@ -4642,7 +4935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="87.5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -4658,6 +4951,9 @@
       <c r="F40" t="s">
         <v>117</v>
       </c>
+      <c r="H40" t="s">
+        <v>25</v>
+      </c>
       <c r="K40" t="s">
         <v>32</v>
       </c>
@@ -4677,7 +4973,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -4693,6 +4989,9 @@
       <c r="F41" t="s">
         <v>22</v>
       </c>
+      <c r="H41" t="s">
+        <v>25</v>
+      </c>
       <c r="I41" t="s">
         <v>22</v>
       </c>
@@ -4718,7 +5017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>38</v>
       </c>
@@ -4734,6 +5033,9 @@
       <c r="F42" t="s">
         <v>22</v>
       </c>
+      <c r="H42" t="s">
+        <v>25</v>
+      </c>
       <c r="I42" t="s">
         <v>22</v>
       </c>
@@ -4759,7 +5061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -4775,6 +5077,9 @@
       <c r="F43" t="s">
         <v>22</v>
       </c>
+      <c r="H43" t="s">
+        <v>25</v>
+      </c>
       <c r="I43" t="s">
         <v>22</v>
       </c>
@@ -4800,7 +5105,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -4816,6 +5121,9 @@
       <c r="F44" t="s">
         <v>573</v>
       </c>
+      <c r="H44" t="s">
+        <v>25</v>
+      </c>
       <c r="K44" t="s">
         <v>32</v>
       </c>
@@ -4835,7 +5143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="102" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>41</v>
       </c>
@@ -4851,6 +5159,9 @@
       <c r="F45" t="s">
         <v>117</v>
       </c>
+      <c r="H45" s="21" t="s">
+        <v>806</v>
+      </c>
       <c r="K45" t="s">
         <v>32</v>
       </c>
@@ -4867,7 +5178,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -4883,6 +5194,9 @@
       <c r="F46" t="s">
         <v>22</v>
       </c>
+      <c r="H46" t="s">
+        <v>25</v>
+      </c>
       <c r="I46" t="s">
         <v>22</v>
       </c>
@@ -4908,7 +5222,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>43</v>
       </c>
@@ -4924,6 +5238,9 @@
       <c r="F47" t="s">
         <v>22</v>
       </c>
+      <c r="H47" t="s">
+        <v>25</v>
+      </c>
       <c r="I47" t="s">
         <v>22</v>
       </c>
@@ -4949,7 +5266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -4965,6 +5282,9 @@
       <c r="F48" t="s">
         <v>22</v>
       </c>
+      <c r="H48" t="s">
+        <v>25</v>
+      </c>
       <c r="I48" t="s">
         <v>22</v>
       </c>
@@ -4990,7 +5310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>45</v>
       </c>
@@ -5006,6 +5326,9 @@
       <c r="F49" t="s">
         <v>22</v>
       </c>
+      <c r="H49" t="s">
+        <v>25</v>
+      </c>
       <c r="I49" t="s">
         <v>22</v>
       </c>
@@ -5031,7 +5354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>46</v>
       </c>
@@ -5047,6 +5370,9 @@
       <c r="F50" t="s">
         <v>22</v>
       </c>
+      <c r="H50" t="s">
+        <v>25</v>
+      </c>
       <c r="I50" t="s">
         <v>22</v>
       </c>
@@ -5072,7 +5398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>47</v>
       </c>
@@ -5088,6 +5414,9 @@
       <c r="F51" t="s">
         <v>22</v>
       </c>
+      <c r="H51" t="s">
+        <v>25</v>
+      </c>
       <c r="I51" t="s">
         <v>22</v>
       </c>
@@ -5113,7 +5442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="73" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>48</v>
       </c>
@@ -5129,6 +5458,9 @@
       <c r="F52" t="s">
         <v>117</v>
       </c>
+      <c r="H52" t="s">
+        <v>807</v>
+      </c>
       <c r="I52" t="s">
         <v>22</v>
       </c>
@@ -5151,7 +5483,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="189" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>49</v>
       </c>
@@ -5170,6 +5502,9 @@
       <c r="F53" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H53" t="s">
+        <v>808</v>
+      </c>
       <c r="I53" t="s">
         <v>117</v>
       </c>
@@ -5189,7 +5524,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>50</v>
       </c>
@@ -5208,6 +5543,9 @@
       <c r="F54" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H54" t="s">
+        <v>809</v>
+      </c>
       <c r="I54" t="s">
         <v>124</v>
       </c>
@@ -5227,7 +5565,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>51</v>
       </c>
@@ -5246,6 +5584,9 @@
       <c r="F55" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H55" t="s">
+        <v>810</v>
+      </c>
       <c r="I55" t="s">
         <v>124</v>
       </c>
@@ -5265,7 +5606,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="160" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>52</v>
       </c>
@@ -5284,6 +5625,9 @@
       <c r="F56" s="4" t="s">
         <v>572</v>
       </c>
+      <c r="H56" t="s">
+        <v>25</v>
+      </c>
       <c r="I56" t="s">
         <v>117</v>
       </c>
@@ -5303,7 +5647,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>53</v>
       </c>
@@ -5322,6 +5666,9 @@
       <c r="F57" s="4" t="s">
         <v>572</v>
       </c>
+      <c r="H57" t="s">
+        <v>25</v>
+      </c>
       <c r="I57" t="s">
         <v>117</v>
       </c>
@@ -5341,7 +5688,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="131" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>54</v>
       </c>
@@ -5360,6 +5707,9 @@
       <c r="F58" t="s">
         <v>572</v>
       </c>
+      <c r="H58" t="s">
+        <v>25</v>
+      </c>
       <c r="I58" t="s">
         <v>22</v>
       </c>
@@ -5379,7 +5729,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="160" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>55</v>
       </c>
@@ -5398,6 +5748,9 @@
       <c r="F59" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H59" s="4" t="s">
+        <v>811</v>
+      </c>
       <c r="I59" t="s">
         <v>117</v>
       </c>
@@ -5417,7 +5770,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="160" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>56</v>
       </c>
@@ -5436,6 +5789,9 @@
       <c r="F60" t="s">
         <v>572</v>
       </c>
+      <c r="H60" s="4" t="s">
+        <v>808</v>
+      </c>
       <c r="I60" t="s">
         <v>146</v>
       </c>
@@ -5455,7 +5811,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:17" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>57</v>
       </c>
@@ -5474,6 +5830,9 @@
       <c r="F61" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H61" s="4" t="s">
+        <v>812</v>
+      </c>
       <c r="I61" t="s">
         <v>117</v>
       </c>
@@ -5493,7 +5852,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -5512,6 +5871,9 @@
       <c r="F62" t="s">
         <v>22</v>
       </c>
+      <c r="H62" t="s">
+        <v>25</v>
+      </c>
       <c r="I62" t="s">
         <v>22</v>
       </c>
@@ -5534,7 +5896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="261.5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -5556,6 +5918,9 @@
       <c r="G63" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="H63" t="s">
+        <v>25</v>
+      </c>
       <c r="I63" t="s">
         <v>22</v>
       </c>
@@ -5581,7 +5946,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>60</v>
       </c>
@@ -5600,6 +5965,9 @@
       <c r="F64" t="s">
         <v>22</v>
       </c>
+      <c r="H64" t="s">
+        <v>25</v>
+      </c>
       <c r="I64" t="s">
         <v>22</v>
       </c>
@@ -5625,7 +5993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="73" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -5644,6 +6012,9 @@
       <c r="F65" t="s">
         <v>22</v>
       </c>
+      <c r="H65" t="s">
+        <v>25</v>
+      </c>
       <c r="I65" t="s">
         <v>22</v>
       </c>
@@ -5669,7 +6040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="261.5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>62</v>
       </c>
@@ -5688,6 +6059,9 @@
       <c r="F66" t="s">
         <v>22</v>
       </c>
+      <c r="H66" t="s">
+        <v>25</v>
+      </c>
       <c r="I66" t="s">
         <v>22</v>
       </c>
@@ -5713,7 +6087,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="247" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>63</v>
       </c>
@@ -5732,6 +6106,9 @@
       <c r="F67" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H67" s="22" t="s">
+        <v>813</v>
+      </c>
       <c r="I67" t="s">
         <v>117</v>
       </c>
@@ -5748,7 +6125,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="189" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>64</v>
       </c>
@@ -5767,6 +6144,9 @@
       <c r="F68" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H68" s="21" t="s">
+        <v>808</v>
+      </c>
       <c r="I68" t="s">
         <v>117</v>
       </c>
@@ -5786,7 +6166,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -5805,6 +6185,9 @@
       <c r="F69" t="s">
         <v>22</v>
       </c>
+      <c r="H69" t="s">
+        <v>25</v>
+      </c>
       <c r="I69" t="s">
         <v>22</v>
       </c>
@@ -5830,7 +6213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>66</v>
       </c>
@@ -5849,6 +6232,9 @@
       <c r="F70" t="s">
         <v>22</v>
       </c>
+      <c r="H70" t="s">
+        <v>25</v>
+      </c>
       <c r="I70" t="s">
         <v>22</v>
       </c>
@@ -5874,7 +6260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="290.5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>67</v>
       </c>
@@ -5893,6 +6279,9 @@
       <c r="F71" t="s">
         <v>22</v>
       </c>
+      <c r="H71" t="s">
+        <v>25</v>
+      </c>
       <c r="I71" t="s">
         <v>22</v>
       </c>
@@ -5918,7 +6307,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="73" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>68</v>
       </c>
@@ -5937,6 +6326,9 @@
       <c r="F72" t="s">
         <v>22</v>
       </c>
+      <c r="H72" t="s">
+        <v>25</v>
+      </c>
       <c r="I72" t="s">
         <v>22</v>
       </c>
@@ -5962,7 +6354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="261.5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>69</v>
       </c>
@@ -5978,6 +6370,9 @@
       <c r="F73" t="s">
         <v>572</v>
       </c>
+      <c r="H73" s="21" t="s">
+        <v>814</v>
+      </c>
       <c r="I73" t="s">
         <v>22</v>
       </c>
@@ -6000,7 +6395,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>70</v>
       </c>
@@ -6016,6 +6411,9 @@
       <c r="F74" t="s">
         <v>572</v>
       </c>
+      <c r="H74" s="21" t="s">
+        <v>815</v>
+      </c>
       <c r="I74" t="s">
         <v>22</v>
       </c>
@@ -6038,7 +6436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="290.5" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>71</v>
       </c>
@@ -6054,6 +6452,9 @@
       <c r="F75" t="s">
         <v>572</v>
       </c>
+      <c r="H75" t="s">
+        <v>816</v>
+      </c>
       <c r="I75" t="s">
         <v>146</v>
       </c>
@@ -6073,7 +6474,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="261.5" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>72</v>
       </c>
@@ -6089,6 +6490,9 @@
       <c r="F76" t="s">
         <v>572</v>
       </c>
+      <c r="H76" t="s">
+        <v>817</v>
+      </c>
       <c r="I76" t="s">
         <v>117</v>
       </c>
@@ -6108,7 +6512,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>73</v>
       </c>
@@ -6124,6 +6528,9 @@
       <c r="F77" t="s">
         <v>22</v>
       </c>
+      <c r="H77" t="s">
+        <v>25</v>
+      </c>
       <c r="I77" t="s">
         <v>22</v>
       </c>
@@ -6149,7 +6556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>74</v>
       </c>
@@ -6165,6 +6572,9 @@
       <c r="F78" t="s">
         <v>22</v>
       </c>
+      <c r="H78" t="s">
+        <v>25</v>
+      </c>
       <c r="I78" t="s">
         <v>22</v>
       </c>
@@ -6190,7 +6600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -6206,6 +6616,9 @@
       <c r="F79" t="s">
         <v>22</v>
       </c>
+      <c r="H79" t="s">
+        <v>25</v>
+      </c>
       <c r="I79" t="s">
         <v>22</v>
       </c>
@@ -6231,7 +6644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>76</v>
       </c>
@@ -6247,6 +6660,9 @@
       <c r="F80" t="s">
         <v>22</v>
       </c>
+      <c r="H80" t="s">
+        <v>25</v>
+      </c>
       <c r="I80" t="s">
         <v>22</v>
       </c>
@@ -6272,7 +6688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>77</v>
       </c>
@@ -6288,6 +6704,9 @@
       <c r="F81" t="s">
         <v>22</v>
       </c>
+      <c r="H81" t="s">
+        <v>25</v>
+      </c>
       <c r="I81" t="s">
         <v>22</v>
       </c>
@@ -6313,7 +6732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>78</v>
       </c>
@@ -6329,6 +6748,9 @@
       <c r="F82" t="s">
         <v>22</v>
       </c>
+      <c r="H82" t="s">
+        <v>25</v>
+      </c>
       <c r="I82" t="s">
         <v>22</v>
       </c>
@@ -6354,7 +6776,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="160" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>79</v>
       </c>
@@ -6370,6 +6792,9 @@
       <c r="F83" t="s">
         <v>117</v>
       </c>
+      <c r="H83" t="s">
+        <v>818</v>
+      </c>
       <c r="I83" t="s">
         <v>22</v>
       </c>
@@ -6392,7 +6817,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="145.5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:17" ht="144" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>80</v>
       </c>
@@ -6411,6 +6836,9 @@
       <c r="F84" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H84" s="4" t="s">
+        <v>819</v>
+      </c>
       <c r="I84" t="s">
         <v>117</v>
       </c>
@@ -6433,7 +6861,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="261.5" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>81</v>
       </c>
@@ -6452,6 +6880,9 @@
       <c r="F85" s="4" t="s">
         <v>572</v>
       </c>
+      <c r="H85" s="4" t="s">
+        <v>820</v>
+      </c>
       <c r="I85" t="s">
         <v>117</v>
       </c>
@@ -6471,7 +6902,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="73" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>82</v>
       </c>
@@ -6490,6 +6921,9 @@
       <c r="F86" t="s">
         <v>572</v>
       </c>
+      <c r="H86" s="4" t="s">
+        <v>821</v>
+      </c>
       <c r="I86" t="s">
         <v>146</v>
       </c>
@@ -6509,7 +6943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="261.5" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>83</v>
       </c>
@@ -6528,6 +6962,9 @@
       <c r="F87" t="s">
         <v>572</v>
       </c>
+      <c r="H87" s="21" t="s">
+        <v>822</v>
+      </c>
       <c r="I87" t="s">
         <v>22</v>
       </c>
@@ -6547,7 +6984,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>84</v>
       </c>
@@ -6563,6 +7000,9 @@
       <c r="F88" t="s">
         <v>22</v>
       </c>
+      <c r="H88" t="s">
+        <v>25</v>
+      </c>
       <c r="I88" t="s">
         <v>22</v>
       </c>
@@ -6588,7 +7028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="319.5" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:17" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>85</v>
       </c>
@@ -6604,6 +7044,9 @@
       <c r="F89" t="s">
         <v>117</v>
       </c>
+      <c r="H89" s="4" t="s">
+        <v>823</v>
+      </c>
       <c r="I89" t="s">
         <v>117</v>
       </c>
@@ -6623,7 +7066,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="218" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:17" ht="216" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>86</v>
       </c>
@@ -6642,6 +7085,9 @@
       <c r="F90" t="s">
         <v>117</v>
       </c>
+      <c r="H90" t="s">
+        <v>824</v>
+      </c>
       <c r="I90" t="s">
         <v>146</v>
       </c>
@@ -6661,7 +7107,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:17" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>87</v>
       </c>
@@ -6677,6 +7123,9 @@
       <c r="F91" t="s">
         <v>572</v>
       </c>
+      <c r="H91" s="21" t="s">
+        <v>825</v>
+      </c>
       <c r="I91" t="s">
         <v>117</v>
       </c>
@@ -6696,7 +7145,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="363" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:17" ht="360" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>88</v>
       </c>
@@ -6715,6 +7164,9 @@
       <c r="F92" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H92" s="21" t="s">
+        <v>826</v>
+      </c>
       <c r="I92" t="s">
         <v>117</v>
       </c>
@@ -6734,7 +7186,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -6750,6 +7202,9 @@
       <c r="F93" t="s">
         <v>22</v>
       </c>
+      <c r="H93" t="s">
+        <v>25</v>
+      </c>
       <c r="I93" t="s">
         <v>22</v>
       </c>
@@ -6775,7 +7230,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>90</v>
       </c>
@@ -6791,6 +7246,9 @@
       <c r="F94" t="s">
         <v>22</v>
       </c>
+      <c r="H94" t="s">
+        <v>25</v>
+      </c>
       <c r="I94" t="s">
         <v>22</v>
       </c>
@@ -6816,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="102" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>91</v>
       </c>
@@ -6832,6 +7290,9 @@
       <c r="F95" t="s">
         <v>572</v>
       </c>
+      <c r="H95" t="s">
+        <v>827</v>
+      </c>
       <c r="K95" t="s">
         <v>32</v>
       </c>
@@ -6848,7 +7309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>92</v>
       </c>
@@ -6864,6 +7325,9 @@
       <c r="F96" t="s">
         <v>572</v>
       </c>
+      <c r="H96" t="s">
+        <v>828</v>
+      </c>
       <c r="K96" t="s">
         <v>32</v>
       </c>
@@ -6880,7 +7344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>93</v>
       </c>
@@ -6896,6 +7360,9 @@
       <c r="F97" t="s">
         <v>22</v>
       </c>
+      <c r="H97" t="s">
+        <v>25</v>
+      </c>
       <c r="K97" t="s">
         <v>23</v>
       </c>
@@ -6918,7 +7385,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>94</v>
       </c>
@@ -6934,6 +7401,9 @@
       <c r="F98" t="s">
         <v>117</v>
       </c>
+      <c r="H98" s="21" t="s">
+        <v>829</v>
+      </c>
       <c r="K98" t="s">
         <v>32</v>
       </c>
@@ -6950,7 +7420,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="131" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>95</v>
       </c>
@@ -6966,6 +7436,9 @@
       <c r="F99" t="s">
         <v>117</v>
       </c>
+      <c r="H99" t="s">
+        <v>830</v>
+      </c>
       <c r="K99" t="s">
         <v>32</v>
       </c>
@@ -6982,7 +7455,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>96</v>
       </c>
@@ -6998,6 +7471,9 @@
       <c r="F100" t="s">
         <v>117</v>
       </c>
+      <c r="H100" s="21" t="s">
+        <v>829</v>
+      </c>
       <c r="K100" t="s">
         <v>32</v>
       </c>
@@ -7014,7 +7490,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>97</v>
       </c>
@@ -7030,6 +7506,9 @@
       <c r="F101" t="s">
         <v>22</v>
       </c>
+      <c r="H101" t="s">
+        <v>25</v>
+      </c>
       <c r="K101" t="s">
         <v>23</v>
       </c>
@@ -7052,7 +7531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>98</v>
       </c>
@@ -7068,6 +7547,9 @@
       <c r="F102" t="s">
         <v>22</v>
       </c>
+      <c r="H102" t="s">
+        <v>25</v>
+      </c>
       <c r="K102" t="s">
         <v>23</v>
       </c>
@@ -7090,7 +7572,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="189" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>99</v>
       </c>
@@ -7106,6 +7588,9 @@
       <c r="F103" t="s">
         <v>117</v>
       </c>
+      <c r="H103" t="s">
+        <v>831</v>
+      </c>
       <c r="K103" t="s">
         <v>32</v>
       </c>
@@ -7122,7 +7607,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:17" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>100</v>
       </c>
@@ -7138,6 +7623,9 @@
       <c r="F104" t="s">
         <v>117</v>
       </c>
+      <c r="H104" s="21" t="s">
+        <v>832</v>
+      </c>
       <c r="K104" t="s">
         <v>32</v>
       </c>
@@ -7154,7 +7642,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="247" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>101</v>
       </c>
@@ -7170,6 +7658,9 @@
       <c r="F105" t="s">
         <v>117</v>
       </c>
+      <c r="H105" s="21" t="s">
+        <v>832</v>
+      </c>
       <c r="K105" t="s">
         <v>32</v>
       </c>
@@ -7186,7 +7677,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>102</v>
       </c>
@@ -7202,6 +7693,9 @@
       <c r="F106" t="s">
         <v>22</v>
       </c>
+      <c r="H106" t="s">
+        <v>25</v>
+      </c>
       <c r="K106" t="s">
         <v>23</v>
       </c>
@@ -7224,7 +7718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="305" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:17" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>103</v>
       </c>
@@ -7240,6 +7734,9 @@
       <c r="F107" t="s">
         <v>117</v>
       </c>
+      <c r="H107" t="s">
+        <v>833</v>
+      </c>
       <c r="K107" t="s">
         <v>32</v>
       </c>
@@ -7256,7 +7753,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="87.5" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>104</v>
       </c>
@@ -7272,6 +7769,9 @@
       <c r="F108" t="s">
         <v>573</v>
       </c>
+      <c r="H108" t="s">
+        <v>25</v>
+      </c>
       <c r="K108" t="s">
         <v>32</v>
       </c>
@@ -7288,7 +7788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="276" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:17" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -7304,6 +7804,9 @@
       <c r="F109" t="s">
         <v>117</v>
       </c>
+      <c r="H109" t="s">
+        <v>25</v>
+      </c>
       <c r="K109" t="s">
         <v>23</v>
       </c>
@@ -7320,7 +7823,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="160" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -7336,6 +7839,9 @@
       <c r="F110" t="s">
         <v>117</v>
       </c>
+      <c r="H110" t="s">
+        <v>25</v>
+      </c>
       <c r="K110" t="s">
         <v>23</v>
       </c>
@@ -7352,7 +7858,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="247" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -7368,6 +7874,9 @@
       <c r="F111" t="s">
         <v>117</v>
       </c>
+      <c r="H111" t="s">
+        <v>834</v>
+      </c>
       <c r="K111" t="s">
         <v>32</v>
       </c>
@@ -7384,7 +7893,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:17" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -7400,6 +7909,9 @@
       <c r="F112" t="s">
         <v>117</v>
       </c>
+      <c r="H112" t="s">
+        <v>25</v>
+      </c>
       <c r="K112" t="s">
         <v>32</v>
       </c>
@@ -7416,7 +7928,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="334" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:17" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -7432,6 +7944,9 @@
       <c r="F113" t="s">
         <v>117</v>
       </c>
+      <c r="H113" t="s">
+        <v>25</v>
+      </c>
       <c r="K113" t="s">
         <v>23</v>
       </c>
@@ -7448,7 +7963,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="319.5" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:17" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -7464,6 +7979,9 @@
       <c r="F114" t="s">
         <v>117</v>
       </c>
+      <c r="H114" s="21" t="s">
+        <v>832</v>
+      </c>
       <c r="K114" t="s">
         <v>32</v>
       </c>
@@ -7480,7 +7998,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="73" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -7496,6 +8014,9 @@
       <c r="F115" t="s">
         <v>117</v>
       </c>
+      <c r="H115" t="s">
+        <v>25</v>
+      </c>
       <c r="K115" t="s">
         <v>32</v>
       </c>
@@ -7510,7 +8031,7 @@
       </c>
       <c r="Q115" s="9"/>
     </row>
-    <row r="116" spans="1:17" ht="32" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>112</v>
       </c>
@@ -7526,6 +8047,9 @@
       <c r="F116" t="s">
         <v>22</v>
       </c>
+      <c r="H116" t="s">
+        <v>25</v>
+      </c>
       <c r="K116" t="s">
         <v>23</v>
       </c>
@@ -7546,7 +8070,7 @@
       </c>
       <c r="Q116" s="9"/>
     </row>
-    <row r="117" spans="1:17" ht="247" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>113</v>
       </c>
@@ -7562,6 +8086,9 @@
       <c r="F117" t="s">
         <v>117</v>
       </c>
+      <c r="H117" t="s">
+        <v>809</v>
+      </c>
       <c r="K117" t="s">
         <v>32</v>
       </c>
@@ -7578,7 +8105,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="189" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>114</v>
       </c>
@@ -7594,6 +8121,9 @@
       <c r="F118" t="s">
         <v>117</v>
       </c>
+      <c r="H118" t="s">
+        <v>809</v>
+      </c>
       <c r="K118" t="s">
         <v>32</v>
       </c>
@@ -7610,7 +8140,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="189" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>115</v>
       </c>
@@ -7626,6 +8156,9 @@
       <c r="F119" t="s">
         <v>117</v>
       </c>
+      <c r="H119" t="s">
+        <v>835</v>
+      </c>
       <c r="K119" t="s">
         <v>32</v>
       </c>
@@ -7642,7 +8175,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="44" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>116</v>
       </c>
@@ -7658,6 +8191,9 @@
       <c r="F120" t="s">
         <v>22</v>
       </c>
+      <c r="H120" t="s">
+        <v>25</v>
+      </c>
       <c r="K120" t="s">
         <v>23</v>
       </c>
@@ -7680,7 +8216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>117</v>
       </c>
@@ -7696,6 +8232,9 @@
       <c r="F121" t="s">
         <v>22</v>
       </c>
+      <c r="H121" t="s">
+        <v>25</v>
+      </c>
       <c r="K121" t="s">
         <v>23</v>
       </c>
@@ -7718,7 +8257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>118</v>
       </c>
@@ -7734,6 +8273,9 @@
       <c r="F122" t="s">
         <v>22</v>
       </c>
+      <c r="H122" t="s">
+        <v>25</v>
+      </c>
       <c r="K122" t="s">
         <v>23</v>
       </c>
@@ -7756,7 +8298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>119</v>
       </c>
@@ -7772,6 +8314,9 @@
       <c r="F123" t="s">
         <v>22</v>
       </c>
+      <c r="H123" t="s">
+        <v>25</v>
+      </c>
       <c r="K123" t="s">
         <v>23</v>
       </c>
@@ -7794,7 +8339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>120</v>
       </c>
@@ -7810,6 +8355,9 @@
       <c r="F124" t="s">
         <v>573</v>
       </c>
+      <c r="H124" t="s">
+        <v>25</v>
+      </c>
       <c r="K124" t="s">
         <v>23</v>
       </c>
@@ -7826,7 +8374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>121</v>
       </c>
@@ -7842,6 +8390,9 @@
       <c r="F125" t="s">
         <v>22</v>
       </c>
+      <c r="H125" t="s">
+        <v>25</v>
+      </c>
       <c r="K125" t="s">
         <v>23</v>
       </c>
@@ -7864,7 +8415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="126" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>122</v>
       </c>
@@ -7880,6 +8431,9 @@
       <c r="F126" t="s">
         <v>22</v>
       </c>
+      <c r="H126" t="s">
+        <v>25</v>
+      </c>
       <c r="K126" t="s">
         <v>23</v>
       </c>
@@ -7902,7 +8456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>123</v>
       </c>
@@ -7918,6 +8472,9 @@
       <c r="F127" t="s">
         <v>117</v>
       </c>
+      <c r="H127" t="s">
+        <v>25</v>
+      </c>
       <c r="K127" t="s">
         <v>23</v>
       </c>
@@ -7934,7 +8491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>124</v>
       </c>
@@ -7950,6 +8507,9 @@
       <c r="F128" t="s">
         <v>573</v>
       </c>
+      <c r="H128" t="s">
+        <v>25</v>
+      </c>
       <c r="K128" t="s">
         <v>23</v>
       </c>
@@ -7966,7 +8526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="87" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>125</v>
       </c>
@@ -7982,6 +8542,9 @@
       <c r="F129" t="s">
         <v>22</v>
       </c>
+      <c r="H129" t="s">
+        <v>25</v>
+      </c>
       <c r="K129" t="s">
         <v>23</v>
       </c>
@@ -8004,7 +8567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>126</v>
       </c>
@@ -8020,6 +8583,9 @@
       <c r="F130" t="s">
         <v>573</v>
       </c>
+      <c r="H130" s="21" t="s">
+        <v>836</v>
+      </c>
       <c r="M130" s="2" t="s">
         <v>765</v>
       </c>
@@ -8033,7 +8599,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>127</v>
       </c>
@@ -8049,6 +8615,9 @@
       <c r="F131" t="s">
         <v>22</v>
       </c>
+      <c r="H131" t="s">
+        <v>25</v>
+      </c>
       <c r="K131" t="s">
         <v>23</v>
       </c>
@@ -8071,7 +8640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>128</v>
       </c>
@@ -8087,6 +8656,9 @@
       <c r="F132" t="s">
         <v>22</v>
       </c>
+      <c r="H132" t="s">
+        <v>25</v>
+      </c>
       <c r="K132" t="s">
         <v>23</v>
       </c>
@@ -8109,7 +8681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>129</v>
       </c>
@@ -8125,6 +8697,9 @@
       <c r="F133" t="s">
         <v>22</v>
       </c>
+      <c r="H133" t="s">
+        <v>25</v>
+      </c>
       <c r="K133" t="s">
         <v>23</v>
       </c>
@@ -8147,7 +8722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>130</v>
       </c>
@@ -8163,6 +8738,9 @@
       <c r="F134" t="s">
         <v>22</v>
       </c>
+      <c r="H134" t="s">
+        <v>25</v>
+      </c>
       <c r="K134" t="s">
         <v>23</v>
       </c>
@@ -8185,7 +8763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:18" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>131</v>
       </c>
@@ -8201,6 +8779,9 @@
       <c r="F135" t="s">
         <v>573</v>
       </c>
+      <c r="H135" t="s">
+        <v>25</v>
+      </c>
       <c r="K135" t="s">
         <v>32</v>
       </c>
@@ -8217,7 +8798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="145.5" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:18" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>132</v>
       </c>
@@ -8233,6 +8814,9 @@
       <c r="F136" t="s">
         <v>573</v>
       </c>
+      <c r="H136" t="s">
+        <v>25</v>
+      </c>
       <c r="K136" t="s">
         <v>32</v>
       </c>
@@ -8249,7 +8833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="44" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>133</v>
       </c>
@@ -8265,6 +8849,9 @@
       <c r="F137" t="s">
         <v>22</v>
       </c>
+      <c r="H137" t="s">
+        <v>25</v>
+      </c>
       <c r="K137" t="s">
         <v>23</v>
       </c>
@@ -8287,7 +8874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="32" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>134</v>
       </c>
@@ -8303,6 +8890,9 @@
       <c r="F138" t="s">
         <v>22</v>
       </c>
+      <c r="H138" t="s">
+        <v>25</v>
+      </c>
       <c r="K138" t="s">
         <v>23</v>
       </c>
@@ -8325,7 +8915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="232.5" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>135</v>
       </c>
@@ -8341,6 +8931,9 @@
       <c r="F139" t="s">
         <v>117</v>
       </c>
+      <c r="H139" s="21" t="s">
+        <v>837</v>
+      </c>
       <c r="K139" t="s">
         <v>32</v>
       </c>
@@ -8357,7 +8950,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>136</v>
       </c>
@@ -8373,6 +8966,9 @@
       <c r="F140" t="s">
         <v>22</v>
       </c>
+      <c r="H140" t="s">
+        <v>25</v>
+      </c>
       <c r="K140" t="s">
         <v>23</v>
       </c>
@@ -8395,7 +8991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>137</v>
       </c>
@@ -8411,6 +9007,9 @@
       <c r="F141" t="s">
         <v>22</v>
       </c>
+      <c r="H141" t="s">
+        <v>25</v>
+      </c>
       <c r="K141" t="s">
         <v>23</v>
       </c>
@@ -8433,7 +9032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="261" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:18" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>138</v>
       </c>
@@ -8452,6 +9051,9 @@
       <c r="F142" s="4" t="s">
         <v>572</v>
       </c>
+      <c r="H142" s="4" t="s">
+        <v>838</v>
+      </c>
       <c r="K142" t="s">
         <v>32</v>
       </c>
@@ -8471,7 +9073,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>139</v>
       </c>
@@ -8490,6 +9092,9 @@
       <c r="F143" t="s">
         <v>22</v>
       </c>
+      <c r="H143" t="s">
+        <v>25</v>
+      </c>
       <c r="K143" t="s">
         <v>23</v>
       </c>
@@ -8510,7 +9115,7 @@
       </c>
       <c r="Q143" s="9"/>
     </row>
-    <row r="144" spans="1:18" ht="319" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:18" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>140</v>
       </c>
@@ -8526,6 +9131,9 @@
       <c r="F144" t="s">
         <v>572</v>
       </c>
+      <c r="H144" t="s">
+        <v>838</v>
+      </c>
       <c r="K144" t="s">
         <v>32</v>
       </c>
@@ -8542,7 +9150,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="261" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>141</v>
       </c>
@@ -8558,6 +9166,9 @@
       <c r="F145" t="s">
         <v>572</v>
       </c>
+      <c r="H145" t="s">
+        <v>838</v>
+      </c>
       <c r="K145" t="s">
         <v>32</v>
       </c>
@@ -8574,7 +9185,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="261" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>142</v>
       </c>
@@ -8590,6 +9201,9 @@
       <c r="F146" t="s">
         <v>572</v>
       </c>
+      <c r="H146" t="s">
+        <v>838</v>
+      </c>
       <c r="K146" t="s">
         <v>32</v>
       </c>
@@ -8606,7 +9220,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="261" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>143</v>
       </c>
@@ -8622,6 +9236,9 @@
       <c r="F147" t="s">
         <v>572</v>
       </c>
+      <c r="H147" t="s">
+        <v>838</v>
+      </c>
       <c r="K147" t="s">
         <v>32</v>
       </c>
@@ -8638,7 +9255,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>144</v>
       </c>
@@ -8654,6 +9271,9 @@
       <c r="F148" t="s">
         <v>22</v>
       </c>
+      <c r="H148" t="s">
+        <v>838</v>
+      </c>
       <c r="K148" t="s">
         <v>23</v>
       </c>
@@ -8676,7 +9296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>145</v>
       </c>
@@ -8692,6 +9312,9 @@
       <c r="F149" t="s">
         <v>22</v>
       </c>
+      <c r="H149" t="s">
+        <v>838</v>
+      </c>
       <c r="K149" t="s">
         <v>23</v>
       </c>
@@ -8714,7 +9337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="261" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>146</v>
       </c>
@@ -8730,6 +9353,9 @@
       <c r="F150" t="s">
         <v>572</v>
       </c>
+      <c r="H150" t="s">
+        <v>838</v>
+      </c>
       <c r="K150" t="s">
         <v>32</v>
       </c>
@@ -8746,7 +9372,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>147</v>
       </c>
@@ -8762,6 +9388,9 @@
       <c r="F151" t="s">
         <v>572</v>
       </c>
+      <c r="H151" t="s">
+        <v>838</v>
+      </c>
       <c r="K151" t="s">
         <v>32</v>
       </c>
@@ -8778,7 +9407,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>148</v>
       </c>
@@ -8794,6 +9423,9 @@
       <c r="F152" t="s">
         <v>22</v>
       </c>
+      <c r="H152" t="s">
+        <v>25</v>
+      </c>
       <c r="K152" t="s">
         <v>23</v>
       </c>
@@ -8816,7 +9448,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>149</v>
       </c>
@@ -8832,6 +9464,9 @@
       <c r="F153" t="s">
         <v>22</v>
       </c>
+      <c r="H153" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K153" t="s">
         <v>23</v>
       </c>
@@ -8854,7 +9489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="261" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>150</v>
       </c>
@@ -8866,6 +9501,9 @@
       </c>
       <c r="D154" s="4" t="s">
         <v>380</v>
+      </c>
+      <c r="H154" s="23" t="s">
+        <v>839</v>
       </c>
       <c r="K154" t="s">
         <v>32</v>
@@ -8887,7 +9525,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>151</v>
       </c>
@@ -8903,6 +9541,9 @@
       <c r="F155" t="s">
         <v>117</v>
       </c>
+      <c r="H155" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K155" t="s">
         <v>32</v>
       </c>
@@ -8919,7 +9560,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>152</v>
       </c>
@@ -8935,6 +9576,9 @@
       <c r="F156" t="s">
         <v>22</v>
       </c>
+      <c r="H156" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K156" t="s">
         <v>23</v>
       </c>
@@ -8957,7 +9601,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>153</v>
       </c>
@@ -8973,6 +9617,9 @@
       <c r="F157" t="s">
         <v>22</v>
       </c>
+      <c r="H157" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K157" t="s">
         <v>23</v>
       </c>
@@ -8995,7 +9642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>154</v>
       </c>
@@ -9011,6 +9658,9 @@
       <c r="F158" t="s">
         <v>22</v>
       </c>
+      <c r="H158" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K158" t="s">
         <v>23</v>
       </c>
@@ -9033,7 +9683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>155</v>
       </c>
@@ -9049,6 +9699,9 @@
       <c r="F159" t="s">
         <v>22</v>
       </c>
+      <c r="H159" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K159" t="s">
         <v>23</v>
       </c>
@@ -9071,7 +9724,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>156</v>
       </c>
@@ -9087,6 +9740,9 @@
       <c r="F160" t="s">
         <v>22</v>
       </c>
+      <c r="H160" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K160" t="s">
         <v>23</v>
       </c>
@@ -9109,7 +9765,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>157</v>
       </c>
@@ -9125,6 +9781,9 @@
       <c r="F161" t="s">
         <v>22</v>
       </c>
+      <c r="H161" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K161" t="s">
         <v>23</v>
       </c>
@@ -9147,7 +9806,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>158</v>
       </c>
@@ -9163,6 +9822,9 @@
       <c r="F162" t="s">
         <v>117</v>
       </c>
+      <c r="H162" s="24" t="s">
+        <v>840</v>
+      </c>
       <c r="K162" t="s">
         <v>32</v>
       </c>
@@ -9179,7 +9841,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>159</v>
       </c>
@@ -9195,6 +9857,9 @@
       <c r="F163" t="s">
         <v>22</v>
       </c>
+      <c r="H163" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K163" t="s">
         <v>23</v>
       </c>
@@ -9217,7 +9882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>160</v>
       </c>
@@ -9233,6 +9898,9 @@
       <c r="F164" s="2" t="s">
         <v>574</v>
       </c>
+      <c r="H164" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K164" t="s">
         <v>23</v>
       </c>
@@ -9249,7 +9917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>161</v>
       </c>
@@ -9265,6 +9933,9 @@
       <c r="F165" t="s">
         <v>572</v>
       </c>
+      <c r="H165" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K165" t="s">
         <v>23</v>
       </c>
@@ -9281,7 +9952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>162</v>
       </c>
@@ -9297,6 +9968,9 @@
       <c r="F166" t="s">
         <v>22</v>
       </c>
+      <c r="H166" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K166" t="s">
         <v>23</v>
       </c>
@@ -9319,7 +9993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>163</v>
       </c>
@@ -9335,6 +10009,9 @@
       <c r="F167" t="s">
         <v>22</v>
       </c>
+      <c r="H167" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K167" t="s">
         <v>23</v>
       </c>
@@ -9351,7 +10028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>164</v>
       </c>
@@ -9367,6 +10044,9 @@
       <c r="F168" t="s">
         <v>22</v>
       </c>
+      <c r="H168" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K168" t="s">
         <v>23</v>
       </c>
@@ -9383,7 +10063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>165</v>
       </c>
@@ -9399,6 +10079,9 @@
       <c r="F169" t="s">
         <v>22</v>
       </c>
+      <c r="H169" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K169" t="s">
         <v>23</v>
       </c>
@@ -9421,7 +10104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>166</v>
       </c>
@@ -9437,6 +10120,9 @@
       <c r="F170" t="s">
         <v>22</v>
       </c>
+      <c r="H170" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K170" t="s">
         <v>23</v>
       </c>
@@ -9459,7 +10145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>167</v>
       </c>
@@ -9475,6 +10161,9 @@
       <c r="F171" t="s">
         <v>22</v>
       </c>
+      <c r="H171" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K171" t="s">
         <v>23</v>
       </c>
@@ -9497,7 +10186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>168</v>
       </c>
@@ -9513,6 +10202,9 @@
       <c r="F172" t="s">
         <v>22</v>
       </c>
+      <c r="H172" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K172" t="s">
         <v>23</v>
       </c>
@@ -9535,7 +10227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>169</v>
       </c>
@@ -9551,6 +10243,9 @@
       <c r="F173" t="s">
         <v>22</v>
       </c>
+      <c r="H173" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K173" t="s">
         <v>23</v>
       </c>
@@ -9573,7 +10268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>170</v>
       </c>
@@ -9589,6 +10284,9 @@
       <c r="F174" t="s">
         <v>22</v>
       </c>
+      <c r="H174" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K174" t="s">
         <v>23</v>
       </c>
@@ -9611,7 +10309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="116" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>171</v>
       </c>
@@ -9627,6 +10325,9 @@
       <c r="F175" t="s">
         <v>117</v>
       </c>
+      <c r="H175" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K175" t="s">
         <v>32</v>
       </c>
@@ -9643,7 +10344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="116" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>172</v>
       </c>
@@ -9659,6 +10360,9 @@
       <c r="F176" t="s">
         <v>117</v>
       </c>
+      <c r="H176" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K176" t="s">
         <v>203</v>
       </c>
@@ -9675,7 +10379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="116" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>173</v>
       </c>
@@ -9691,6 +10395,9 @@
       <c r="F177" t="s">
         <v>117</v>
       </c>
+      <c r="H177" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K177" t="s">
         <v>203</v>
       </c>
@@ -9707,7 +10414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>174</v>
       </c>
@@ -9723,6 +10430,9 @@
       <c r="F178" t="s">
         <v>22</v>
       </c>
+      <c r="H178" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K178" t="s">
         <v>32</v>
       </c>
@@ -9739,7 +10449,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>175</v>
       </c>
@@ -9755,6 +10465,9 @@
       <c r="F179" t="s">
         <v>22</v>
       </c>
+      <c r="H179" s="23" t="s">
+        <v>805</v>
+      </c>
       <c r="K179" t="s">
         <v>23</v>
       </c>
@@ -9777,7 +10490,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>176</v>
       </c>
@@ -9793,6 +10506,9 @@
       <c r="F180" t="s">
         <v>117</v>
       </c>
+      <c r="H180" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K180" t="s">
         <v>32</v>
       </c>
@@ -9809,7 +10525,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="290.5" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>177</v>
       </c>
@@ -9825,6 +10541,9 @@
       <c r="F181" t="s">
         <v>572</v>
       </c>
+      <c r="H181" s="24" t="s">
+        <v>841</v>
+      </c>
       <c r="K181" t="s">
         <v>32</v>
       </c>
@@ -9838,7 +10557,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>178</v>
       </c>
@@ -9854,6 +10573,9 @@
       <c r="F182" t="s">
         <v>22</v>
       </c>
+      <c r="H182" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K182" t="s">
         <v>23</v>
       </c>
@@ -9876,7 +10598,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>179</v>
       </c>
@@ -9892,6 +10614,9 @@
       <c r="F183" t="s">
         <v>22</v>
       </c>
+      <c r="H183" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K183" t="s">
         <v>23</v>
       </c>
@@ -9914,7 +10639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>180</v>
       </c>
@@ -9930,6 +10655,9 @@
       <c r="F184" t="s">
         <v>22</v>
       </c>
+      <c r="H184" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K184" t="s">
         <v>23</v>
       </c>
@@ -9952,7 +10680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>181</v>
       </c>
@@ -9968,6 +10696,9 @@
       <c r="F185" t="s">
         <v>22</v>
       </c>
+      <c r="H185" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K185" t="s">
         <v>23</v>
       </c>
@@ -9990,7 +10721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>182</v>
       </c>
@@ -10006,6 +10737,9 @@
       <c r="F186" t="s">
         <v>22</v>
       </c>
+      <c r="H186" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K186" t="s">
         <v>23</v>
       </c>
@@ -10028,7 +10762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>183</v>
       </c>
@@ -10044,6 +10778,9 @@
       <c r="F187" t="s">
         <v>22</v>
       </c>
+      <c r="H187" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K187" t="s">
         <v>23</v>
       </c>
@@ -10066,7 +10803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>184</v>
       </c>
@@ -10082,6 +10819,9 @@
       <c r="F188" t="s">
         <v>22</v>
       </c>
+      <c r="H188" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K188" t="s">
         <v>23</v>
       </c>
@@ -10104,7 +10844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>185</v>
       </c>
@@ -10120,6 +10860,9 @@
       <c r="F189" t="s">
         <v>22</v>
       </c>
+      <c r="H189" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K189" t="s">
         <v>23</v>
       </c>
@@ -10142,7 +10885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>186</v>
       </c>
@@ -10158,6 +10901,9 @@
       <c r="F190" t="s">
         <v>22</v>
       </c>
+      <c r="H190" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K190" t="s">
         <v>23</v>
       </c>
@@ -10180,7 +10926,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>187</v>
       </c>
@@ -10196,6 +10942,9 @@
       <c r="F191" t="s">
         <v>22</v>
       </c>
+      <c r="H191" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K191" t="s">
         <v>23</v>
       </c>
@@ -10218,7 +10967,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>188</v>
       </c>
@@ -10234,6 +10983,9 @@
       <c r="F192" t="s">
         <v>22</v>
       </c>
+      <c r="H192" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K192" t="s">
         <v>23</v>
       </c>
@@ -10256,7 +11008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>189</v>
       </c>
@@ -10272,6 +11024,9 @@
       <c r="F193" t="s">
         <v>22</v>
       </c>
+      <c r="H193" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K193" t="s">
         <v>23</v>
       </c>
@@ -10294,7 +11049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>190</v>
       </c>
@@ -10310,6 +11065,9 @@
       <c r="F194" t="s">
         <v>22</v>
       </c>
+      <c r="H194" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K194" t="s">
         <v>23</v>
       </c>
@@ -10332,7 +11090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="218" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:18" ht="216" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>191</v>
       </c>
@@ -10351,6 +11109,9 @@
       <c r="F195" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="H195" s="25" t="s">
+        <v>836</v>
+      </c>
       <c r="K195" t="s">
         <v>32</v>
       </c>
@@ -10367,7 +11128,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="196" spans="1:18" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>192</v>
       </c>
@@ -10383,6 +11144,9 @@
       <c r="F196" t="s">
         <v>22</v>
       </c>
+      <c r="H196" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K196" t="s">
         <v>23</v>
       </c>
@@ -10405,7 +11169,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:18" ht="16" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>193</v>
       </c>
@@ -10421,6 +11185,9 @@
       <c r="F197" t="s">
         <v>22</v>
       </c>
+      <c r="H197" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K197" t="s">
         <v>23</v>
       </c>
@@ -10443,7 +11210,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>194</v>
       </c>
@@ -10459,6 +11226,9 @@
       <c r="F198" t="s">
         <v>22</v>
       </c>
+      <c r="H198" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K198" t="s">
         <v>23</v>
       </c>
@@ -10481,7 +11251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="203.5" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:18" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>195</v>
       </c>
@@ -10497,6 +11267,9 @@
       <c r="F199" t="s">
         <v>22</v>
       </c>
+      <c r="H199" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K199" t="s">
         <v>23</v>
       </c>
@@ -10519,7 +11292,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="200" spans="1:18" ht="16" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>196</v>
       </c>
@@ -10535,6 +11308,9 @@
       <c r="F200" t="s">
         <v>22</v>
       </c>
+      <c r="H200" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K200" t="s">
         <v>23</v>
       </c>
@@ -10557,7 +11333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:18" ht="16" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>197</v>
       </c>
@@ -10573,6 +11349,9 @@
       <c r="F201" t="s">
         <v>22</v>
       </c>
+      <c r="H201" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K201" t="s">
         <v>23</v>
       </c>
@@ -10595,7 +11374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:18" ht="16" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>198</v>
       </c>
@@ -10611,6 +11390,9 @@
       <c r="F202" t="s">
         <v>22</v>
       </c>
+      <c r="H202" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K202" t="s">
         <v>23</v>
       </c>
@@ -10633,7 +11415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="203" spans="1:18" ht="16" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>199</v>
       </c>
@@ -10649,6 +11431,9 @@
       <c r="F203" t="s">
         <v>22</v>
       </c>
+      <c r="H203" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K203" t="s">
         <v>23</v>
       </c>
@@ -10671,7 +11456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="204" spans="1:18" ht="232.5" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>200</v>
       </c>
@@ -10687,6 +11472,9 @@
       <c r="F204" t="s">
         <v>117</v>
       </c>
+      <c r="H204" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K204" t="s">
         <v>32</v>
       </c>
@@ -10703,7 +11491,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>201</v>
       </c>
@@ -10719,6 +11507,9 @@
       <c r="F205" t="s">
         <v>22</v>
       </c>
+      <c r="H205" s="23" t="s">
+        <v>842</v>
+      </c>
       <c r="K205" t="s">
         <v>23</v>
       </c>
@@ -10741,7 +11532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="206" spans="1:18" ht="232.5" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>202</v>
       </c>
@@ -10757,6 +11548,9 @@
       <c r="F206" t="s">
         <v>22</v>
       </c>
+      <c r="H206" s="23" t="s">
+        <v>822</v>
+      </c>
       <c r="K206" t="s">
         <v>23</v>
       </c>
@@ -10779,7 +11573,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="207" spans="1:18" ht="276" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:18" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>203</v>
       </c>
@@ -10795,6 +11589,9 @@
       <c r="F207" t="s">
         <v>22</v>
       </c>
+      <c r="H207" s="23" t="s">
+        <v>843</v>
+      </c>
       <c r="K207" t="s">
         <v>23</v>
       </c>
@@ -10820,7 +11617,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="208" spans="1:18" ht="145.5" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:18" ht="144" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>204</v>
       </c>
@@ -10842,6 +11639,9 @@
       <c r="G208" s="4" t="s">
         <v>503</v>
       </c>
+      <c r="H208" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="K208" t="s">
         <v>504</v>
       </c>
@@ -10858,7 +11658,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="209" spans="1:18" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:18" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>205</v>
       </c>
@@ -10877,6 +11677,9 @@
       <c r="F209" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H209" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="K209" t="s">
         <v>510</v>
       </c>
@@ -10893,7 +11696,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="210" spans="1:18" ht="131" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:18" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>206</v>
       </c>
@@ -10909,6 +11712,9 @@
       <c r="F210" t="s">
         <v>117</v>
       </c>
+      <c r="H210" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K210" t="s">
         <v>23</v>
       </c>
@@ -10928,7 +11734,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="174.5" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:18" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>207</v>
       </c>
@@ -10944,6 +11750,9 @@
       <c r="F211" t="s">
         <v>117</v>
       </c>
+      <c r="H211" s="23" t="s">
+        <v>839</v>
+      </c>
       <c r="K211" t="s">
         <v>510</v>
       </c>
@@ -10960,7 +11769,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="377.5" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:18" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>208</v>
       </c>
@@ -10979,6 +11788,9 @@
       <c r="F212" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H212" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="K212" t="s">
         <v>524</v>
       </c>
@@ -10995,7 +11807,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="213" spans="1:18" ht="102" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>209</v>
       </c>
@@ -11017,6 +11829,9 @@
       <c r="G213" s="4" t="s">
         <v>503</v>
       </c>
+      <c r="H213" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="K213" t="s">
         <v>529</v>
       </c>
@@ -11033,7 +11848,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A214" s="3">
         <v>210</v>
       </c>
@@ -11052,6 +11867,9 @@
       <c r="F214" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H214" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="K214" t="s">
         <v>535</v>
       </c>
@@ -11068,7 +11886,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="160" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:18" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A215" s="3">
         <v>211</v>
       </c>
@@ -11084,6 +11902,9 @@
       <c r="F215" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H215" s="26" t="s">
+        <v>839</v>
+      </c>
       <c r="K215" t="s">
         <v>538</v>
       </c>
@@ -11103,7 +11924,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="3">
         <v>212</v>
       </c>
@@ -11119,6 +11940,9 @@
       <c r="F216" t="s">
         <v>22</v>
       </c>
+      <c r="H216" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K216" t="s">
         <v>23</v>
       </c>
@@ -11139,7 +11963,7 @@
       </c>
       <c r="Q216" s="9"/>
     </row>
-    <row r="217" spans="1:18" ht="16" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="3">
         <v>213</v>
       </c>
@@ -11155,6 +11979,9 @@
       <c r="F217" t="s">
         <v>22</v>
       </c>
+      <c r="H217" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K217" t="s">
         <v>23</v>
       </c>
@@ -11175,7 +12002,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:18" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A218" s="3">
         <v>214</v>
       </c>
@@ -11191,6 +12018,9 @@
       <c r="F218" t="s">
         <v>22</v>
       </c>
+      <c r="H218" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K218" t="s">
         <v>23</v>
       </c>
@@ -11211,7 +12041,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:18" ht="174.5" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:18" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A219" s="3">
         <v>215</v>
       </c>
@@ -11227,6 +12057,9 @@
       <c r="F219" t="s">
         <v>117</v>
       </c>
+      <c r="H219" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K219" t="s">
         <v>547</v>
       </c>
@@ -11243,7 +12076,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="116.5" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A220" s="3">
         <v>216</v>
       </c>
@@ -11259,6 +12092,9 @@
       <c r="F220" t="s">
         <v>117</v>
       </c>
+      <c r="H220" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="K220" t="s">
         <v>547</v>
       </c>
@@ -11275,7 +12111,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="131" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:18" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A221" s="3">
         <v>217</v>
       </c>
@@ -11294,6 +12130,9 @@
       <c r="F221" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H221" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="K221" t="s">
         <v>557</v>
       </c>
@@ -11313,7 +12152,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="174.5" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:18" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A222" s="3">
         <v>218</v>
       </c>
@@ -11332,6 +12171,9 @@
       <c r="F222" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H222" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="K222" t="s">
         <v>547</v>
       </c>
@@ -11348,7 +12190,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="160" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:18" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A223" s="3">
         <v>219</v>
       </c>
@@ -11367,6 +12209,9 @@
       <c r="F223" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="H223" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="K223" t="s">
         <v>565</v>
       </c>
@@ -11383,7 +12228,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="224" spans="1:18" ht="232.5" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A224" s="3">
         <v>220</v>
       </c>
@@ -11399,6 +12244,9 @@
       <c r="F224" t="s">
         <v>117</v>
       </c>
+      <c r="H224" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="K224" t="s">
         <v>569</v>
       </c>
@@ -11415,12 +12263,12 @@
         <v>570</v>
       </c>
     </row>
-    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" spans="18:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R230" t="s">
         <v>571</v>
       </c>

</xml_diff>